<commit_message>
Updating v3 of webapp with modified taxonomy, asr output panel and severity scaling
</commit_message>
<xml_diff>
--- a/annotation_tool/selected_sessions_normalized.xlsx
+++ b/annotation_tool/selected_sessions_normalized.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AB4"/>
+  <dimension ref="A1:AM4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,286 +461,474 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Phi-4-ASR</t>
+          <t>phi4-asr</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Whisper-ASR</t>
+          <t>whisper-asr</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
+          <t>nvidia-parakeet-asr</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
           <t>norm_human_transcript</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>norm_whisper_asr</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>norm_phi4_asr</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>norm_parakeet_asr</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>norm_whisper_asr_wer</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>norm_whisper_asr_ins</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>norm_whisper_asr_del</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>norm_whisper_asr_sub</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>norm_phi4_asr_wer</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>norm_phi4_asr_ins</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>norm_phi4_asr_del</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>norm_phi4_asr_sub</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>norm_whisper_asr_Deletions</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>norm_whisper_asr_Insertions</t>
-        </is>
-      </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>norm_whisper_asr_Substitutions</t>
+          <t>norm_parakeet_asr_wer</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>norm_phi4_asr_Deletions</t>
+          <t>norm_parakeet_asr_ins</t>
         </is>
       </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
-          <t>norm_phi4_asr_Insertions</t>
+          <t>norm_parakeet_asr_del</t>
         </is>
       </c>
       <c r="X1" s="1" t="inlineStr">
         <is>
-          <t>norm_phi4_asr_Substitutions</t>
+          <t>norm_parakeet_asr_sub</t>
         </is>
       </c>
       <c r="Y1" s="1" t="inlineStr">
         <is>
+          <t>norm_whisper_asr_deletions</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>norm_whisper_asr_insertions</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>norm_whisper_asr_substitutions</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>norm_phi4_asr_deletions</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>norm_phi4_asr_insertions</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>norm_phi4_asr_substitutions</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>norm_parakeet_asr_deletions</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>norm_parakeet_asr_insertions</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>norm_parakeet_asr_substitutions</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
           <t>whisper_aligned_df</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>phi4_aligned_df</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>parakeet_aligned_df</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>whisper_reconstructed_ref</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>phi4_reconstructed_ref</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>parakeet_reconstructed_ref</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>day4_consultation07</t>
+          <t>46aacf84-fdd1-490b-a857-633d2e7763a0_7d4de4c9d3488a4bbd35634cbd3a2b66_l1RjPEwA</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>data/final_audio/day4_consultation07_stereo.wav</t>
+          <t>data/final_audio/46aacf84-fdd1-490b-a857-633d2e7763a0_7d4de4c9d3488a4bbd35634cbd3a2b66_l1RjPEwA.wav</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>DOCTOR: Hello. Can you hear me OK? PATIENT: &lt;UNSURE&gt;Ohh&lt;/UNSURE&gt; yes, I can. Can you hear me? DOCTOR: Yeah, good, good. So, my name is Joe. I'm a doctor, um, here &lt;UNSURE&gt;at&lt;/UNSURE&gt; Babylon. Can I just confirm your name, please? PATIENT: &lt;UNSURE&gt;Uh&lt;/UNSURE&gt;, my name's Vincent. DOCTOR: And, your date of birth? PATIENT: Uh. PATIENT: Uh, ninth of May, two thousand and sixteen. DOCTOR: OK, great. PATIENT: &lt;INAUDIBLE_SPEECH/&gt; DOCTOR: And are you in a, uh, a safe place, ohh sorry, a safe and &lt;UNIN/&gt;, confidential place to talk and just, &lt;INAUDIBLE_SPEECH/&gt; happy to go ahead with the consultation? PATIENT: &lt;UNSURE&gt;Yeah. Yeah&lt;/UNSURE&gt;, I am. PATIENT: Yes, yes I am. DOCTOR: Great. So, how can I help? PATIENT: Yeah, so, &lt;UNSURE&gt;have a&lt;/UNSURE&gt; &lt;INAUDIBLE_SPEECH/&gt;. I've been having a cough and a sore throat, for about a week, and, it's been causing me problems. I've had to stay away from work, for about three or four of those days, because of how bad &lt;UNSURE&gt;is&lt;/UNSURE&gt;. DOCTOR: OK, I'm sorry to hear that. So, you've had a cough, and a sore throat, for about a week? DOCTOR: And what came, what, what came first? PATIENT: Yes. PATIENT: Uh, the, sore throat came first, and then, after a day or two, the cough. DOCTOR: OK, OK. And, uh, are you &lt;UNSURE&gt;coughing&lt;/UNSURE&gt; up anything? PATIENT: No, it's very dry. DOCTOR: OK, So I'm, I'm just gonna ask a few questions about the, uh, your current symptoms. And a little bit about your background. DOCTOR: Um, and, something else about what we can do, a little bit later on in the consultation, to help you. So, before we go on. &lt;UNIN/&gt; anything you're particularly concerned about? Um, or have any ideas, what might be going on? You said that you had a cold. PATIENT: &lt;UNSURE&gt;OK&lt;/UNSURE&gt;. PATIENT: &lt;UNIN/&gt;, well. PATIENT: I mean, you &lt;UNIN/&gt;, you know how, we all are. Once this happens, you Google it and, there seems to be, all kinds of bad things it could be. It could be, could be a cold or, flu obviously, but it could also be tuberculosis. It &lt;UNSURE&gt;could&lt;/UNSURE&gt; be, cancer always comes up so. PATIENT: &lt;UNSURE&gt;It'll&lt;/UNSURE&gt; be good if, none of those. DOCTOR: Great, so, so yeah. I can provide a bit of reassurance, um, and uh, we can talk about those a little bit, as well. And was &lt;UNSURE&gt;there anything&lt;/UNSURE&gt; you were particularly expecting, or hoping to get out of this consultation? Um. PATIENT: OK. PATIENT: Uh. &lt;UNSURE&gt;Uh&lt;/UNSURE&gt;, well, uh yeah, so reassurance. So like, hopefully some sense that it's not anything too serious. But also, &lt;UNSURE&gt;is there&lt;/UNSURE&gt; anything you can prescribe me to make it better? Or any advice? PATIENT: Or maybe even a sick note. So that, if I need to stay away from work for a bit longer, I can get one. DOCTOR: Sure, sure, OK. All right, so, we'll talk a little bit about the symptoms, and I'm sure we can &lt;UNIN/&gt;, get a, um, those things, uh, &lt;INAUDIBLE_SPEECH/&gt; and some reassurance, um, about your concerns. PATIENT: &lt;UNSURE&gt;OK&lt;/UNSURE&gt;. DOCTOR: So, um, you mentioned that you started with sore throat about a week ago, developed into bit of a dry cough. Um, &lt;UNIN/&gt;, I'll just ask a few questions around those. So, um, do you have any shortness of breath? PATIENT: &lt;UNSURE&gt;No&lt;/UNSURE&gt;. PATIENT: Yes, yes, I've been having shortness of, &lt;UNIN/&gt;. Yeah, I've been having shortness of breath, yeah. DOCTOR: You are short of breath. And, uh, do you have any wheeze? Or chest pain? PATIENT: &lt;UNSURE&gt;Uh&lt;/UNSURE&gt;, yeah, a bit of both &lt;UNIN/&gt;. DOCTOR: You're, you're feeling a bit wheezy, with some chest pain as well. PATIENT: Yes. DOCTOR: OK. And, how, ah, when did you start to develop the shortness of breath? PATIENT: &lt;INAUDIBLE_SPEECH/&gt;. So, so the sore throat, so today's &lt;UNSURE&gt;Friday&lt;/UNSURE&gt;, sore throat was about, last week, Friday or Thursday. PATIENT: Cough was Saturday or Sunday. So the, so the, shortness of breath was I think, shortly after the cough. So maybe a day or two later. So, three, four days ago. DOCTOR: Three or four days ago, you started develop &lt;UNIN/&gt;. And is the cough worse at night-time? PATIENT: No, no, it's the same throughout the &lt;UNSURE&gt;whole&lt;/UNSURE&gt; day. DOCTOR: Same throughout the day. Um, and, uh, when you say you're short of breath. DOCTOR: Just need to try and get an idea about how short of breath you are. So, are you able to, &lt;UNSURE&gt;so&lt;/UNSURE&gt; &lt;UNIN/&gt;, um, so, uh, like walk up a flight of stairs, for example? Um, or, or, are you short of breath at rest? PATIENT: Ohh yeah, it's, it's like, &lt;UNSURE&gt;so&lt;/UNSURE&gt; when I'm doing &lt;UNSURE&gt;walking&lt;/UNSURE&gt;. Um, and I do exercises &lt;UNSURE&gt;now and then&lt;/UNSURE&gt;. So it, it hasn't been . PATIENT: Superbad like, hasn't stopped me from doing any of those things, but it's been pretty unusual, and a little bit worrying. DOCTOR: And you're a bit concerned about that, OK. DOCTOR: So, I just need to ask a few, uh, things about your background as well. So, um, do you have any other medical conditions, or medical history? PATIENT: No, just, no, no &lt;UNIN/&gt;, past medical history, no. DOCTOR: No &lt;INAUDIBLE_SPEECH/&gt;. No history of asthma? PATIENT: No. DOCTOR: Um, and any, uh, uh, history of, uh, clots on your legs, or your lungs? DOCTOR: &lt;UNSURE&gt;So these&lt;/UNSURE&gt; &lt;INAUDIBLE_SPEECH/&gt;. Uh, no one in your family's had those? Clots on the legs, or the lungs? PATIENT: &lt;INAUDIBLE_SPEECH/&gt; PATIENT: Well, my mother had lung cancer. DOCTOR: Your mother had lung cancer. Do you smoke? PATIENT: No. DOCTOR: You ever smoked? Or been exposed to asbestos? That you know of? PATIENT: Don't know with asbestos. Ever smoked, &lt;UNIN/&gt;. I mean, once or twice in Amsterdam, if that counts, but, not really. DOCTOR: OK. Um, and, uh, this, so just going back to the, your symptoms of shortness of breath, with the cough. It's a dry cough, no, you're not coughing up any flem? DOCTOR: Um, do, do you have, uh, and you don't, you say you don't have any chest pain, as such? DOCTOR: Um. Uh, are you taking any medications, currently, at the moment? PATIENT: Uh. No, no. DOCTOR: OK. Are you allergic to any medications? PATIENT: Not to any medication, but I'm allergic to peanuts. DOCTOR: Peanuts. OK. Um, and, uh. DOCTOR: You mentioned that your mother had, uh, lung cancer. Um, any other, family history of any significant illnesses, uh, run, running in your family? PATIENT: No, no, that's the only one. Just lung cancer, from my mother. DOCTOR: Just lung cancer. OK. DOCTOR: And you say you have a cold. So, do you have &lt;UNIN/&gt;, sinus congestion? Or, um. PATIENT: No, it seems to be &lt;INAUDIBLE_SPEECH/&gt;, &lt;UNIN/&gt; entirely with just my throat. So like, my nose is &lt;INAUDIBLE_SPEECH/&gt; like, &lt;UNIN/&gt;. DOCTOR: So, &lt;UNIN/&gt;, just your, just your throat. And, any recent travel? Or have you always lived in the UK? PATIENT: Uh, no, so &lt;UNSURE&gt;I, I&lt;/UNSURE&gt;, I haven't always lived in the UK. Like, so I was born in the US, and moved over. PATIENT: Well, it was twelve years ago, but, in terms of recent travel. Just to Europe, nowhere too exotic. DOCTOR: OK, so no, so no recent travel, no significant recent travel any, anywhere. Um, OK. DOCTOR: And, are you coughing up anything other than, &lt;UNIN/&gt;. Um, uh, so you, you're not coughing up blood, or anything like that? No, no. DOCTOR: Um, good. And, uh, are you feeling feverish, hot, cold, sweaty? PATIENT: Yeah, so, a little bit feverish, uh, um, at first. So the first three or so days of this, but then it, the fever's gone away. DOCTOR: OK. And in general, do you &lt;UNIN/&gt;. Sorry? Yeah. PATIENT: &lt;INAUDIBLE_SPEECH/&gt; PATIENT: Yeah, I was just gonna say, also had a bit of a headache. But like, headaches that come and go rather, but like, right now it's fine. DOCTOR: &lt;UNSURE&gt;Uh&lt;/UNSURE&gt;. DOCTOR: OK. And in general, would you say you're feeling, you're, you're beginning to, to feel better? Worse? Or, or sort of, um, staying the same? PATIENT: &lt;UNIN/&gt;, so it's like, it's up and down. So, so let's see, so I, &lt;UNIN/&gt;, it started last week, and I stayed home from work two days this week. PATIENT: I think it was maybe, Tuesday and then Thursday. So like, I felt better and then worse again, and then better and then worse again. So it's been, yeah, a kind of constant, but constant and being, variable, if that makes &lt;UNIN/&gt;. DOCTOR: OK. DOCTOR: And I just &lt;UNIN/&gt;, need to ask any, other sort of risk factors. Um. DOCTOR: That you may have. So, &lt;UNIN/&gt;, um, no sort of significant weight loss? Um, or unexplained weight loss? Any &lt;INAUDIBLE_SPEECH/&gt;? PATIENT: So no weight loss, but I have been, have been losing my appetite recently. And I mean, I usually eat a lot so, and I, and I enjoy eating as well, but like, so that's been a bit concerning. DOCTOR: You've been losing your appetite recently? PATIENT: Yes. DOCTOR: And you're a little bit concerned about that? But you haven't, you haven't lost any weight, that you think of? PATIENT: Yes. PATIENT: No. Not that &lt;UNIN/&gt;. DOCTOR: And any, um, sort of rashes or anything? &lt;UNSURE&gt;Or&lt;/UNSURE&gt;, uh, &lt;UNIN/&gt;, and you. PATIENT: No. Not &lt;UNIN/&gt;. DOCTOR: &lt;UNSURE&gt;Not that&lt;/UNSURE&gt;, not that you can think of. OK. DOCTOR: Um. So, I would ask to examine you now, but um, I, I don't know if I could sort of look inside your throat, at least. To see if there's a, probably, &lt;UNSURE&gt;there's&lt;/UNSURE&gt;. PATIENT: Ohh, we can try &lt;INAUDIBLE_SPEECH/&gt;. DOCTOR: Ohh no, well, no, it's OK, I &lt;UNIN/&gt;, might think about doing &lt;UNSURE&gt;a&lt;/UNSURE&gt;. Have you got any lumps or bumps around your neck? That you can feel? PATIENT: &lt;INAUDIBLE_SPEECH/&gt; PATIENT: Uh. PATIENT: No. DOCTOR: No that you, no, OK. DOCTOR: Um. And, so finally, you, you were talking about, uh, &lt;UNIN/&gt;. I mean, it sounds to me that, um, you've been a little bit up and down. Sore throat. Developed a dry cough. DOCTOR: Um, you are slightly short of breath, but not too overly concerningly short of breath. What I would say, we're just coming to the end of consultation now, &lt;UNIN/&gt;. If you feel significantly worse . PATIENT: &lt;UNSURE&gt;Mm-hmm&lt;/UNSURE&gt;. DOCTOR: Um. Uh, if you get more short of breath, or sudden change in your breathlessness. Um, or breathlessness that you are concerned about. Then I would advise you to &lt;UNSURE&gt;see, no&lt;/UNSURE&gt; &lt;INAUDIBLE_SPEECH/&gt;, go and see a GP. Um, and actually see somebody physically. DOCTOR: Um, uh, but I think, for now I can sort of, uh, try and reassure you that, um, if this clears up, as I expect it would. So, I expect this to sort of be getting better in the next, four or five days. Um, if it's not, please get in touch with a medical professional again. DOCTOR: Um, and, uh, I would expect it to, and so therefore, I wouldn't be concerned about tuberculosis DOCTOR: Um, your concerns about lung cancer, are. And, was that the other thing &lt;UNSURE&gt;you're&lt;/UNSURE&gt; concerned about? PATIENT: Ohh yeah, yeah. Yeah. DOCTOR: Yeah. So, so, um, again, if you're not getting better, please see somebody again. DOCTOR: Um, I've just got four seconds now. So, nice talking to you. And, have we gotta? We gotta, tidy up, yeah. OK, so, uh. PATIENT: &lt;UNSURE&gt;All right&lt;/UNSURE&gt;. DOCTOR: Uh, and I'll provide you with a sick note, just to give you a few more days off work. DOCTOR: Um, and paracetemol. Lots of fluids. Um, and, uh, rest up. And, as I say, if you're not feeling better, please get in touch. OK? PATIENT: &lt;INAUDIBLE_SPEECH/&gt; PATIENT: Have a good day. DOCTOR: &lt;UNIN/&gt;. Thank you. PATIENT: Bye.</t>
+          <t>[Speaker 1]: Male or a female?
+[Speaker 2]: A male
+[Speaker 1]: How old are you?
+[Speaker 2]: I am 65 years old
+[Speaker 1]: Hope you don't mind if i address you as mr emeka
+[Speaker 2]: I don't mind
+[Speaker 1]: Ok. Thank you very much. So what brought you to the clinic today?
+[Speaker 2]: I am having difficulty in urinating 
+[Speaker 1]: Ok. You have been having difficulty in urinating. For how long has this been?
+[Speaker 2]: It has started for two weeks
+[Speaker 1]: You have been having difficulty in urinating for two weeks?
+[Speaker 2]: Yes
+[Speaker 1]: Did it started gradually? Or
+[Speaker 2]: It was gradual in onset
+[Speaker 1]: Ok. It was gradual in onset. Has it been constant? Has it always been there or it just comes and goes? Or you feel this within a particular period of the day?
+[Speaker 2]: I think it goes bad of recent. It was not constant before but now it is constant 
+[Speaker 1]: Ok. Thank you very much. Is this pain while urinating associated with a burning sensation?
+[Speaker 2]: Is not associated with pain or a burning sensation 
+[Speaker 1]: Ok. It is not associated with any pain or a burning sensation?
+[Speaker 2]: Yes. It is not
+[Speaker 1]: Do you feel urgency to urinate?
+[Speaker 2]: Yes. I feel urgency to urinate 
+[Speaker 1]: And then are you able to pass out this urine when you feel this urgency to urinate? 
+[Speaker 2]: I am unable to pass out urine
+[Speaker 1]: Ok. Do you feel frequent urination? The urge to always go to the toilet? 
+[Speaker 2]: Yes. I am always visiting the toilet especially in the night.
+[Speaker 1]: Ok. Nocturia, you always visit the toilet in the night?
+[Speaker 2]: Yes, at morning. At night, at night 
+[Speaker 1]: Like how many times do you urinate in the night?
+[Speaker 2]: It is very frequent. I can't tell
+[Speaker 1]: More than you used to before?
+[Speaker 2]: Yes. It's more than the usual two times to zero times i usually use the toilet but now it's about five times
+[Speaker 1]: Do you straint in urinate? 
+[Speaker 2]: Yes. I strain alot and my urine dripples 
+[Speaker 1]: Ok. It dripples? 
+[Speaker 2]: Yeah. After urination 
+[Speaker 1]: May i know if there is blood in the urine?
+[Speaker 2]: There's no blood in this urine. There's no fever. I don't have fever 
+[Speaker 1]: Is there pause? 
+[Speaker 2]:  There's no pause oo 
+[Speaker 1]: Do you have lower abdominal pain?
+[Speaker 2]: I don't have abdominal pain
+[Speaker 1]: Ok. Thank you very much. Is there a history of trauma? Or recent catherization or urethra instrumentation?
+[Speaker 2]: No. There's not 
+[Speaker 1]: There's not history of trauma or catherization?
+[Speaker 2]: I do not have any history of that
+[Speaker 1]: Ok. Thank you very much. Are you a main hypertensive patient? Are you hypertensive?
+[Speaker 2]: Yes. I have been hypertensive for 10 years now
+[Speaker 1]: Ok. You have been hypertensive for 10 years. How do you know that you are hypertensive?
+[Speaker 2]: I was told at the hospital that i was diagnosed there
+[Speaker 1]: You were diagnosed in a hospital 10 years ago?
+[Speaker 2]: Yes
+[Speaker 1]: And you have been on medications?
+[Speaker 2]: Yes. It has been controlled by medications
+[Speaker 1]: Ok. Thank you very much. How about diabetic? Are you diabetic? 
+[Speaker 2]: No. I am not diabetic 
+[Speaker 1]: You are not diabetic. Ok. Is there a family history of similar condition? Is there anyone in your family that has similar condition?
+[Speaker 2]: Yeah. I can remember my dad have similar condition when he was old
+[Speaker 1]: When he was old? What exactly was the problem? Did he also feel pain while trying to urinate?
+[Speaker 2]: He has some urinal problem i can tell exactly. I was young at that time
+[Speaker 1]: Ok. Thank you very much. Are you a smoker?
+[Speaker 2]: I don't smoke 
+[Speaker 1]: Do you take alcohol?
+[Speaker 2]: Yeah. I consume alcohol occasionally 
+[Speaker 1]: Do you take any recreational drugs substance abuse?
+[Speaker 2]: No
+[Speaker 1]: Thank you very much. Are you on your hypertensive agents?
+[Speaker 2]: Yes. I am on some drugs they give me to control the hypertension 
+[Speaker 1]: Can you tell me the name of the drug you are on? 
+[Speaker 2]: amlodepine 
+[Speaker 1]: Ok. You are on amlodepine? Is there any drug you are on?
+[Speaker 2]: I am not on any other. They give me just that one
+[Speaker 1]: Ok. Thank you very much. Do you have any other allergies? Do you have, are you allergic to any drug or medication?
+[Speaker 2]: I am not 
+[Speaker 1]: Ok. Thank you very much</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>626.7</v>
+        <v>247.1079819</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>UK-Dataset</t>
+          <t>afrispeech_medical</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>hello can you hear me okay hey yes i can can you hear me yeah good good so my name is joe i'm a doctor here at babylon can i just confirm your name please hey my name is vincent and your date of birth ah nine of may two thousand and sixteen okay great sorry and are you in a be a safe place oh sorry a safe and confidential place to talk and discuss yeah i'm happy to go ahead with the consultation yes yes i am great so how can i help yeah so i have a call up i've been having a cough and a sore throat for about a week and it's been causing me problems i've had to stay away from work for about three or four of those days because of it okay i'm sorry to hear that so you've had a cough and a sore throat for about a week and what came what came first the sore throat came first and then after a day or two the cough okay and are you coughing up anything no it's very dry okay so i'm just going to ask a few questions about the your current symptoms and then a little bit about your background and something else about what we can do a little bit later on in the consultation to help you but before we go on anything you're particularly concerned about or have any Right so so yeah i can provide a little bit of reassurance um and uh we can talk about those a little bit as well. Was there anything you were particularly expecting or hoping to get out of this consultation? Well yeah, so reassurance, so like hopefully in some sense that's not anything too serious, but also is there anything you can prescribe me to make it better or any advice or maybe even a sick note so that if i need to stay away from work for a bit longer i can get one? Sure, sure. Okay. All right. So we'll talk a little bit about the symptoms and i'm sure we can get a those things sorted. and some reassurance thank you about your concerns so um you mentioned that you started with a sore throat about a week ago developed into a bit of a dry cough and i'll just ask a few questions around those so um do you have any shortness of breath yes yes i've been having shortness of oh yeah i've been having shortness of breath yeah you are short of breath and uh do you have any wheeze or chest pain Yeah, you're feeling a bit wheezy with some chest pain as well. Yes. Okay. And how when did you start to develop the shortness of breath? So the sore throat so today is friday sore throat was about friday or thursday cough was saturday or sunday so the shortness of breath was i think shortly after the cough so maybe a day or two later so three or four days ago? Two or four days ago. you start to develop symptoms and is the cough worse at night time no no it's the same throughout the day same throughout the day and when you say you're short of breath just need to try and get an idea about how short of breath you are so are you able to like walk up a flight of stairs for example or are you short of breath at rest oh yeah it's like when i'm doing walking and i do exercise now and then so it It hasn't been super bad, like hasn't stopped me from doing any of those things, but it's been pretty unusual and a little bit worrying. And you're a bit concerned about that. Okay. So I just need to ask a few things about your background as well. So do you have any other medical conditions or medical history? No, just no, no past medical history, no. No history of asthma? No. And any history of... clots on your legs or your lungs so these are ddp's or p's and none of your families had those clots in the legs or lungs well my mother had lung cancer your mother had lung cancer do you smoke no you ever smoked or been exposed to asbestos you know don't know if asbestos ever smoked i mean once or twice in amsterdam with that car but not really okay um and ah this so just going back to the your symptoms of shortness of breath with the cough it's a dry cough no you're not coughing up any phlegm um do you do you have and you say you don't have any chest pain as such um are you taking any medications currently at the moment no i'm not okay are you allergic to any medications not any medication but i'm allergic to peanuts peanuts okay and and you mentioned that your mother had lung cancer and any other family history of any significant illnesses when running in your family no no that's the only one just lung cancer from my mother just lung cancer okay and you say you have a cold so do you have sinus congestion or um no it seems to be almost entirely just my throat like J just your just your throat and any recent travel or have you always lived in the u. k. uh no so i i haven't always lived in the u. k. like so i was born in the u. s. and moved over about twelve years ago but in terms of recent travel just to europe nowhere to exotic. okay so no so no recent travel no significant recent travel anywhere um okay and are you coughing up anything other than um so you're not coughing up blood or anything like that no um good and are you feeling feverish hot cold sweaty yeah so a little bit feverish um at first so the first three or so days of this but then the fever's gone away okay and in general do you sorry yeah i was just going to say also had a bit of a headache like headaches that come and go rather but Like right now it's fine. Okay. And in general would you say you're feeling you're you're beginning to to feel better worse or or sort of staying the same? So it's like it's up and down so so let's see so i started last week and i stayed home from work two days this week i think it was maybe tuesday and then thursday so like i felt better and then worse again and then better and then worse again so it's been yeah a kind of constant but constant in being variable but okay and i just really need to ask any other sort of risk factors um that you may have so um no sort of significant weight loss um or unexplained weight loss any so no weight loss but i have been have been losing my appetite recently and i mean i usually eat a lot so i enjoy eating as well but like that's been a bit concerning you've been losing your appetite recently Yes, and you're a little bit concerned about that, but you haven't you haven't lost any weight that you think no, not that and any um sort of rashes or anything uh and you no rash no you can go okay um so i would ask to examine you now but um i i don't know if i could sort of look inside your throat at least to see if there's a probably there's oh we can try it on oh no well no it's okay i might think about doing it have you got any lumps or bumps around your neck that you can feel ah no not the no okay and and so finally you you were talking about i mean it sounds to me that um you've been a little bit up and down sore throat developed a dry cough and you are slightly short of breath but not too overly concerningly short of breath what i would say we're just coming to the end So consultation hours is if you feel significantly worse, um, uh, if you get more short of breath or sudden change in your breathlessness, um, or breathlessness that you are concerned about, and I would advise you to see your GP and actually see somebody physically, um, uh, but I think for now I can sort of try and reassure you that, um, if this clears up as I expected it would, so expect this to sort of be getting better in the next, four or five days if it's not please get in touch with the medical professional again and i'll expect it to and so therefore i wouldn't be concerned about tuberculosis your concerns about lung cancer was that the other thing you were concerned about yeah yeah so so um again if you're not getting better please see somebody again i've just got four seconds now so nice talking to you and we've got to we've got to tidy up yeah okay so and i'll provide you with a sick note just to give you a few more days off work and paracetamol lots of fluids and rest up and as i say if you're not feeling better please get in touch okay alright have a good day thank you alright</t>
+          <t>Male or a female? I'm a male. How old are you? I'm 65 years old. I hope you don't mind I address you as Mr. I maker. I don't mind. Okay, thank you very much. So what brought you to the clinic today? I've been having difficulty in urinating. You've been having difficulty in urinating. For how long has this been? That's lasted for two weeks. You've been having difficulty urinating for two weeks. Yes. Did this start as gradually or? It was gradual in onset. It was gradual in onset. Has it been constant? Has he always been there or he just comes and goes or he feels this within a particular period of the day? I think he got bad of recent. It was not constant before but now it's constant. Okay, thank you very much. Is this pain, while urinating, associated with the burning sensation? It's not associated with pain. burning sensation it's not associated with any pain or a burning sensation yes it's not do you feel the urgency to you know and then are you able to pass out this urine when you feel this urgency to you know i'm unable to pass out okay do you feel frequent urination the urge to always go to the toilet yes i'm always using the toilet especially in the night okay nocturia so you always use the toilet in the night yes at morning at night at night like how many times you you need in the night it's very frequent i can't tell more than it used to be for yes it's more than the usual two times to zero times i usually use the toilet but now it's about five times do you strain to urinate yes i strain a lot and my urine bubbles okay it bubbles yes after urination um i know if there's blood in the urine There's no blood in this urine. There's no fever. I don't have a fever. Is there pus? There's no pus. So okay. So do you have lower abdominal pain? I don't have any abdominal pain. Oh, thank you very much. Is there a history of trauma or any recent catheterization or ureteral instrumentation? No, there is none. There's no history of trauma or catheterization. I don't have any history of that. Oh, thank you very much. Are you a known hypertensive? Yes, I've been hypertensive for 10 years now. Okay, you've been hypertensive for 10 years. How do you know you are hypertensive? I was told that I was diagnosed in the hospital. I was diagnosed in the hospital 10 years ago. Yes, and you have been on medications? Yes, that has been controlled by medications. Okay, thank you very much. How about being diabetic? Are you diabetic? No, I'm not diabetic. Is there anyone in your family that has similar condition? Yeah, I can remember my dad had similar condition when he was old. When he was old, what exactly was the problem? Did he also feel pain while trying to urinate? He had some urinary problem. I can't tell exactly. I was young at that time. Okay, thank you very much. Are you a smoker? I don't smoke. Do you take alcohol? Yeah, I consume alcohol occasionally. Are you on your hypertensive agents? Yes, I'm on some drugs they gave me to control the hypertension. Can you tell me the name of the drug you're on? I'm on load the pin. Is there any other drug you're on? I'm not on any other drug. They gave me just that one. Thank you very much. Do you have any other justifications? Are you allergic to any drug or medication? No, I'm not. Okay, thank you very much.</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Hello, can you hear me okay? Yes, I can. Can you hear me? Yeah, good, good. So my name is Joe. I'm a doctor here at Babylon. Can I just confirm your name, please? My name is Vincent. And your date of birth? 9th of may 2016. okay great sorry i know you in a uh a safe place oh sorry a safe and confidential place to talk and just i have to go ahead with the consultation yes yes i am great so how can i help yeah so i have a call that I've been having a cough and a sore throat for about a week and it's been causing me problems. I've had to stay away from work for about three or four of those days because of a bad history. Okay, I'm sorry to hear that. So you've had a cough and a sore throat for about a week. And what came first? The sore throat came first and then after a day or two, the cough. Okay. And I just want to thank a few questions about your current symptoms and then a little bit about your background and something else about what we can do a little bit later on in the consultation to help you. But before we go on, anything you're particularly concerned about or have any ideas what might be going on? You said that you had a cold. Well, I mean, you know how we all are. Once this happens, you Google it, and it seems to be all kinds of bad things. It could be a cold or flu, obviously, obviously because we tuberculosis the cancer always comes up so it'll be good if those right say say yeah I can provide a little bit of reassurance and we can talk about those a little bit as well and was there any you're particularly expecting or hoping to get out of this consultation? Well, yeah, so reassurance, so hopefully some sense that it's not anything too serious, but also, if there's anything you can prescribe me to make it better, or any advice, or maybe even a sick note, so if I need to stay away from work for a bit longer, I can get one. Sure, sure, okay. All right. So we'll talk a little bit about the symptoms and I'm sure we can get those things, some secrets and some reassurance. Thank you. About your concerns. So you mentioned that you started with a sore throat about a week ago, developed into a bit of a dry cough. And I just ask a few questions around those those so do you have any shortness of breath yes yes we're having shorts oh yeah I've been having shortness of breath you are short of breath and do you have any wheeze or chest pain yeah you're feeling a bit wheezy with some chest pain as well? Yes. Okay. And when did you start to develop a shortness of breath? Let's see. So the sore throat, so today is Friday. Sore throat was about last Friday or Thursday. Cough was Saturday or Sunday. So the shortness of breath was I think shortly after the cough, so maybe a day or two later, so three or four days ago. Three or four days ago you started developing and is the cough worse at night time? No, it's the same throughout the day. And when you say you're short of breath, just need to try and get an idea about how short of breath you are so are you able to like walk up flights of stairs for example or are you short breath of rest oh yeah it's like when I'm doing walking and I do exercise now and then so it hasn't been super bad like hasn't stopped me from doing any of those things but it's been pretty unusual and a little bit worried and you're a bit concerned about that okay so I just need to ask a few things about your background as well so do you have any other medical conditions or medical history no just no no No history of asthma? No. And any history of clots on your legs or your lungs? These are DDT's or P's. No one in your family's had those? Clots on the legs or the lungs? Well my mother had lung cancer. Your mother had lung cancer. Do you smoke? No. Have you ever smoked or been exposed to asbestos? I don't know if asbestos ever smoked. I mean once or twice in Amsterdam, in Dakar, but not really. Okay and this, just going back to your symptoms of shortness of breath with the cough, it's a dry cough, not cough, cap, flem. Do you have, and you say you don't have any chest pain as such. Are you taking any medications currently at the moment? No, I'm not. Okay. Are you allergic to any medications? Not to any medication, but I'm allergic to peanuts. Peanuts, okay. And you mentioned that your mother had lung cancer. Any other family history of any significant illnesses when running into family? No, no, that's the only one just lung cancer from my mother. Okay and you say you have a cold so do you have sinus congestion or? No it seems to be all entirely with just my throat, like my nose is just running out. Just your throat and any recent travel or have you always lived in the UK no so I I haven't always lived in the UK like so I was born in the US and 12 years ago but it's a recent travel just to Europe nowhere to exotic okay so no so no recent travel no significant recent travel anywhere um okay and are you coughing up anything other than um so you're not coughing up blood or anything like that um good and uh are you feeling feverish hot cold sweaty, so a little bit feverish at first. So the first three or so days of this, but then the fever's gone away. OK. And in general, do you feel better? Sorry. Yeah. Yeah, I was just going to say I also had a bit of a headache. Like, headaches that come and go, rather. But right now, it's fine. OK. And in general, would you say you're beginning to feel better, worse, or sort of staying the same? So it's like, it's up and down. So let's see. So I started last week and I stayed home from work two days this week. I think it was maybe Tuesday and then Thursday. So like I felt better and then worse again, and then better and then worse again. So it's been a kind of constant, but constant in being variable. Okay. And I just need to ask any other sort of risk factors, um, that you may have. So, um, no sort of significant weight loss, um, or unexplained weight loss. Any? So no no weight loss but I have been losing my appetite recently and I mean I usually eat a lot so I enjoy eating as well but that's been a bit concerning. You've been losing your appetite recently? Yes. And you're a little bit concerned about that but you haven't lost any weight lost any weight that you think no not that and any um sort of rashes or anything uh and you no no okay um so i would ask to examine you now but um i i don't know if i could sort of look inside your throat at least see if there's a probably we can try oh no well no it's okay I might think about doing have you got any lumps or bumps around your neck that you could feel no not the no okay and and so finally you were talking about I, it sounds to me that you've been a little bit up and down, sore throat, developed a dry cough, you are slightly short of breath, but not too overly concerningly short of breath. What I would say, we're just coming to the end of the consultation now, is if you feel significantly worse, if you get more short of breath or sudden change in your breathlessness or breathlessness that you are concerned about and I would advise you to see a GP and actually see something physically but I think for now I can sort of try and reassure you that if this clears up as I expect it would, so expect this to sort of be getting better in the next four or five days. If it's not, please get in touch with the medical professional again. And I would expect it to, and so therefore I wouldn't be concerned about tuberculosis. Your concerns about lung cancer are... Was that the other thing you were concerned about? Oh yeah, yeah. So again, if you're not getting better, please see somebody again. I've just got four seconds now, so nice talking to you. And we've got to tidy up, yeah. Okay, okay so and I'll provide you with a sick note just to give you a few more days of work and paracetamol lots of fluids and rest up and as I say if you're not feeling better please get in touch okay all right thank you</t>
+          <t xml:space="preserve"> male or a female i'm a male how old are you i'm 65 years old i hope you don't mind i address you as mr emeka i don't mind okay thank you very much so what brought you to the clinic today i'm having difficulty in urinating you've been having difficulty in urinating for how long has this been that's nothing for two weeks you've been having difficulty urinating for two weeks Yes. Did this started gradually or...? It was gradual in onset. It was gradual in onset. Has it been constant? Has it always been there or it just comes and goes or you feel this within a particular period of the day? I think it got bad recently. It was not constant before but now it's constant okay thank you very much is this pain while urinating associated with the burning sensation it's it's not associated with pain or a burning sensation okay so it's not associated with any pain or a burning sensation yes it's not do you feel the urgency to urinate yes i feel the urgency to you ring it and then are you able to pass out this urine when you feel this urgency to you in it i'm unable to pass out here okay do you feel frequent urination the urge to always go to the toilet yes i'm always just into it especially the night okay nocturia so you always use the toilet in the night yes at morning at night at night like how many times you you need in the night it's very frequent i can't tell more than you used to before yes it's more than the usual two times to zero times i usually use the toilet but now it's about five times do you strain to urinate yes i strain a lot and my urine dribbles okay it dribbles yes after i might know if there's blood in the urine there's no blood in this urine there's no fever i don't have is't have fever. Is there pus? There's no pus. Okay. So, do you have lower abdominal pain? I don't have abdominal pain. Oh, thank you very much. Is there a history of trauma or any recent catarization or urethra instrumentation? No, there is none. There's no history of trauma or catarization? I don't have any history oh thank you very much are you a known hypertensive patient are you hypertensive yes i've been hypertensive for 10 years now okay you've been hypertensive for 10 years how do you know you are hypertensive i was told that the hospital uh i was diagnosed there you were diagnosed in the hospital 10 years ago yes Yes. And you have been on medications? Yes, that's been controlled by medications. Okay, thank you very much. How about being diabetic? Are you diabetic? No, I'm not diabetic. You're not diabetic. Okay, is there a family history of similar condition? Is there anyone in your family that has similar condition? Yeah, I can remember my dad had similar condition when he was old. When he was old, what exactly was the problem? Did he also feel pain while trying to urinate? He had some urinary problem. I can't tell exactly. I was young at that time. Okay, thank you very much. Are you a smoker? I don't smoke. Do you take alcohol? Yeah, I consume alcohol occasionally. Do you take any recreational drugs, substance abuse? No. Thank you very much. Are you on your hypertensive agent? Yes, I'm on some drugs they gave me to control the hypertension. Can you tell me the name of the drug you're on? I'm on Lodipine. Okay, you're on Lodipine. Is there any other drug you're on? I'm not on any other drug. They gave me just that one. Oh, thank you very much. Do you have any allergies? Are you allergic to any drug or medication? No, I'm not. Okay, thank you very much.</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>hello can you hear me ok ohh yes i can can you hear me yeah good good so my name is joe i am a doctor um here at babylon can i just confirm your name please uh my names vincent and your date of birth uh uh ninth of may two thousand and sixteen ok great  and are you in a uh a safe place ohh sorry a safe and  confidential place to talk and just  happy to go ahead with the consultation yeah yeah i am yes yes i am great so how can i help yeah so have a  i have been having a cough and a sore throat for about a week and its been causing me problems i have had to stay away from work for about three or four of those days because of how bad is ok i am sorry to hear that so you have had a cough and a sore throat for about a week and what came what what came first yes uh the sore throat came first and then after a day or two the cough ok ok and uh are you coughing up anything no its very dry ok so i am i am just going to ask a few questions about the uh your current symptoms and a little bit about your background um and something else about what we can do a little bit later on in the consultation to help you so before we go on  anything you are particularly concerned about um or have any ideas what might be going on you said that you had a cold ok  well i mean you  you know how we all are once this happens you google it and there seems to be all kinds of bad things it could be it could be could be a cold or flu obviously but it could also be tuberculosis it could be cancer always comes up so it will be good if none of those great so so yeah i can provide a bit of reassurance um and uh we can talk about those a little bit as well and was there anything you were particularly expecting or hoping to get out of this consultation um ok uh uh well uh yeah so reassurance so like hopefully some sense that its not anything too serious but also is there anything you can prescribe me to make it better or any advice or maybe even a sick note so that if i need to stay away from work for a bit longer i can get one sure sure ok all right so well talk a little bit about the symptoms and i am sure we can  get a um those things uh  and some reassurance um about your concerns ok so um you mentioned that you started with sore throat about a week ago developed into bit of a dry cough um  ill just ask a few questions around those so um do you have any shortness of breath no yes yes i have been having shortness of  yeah i have been having shortness of breath yeah you are short of breath and uh do you have any wheeze or chest pain uh yeah a bit of both  you are you are feeling a bit wheezy with some chest pain as well yes ok and how ah when did you start to develop the shortness of breath  so so the sore throat so todays friday sore throat was about last week friday or thursday cough was saturday or sunday so the so the shortness of breath was i think shortly after the cough so maybe a day or two later so three four days ago three or four days ago you started develop  and is the cough worse at nighttime no no its the same throughout the whole day same throughout the day um and uh when you say you are short of breath just need to try and get an idea about how short of breath you are so are you able to so  um so uh like walk up a flight of stairs for example um or or are you short of breath at rest ohh yeah its its like so when i am doing walking um and i do exercises now and then so it it has not been  superbad like has not stopped me from doing any of those things but its been pretty unusual and a little bit worrying and you are a bit concerned about that ok so i just need to ask a few uh things about your background as well so um do you have any other medical conditions or medical history no just no no  past medical history no no  no history of asthma no um and any uh uh history of uh clots on your legs or your lungs so these  uh no one in your familys had those clots on the legs or the lungs  well my mother had lung cancer your mother had lung cancer do you smoke no you ever smoked or been exposed to asbestos that you know of do not know with asbestos ever smoked  i mean once or twice in amsterdam if that counts but not really ok um and uh this so just going back to the your symptoms of shortness of breath with the cough its a dry cough no you are not coughing up any flem um do do you have uh and you do not you say you do not have any chest pain as such um uh are you taking any medications currently at the moment uh no no ok are you allergic to any medications not to any medication but i am allergic to peanuts peanuts ok um and uh you mentioned that your mother had uh lung cancer um any other family history of any significant illnesses uh run running in your family no no that is the only one just lung cancer from my mother just lung cancer ok and you say you have a cold so do you have  sinus congestion or um no it seems to be   entirely with just my throat so like my nose is  like  so  just your just your throat and any recent travel or have you always lived in the uk uh no so i i i have not always lived in the uk like so i was born in the us and moved over well it was twelve years ago but in terms of recent travel just to europe nowhere too exotic ok so no so no recent travel no significant recent travel any anywhere um ok and are you coughing up anything other than  um uh so you you are not coughing up blood or anything like that no no um good and uh are you feeling feverish hot cold sweaty yeah so a little bit feverish uh um at first so the first three or so days of this but then it the fevers gone away ok and in general do you  sorry yeah  yeah i was just going to say also had a bit of a headache but like headaches that come and go rather but like right now its fine uh ok and in general would you say you are feeling you are you are beginning to to feel better worse or or sort of um staying the same  so its like its up and down so so let us see so i  it started last week and i stayed home from work two days this week i think it was maybe tuesday and then thursday so like i felt better and then worse again and then better and then worse again so its been yeah a kind of constant but constant and being variable if that makes  ok and i just  need to ask any other sort of risk factors um that you may have so  um no sort of significant weight loss um or unexplained weight loss any  so no weight loss but i have been have been losing my appetite recently and i mean i usually eat a lot so and i and i enjoy eating as well but like so that is been a bit concerning you have been losing your appetite recently yes and you are a little bit concerned about that but you have not you have not lost any weight that you think of yes no not that  and any um sort of rashes or anything or uh  and you no not  not that not that you can think of ok um so i would ask to examine you now but um i i do not know if i could sort of look inside your throat at least to see if there is a probably there is ohh we can try  ohh no well no its ok i  might think about doing a have you got any lumps or bumps around your neck that you can feel  uh no no that you no ok um and so finally you you were talking about uh  i mean it sounds to me that um you have been a little bit up and down sore throat developed a dry cough um you are slightly short of breath but not too overly concerningly short of breath what i would say were just coming to the end of consultation now  if you feel significantly worse  mmhmm um uh if you get more short of breath or sudden change in your breathlessness um or breathlessness that you are concerned about then i would advise you to see no  go and see a gp um and actually see somebody physically um uh but i think for now i can sort of uh try and reassure you that um if this clears up as i expect it would so i expect this to sort of be getting better in the next four or five days um if its not please get in touch with a medical professional again um and uh i would expect it to and so therefore i would not be concerned about tuberculosis um your concerns about lung cancer are and was that the other thing you are concerned about ohh yeah yeah yeah yeah so so um again if you are not getting better please see somebody again um i have just got four seconds now so nice talking to you and have we got to we got to tidy up yeah ok so uh all right uh and ill provide you with a sick note just to give you a few more days off work um and paracetemol lots of fluids um and uh rest up and as i say if you are not feeling better please get in touch ok  have a good day  thank you bye</t>
+          <t>Male or a female? Male. How old are you? I'm 65 years old. I hope you don't mind. I address you as Mr. Emeka. I don't mind. Okay, thank you very much. So, what brought you to the clinic today? I'm having difficulty in urinating. You've been having difficulty in urinating. For how long has this been? It has lasted for two weeks. You've been having difficulty urinating for two weeks. Yes. Did this start gradually or it was gradual nonsense? Okay, it was gradual in on set. Has it been constant? Has it always been there, or it just comes and goes, or you feel this within the particular period of the day? I think it got bad of recent. It was not constant before, but now it's constant. Okay, thank you very much. Is this pain while urinating associated with a burning sensation? It's not associated with pain or a burning sensation. Okay, so it's not associated with any pain or a burning sensation. Yes, it's not. Do you feel the urgency to urinate? Yes, I feel the urgency to urinate. And then are you able to pass out this urine when you feel this urgency to urinate? I'm unable to pass out urine. Okay, do you feel frequent urination? The urge to always go to the toilet? Yes, I'm always using the toilet, especially in the night. Okay, Nocturia. So you always use the toilet in the night? Yes, at morning, at night, at night. Like how many times do you urinate in the night? It's very frequent. I can't tell. More than it used to before? Yes, it's more than the usual two times to zero times. I usually use the toilet, but now it's about five times. Do you strain to urinate? Yes, I strain a lot and my urine dribbles. Okay, it dribbles. Yes, after urination. May I know if there's blood in the urine? There's no blood in this urine. There's no fever. I don't have fever. Is there pulse? There's no pulse. Okay. So, do you have lower abdominal pain? I don't have abdominal pain. Oh, thank you very much. Is there a history of trauma or any recent caterization or urethra instrumentation? No, there is none. There's no history of trauma or catheterization? I don't have any history of that. Oh, thank you very much. Are you a known hypertensive patient? Are you hypertensive? Yes, I've been hypertensive for 10 years now. Okay, you've been hypertensive for 10 years. How do you know you are hypertensive? I was told at the hospital I was diagnosed there. You were diagnosed in a hospital 10 years ago? Yes. And you have been on medications? Yes, that's been controlled by medications. Okay, thank you very much. How about being diabetic? Are you diabetic? No, I'm not diabetic. You're not diabetic. Okay, is there a family history of similar conditions? Is there anyone in your family that has similar conditions? Yeah, I can remember my dad had a similar condition when he was old. When he was old, what exactly was the problem? Did he also feel pain while trying to urinate? He had some urinal problem. I can't tell exactly. I was young at that time. Okay, thank you very much. Are you a smoker? I don't smoke. Do you take alcohol? Yeah, I consume alcohol occasionally. Do you take any recreational drug substance abuse? No. Thank you very much. Are you on your hypertensive agent? Yes, I'm on some drugs they gave me to control the hypertension. Can you tell me the name of the drug you're on? I'm not pain. Okay, you're on and you know the pain. Is there any other drug you are on? I'm not on any other drug. They gave me just that one. Oh, thank you very much. Do you have any allergies? Do you have are you allergic to any drug or medication? No, I'm not. Okay, thank you very much, ma'am.</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>hello can you hear me okay yes i can can you hear me yeah good good so my name is joe i am a doctor here at babylon can i just confirm your name please my name is vincent and your date of birth nineth of may two thousand and sixteen okay great sorry i know you in a uh a safe place oh sorry a safe and confidential place to talk and just i have to go ahead with the consultation yes yes i am great so how can i help yeah so i have a call that i have been having a cough and a sore throat for about a week and its been causing me problems i have had to stay away from work for about three or four of those days because of a bad history okay i am sorry to hear that so you have had a cough and a sore throat for about a week and what came first the sore throat came first and then after a day or two the cough okay and i just want to thank a few questions about your current symptoms and then a little bit about your background and something else about what we can do a little bit later on in the consultation to help you but before we go on anything you are particularly concerned about or have any ideas what might be going on you said that you had a cold well i mean you know how we all are once this happens you google it and it seems to be all kinds of bad things it could be a cold or flu obviously obviously because we tuberculosis the cancer always comes up so it will be good if those right say say yeah i can provide a little bit of reassurance and we can talk about those a little bit as well and was there any you are particularly expecting or hoping to get out of this consultation well yeah so reassurance so hopefully some sense that its not anything too serious but also if there is anything you can prescribe me to make it better or any advice or maybe even a sick note so if i need to stay away from work for a bit longer i can get one sure sure okay all right so well talk a little bit about the symptoms and i am sure we can get those things some secrets and some reassurance thank you about your concerns so you mentioned that you started with a sore throat about a week ago developed into a bit of a dry cough and i just ask a few questions around those those so do you have any shortness of breath yes yes were having shorts oh yeah i have been having shortness of breath you are short of breath and do you have any wheeze or chest pain yeah you are feeling a bit wheezy with some chest pain as well yes okay and when did you start to develop a shortness of breath let us see so the sore throat so today is friday sore throat was about last friday or thursday cough was saturday or sunday so the shortness of breath was i think shortly after the cough so maybe a day or two later so three or four days ago three or four days ago you started developing and is the cough worse at night time no its the same throughout the day and when you say you are short of breath just need to try and get an idea about how short of breath you are so are you able to like walk up flights of stairs for example or are you short breath of rest oh yeah its like when i am doing walking and i do exercise now and then so it has not been super bad like has not stopped me from doing any of those things but its been pretty unusual and a little bit worried and you are a bit concerned about that okay so i just need to ask a few things about your background as well so do you have any other medical conditions or medical history no just no no no history of asthma no and any history of clots on your legs or your lungs these are ddts or ps no one in your familys had those clots on the legs or the lungs well my mother had lung cancer your mother had lung cancer do you smoke no have you ever smoked or been exposed to asbestos i do not know if asbestos ever smoked i mean once or twice in amsterdam in dakar but not really okay and this just going back to your symptoms of shortness of breath with the cough its a dry cough not cough cap flem do you have and you say you do not have any chest pain as such are you taking any medications currently at the moment no i am not okay are you allergic to any medications not to any medication but i am allergic to peanuts peanuts okay and you mentioned that your mother had lung cancer any other family history of any significant illnesses when running into family no no that is the only one just lung cancer from my mother okay and you say you have a cold so do you have sinus congestion or no it seems to be all entirely with just my throat like my nose is just running out just your throat and any recent travel or have you always lived in the uk no so i i have not always lived in the uk like so i was born in the us and twelve years ago but its a recent travel just to europe nowhere to exotic okay so no so no recent travel no significant recent travel anywhere um okay and are you coughing up anything other than um so you are not coughing up blood or anything like that um good and uh are you feeling feverish hot cold sweaty so a little bit feverish at first so the first three or so days of this but then the fevers gone away ok and in general do you feel better sorry yeah yeah i was just going to say i also had a bit of a headache like headaches that come and go rather but right now its fine ok and in general would you say you are beginning to feel better worse or sort of staying the same so its like its up and down so let us see so i started last week and i stayed home from work two days this week i think it was maybe tuesday and then thursday so like i felt better and then worse again and then better and then worse again so its been a kind of constant but constant in being variable okay and i just need to ask any other sort of risk factors um that you may have so um no sort of significant weight loss um or unexplained weight loss any so no no weight loss but i have been losing my appetite recently and i mean i usually eat a lot so i enjoy eating as well but that is been a bit concerning you have been losing your appetite recently yes and you are a little bit concerned about that but you have not lost any weight lost any weight that you think no not that and any um sort of rashes or anything uh and you no no okay um so i would ask to examine you now but um i i do not know if i could sort of look inside your throat at least see if there is a probably we can try oh no well no its okay i might think about doing have you got any lumps or bumps around your neck that you could feel no not the no okay and and so finally you were talking about i it sounds to me that you have been a little bit up and down sore throat developed a dry cough you are slightly short of breath but not too overly concerningly short of breath what i would say were just coming to the end of the consultation now is if you feel significantly worse if you get more short of breath or sudden change in your breathlessness or breathlessness that you are concerned about and i would advise you to see a gp and actually see something physically but i think for now i can sort of try and reassure you that if this clears up as i expect it would so expect this to sort of be getting better in the next four or five days if its not please get in touch with the medical professional again and i would expect it to and so therefore i would not be concerned about tuberculosis your concerns about lung cancer are was that the other thing you were concerned about oh yeah yeah so again if you are not getting better please see somebody again i have just got four seconds now so nice talking to you and we have got to tidy up yeah okay okay so and ill provide you with a sick note just to give you a few more days of work and paracetamol lots of fluids and rest up and as i say if you are not feeling better please get in touch okay all right thank you</t>
+          <t xml:space="preserve"> male or a female  a male  how old are you  i am sixtyfive years old  hope you do not mind if i address you as mr emeka  i do not mind  okay thank you very much so what brought you to the clinic today  i am having difficulty in urinating  okay you have been having difficulty in urinating for how long has this been  it has started for two weeks  you have been having difficulty in urinating for two weeks  yes  did it started gradually or  it was gradual in onset  okay it was gradual in onset has it been constant has it always been there or it just comes and goes or you feel this within a particular period of the day  i think it goes bad of recent it was not constant before but now it is constant  okay thank you very much is this pain while urinating associated with a burning sensation  is not associated with pain or a burning sensation  okay it is not associated with any pain or a burning sensation  yes it is not  do you feel urgency to urinate  yes i feel urgency to urinate  and then are you able to pass out this urine when you feel this urgency to urinate  i am unable to pass out urine  okay do you feel frequent urination the urge to always go to the toilet  yes i am always visiting the toilet especially in the night  okay nocturia you always visit the toilet in the night  yes at morning at night at night  like how many times do you urinate in the night  it is very frequent i cannot tell  more than you used to before  yes it is more than the usual two times to zero times i usually use the toilet but now it is about five times  do you straint in urinate  yes i strain alot and my urine dripples  okay it dripples  yeah after urination  may i know if there is blood in the urine  there is no blood in this urine there is no fever i do not have fever  is there pause  there is no pause oo  do you have lower abdominal pain  i do not have abdominal pain  okay thank you very much is there a history of trauma or recent catherization or urethra instrumentation  no there is not  there is not history of trauma or catherization  i do not have any history of that  okay thank you very much are you a main hypertensive patient are you hypertensive  yes i have been hypertensive for ten years now  okay you have been hypertensive for ten years how do you know that you are hypertensive  i was told at the hospital that i was diagnosed there  you were diagnosed in a hospital ten years ago  yes  and you have been on medications  yes it has been controlled by medications  okay thank you very much how about diabetic are you diabetic  no i am not diabetic  you are not diabetic okay is there a family history of similar condition is there anyone in your family that has similar condition  yeah i can remember my dad have similar condition when he was old  when he was old what exactly was the problem did he also feel pain while trying to urinate  he has some urinal problem i can tell exactly i was young at that time  okay thank you very much are you a smoker  i do not smoke  do you take alcohol  yeah i consume alcohol occasionally  do you take any recreational drugs substance abuse  no  thank you very much are you on your hypertensive agents  yes i am on some drugs they give me to control the hypertension  can you tell me the name of the drug you are on  amlodepine  okay you are on amlodepine is there any drug you are on  i am not on any other they give me just that one  okay thank you very much do you have any other allergies do you have are you allergic to any drug or medication  i am not  okay thank you very much</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>hello can you hear me okay hey yes i can can you hear me yeah good good so my name is joe i am a doctor here at babylon can i just confirm your name please hey my name is vincent and your date of birth ah nine of may two thousand and sixteen okay great sorry and are you in a be a safe place oh sorry a safe and confidential place to talk and discuss yeah i am happy to go ahead with the consultation yes yes i am great so how can i help yeah so i have a call up i have been having a cough and a sore throat for about a week and its been causing me problems i have had to stay away from work for about three or four of those days because of it okay i am sorry to hear that so you have had a cough and a sore throat for about a week and what came what came first the sore throat came first and then after a day or two the cough okay and are you coughing up anything no its very dry okay so i am just going to ask a few questions about the your current symptoms and then a little bit about your background and something else about what we can do a little bit later on in the consultation to help you but before we go on anything you are particularly concerned about or have any right so so yeah i can provide a little bit of reassurance um and uh we can talk about those a little bit as well was there anything you were particularly expecting or hoping to get out of this consultation well yeah so reassurance so like hopefully in some sense that is not anything too serious but also is there anything you can prescribe me to make it better or any advice or maybe even a sick note so that if i need to stay away from work for a bit longer i can get one sure sure okay all right so well talk a little bit about the symptoms and i am sure we can get a those things sorted and some reassurance thank you about your concerns so um you mentioned that you started with a sore throat about a week ago developed into a bit of a dry cough and ill just ask a few questions around those so um do you have any shortness of breath yes yes i have been having shortness of oh yeah i have been having shortness of breath yeah you are short of breath and uh do you have any wheeze or chest pain yeah you are feeling a bit wheezy with some chest pain as well yes okay and how when did you start to develop the shortness of breath so the sore throat so today is friday sore throat was about friday or thursday cough was saturday or sunday so the shortness of breath was i think shortly after the cough so maybe a day or two later so three or four days ago two or four days ago you start to develop symptoms and is the cough worse at night time no no its the same throughout the day same throughout the day and when you say you are short of breath just need to try and get an idea about how short of breath you are so are you able to like walk up a flight of stairs for example or are you short of breath at rest oh yeah its like when i am doing walking and i do exercise now and then so it it has not been super bad like has not stopped me from doing any of those things but its been pretty unusual and a little bit worrying and you are a bit concerned about that okay so i just need to ask a few things about your background as well so do you have any other medical conditions or medical history no just no no past medical history no no history of asthma no and any history of clots on your legs or your lungs so these are ddps or ps and none of your families had those clots in the legs or lungs well my mother had lung cancer your mother had lung cancer do you smoke no you ever smoked or been exposed to asbestos you know do not know if asbestos ever smoked i mean once or twice in amsterdam with that car but not really okay um and ah this so just going back to the your symptoms of shortness of breath with the cough its a dry cough no you are not coughing up any phlegm um do you do you have and you say you do not have any chest pain as such um are you taking any medications currently at the moment no i am not okay are you allergic to any medications not any medication but i am allergic to peanuts peanuts okay and and you mentioned that your mother had lung cancer and any other family history of any significant illnesses when running in your family no no that is the only one just lung cancer from my mother just lung cancer okay and you say you have a cold so do you have sinus congestion or um no it seems to be almost entirely just my throat like j just your just your throat and any recent travel or have you always lived in the you k uh no so i i have not always lived in the you k like so i was born in the you s and moved over about twelve years ago but in terms of recent travel just to europe nowhere to exotic okay so no so no recent travel no significant recent travel anywhere um okay and are you coughing up anything other than um so you are not coughing up blood or anything like that no um good and are you feeling feverish hot cold sweaty yeah so a little bit feverish um at first so the first three or so days of this but then the fevers gone away okay and in general do you sorry yeah i was just going to say also had a bit of a headache like headaches that come and go rather but like right now its fine okay and in general would you say you are feeling you are you are beginning to to feel better worse or or sort of staying the same so its like its up and down so so let us see so i started last week and i stayed home from work two days this week i think it was maybe tuesday and then thursday so like i felt better and then worse again and then better and then worse again so its been yeah a kind of constant but constant in being variable but okay and i just really need to ask any other sort of risk factors um that you may have so um no sort of significant weight loss um or unexplained weight loss any so no weight loss but i have been have been losing my appetite recently and i mean i usually eat a lot so i enjoy eating as well but like that is been a bit concerning you have been losing your appetite recently yes and you are a little bit concerned about that but you have not you have not lost any weight that you think no not that and any um sort of rashes or anything uh and you no rash no you can go okay um so i would ask to examine you now but um i i do not know if i could sort of look inside your throat at least to see if there is a probably there is oh we can try it on oh no well no its okay i might think about doing it have you got any lumps or bumps around your neck that you can feel ah no not the no okay and and so finally you you were talking about i mean it sounds to me that um you have been a little bit up and down sore throat developed a dry cough and you are slightly short of breath but not too overly concerningly short of breath what i would say were just coming to the end so consultation hours is if you feel significantly worse um uh if you get more short of breath or sudden change in your breathlessness um or breathlessness that you are concerned about and i would advise you to see your gp and actually see somebody physically um uh but i think for now i can sort of try and reassure you that um if this clears up as i expected it would so expect this to sort of be getting better in the next four or five days if its not please get in touch with the medical professional again and ill expect it to and so therefore i would not be concerned about tuberculosis your concerns about lung cancer was that the other thing you were concerned about yeah yeah so so um again if you are not getting better please see somebody again i have just got four seconds now so nice talking to you and we have got to we have got to tidy up yeah okay so and ill provide you with a sick note just to give you a few more days off work and paracetamol lots of fluids and rest up and as i say if you are not feeling better please get in touch okay alright have a good day thank you alright</t>
-        </is>
-      </c>
-      <c r="K2" t="n">
-        <v>0.2046204620462046</v>
-      </c>
-      <c r="L2" t="n">
-        <v>30</v>
+          <t>male or a female i am a male how old are you i am sixtyfive years old i hope you do not mind i address you as mr emeka i do not mind okay thank you very much so what brought you to the clinic today i am having difficulty in urinating you have been having difficulty in urinating for how long has this been that is nothing for two weeks you have been having difficulty urinating for two weeks yes did this started gradually or it was gradual in onset it was gradual in onset has it been constant has it always been there or it just comes and goes or you feel this within a particular period of the day i think it got bad recently it was not constant before but now it is constant okay thank you very much is this pain while urinating associated with the burning sensation it is it is not associated with pain or a burning sensation okay so it is not associated with any pain or a burning sensation yes it is not do you feel the urgency to urinate yes i feel the urgency to you ring it and then are you able to pass out this urine when you feel this urgency to you in it i am unable to pass out here okay do you feel frequent urination the urge to always go to the toilet yes i am always just into it especially the night okay nocturia so you always use the toilet in the night yes at morning at night at night like how many times you you need in the night it is very frequent i cannot tell more than you used to before yes it is more than the usual two times to zero times i usually use the toilet but now it is about five times do you strain to urinate yes i strain a lot and my urine dribbles okay it dribbles yes after i might know if there is blood in the urine there is no blood in this urine there is no fever i do not have ist have fever is there pus there is no pus okay so do you have lower abdominal pain i do not have abdominal pain oh thank you very much is there a history of trauma or any recent catarization or urethra instrumentation no there is none there is no history of trauma or catarization i do not have any history oh thank you very much are you a known hypertensive patient are you hypertensive yes i have been hypertensive for ten years now okay you have been hypertensive for ten years how do you know you are hypertensive i was told that the hospital  i was diagnosed there you were diagnosed in the hospital ten years ago yes yes and you have been on medications yes that is been controlled by medications okay thank you very much how about being diabetic are you diabetic no i am not diabetic you are not diabetic okay is there a family history of similar condition is there anyone in your family that has similar condition yeah i can remember my dad had similar condition when he was old when he was old what exactly was the problem did he also feel pain while trying to urinate he had some urinary problem i cannot tell exactly i was young at that time okay thank you very much are you a smoker i do not smoke do you take alcohol yeah i consume alcohol occasionally do you take any recreational drugs substance abuse no thank you very much are you on your hypertensive agent yes i am on some drugs they gave me to control the hypertension can you tell me the name of the drug you are on i am on lodipine okay you are on lodipine is there any other drug you are on i am not on any other drug they gave me just that one oh thank you very much do you have any allergies are you allergic to any drug or medication no i am not okay thank you very much</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>male or a female i am a male how old are you i am sixtyfive years old i hope you do not mind i address you as mr i maker i do not mind okay thank you very much so what brought you to the clinic today i have been having difficulty in urinating you have been having difficulty in urinating for how long has this been that is lasted for two weeks you have been having difficulty urinating for two weeks yes did this start as gradually or it was gradual in onset it was gradual in onset has it been constant has he always been there or he just comes and goes or he feels this within a particular period of the day i think he got bad of recent it was not constant before but now it is constant okay thank you very much is this pain while urinating associated with the burning sensation it is not associated with pain burning sensation it is not associated with any pain or a burning sensation yes it is not do you feel the urgency to you know and then are you able to pass out this urine when you feel this urgency to you know i am unable to pass out okay do you feel frequent urination the urge to always go to the toilet yes i am always using the toilet especially in the night okay nocturia so you always use the toilet in the night yes at morning at night at night like how many times you you need in the night it is very frequent i cannot tell more than it used to be for yes it is more than the usual two times to zero times i usually use the toilet but now it is about five times do you strain to urinate yes i strain a lot and my urine bubbles okay it bubbles yes after urination  i know if there is blood in the urine there is no blood in this urine there is no fever i do not have a fever is there pus there is no pus so okay so do you have lower abdominal pain i do not have any abdominal pain oh thank you very much is there a history of trauma or any recent catheterization or ureteral instrumentation no there is none there is no history of trauma or catheterization i do not have any history of that oh thank you very much are you a known hypertensive yes i have been hypertensive for ten years now okay you have been hypertensive for ten years how do you know you are hypertensive i was told that i was diagnosed in the hospital i was diagnosed in the hospital ten years ago yes and you have been on medications yes that has been controlled by medications okay thank you very much how about being diabetic are you diabetic no i am not diabetic is there anyone in your family that has similar condition yeah i can remember my dad had similar condition when he was old when he was old what exactly was the problem did he also feel pain while trying to urinate he had some urinary problem i cannot tell exactly i was young at that time okay thank you very much are you a smoker i do not smoke do you take alcohol yeah i consume alcohol occasionally are you on your hypertensive agents yes i am on some drugs they gave me to control the hypertension can you tell me the name of the drug you are on i am on load the pin is there any other drug you are on i am not on any other drug they gave me just that one thank you very much do you have any other justifications are you allergic to any drug or medication no i am not okay thank you very much</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>male or a female male how old are you i am sixtyfive years old i hope you do not mind i address you as mr emeka i do not mind okay thank you very much so what brought you to the clinic today i am having difficulty in urinating you have been having difficulty in urinating for how long has this been it has lasted for two weeks you have been having difficulty urinating for two weeks yes did this start gradually or it was gradual nonsense okay it was gradual in on set has it been constant has it always been there or it just comes and goes or you feel this within the particular period of the day i think it got bad of recent it was not constant before but now it is constant okay thank you very much is this pain while urinating associated with a burning sensation it is not associated with pain or a burning sensation okay so it is not associated with any pain or a burning sensation yes it is not do you feel the urgency to urinate yes i feel the urgency to urinate and then are you able to pass out this urine when you feel this urgency to urinate i am unable to pass out urine okay do you feel frequent urination the urge to always go to the toilet yes i am always using the toilet especially in the night okay nocturia so you always use the toilet in the night yes at morning at night at night like how many times do you urinate in the night it is very frequent i cannot tell more than it used to before yes it is more than the usual two times to zero times i usually use the toilet but now it is about five times do you strain to urinate yes i strain a lot and my urine dribbles okay it dribbles yes after urination may i know if there is blood in the urine there is no blood in this urine there is no fever i do not have fever is there pulse there is no pulse okay so do you have lower abdominal pain i do not have abdominal pain oh thank you very much is there a history of trauma or any recent caterization or urethra instrumentation no there is none there is no history of trauma or catheterization i do not have any history of that oh thank you very much are you a known hypertensive patient are you hypertensive yes i have been hypertensive for ten years now okay you have been hypertensive for ten years how do you know you are hypertensive i was told at the hospital i was diagnosed there you were diagnosed in a hospital ten years ago yes and you have been on medications yes that is been controlled by medications okay thank you very much how about being diabetic are you diabetic no i am not diabetic you are not diabetic okay is there a family history of similar conditions is there anyone in your family that has similar conditions yeah i can remember my dad had a similar condition when he was old when he was old what exactly was the problem did he also feel pain while trying to urinate he had some urinal problem i cannot tell exactly i was young at that time okay thank you very much are you a smoker i do not smoke do you take alcohol yeah i consume alcohol occasionally do you take any recreational drug substance abuse no thank you very much are you on your hypertensive agent yes i am on some drugs they gave me to control the hypertension can you tell me the name of the drug you are on i am not pain okay you are on and you know the pain is there any other drug you are on i am not on any other drug they gave me just that one oh thank you very much do you have any allergies do you have are you allergic to any drug or medication no i am not okay thank you very much madam</t>
+        </is>
       </c>
       <c r="M2" t="n">
-        <v>240</v>
+        <v>0.1311953352769679</v>
       </c>
       <c r="N2" t="n">
-        <v>102</v>
+        <v>27</v>
       </c>
       <c r="O2" t="n">
-        <v>0.1848184818481848</v>
+        <v>15</v>
       </c>
       <c r="P2" t="n">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="Q2" t="n">
-        <v>209</v>
+        <v>0.1938775510204082</v>
       </c>
       <c r="R2" t="n">
-        <v>90</v>
-      </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>['ohh', 'um', 'uh', 'ninth', 'yeah', 'yeah', 'i', 'am', 'what', 'what', 'came', 'yes', 'uh', 'ok', 'uh', 'are', 'you', 'coughing', 'up', 'anything', 'no', 'its', 'very', 'dry', 'ok', 'so', 'am', 'i', 'am', 'the', 'uh', 'um', 'um', 'ok', 'you', 'it', 'could', 'be', 'could', 'be', 'also', 'be', 'could', 'be', 'none', 'of', 'um', 'uh', 'um', 'ok', 'uh', 'uh', 'uh', 'like', 'that', 'a', 'um', 'ok', 'um', 'um', 'no', 'have', 'been', 'yeah', 'uh', 'uh', 'a', 'bit', 'of', 'both', 'you', 'are', 'how', 'ah', 'week', 'so', 'the', 'whole', 'same', 'throughout', 'the', 'day', 'um', 'uh', 'so', 'um', 'so', 'uh', 'flight', 'um', 'or', 'of', 'its', 'so', 'um', 'it', 'uh', 'um', 'past', 'medical', 'history', 'no', 'no', 'um', 'uh', 'uh', 'uh', 'you', 'know', 'of', 'counts', 'um', 'uh', 'so', 'the', 'no', 'you', 'are', 'any', 'um', 'do', 'uh', 'do', 'not', 'you', 'um', 'uh', 'um', 'uh', 'uh', 'um', 'run', 'your', 'lung', 'cancer', 'ok', 'um', 'so', 'your', 'uh', 'i', 'moved', 'over', 'well', 'it', 'was', 'of', 'any', 'uh', 'you', 'no', 'no', 'yeah', 'uh', 'um', 'it', 'but', 'like', 'uh', 'feeling', 'you', 'are', 'you', 'are', 'to', 'or', 'um', 'so', 'it', 'yeah', 'that', 'makes', 'ok', 'have', 'been', 'and', 'and', 'i', 'like', 'so', 'of', 'yes', 'or', 'that', 'not', 'that', 'you', 'can', 'think', 'of', 'ok', 'to', 'there', 'is', 'ohh', 'a', 'uh', 'you', 'you', 'uh', 'mean', 'um', 'um', 'mmhmm', 'um', 'uh', 'um', 'no', 'go', 'and', 'see', 'um', 'um', 'uh', 'uh', 'um', 'i', 'um', 'um', 'uh', 'um', 'and', 'yeah', 'yeah', 'so', 'um', 'um', 'have', 'to', 'we', 'uh', 'all', 'right', 'uh', 'um', 'um', 'uh', 'good', 'day', 'bye']</t>
-        </is>
-      </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>['sorry', 'i', 'i', 'call', 'that', 'then', 'little', 'is', 'some', 'thank', 'a', 'a', 'those', 'let', 'us', 'today', 'or', 'super', 'these', 'are', 'have', 'no', 'all', 'feel', 'better', 'i', 'no', 'the', 'is', 'okay']</t>
-        </is>
-      </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>['ok', 'uh', 'my', 'names', 'uh', 'ok', 'and', 'are', 'ohh', 'happy', 'how', 'is', 'ok', 'ok', 'going', 'ask', 'so', 'there', 'but', 'it', 'could', 'it', 'great', 'so', 'so', 'anything', 'were', 'is', 'ok', 'uh', 'um', 'um', 'ill', 'i', 'shortness', 'of', 'ok', 'the', 'so', 'todays', 'develop', 'nighttime', 'no', 'a', 'at', 'ohh', 'exercises', 'superbad', 'worrying', 'ok', 'so', 'these', 'uh', 'that', 'with', 'if', 'that', 'ok', 'coughing', 'up', 'uh', 'no', 'no', 'ok', 'ok', 'uh', 'in', 'just', 'like', 'so', 'just', 'in', 'terms', 'too', 'ok', 'ok', 'and', 'if', 'you', 'have', 'not', 'not', 'not', 'ohh', 'ok', 'can', 'no', 'that', 'ok', 'um', 'then', 'somebody', 'a', 'are', 'ohh', 'got', 'ok', 'off', 'paracetemol', 'ok', 'have', 'a']</t>
-        </is>
-      </c>
-      <c r="V2" t="inlineStr">
-        <is>
-          <t>['um', 'ninth', 'yeah', 'yeah', 'i', 'am', 'is', 'ok', 'what', 'yes', 'uh', 'ok', 'uh', 'i', 'am', 'uh', 'um', 'um', 'what', 'might', 'be', 'going', 'on', 'you', 'said', 'that', 'you', 'had', 'a', 'cold', 'ok', 'well', 'i', 'mean', 'you', 'you', 'know', 'how', 'we', 'all', 'are', 'once', 'this', 'happens', 'you', 'google', 'it', 'and', 'there', 'seems', 'to', 'be', 'all', 'kinds', 'of', 'bad', 'things', 'it', 'could', 'be', 'it', 'could', 'be', 'could', 'be', 'a', 'cold', 'or', 'flu', 'obviously', 'but', 'it', 'could', 'also', 'be', 'tuberculosis', 'it', 'could', 'be', 'cancer', 'always', 'comes', 'up', 'it', 'will', 'be', 'good', 'if', 'none', 'of', 'those', 'great', 'so', 'and', 'um', 'ok', 'uh', 'uh', 'uh', 'um', 'ok', 'no', 'uh', 'a', 'bit', 'of', 'both', 'you', 'are', 'ah', 'so', 'last', 'week', 'so', 'the', 'whole', 'um', 'uh', 'so', 'um', 'so', 'uh', 'um', 'or', 'its', 'so', 'um', 'uh', 'um', 'no', 'um', 'uh', 'uh', 'uh', 'the', 'that', 'of', 'uh', 'do', 'not', 'you', 'uh', 'to', 'uh', 'uh', 'run', 'with', 'so', 'nose', 'is', 'like', 'so', 'i', 'it', 'was', 'any', 'uh', 'you', 'no', 'uh', 'uh', 'it', 'yeah', 'but', 'ok', 'um', 'it', 'makes', 'ok', 'and', 'and', 'i', 'so', 'of', 'yes', 'or', 'that', 'not', 'that', 'ok', 'you', 'uh', 'mmhmm', 'go', 'and', 'see', 'a', 'um', 'uh', 'i', 'um', 'um', 'i', 'would', 'um', 'are', 'and', 'ohh', 'yeah', 'yeah', 'um', 'we', 'uh', 'all', 'right', 'uh', 'um', 'um', 'uh']</t>
-        </is>
-      </c>
-      <c r="W2" t="inlineStr">
-        <is>
-          <t>['name', 'sorry', 'discuss', 'yeah', 'i', 'i', 'call', 'up', 'then', 'little', 'in', 'thank', 'a', 'a', 'oh', 'today', 'or', 'start', 'symptoms', 'night', 'super', 'are', 'ddps', 'or', 'you', 'no', 'almost', 'you', 'you', 'you', 'really', 'it', 'on', 'hours', 'we', 'have', 'okay']</t>
-        </is>
-      </c>
-      <c r="X2" t="inlineStr">
-        <is>
-          <t>['ok', 'ohh', 'uh', 'names', 'uh', 'uh', 'ok', 'uh', 'ohh', 'just', 'how', 'bad', 'ok', 'ok', 'so', 'ideas', 'its', 'ok', 'uh', 'um', 'um', 'ok', 'todays', 'three', 'started', 'nighttime', 'ohh', 'exercises', 'superbad', 'ok', 'uh', 'no', 'one', 'in', 'familys', 'on', 'with', 'if', 'counts', 'ok', 'uh', 'flem', 'uh', 'no', 'no', 'ok', 'ok', 'um', 'um', 'uh', 'ok', 'my', 'uk', 'uk', 'us', 'well', 'too', 'ok', 'ok', 'ok', 'uh', 'and', 'if', 'that', 'not', 'not', 'think', 'of', 'ohh', 'ohh', 'ok', 'a', 'uh', 'no', 'that', 'ok', 'um', 'um', 'of', 'now', 'then', 'no', 'expect', 'a', 'uh', 'are', 'ok', 'paracetemol', 'ok', 'bye']</t>
-        </is>
+        <v>23</v>
+      </c>
+      <c r="S2" t="n">
+        <v>52</v>
+      </c>
+      <c r="T2" t="n">
+        <v>58</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0.1034985422740525</v>
+      </c>
+      <c r="V2" t="n">
+        <v>23</v>
+      </c>
+      <c r="W2" t="n">
+        <v>8</v>
+      </c>
+      <c r="X2" t="n">
+        <v>40</v>
       </c>
       <c r="Y2" t="inlineStr">
         <is>
-          <t xml:space="preserve">      ref_ix  hyp_ix reference hypothesis operation  index_edit_ops
-0          0       0     hello      hello         =            &lt;NA&gt;
-1          1       1       can        can         =            &lt;NA&gt;
-2          2       2       you        you         =            &lt;NA&gt;
-3          3       3      hear       hear         =            &lt;NA&gt;
-4          4       4        me         me         =            &lt;NA&gt;
-...      ...     ...       ...        ...       ...             ...
-1843    1813    &lt;NA&gt;      good          _       del             369
-1844    1814    &lt;NA&gt;       day          _       del             370
-1845    1815    1606     thank      thank         =            &lt;NA&gt;
-1846    1816    1607       you        you         =            &lt;NA&gt;
-1847    1817    &lt;NA&gt;       bye          _       del             371
-[1848 rows x 6 columns]</t>
+          <t>['if', 'okay', 'in', 'okay', 'recent', 'in', 'i', 'that', 'okay', 'that', 'that', 'other', 'do', 'you', 'have']</t>
         </is>
       </c>
       <c r="Z2" t="inlineStr">
         <is>
-          <t xml:space="preserve">      ref_ix  hyp_ix reference hypothesis operation  index_edit_ops
-0          0       0     hello      hello         =            &lt;NA&gt;
-1          1       1       can        can         =            &lt;NA&gt;
-2          2       2       you        you         =            &lt;NA&gt;
-3          3       3      hear       hear         =            &lt;NA&gt;
-4          4       4        me         me         =            &lt;NA&gt;
-...      ...     ...       ...        ...       ...             ...
-1850    1813    1641      good       good         =            &lt;NA&gt;
-1851    1814    1642       day        day         =            &lt;NA&gt;
-1852    1815    1643     thank      thank         =            &lt;NA&gt;
-1853    1816    1644       you        you         =            &lt;NA&gt;
-1854    1817    1645       bye    alright       sub             335
-[1855 rows x 6 columns]</t>
+          <t>['i', 'am', 'i', 'it', 'it', 'is', 'so', 'the', 'the', 'you', 'ring', 'you', 'in', 'so', 'a', 'ist', 'have', 'pus', 'any', 'yes', 'being', 'i', 'am', 'on', 'other', 'drug', 'no']</t>
         </is>
       </c>
       <c r="AA2" t="inlineStr">
         <is>
-          <t>hello can you hear me [SUB:ok-&gt;okay] [DEL:ohh] yes i can can you hear me yeah good good so my name is joe i am a doctor [DEL:um] here at babylon can i just confirm your name please [SUB:uh-&gt;my] [SUB:my-&gt;name] [SUB:names-&gt;is] vincent and your date of birth [SUB:uh-&gt;nineth] [DEL:uh] [DEL:ninth] of may two thousand and sixteen [SUB:ok-&gt;okay] great [INS:sorry] [SUB:and-&gt;i] [SUB:are-&gt;know] you in a uh a safe place [SUB:ohh-&gt;oh] sorry a safe and confidential place to talk and just [INS:i] [SUB:happy-&gt;have] to go ahead with the consultation [DEL:yeah] [DEL:yeah] [DEL:i] [DEL:am] yes yes i am great so how can i help yeah so [INS:i] have a [INS:call] [INS:that] i have been having a cough and a sore throat for about a week and its been causing me problems i have had to stay away from work for about three or four of those days because of [SUB:how-&gt;a] bad [SUB:is-&gt;history] [SUB:ok-&gt;okay] i am sorry to hear that so you have had a cough and a sore throat for about a week and what came [DEL:what] [DEL:what] [DEL:came] first [DEL:yes] [DEL:uh] the sore throat came first and then after a day or two the cough [SUB:ok-&gt;okay] [DEL:ok] and [DEL:uh] [DEL:are] [DEL:you] [DEL:coughing] [DEL:up] [DEL:anything] [DEL:no] [DEL:its] [DEL:very] [DEL:dry] [DEL:ok] [DEL:so] i [DEL:am] [DEL:i] [DEL:am] just [SUB:going-&gt;want] to [SUB:ask-&gt;thank] a few questions about [DEL:the] [DEL:uh] your current symptoms and [INS:then] a little bit about your background [DEL:um] and something else about what we can do a little bit later on in the consultation to help you [SUB:so-&gt;but] before we go on anything you are particularly concerned about [DEL:um] or have any ideas what might be going on you said that you had a cold [DEL:ok] well i mean you [DEL:you] know how we all are once this happens you google it and [SUB:there-&gt;it] seems to be all kinds of bad things it could be [DEL:it] [DEL:could] [DEL:be] [DEL:could] [DEL:be] a cold or flu obviously [SUB:but-&gt;obviously] [SUB:it-&gt;because] [SUB:could-&gt;we] [DEL:also] [DEL:be] tuberculosis [SUB:it-&gt;the] [DEL:could] [DEL:be] cancer always comes up so it will be good if [DEL:none] [DEL:of] those [SUB:great-&gt;right] [SUB:so-&gt;say] [SUB:so-&gt;say] yeah i can provide a [INS:little] bit of reassurance [DEL:um] and [DEL:uh] we can talk about those a little bit as well and was there [SUB:anything-&gt;any] you [SUB:were-&gt;are] particularly expecting or hoping to get out of this consultation [DEL:um] [DEL:ok] [DEL:uh] [DEL:uh] well [DEL:uh] yeah so reassurance so [DEL:like] hopefully some sense that its not anything too serious but also [SUB:is-&gt;if] there [INS:is] anything you can prescribe me to make it better or any advice or maybe even a sick note so [DEL:that] if i need to stay away from work for a bit longer i can get one sure sure [SUB:ok-&gt;okay] all right so well talk a little bit about the symptoms and i am sure we can get [DEL:a] [DEL:um] those things [INS:some] [SUB:uh-&gt;secrets] and some reassurance [INS:thank] [SUB:um-&gt;you] about your concerns [DEL:ok] so [DEL:um] you mentioned that you started with [INS:a] sore throat about a week ago developed into [INS:a] bit of a dry cough [SUB:um-&gt;and] [SUB:ill-&gt;i] just ask a few questions around those [INS:those] so [DEL:um] do you have any shortness of breath [DEL:no] yes yes [SUB:i-&gt;were] [DEL:have] [DEL:been] having [SUB:shortness-&gt;shorts] [SUB:of-&gt;oh] yeah i have been having shortness of breath [DEL:yeah] you are short of breath and [DEL:uh] do you have any wheeze or chest pain [DEL:uh] yeah [DEL:a] [DEL:bit] [DEL:of] [DEL:both] you are [DEL:you] [DEL:are] feeling a bit wheezy with some chest pain as well yes [SUB:ok-&gt;okay] and [DEL:how] [DEL:ah] when did you start to develop [SUB:the-&gt;a] shortness of breath [INS:let] [INS:us] [SUB:so-&gt;see] so the sore throat so [INS:today] [SUB:todays-&gt;is] friday sore throat was about last [DEL:week] friday or thursday cough was saturday or sunday so the [DEL:so] [DEL:the] shortness of breath was i think shortly after the cough so maybe a day or two later so three [INS:or] four days ago three or four days ago you started [SUB:develop-&gt;developing] and is the cough worse at [SUB:nighttime-&gt;night] [SUB:no-&gt;time] no its the same throughout the [DEL:whole] day [DEL:same] [DEL:throughout] [DEL:the] [DEL:day] [DEL:um] and [DEL:uh] when you say you are short of breath just need to try and get an idea about how short of breath you are so are you able to [DEL:so] [DEL:um] [DEL:so] [DEL:uh] like walk up [SUB:a-&gt;flights] [DEL:flight] of stairs for example [DEL:um] or [DEL:or] are you short [DEL:of] breath [SUB:at-&gt;of] rest [SUB:ohh-&gt;oh] yeah its [DEL:its] like [DEL:so] when i am doing walking [DEL:um] and i do [SUB:exercises-&gt;exercise] now and then so it [DEL:it] has not been [INS:super] [SUB:superbad-&gt;bad] like has not stopped me from doing any of those things but its been pretty unusual and a little bit [SUB:worrying-&gt;worried] and you are a bit concerned about that [SUB:ok-&gt;okay] so i just need to ask a few [DEL:uh] things about your background as well so [DEL:um] do you have any other medical conditions or medical history no just no no [DEL:past] [DEL:medical] [DEL:history] no [DEL:no] [DEL:no] history of asthma no [DEL:um] and any [DEL:uh] [DEL:uh] history of [DEL:uh] clots on your legs or your lungs [INS:these] [INS:are] [SUB:so-&gt;ddts] [SUB:these-&gt;or] [SUB:uh-&gt;ps] no one in your familys had those clots on the legs or the lungs well my mother had lung cancer your mother had lung cancer do you smoke no [INS:have] you ever smoked or been exposed to asbestos [SUB:that-&gt;i] [DEL:you] [DEL:know] [DEL:of] do not know [SUB:with-&gt;if] asbestos ever smoked i mean once or twice in amsterdam [SUB:if-&gt;in] [SUB:that-&gt;dakar] [DEL:counts] but not really [SUB:ok-&gt;okay] [DEL:um] and [DEL:uh] this [DEL:so] just going back to [DEL:the] your symptoms of shortness of breath with the cough its a dry cough [DEL:no] [DEL:you] [DEL:are] not [SUB:coughing-&gt;cough] [SUB:up-&gt;cap] [DEL:any] flem [DEL:um] do [DEL:do] you have [DEL:uh] and you [DEL:do] [DEL:not] [DEL:you] say you do not have any chest pain as such [DEL:um] [DEL:uh] are you taking any medications currently at the moment [INS:no] [SUB:uh-&gt;i] [SUB:no-&gt;am] [SUB:no-&gt;not] [SUB:ok-&gt;okay] are you allergic to any medications not to any medication but i am allergic to peanuts peanuts [SUB:ok-&gt;okay] [DEL:um] and [DEL:uh] you mentioned that your mother had [DEL:uh] lung cancer [DEL:um] any other family history of any significant illnesses [SUB:uh-&gt;when] [DEL:run] running [SUB:in-&gt;into] [DEL:your] family no no that is the only one just lung cancer from my mother [SUB:just-&gt;okay] [DEL:lung] [DEL:cancer] [DEL:ok] and you say you have a cold so do you have sinus congestion or [DEL:um] no it seems to be [INS:all] entirely with just my throat [DEL:so] like my nose is [SUB:like-&gt;just] [SUB:so-&gt;running] [SUB:just-&gt;out] [DEL:your] just your throat and any recent travel or have you always lived in the uk [DEL:uh] no so i i [DEL:i] have not always lived in the uk like so i was born in the us and [DEL:moved] [DEL:over] [DEL:well] [DEL:it] [DEL:was] twelve years ago but [SUB:in-&gt;its] [SUB:terms-&gt;a] [DEL:of] recent travel just to europe nowhere [SUB:too-&gt;to] exotic [SUB:ok-&gt;okay] so no so no recent travel no significant recent travel [DEL:any] anywhere um [SUB:ok-&gt;okay] and are you coughing up anything other than um [DEL:uh] so you [DEL:you] are not coughing up blood or anything like that [DEL:no] [DEL:no] um good and uh are you feeling feverish hot cold sweaty [DEL:yeah] so a little bit feverish [DEL:uh] [DEL:um] at first so the first three or so days of this but then [DEL:it] the fevers gone away ok and in general do you [INS:feel] [INS:better] sorry yeah yeah i was just going to say [INS:i] also had a bit of a headache [DEL:but] like headaches that come and go rather but [DEL:like] right now its fine [DEL:uh] ok and in general would you say you are [DEL:feeling] [DEL:you] [DEL:are] [DEL:you] [DEL:are] beginning to [DEL:to] feel better worse or [DEL:or] sort of [DEL:um] staying the same so its like its up and down so [DEL:so] let us see so i [DEL:it] started last week and i stayed home from work two days this week i think it was maybe tuesday and then thursday so like i felt better and then worse again and then better and then worse again so its been [DEL:yeah] a kind of constant but constant [SUB:and-&gt;in] being variable [SUB:if-&gt;okay] [DEL:that] [DEL:makes] [DEL:ok] and i just need to ask any other sort of risk factors um that you may have so um no sort of significant weight loss um or unexplained weight loss any so no [INS:no] weight loss but i have been [DEL:have] [DEL:been] losing my appetite recently and i mean i usually eat a lot so [DEL:and] i [DEL:and] [DEL:i] enjoy eating as well but [DEL:like] [DEL:so] that is been a bit concerning you have been losing your appetite recently yes and you are a little bit concerned about that but you have not [SUB:you-&gt;lost] [SUB:have-&gt;any] [SUB:not-&gt;weight] lost any weight that you think [DEL:of] [DEL:yes] no not that and any um sort of rashes or anything [DEL:or] uh and you no [SUB:not-&gt;no] [SUB:not-&gt;okay] [DEL:that] [DEL:not] [DEL:that] [DEL:you] [DEL:can] [DEL:think] [DEL:of] [DEL:ok] um so i would ask to examine you now but um i i do not know if i could sort of look inside your throat at least [DEL:to] see if there is a probably [DEL:there] [DEL:is] [DEL:ohh] we can try [SUB:ohh-&gt;oh] no well no its [SUB:ok-&gt;okay] i might think about doing [DEL:a] have you got any lumps or bumps around your neck that you [SUB:can-&gt;could] feel [DEL:uh] no [SUB:no-&gt;not] [SUB:that-&gt;the] [DEL:you] no [SUB:ok-&gt;okay] [SUB:um-&gt;and] and so finally you [DEL:you] were talking about [DEL:uh] i [DEL:mean] it sounds to me that [DEL:um] you have been a little bit up and down sore throat developed a dry cough [DEL:um] you are slightly short of breath but not too overly concerningly short of breath what i would say were just coming to the end of [INS:the] consultation now [INS:is] if you feel significantly worse [DEL:mmhmm] [DEL:um] [DEL:uh] if you get more short of breath or sudden change in your breathlessness [DEL:um] or breathlessness that you are concerned about [SUB:then-&gt;and] i would advise you to see [DEL:no] [DEL:go] [DEL:and] [DEL:see] a gp [DEL:um] and actually see [SUB:somebody-&gt;something] physically [DEL:um] [DEL:uh] but i think for now i can sort of [DEL:uh] try and reassure you that [DEL:um] if this clears up as i expect it would so [DEL:i] expect this to sort of be getting better in the next four or five days [DEL:um] if its not please get in touch with [SUB:a-&gt;the] medical professional again [DEL:um] and [DEL:uh] i would expect it to and so therefore i would not be concerned about tuberculosis [DEL:um] your concerns about lung cancer are [DEL:and] was that the other thing you [SUB:are-&gt;were] concerned about [SUB:ohh-&gt;oh] yeah yeah [DEL:yeah] [DEL:yeah] so [DEL:so] [DEL:um] again if you are not getting better please see somebody again [DEL:um] i have just got four seconds now so nice talking to you and [DEL:have] we [SUB:got-&gt;have] [DEL:to] [DEL:we] got to tidy up yeah [INS:okay] [SUB:ok-&gt;okay] so [DEL:uh] [DEL:all] [DEL:right] [DEL:uh] and ill provide you with a sick note just to give you a few more days [SUB:off-&gt;of] work [DEL:um] and [SUB:paracetemol-&gt;paracetamol] lots of fluids [DEL:um] and [DEL:uh] rest up and as i say if you are not feeling better please get in touch [SUB:ok-&gt;okay] [SUB:have-&gt;all] [SUB:a-&gt;right] [DEL:good] [DEL:day] thank you [DEL:bye]</t>
+          <t>['it', 'has', 'started', 'it', 'goes', 'of', 'a', 'urinate', 'urinate', 'urine', 'visiting', 'the', 'toilet', 'visit', 'do', 'urinate', 'straint', 'in', 'alot', 'dripples', 'dripples', 'yeah', 'urination', 'may', 'pause', 'pause', 'oo', 'okay', 'catherization', 'not', 'not', 'catherization', 'of', 'main', 'at', 'a', 'it', 'has', 'have', 'has', 'urinal', 'can', 'agents', 'give', 'amlodepine', 'amlodepine', 'give', 'okay']</t>
         </is>
       </c>
       <c r="AB2" t="inlineStr">
         <is>
-          <t>hello can you hear me [SUB:ok-&gt;okay] [SUB:ohh-&gt;hey] yes i can can you hear me yeah good good so my name is joe i am a doctor [DEL:um] here at babylon can i just confirm your name please [SUB:uh-&gt;hey] my [INS:name] [SUB:names-&gt;is] vincent and your date of birth [SUB:uh-&gt;ah] [SUB:uh-&gt;nine] [DEL:ninth] of may two thousand and sixteen [SUB:ok-&gt;okay] great [INS:sorry] and are you in a [SUB:uh-&gt;be] a safe place [SUB:ohh-&gt;oh] sorry a safe and confidential place to talk and [INS:discuss] [INS:yeah] [INS:i] [SUB:just-&gt;am] happy to go ahead with the consultation [DEL:yeah] [DEL:yeah] [DEL:i] [DEL:am] yes yes i am great so how can i help yeah so [INS:i] have a [INS:call] [INS:up] i have been having a cough and a sore throat for about a week and its been causing me problems i have had to stay away from work for about three or four of those days because of [SUB:how-&gt;it] [SUB:bad-&gt;okay] [DEL:is] [DEL:ok] i am sorry to hear that so you have had a cough and a sore throat for about a week and what came what [DEL:what] came first [DEL:yes] [DEL:uh] the sore throat came first and then after a day or two the cough [SUB:ok-&gt;okay] [DEL:ok] and [DEL:uh] are you coughing up anything no its very dry [SUB:ok-&gt;okay] so i am [DEL:i] [DEL:am] just going to ask a few questions about the [DEL:uh] your current symptoms and [INS:then] a little bit about your background [DEL:um] and something else about what we can do a little bit later on in the consultation to help you [SUB:so-&gt;but] before we go on anything you are particularly concerned about [DEL:um] or have any [SUB:ideas-&gt;right] [DEL:what] [DEL:might] [DEL:be] [DEL:going] [DEL:on] [DEL:you] [DEL:said] [DEL:that] [DEL:you] [DEL:had] [DEL:a] [DEL:cold] [DEL:ok] [DEL:well] [DEL:i] [DEL:mean] [DEL:you] [DEL:you] [DEL:know] [DEL:how] [DEL:we] [DEL:all] [DEL:are] [DEL:once] [DEL:this] [DEL:happens] [DEL:you] [DEL:google] [DEL:it] [DEL:and] [DEL:there] [DEL:seems] [DEL:to] [DEL:be] [DEL:all] [DEL:kinds] [DEL:of] [DEL:bad] [DEL:things] [DEL:it] [DEL:could] [DEL:be] [DEL:it] [DEL:could] [DEL:be] [DEL:could] [DEL:be] [DEL:a] [DEL:cold] [DEL:or] [DEL:flu] [DEL:obviously] [DEL:but] [DEL:it] [DEL:could] [DEL:also] [DEL:be] [DEL:tuberculosis] [DEL:it] [DEL:could] [DEL:be] [DEL:cancer] [DEL:always] [DEL:comes] [DEL:up] so [DEL:it] [DEL:will] [DEL:be] [DEL:good] [DEL:if] [DEL:none] [DEL:of] [DEL:those] [DEL:great] so [DEL:so] yeah i can provide a [INS:little] bit of reassurance um and uh we can talk about those a little bit as well [DEL:and] was there anything you were particularly expecting or hoping to get out of this consultation [DEL:um] [DEL:ok] [DEL:uh] [DEL:uh] well [DEL:uh] yeah so reassurance so like hopefully [INS:in] some sense that [SUB:its-&gt;is] not anything too serious but also is there anything you can prescribe me to make it better or any advice or maybe even a sick note so that if i need to stay away from work for a bit longer i can get one sure sure [SUB:ok-&gt;okay] all right so well talk a little bit about the symptoms and i am sure we can get a [DEL:um] those things [SUB:uh-&gt;sorted] and some reassurance [INS:thank] [SUB:um-&gt;you] about your concerns [DEL:ok] so um you mentioned that you started with [INS:a] sore throat about a week ago developed into [INS:a] bit of a dry cough [SUB:um-&gt;and] ill just ask a few questions around those so um do you have any shortness of breath [DEL:no] yes yes i have been having shortness of [INS:oh] yeah i have been having shortness of breath yeah you are short of breath and uh do you have any wheeze or chest pain [DEL:uh] yeah [DEL:a] [DEL:bit] [DEL:of] [DEL:both] you are [DEL:you] [DEL:are] feeling a bit wheezy with some chest pain as well yes [SUB:ok-&gt;okay] and how [DEL:ah] when did you start to develop the shortness of breath so [DEL:so] the sore throat so [INS:today] [SUB:todays-&gt;is] friday sore throat was about [DEL:last] [DEL:week] friday or thursday cough was saturday or sunday so the [DEL:so] [DEL:the] shortness of breath was i think shortly after the cough so maybe a day or two later so three [INS:or] four days ago [SUB:three-&gt;two] or four days ago you [INS:start] [SUB:started-&gt;to] develop [INS:symptoms] and is the cough worse at [INS:night] [SUB:nighttime-&gt;time] no no its the same throughout the [DEL:whole] day same throughout the day [DEL:um] and [DEL:uh] when you say you are short of breath just need to try and get an idea about how short of breath you are so are you able to [DEL:so] [DEL:um] [DEL:so] [DEL:uh] like walk up a flight of stairs for example [DEL:um] or [DEL:or] are you short of breath at rest [SUB:ohh-&gt;oh] yeah its [DEL:its] like [DEL:so] when i am doing walking [DEL:um] and i do [SUB:exercises-&gt;exercise] now and then so it it has not been [INS:super] [SUB:superbad-&gt;bad] like has not stopped me from doing any of those things but its been pretty unusual and a little bit worrying and you are a bit concerned about that [SUB:ok-&gt;okay] so i just need to ask a few [DEL:uh] things about your background as well so [DEL:um] do you have any other medical conditions or medical history no just no no past medical history no no [DEL:no] history of asthma no [DEL:um] and any [DEL:uh] [DEL:uh] history of [DEL:uh] clots on your legs or your lungs so these [INS:are] [INS:ddps] [INS:or] [SUB:uh-&gt;ps] [SUB:no-&gt;and] [SUB:one-&gt;none] [SUB:in-&gt;of] your [SUB:familys-&gt;families] had those clots [SUB:on-&gt;in] the legs or [DEL:the] lungs well my mother had lung cancer your mother had lung cancer do you smoke no you ever smoked or been exposed to asbestos [DEL:that] you know [DEL:of] do not know [SUB:with-&gt;if] asbestos ever smoked i mean once or twice in amsterdam [SUB:if-&gt;with] that [SUB:counts-&gt;car] but not really [SUB:ok-&gt;okay] um and [SUB:uh-&gt;ah] this so just going back to the your symptoms of shortness of breath with the cough its a dry cough no you are not coughing up any [SUB:flem-&gt;phlegm] um do [INS:you] do you have [DEL:uh] and you [DEL:do] [DEL:not] [DEL:you] say you do not have any chest pain as such um [DEL:uh] are you taking any medications currently at the moment [INS:no] [SUB:uh-&gt;i] [SUB:no-&gt;am] [SUB:no-&gt;not] [SUB:ok-&gt;okay] are you allergic to any medications not [DEL:to] any medication but i am allergic to peanuts peanuts [SUB:ok-&gt;okay] [SUB:um-&gt;and] and [DEL:uh] you mentioned that your mother had [DEL:uh] lung cancer [SUB:um-&gt;and] any other family history of any significant illnesses [SUB:uh-&gt;when] [DEL:run] running in your family no no that is the only one just lung cancer from my mother just lung cancer [SUB:ok-&gt;okay] and you say you have a cold so do you have sinus congestion or um no it seems to be [INS:almost] entirely [DEL:with] just my throat [DEL:so] like [SUB:my-&gt;j] [DEL:nose] [DEL:is] [DEL:like] [DEL:so] just your just your throat and any recent travel or have you always lived in the [INS:you] [SUB:uk-&gt;k] uh no so i i [DEL:i] have not always lived in the [INS:you] [SUB:uk-&gt;k] like so i was born in the [INS:you] [SUB:us-&gt;s] and moved over [SUB:well-&gt;about] [DEL:it] [DEL:was] twelve years ago but in terms of recent travel just to europe nowhere [SUB:too-&gt;to] exotic [SUB:ok-&gt;okay] so no so no recent travel no significant recent travel [DEL:any] anywhere um [SUB:ok-&gt;okay] and are you coughing up anything other than um [DEL:uh] so you [DEL:you] are not coughing up blood or anything like that no [DEL:no] um good and [DEL:uh] are you feeling feverish hot cold sweaty yeah so a little bit feverish [DEL:uh] um at first so the first three or so days of this but then [DEL:it] the fevers gone away [SUB:ok-&gt;okay] and in general do you sorry yeah [DEL:yeah] i was just going to say also had a bit of a headache [DEL:but] like headaches that come and go rather but like right now its fine [SUB:uh-&gt;okay] [DEL:ok] and in general would you say you are feeling you are you are beginning to to feel better worse or or sort of [DEL:um] staying the same so its like its up and down so so let us see so i [DEL:it] started last week and i stayed home from work two days this week i think it was maybe tuesday and then thursday so like i felt better and then worse again and then better and then worse again so its been yeah a kind of constant but constant [SUB:and-&gt;in] being variable [SUB:if-&gt;but] [SUB:that-&gt;okay] [DEL:makes] [DEL:ok] and i just [INS:really] need to ask any other sort of risk factors um that you may have so um no sort of significant weight loss um or unexplained weight loss any so no weight loss but i have been have been losing my appetite recently and i mean i usually eat a lot so [DEL:and] i [DEL:and] [DEL:i] enjoy eating as well but like [DEL:so] that is been a bit concerning you have been losing your appetite recently yes and you are a little bit concerned about that but you have not you have not lost any weight that you think [DEL:of] [DEL:yes] no not that and any um sort of rashes or anything [DEL:or] uh and you no [SUB:not-&gt;rash] [SUB:not-&gt;no] [DEL:that] [DEL:not] [DEL:that] you can [SUB:think-&gt;go] [SUB:of-&gt;okay] [DEL:ok] um so i would ask to examine you now but um i i do not know if i could sort of look inside your throat at least to see if there is a probably there is [SUB:ohh-&gt;oh] we can try [INS:it] [INS:on] [SUB:ohh-&gt;oh] no well no its [SUB:ok-&gt;okay] i might think about doing [SUB:a-&gt;it] have you got any lumps or bumps around your neck that you can feel [SUB:uh-&gt;ah] no [SUB:no-&gt;not] [SUB:that-&gt;the] [DEL:you] no [SUB:ok-&gt;okay] [SUB:um-&gt;and] and so finally you you were talking about [DEL:uh] i mean it sounds to me that um you have been a little bit up and down sore throat developed a dry cough [SUB:um-&gt;and] you are slightly short of breath but not too overly concerningly short of breath what i would say were just coming to the end [SUB:of-&gt;so] consultation [INS:hours] [SUB:now-&gt;is] if you feel significantly worse [DEL:mmhmm] um uh if you get more short of breath or sudden change in your breathlessness um or breathlessness that you are concerned about [SUB:then-&gt;and] i would advise you to see [SUB:no-&gt;your] [DEL:go] [DEL:and] [DEL:see] [DEL:a] gp [DEL:um] and actually see somebody physically um uh but i think for now i can sort of [DEL:uh] try and reassure you that um if this clears up as i [SUB:expect-&gt;expected] it would so [DEL:i] expect this to sort of be getting better in the next four or five days [DEL:um] if its not please get in touch with [SUB:a-&gt;the] medical professional again [DEL:um] and [SUB:uh-&gt;ill] [DEL:i] [DEL:would] expect it to and so therefore i would not be concerned about tuberculosis [DEL:um] your concerns about lung cancer [DEL:are] [DEL:and] was that the other thing you [SUB:are-&gt;were] concerned about [DEL:ohh] yeah yeah [DEL:yeah] [DEL:yeah] so so um again if you are not getting better please see somebody again [DEL:um] i have just got four seconds now so nice talking to you and [INS:we] have [DEL:we] got to we [INS:have] got to tidy up yeah [SUB:ok-&gt;okay] so [DEL:uh] [DEL:all] [DEL:right] [DEL:uh] and ill provide you with a sick note just to give you a few more days off work [DEL:um] and [SUB:paracetemol-&gt;paracetamol] lots of fluids [DEL:um] and [DEL:uh] rest up and as i say if you are not feeling better please get in touch [INS:okay] [SUB:ok-&gt;alright] have a good day thank you [SUB:bye-&gt;alright]</t>
+          <t>['if', 'okay', 'in', 'okay', 'or', 'a', 'okay', 'i', 'feel', 'urgency', 'to', 'urinate', 'urine', 'may', 'patient', 'are', 'you', 'hypertensive', 'that', 'at', 'the', 'hospital', 'you', 'are', 'not', 'diabetic', 'okay', 'a', 'family', 'history', 'of', 'similar', 'condition', 'is', 'there', 'do', 'you', 'take', 'any', 'recreational', 'drugs', 'substance', 'abuse', 'no', 'thank', 'you', 'very', 'much', 'okay', 'do', 'you', 'have']</t>
+        </is>
+      </c>
+      <c r="AC2" t="inlineStr">
+        <is>
+          <t>['i', 'am', 'i', 'i', 'have', 'this', 'it', 'the', 'you', 'so', 'be', 'a', 'a', 'pus', 'so', 'any', 'any', 'in', 'the', 'being', 'other', 'drug', 'no']</t>
+        </is>
+      </c>
+      <c r="AD2" t="inlineStr">
+        <is>
+          <t>['emeka', 'am', 'it', 'has', 'started', 'it', 'started', 'it', 'it', 'you', 'feel', 'it', 'goes', 'a', 'urinate', 'yes', 'urinate', 'visiting', 'visit', 'do', 'urinate', 'you', 'before', 'straint', 'in', 'alot', 'dripples', 'dripples', 'yeah', 'pause', 'pause', 'oo', 'okay', 'catherization', 'urethra', 'not', 'not', 'catherization', 'okay', 'main', 'there', 'you', 'were', 'a', 'it', 'have', 'has', 'urinal', 'can', 'give', 'amlodepine', 'okay', 'you', 'are', 'on', 'amlodepine', 'give', 'allergies']</t>
+        </is>
+      </c>
+      <c r="AE2" t="inlineStr">
+        <is>
+          <t>['a', 'if', 'okay', 'in', 'onset', 'that', 'that', 'other']</t>
+        </is>
+      </c>
+      <c r="AF2" t="inlineStr">
+        <is>
+          <t>['i', 'on', 'it', 'so', 'the', 'the', 'so', 'a', 'pulse', 'any', 'being', 'had', 'i', 'am', 'not', 'and', 'you', 'know', 'the', 'other', 'drug', 'no', 'madam']</t>
+        </is>
+      </c>
+      <c r="AG2" t="inlineStr">
+        <is>
+          <t>['started', 'it', 'started', 'in', 'onset', 'a', 'goes', 'visiting', 'visit', 'you', 'straint', 'in', 'alot', 'dripples', 'dripples', 'yeah', 'pause', 'pause', 'oo', 'okay', 'catherization', 'not', 'not', 'catherization', 'okay', 'main', 'it', 'has', 'condition', 'condition', 'have', 'has', 'can', 'drugs', 'agents', 'give', 'amlodepine', 'amlodepine', 'give', 'okay']</t>
+        </is>
+      </c>
+      <c r="AH2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     ref_ix  hyp_ix reference hypothesis operation  index_edit_ops
+0         0       0      male       male         =            &lt;NA&gt;
+1         1       1        or         or         =            &lt;NA&gt;
+2         2       2         a          a         =            &lt;NA&gt;
+3         3       3    female     female         =            &lt;NA&gt;
+4      &lt;NA&gt;       4         _          i       ins               0
+..      ...     ...       ...        ...       ...             ...
+708     681     693      okay       okay         =            &lt;NA&gt;
+709     682     694     thank      thank         =            &lt;NA&gt;
+710     683     695       you        you         =            &lt;NA&gt;
+711     684     696      very       very         =            &lt;NA&gt;
+712     685     697      much       much         =            &lt;NA&gt;
+[713 rows x 6 columns]</t>
+        </is>
+      </c>
+      <c r="AI2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     ref_ix  hyp_ix reference hypothesis operation  index_edit_ops
+0         0       0      male       male         =            &lt;NA&gt;
+1         1       1        or         or         =            &lt;NA&gt;
+2         2       2         a          a         =            &lt;NA&gt;
+3         3       3    female     female         =            &lt;NA&gt;
+4      &lt;NA&gt;       4         _          i       ins               0
+..      ...     ...       ...        ...       ...             ...
+704     681     652      okay       okay         =            &lt;NA&gt;
+705     682     653     thank      thank         =            &lt;NA&gt;
+706     683     654       you        you         =            &lt;NA&gt;
+707     684     655      very       very         =            &lt;NA&gt;
+708     685     656      much       much         =            &lt;NA&gt;
+[709 rows x 6 columns]</t>
+        </is>
+      </c>
+      <c r="AJ2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     ref_ix  hyp_ix reference hypothesis operation  index_edit_ops
+0         0       0      male       male         =            &lt;NA&gt;
+1         1       1        or         or         =            &lt;NA&gt;
+2         2       2         a          a         =            &lt;NA&gt;
+3         3       3    female     female         =            &lt;NA&gt;
+4         4    &lt;NA&gt;         a          _       del               0
+..      ...     ...       ...        ...       ...             ...
+704     682     696     thank      thank         =            &lt;NA&gt;
+705     683     697       you        you         =            &lt;NA&gt;
+706     684     698      very       very         =            &lt;NA&gt;
+707     685     699      much       much         =            &lt;NA&gt;
+708    &lt;NA&gt;     700         _      madam       ins              70
+[709 rows x 6 columns]</t>
+        </is>
+      </c>
+      <c r="AK2" t="inlineStr">
+        <is>
+          <t>male or a female [INS:i] [INS:am] a male how old are you i am sixtyfive years old [INS:i] hope you do not mind [DEL:if] i address you as mr emeka i do not mind okay thank you very much so what brought you to the clinic today i am having difficulty in urinating [DEL:okay] you have been having difficulty in urinating for how long has this been [SUB:it-&gt;that] [SUB:has-&gt;is] [SUB:started-&gt;nothing] for two weeks you have been having difficulty [DEL:in] urinating for two weeks yes did [SUB:it-&gt;this] started gradually or it was gradual in onset [DEL:okay] it was gradual in onset has it been constant has it always been there or it just comes and goes or you feel this within a particular period of the day i think it [SUB:goes-&gt;got] bad [SUB:of-&gt;recently] [DEL:recent] it was not constant before but now it is constant okay thank you very much is this pain while urinating associated with [SUB:a-&gt;the] burning sensation [INS:it] is [INS:it] [INS:is] not associated with pain or a burning sensation okay [INS:so] it is not associated with any pain or a burning sensation yes it is not do you feel [INS:the] urgency to urinate yes i feel [INS:the] urgency to [INS:you] [INS:ring] [SUB:urinate-&gt;it] and then are you able to pass out this urine when you feel this urgency to [INS:you] [INS:in] [SUB:urinate-&gt;it] i am unable to pass out [SUB:urine-&gt;here] okay do you feel frequent urination the urge to always go to the toilet yes i am always [SUB:visiting-&gt;just] [SUB:the-&gt;into] [SUB:toilet-&gt;it] especially [DEL:in] the night okay nocturia [INS:so] you always [SUB:visit-&gt;use] the toilet in the night yes at morning at night at night like how many times [SUB:do-&gt;you] you [SUB:urinate-&gt;need] in the night it is very frequent i cannot tell more than you used to before yes it is more than the usual two times to zero times i usually use the toilet but now it is about five times do you [SUB:straint-&gt;strain] [SUB:in-&gt;to] urinate yes i strain [INS:a] [SUB:alot-&gt;lot] and my urine [SUB:dripples-&gt;dribbles] okay it [SUB:dripples-&gt;dribbles] [SUB:yeah-&gt;yes] after [SUB:urination-&gt;i] [SUB:may-&gt;might] [DEL:i] know if there is blood in the urine there is no blood in this urine there is no fever i do not have [INS:ist] [INS:have] fever is there [SUB:pause-&gt;pus] there is no [INS:pus] [SUB:pause-&gt;okay] [SUB:oo-&gt;so] do you have lower abdominal pain i do not have abdominal pain [SUB:okay-&gt;oh] thank you very much is there a history of trauma or [INS:any] recent [SUB:catherization-&gt;catarization] or urethra instrumentation no there is [SUB:not-&gt;none] there is [SUB:not-&gt;no] history of trauma or [SUB:catherization-&gt;catarization] i do not have any history [SUB:of-&gt;oh] [DEL:that] [DEL:okay] thank you very much are you a [SUB:main-&gt;known] hypertensive patient are you hypertensive yes i have been hypertensive for ten years now okay you have been hypertensive for ten years how do you know [DEL:that] you are hypertensive i was told [SUB:at-&gt;that] the hospital [DEL:that] i was diagnosed there you were diagnosed in [SUB:a-&gt;the] hospital ten years ago yes [INS:yes] and you have been on medications yes [SUB:it-&gt;that] [SUB:has-&gt;is] been controlled by medications okay thank you very much how about [INS:being] diabetic are you diabetic no i am not diabetic you are not diabetic okay is there a family history of similar condition is there anyone in your family that has similar condition yeah i can remember my dad [SUB:have-&gt;had] similar condition when he was old when he was old what exactly was the problem did he also feel pain while trying to urinate he [SUB:has-&gt;had] some [SUB:urinal-&gt;urinary] problem i [SUB:can-&gt;cannot] tell exactly i was young at that time okay thank you very much are you a smoker i do not smoke do you take alcohol yeah i consume alcohol occasionally do you take any recreational drugs substance abuse no thank you very much are you on your hypertensive [SUB:agents-&gt;agent] yes i am on some drugs they [SUB:give-&gt;gave] me to control the hypertension can you tell me the name of the drug you are on [INS:i] [INS:am] [INS:on] [SUB:amlodepine-&gt;lodipine] okay you are on [SUB:amlodepine-&gt;lodipine] is there any [INS:other] drug you are on i am not on any other [INS:drug] they [SUB:give-&gt;gave] me just that one [SUB:okay-&gt;oh] thank you very much do you have any [DEL:other] allergies [DEL:do] [DEL:you] [DEL:have] are you allergic to any drug or medication [INS:no] i am not okay thank you very much</t>
+        </is>
+      </c>
+      <c r="AL2" t="inlineStr">
+        <is>
+          <t>male or a female [INS:i] [INS:am] a male how old are you i am sixtyfive years old [INS:i] hope you do not mind [DEL:if] i address you as mr [INS:i] [SUB:emeka-&gt;maker] i do not mind okay thank you very much so what brought you to the clinic today i [INS:have] [SUB:am-&gt;been] having difficulty in urinating [DEL:okay] you have been having difficulty in urinating for how long has this been [SUB:it-&gt;that] [SUB:has-&gt;is] [SUB:started-&gt;lasted] for two weeks you have been having difficulty [DEL:in] urinating for two weeks yes did [INS:this] [SUB:it-&gt;start] [SUB:started-&gt;as] gradually or it was gradual in onset [DEL:okay] it was gradual in onset has it been constant has [SUB:it-&gt;he] always been there or [SUB:it-&gt;he] just comes and goes or [SUB:you-&gt;he] [SUB:feel-&gt;feels] this within a particular period of the day i think [SUB:it-&gt;he] [SUB:goes-&gt;got] bad of recent it was not constant before but now it is constant okay thank you very much is this pain while urinating associated with [SUB:a-&gt;the] burning sensation [INS:it] is not associated with pain [DEL:or] [DEL:a] burning sensation [DEL:okay] it is not associated with any pain or a burning sensation yes it is not do you feel [INS:the] urgency to [SUB:urinate-&gt;you] [SUB:yes-&gt;know] [DEL:i] [DEL:feel] [DEL:urgency] [DEL:to] [DEL:urinate] and then are you able to pass out this urine when you feel this urgency to [INS:you] [SUB:urinate-&gt;know] i am unable to pass out [DEL:urine] okay do you feel frequent urination the urge to always go to the toilet yes i am always [SUB:visiting-&gt;using] the toilet especially in the night okay nocturia [INS:so] you always [SUB:visit-&gt;use] the toilet in the night yes at morning at night at night like how many times [SUB:do-&gt;you] you [SUB:urinate-&gt;need] in the night it is very frequent i cannot tell more than [SUB:you-&gt;it] used to [INS:be] [SUB:before-&gt;for] yes it is more than the usual two times to zero times i usually use the toilet but now it is about five times do you [SUB:straint-&gt;strain] [SUB:in-&gt;to] urinate yes i strain [INS:a] [SUB:alot-&gt;lot] and my urine [SUB:dripples-&gt;bubbles] okay it [SUB:dripples-&gt;bubbles] [SUB:yeah-&gt;yes] after urination [DEL:may] i know if there is blood in the urine there is no blood in this urine there is no fever i do not have [INS:a] fever is there [SUB:pause-&gt;pus] there is no [INS:pus] [INS:so] [SUB:pause-&gt;okay] [SUB:oo-&gt;so] do you have lower abdominal pain i do not have [INS:any] abdominal pain [SUB:okay-&gt;oh] thank you very much is there a history of trauma or [INS:any] recent [SUB:catherization-&gt;catheterization] or [SUB:urethra-&gt;ureteral] instrumentation no there is [SUB:not-&gt;none] there is [SUB:not-&gt;no] history of trauma or [SUB:catherization-&gt;catheterization] i do not have any history of that [SUB:okay-&gt;oh] thank you very much are you a [SUB:main-&gt;known] hypertensive [DEL:patient] [DEL:are] [DEL:you] [DEL:hypertensive] yes i have been hypertensive for ten years now okay you have been hypertensive for ten years how do you know [DEL:that] you are hypertensive i was told [DEL:at] [DEL:the] [DEL:hospital] that i was diagnosed [INS:in] [INS:the] [SUB:there-&gt;hospital] [SUB:you-&gt;i] [SUB:were-&gt;was] diagnosed in [SUB:a-&gt;the] hospital ten years ago yes and you have been on medications yes [SUB:it-&gt;that] has been controlled by medications okay thank you very much how about [INS:being] diabetic are you diabetic no i am not diabetic [DEL:you] [DEL:are] [DEL:not] [DEL:diabetic] [DEL:okay] is there [DEL:a] [DEL:family] [DEL:history] [DEL:of] [DEL:similar] [DEL:condition] [DEL:is] [DEL:there] anyone in your family that has similar condition yeah i can remember my dad [SUB:have-&gt;had] similar condition when he was old when he was old what exactly was the problem did he also feel pain while trying to urinate he [SUB:has-&gt;had] some [SUB:urinal-&gt;urinary] problem i [SUB:can-&gt;cannot] tell exactly i was young at that time okay thank you very much are you a smoker i do not smoke do you take alcohol yeah i consume alcohol occasionally [DEL:do] [DEL:you] [DEL:take] [DEL:any] [DEL:recreational] [DEL:drugs] [DEL:substance] [DEL:abuse] [DEL:no] [DEL:thank] [DEL:you] [DEL:very] [DEL:much] are you on your hypertensive agents yes i am on some drugs they [SUB:give-&gt;gave] me to control the hypertension can you tell me the name of the drug you are on [SUB:amlodepine-&gt;i] [SUB:okay-&gt;am] [SUB:you-&gt;on] [SUB:are-&gt;load] [SUB:on-&gt;the] [SUB:amlodepine-&gt;pin] is there any [INS:other] drug you are on i am not on any other [INS:drug] they [SUB:give-&gt;gave] me just that one [DEL:okay] thank you very much do you have any other [SUB:allergies-&gt;justifications] [DEL:do] [DEL:you] [DEL:have] are you allergic to any drug or medication [INS:no] i am not okay thank you very much</t>
+        </is>
+      </c>
+      <c r="AM2" t="inlineStr">
+        <is>
+          <t>male or a female [DEL:a] male how old are you i am sixtyfive years old [INS:i] hope you do not mind [DEL:if] i address you as mr emeka i do not mind okay thank you very much so what brought you to the clinic today i am having difficulty in urinating [DEL:okay] you have been having difficulty in urinating for how long has this been it has [SUB:started-&gt;lasted] for two weeks you have been having difficulty [DEL:in] urinating for two weeks yes did [SUB:it-&gt;this] [SUB:started-&gt;start] gradually or it was gradual [SUB:in-&gt;nonsense] [DEL:onset] okay it was gradual in [INS:on] [SUB:onset-&gt;set] has it been constant has it always been there or it just comes and goes or you feel this within [SUB:a-&gt;the] particular period of the day i think it [SUB:goes-&gt;got] bad of recent it was not constant before but now it is constant okay thank you very much is this pain while urinating associated with a burning sensation [INS:it] is not associated with pain or a burning sensation okay [INS:so] it is not associated with any pain or a burning sensation yes it is not do you feel [INS:the] urgency to urinate yes i feel [INS:the] urgency to urinate and then are you able to pass out this urine when you feel this urgency to urinate i am unable to pass out urine okay do you feel frequent urination the urge to always go to the toilet yes i am always [SUB:visiting-&gt;using] the toilet especially in the night okay nocturia [INS:so] you always [SUB:visit-&gt;use] the toilet in the night yes at morning at night at night like how many times do you urinate in the night it is very frequent i cannot tell more than [SUB:you-&gt;it] used to before yes it is more than the usual two times to zero times i usually use the toilet but now it is about five times do you [SUB:straint-&gt;strain] [SUB:in-&gt;to] urinate yes i strain [INS:a] [SUB:alot-&gt;lot] and my urine [SUB:dripples-&gt;dribbles] okay it [SUB:dripples-&gt;dribbles] [SUB:yeah-&gt;yes] after urination may i know if there is blood in the urine there is no blood in this urine there is no fever i do not have fever is there [SUB:pause-&gt;pulse] there is no [INS:pulse] [SUB:pause-&gt;okay] [SUB:oo-&gt;so] do you have lower abdominal pain i do not have abdominal pain [SUB:okay-&gt;oh] thank you very much is there a history of trauma or [INS:any] recent [SUB:catherization-&gt;caterization] or urethra instrumentation no there is [SUB:not-&gt;none] there is [SUB:not-&gt;no] history of trauma or [SUB:catherization-&gt;catheterization] i do not have any history of that [SUB:okay-&gt;oh] thank you very much are you a [SUB:main-&gt;known] hypertensive patient are you hypertensive yes i have been hypertensive for ten years now okay you have been hypertensive for ten years how do you know [DEL:that] you are hypertensive i was told at the hospital [DEL:that] i was diagnosed there you were diagnosed in a hospital ten years ago yes and you have been on medications yes [SUB:it-&gt;that] [SUB:has-&gt;is] been controlled by medications okay thank you very much how about [INS:being] diabetic are you diabetic no i am not diabetic you are not diabetic okay is there a family history of similar [SUB:condition-&gt;conditions] is there anyone in your family that has similar [SUB:condition-&gt;conditions] yeah i can remember my dad [INS:had] [SUB:have-&gt;a] similar condition when he was old when he was old what exactly was the problem did he also feel pain while trying to urinate he [SUB:has-&gt;had] some urinal problem i [SUB:can-&gt;cannot] tell exactly i was young at that time okay thank you very much are you a smoker i do not smoke do you take alcohol yeah i consume alcohol occasionally do you take any recreational [SUB:drugs-&gt;drug] substance abuse no thank you very much are you on your hypertensive [SUB:agents-&gt;agent] yes i am on some drugs they [SUB:give-&gt;gave] me to control the hypertension can you tell me the name of the drug you are on [INS:i] [INS:am] [INS:not] [SUB:amlodepine-&gt;pain] okay you are on [INS:and] [INS:you] [INS:know] [INS:the] [SUB:amlodepine-&gt;pain] is there any [INS:other] drug you are on i am not on any other [INS:drug] they [SUB:give-&gt;gave] me just that one [SUB:okay-&gt;oh] thank you very much do you have any [DEL:other] allergies do you have are you allergic to any drug or medication [INS:no] i am not okay thank you very much [INS:madam]</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1_Malaria</t>
+          <t>18_Pneumonia</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>data/final_audio/1_Malaria.wav</t>
+          <t>data/final_audio/18_Pneumonia.wav</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Hello. Hello. Good afternoon. Good afternoon. I'm Doctor Yemi and I'll be the one attending to you this afternoon. All right, So can you tell me what brought you to the hospital? I've been having..erm… My body has been feeling hot for a while now, As in very hot. Oh, I'm so sorry to hear about that. So I'd like to know more about this so I would know how best to, you know, help you. So when did it start? Started a week ago. Was is sudden in onset or it was gradual? It was gradual. And how has it been since then, has it progressed, has it gotten better Or It has gotten worse? It has gotten worse. OK, aside from this high body temperature, do you have any other associated symptom? Yes. I've been having this very bad headache. OK. Body pains. OK OK, OK. So, all these symptoms now, did it starts with the high body temperature? yes. And it… especially it gets worse at night. At night, OK, OK, so you feel like… what of during the day? How… How do you feel during the day? During the day erm… I vomit like I vomited, for example today now, I vomited like four times. OK this morning. OK, so the headache, what part of your head are you have… having this headache? the… my… front part of my head front part of your head, I will… do you Describe It like… any associated eye pain. No. OK. Hmm, last month. OK. So, you've not you've not had a missed. Yeah. OK, Alright. Thank you very much. So aside from this I'd like to erm…So what have you done since it started so far? I haven't done… I've… I’ve only taken Paracetamol You’ve only taken para…, and any, any, any relief with paracetamol? just for a short while. OK. OK. OK. So erm, I'd just like to ask some other systemic questions to be sure that everything is fine with other systems. So, from… any uhm… neck pain or stiffness? No. Any cough or chest pain? No. Have you been going to... have you… any urinary symptoms? No. Any diarrhea? No. OK. So, like from what you told me so far you said you've been having high body temperature. Yes There was headache and body pain and you, Shiver, for about a week now, am I correct? And also this happens more in the evenings. OK. And there's also been vomiting. How about  your appetite? Has your appetite been fine? It has reduced. Reduced appetite OK, OK. So are you being erm… I would like to ask for your past medical history now. Are you been managed for any medical condition? No. In the past? Are you on any routine medications? No. Do you drink alcohol? No. Do you smoke cigarettes? No. Have you had surgery before, in the past? No. Have you ever been admitted in the hospital? No. Have you ever been transfused with blood? No. OK. Erm… Are you married? No. OK. Are you sexually active? No. OK, that's that's that's that's OK. And what do you do for work? I'm a student. Oh, OK. Where do you school? Unilag OK, now I'm most… I would like to ask, for this erm… consultation, Are you paying out of pocket or you’re under insurance, I'm paying out of pocket. And how are your finances like, you know? well, depend… I’m depending on my parents. OK, OK, OK, alright that's that's very good. So erm… asides this is there any other thing that you think it's important that I might have missed out in the course of this conversation. None for now. OK. Alright. Thank you very much. So, I'd like to examine you now I'll do a general examination and for… and focus and systemic examinations. So, well from what you've told me so far let's just you know do a quick recap, you said you've been having headache, body pains, and fever for about a week, with vomiting. so and this… it occurs more in the evenings. So, I'm thinking you're having a condition, you're having malaria. So, but what what would need to do is we'll need to confirm. We'll take blood samples to the lab, we'll do erm… malaria parasite test. So, if it comes out positive, we'll give you medications for malaria, but for now we'd give you paracetamol for the fever and the erm… headache and the body pains. So, we’d also like you to, you know,  bed rest if you need erm… notes for school to maybe exempt you from school, we can also issue that for you. Do you have any other thing you’d like you know like me to help with? So I'll direct you to the lab, where they’ll do the test and while we await the test results alright. Have… any other thing? No. Alright, Thank you so much for your time. Thank you very much. Alright, Have a lovely day. You too. Bye.</t>
+          <t>Good afternoon, Sir. I am Doctor Sadeko. Good afternoon. Good afternoon, Doctor. How are you doing today, Sir? Doctor, I'm not… I'm not too fine… not too fine, that's why I came to the hospital today. What was the complaints? So, Doctor, I've been coughing for about a week now and I've been also.. also have… you also have what? So, and I also have erm… I've also been running temperature for about 5 days. So, you have running temperature for five days. Yes, Yes. For about a week now. A week? Yes. OK all right. So, the cough, did it start suddenly or gradually? The cough started suddenly, just started like that, I just… just woke up more morning and started coughing, about a week ago, yes. Was there Was there any symptoms like Catarrh or erm… any, erm… any difficulty in swallowing before the cough started? No, none like that. I had nothing like that. Nothing like that. You had nothing like that. Yes. OK, so now the cough, how does it sound? Does it sound like barking? Does it sound like it's comes in bouts and then you have to take a deep breath? When… when you say barking, do you… are you… do you mean like a dog or what do you mean by barking? Yes, yes, sounds like a dog barking. No, no, no, no, no, no, Mine is not that. I did not... I didn't experience anything like that. OK. So, is the cough productive of phlegm? Yes. Yes. It's productive when I, Yes… When I cough, I bring out some, some substance from my mouth, yes. So, what's the colour of the substance? Err, it's about, erm, it's clear. It's whitish, It's not, it's just normal. It's looking like saliva, but it's very thick. It's very thick. Was there blood in it, at any point? No, there was no blood in it. There was no blood in it. There was no blood in it at any point. Yes. And after you cough, do you feel like vomiting, or do you vomit? No, I don't. I don't. I don't feel like vomiting. I don't vomit at all. OK And you did not have catarrh or difficulty in swallowing prior to onset of the cough? No, no. There was nothing. I was not, I had nothing. My… my… even when I was coughing, my chest was not paining me nothing it was just the cough then I… I discovered after a few days after that I just started running temperature too. My body was very, very hot. It was very hot that I was shivering. So, you're telling me there is no, there is no cough, there is no chest pain. No, there's… there's no chest pain, my chest was not paining me at all. Your chest was not paining me. Is there anybody coughing around you? No, there nobody. I stay alone right now so I have nobody around me. I don't stay with people, so I don't have anybody around me that's coughing too. And at work too there's nobody coughing around me. So, OK, so you stay alone. You're not here in an overcrowded place. Yes, but yes. But Doctor, I noticed. What actually prompted me to come is the fact that about two days ago I noticed that the cough became worsened, and I was… I started to have some difficulty in breathing. So, like that got me really scared, like I was, I was, I was just feeling breathless for a moment. Comes and goes then, and since that, since then, the breathlessness has become more worsened. So that's what exactly prompted me to completely to see you. You're finding it difficult to breathe, Yes, Yes When you sleep at night, you sweat excessively. No, at all. I don't, I don't slept… I don't sweat when I sleep at night? OK, so what's what relieves the breathlessness? Any change in position that relieves the breathlessness or it’s constant? No, it's not associated with erm, any… any position, nothing. I just… it just comes and goes, like I just feel breathless for a while, then it relieves me. Then it comes again, especially when I'm especially when I'm coughing. OK. Has this worsened progressively? Yes, Yes… It has gotten very bad, doctor, that's why I came to the hospital. Does it affect, does it affect your daily activities? Yes, it does, doctor. I've not been able to work for the past two days because of the cough and the fact that I have, I've not been feeling well, generally in my body, so that's so, Now this fever that you were having, was it… did it start suddenly or gradually? It started. It started gradually, then became I became very hot and it has been like that, it has been like that. So, the fever is high grade, You're very hot? Yes… Yes, it's high. Did you at any point? Yes. Check by yourself at home your temperature? Yes, I did… I did, I have a thermometer, it was about was about 38.9. 38.9 OK and what does… what do you do that relieves the fever. I took some, I took some paracetamol. It relieved a bit, then but it did… didn't last long. I just I I became hot again and it has been like that ever since. So I just want to ask you some questions. Has anything happened before in the past? OK, Has it happened in the past? No, no, no, no. This is the first time I'm experiencing, that's why I'm… this is the first time I'm experiencing this kind of thing. OK, this is the first time. Are you.. do you have any medical condition? Like, are you asthmatic during your blood group and genotype? No, I'm not doctor, I'm fine. No, I have nothing. And that’s why this is Surprising. Are you hypertensive? What did you say? I can't hear you properly, Sir. Are you hypertensive or diabetic? None. None. None. None No, no. I have none of them… I have none of them. So, what have you... what have you done to care for yourself so far? I just… I just… I just tried to get some cough syrup, but they didn't… They didn't seem to work properly. They didn't seem to work and since the difficulty breathing started, I knew, I knew, I know I needed to like, come to speak to someone, to a doctor. So, that's why I came today, for you to like, for me to like, know what's wrong with me and treat myself, basically. Have you been, have you been admitted before? No, not, not, not that I can remember. Have you done any surgical procedure before? No, No. OK. So, I'm just going to ask you some other questions just to know what exactly could be related to your, to the symptoms you're having. So, do you have headache? Headache just comes once in a while, maybe 'cause the cough. I've not been able to sleep really. So, kind of, yeah, kind of, yes. OK. So, any loss of consciousness? No. No. No, No. OK, OK. Do you have Catarrh? No, at all. OK. Do you have any abdominal pain? No. No, I don't have any. Diarrhea or vomiting? No, I've not vomited at all. You have any bone pain? Yes. No, the no, the most. It's just, it's just the shortest of breath I've been having. The difficulty in breathing I've been having. That's just, that's just… So, in summary you're telling me, in summary you're telling me you had, you… you've had cough, fever and difficulty in breathing. Yes. Right and your cough is productive. Yes. All right, So I'm going to have to have to examine you, right. I'm going to have to examine you and I'm going to have to listen to your chest to know if, to know whatever is going on in your chest, whether there's a chest infection that is causing you to have a fever and the and the cough. Do you understand? And then we are going to have you do some investigations like a chest X-ray, a complete blood count, a full blood count which will tell us whether there's an infection going on, depending on the parameters that are elevated or reduced, do you understand? We are going to do you know, electrocyte segmentation rates to know whether there's an inflammatory process going on. Do you understand? And then we're also going to take your sputum, your… the phlegm and we're going to send it for culture, sensitivity to know what bacteria is, is being cultured. Erm, please, I just want to ask you, do you smoke? No. No, I don't, doctor, I'm a good Christian. I don’t smoke. I don't drink. You don't… You don't drink alcohol either. I don't, I don't do any of those, I don't do drugs, I don't do any of that. I'm going to ask you some other questions. Do you have… their kind of personal questions? Can I go ahead? Yeah. I just want to know, doctor, I just want to… I just want to be fine. I just want to know how soon you can start treating me and what I’ll need to take basically. I just want to ask if…I just want to ask if you have multiple sexual partners and then your sexual practices. No, no. You have oral sex? I'm married. No, not at all. Not at all. I'm married. So, we are going to start you, from the history and the examination we have done and then we're going to ask you to do some investigations. However, we have some differentials like diagnosis, the cause, the cause of what is causing the cough and the fever. We have some, this thing at the back of our mind, which could be the cause. Do you understand? We think you have a pneumonia, pneumonia, a chest infection. So, we're going to start you on a broad spectrum antibiotics, right? And then we're going to start you on the cough syrup, right, to treat the cough while we wait for the results of our investigations. Do you understand? OK And then since there's no history of asthma by the time you'll start treatment with the antibiotics and… and the cough syrup there will be… the breathlessness is going to reduce. But we… your... we would have checked your… your oxygen saturation and we'll see that it is fine. So, there'll be no need to place you on… on oxygen. So, you're going to have you do a full blood count in sputum and microscopy culture sensitivity. You're going to have you do any Erythrocyte segmentation rate and you're going to do a chest X-ray. So, let's see if it's a structural problem or a functional problem. Do you understand? OK, doctor. So doctor, do I.. Do you want to ask the question if you have any questions, Yes, I was going to ask that are you going to keep me in the hospital or do I… that… can I… can I be treated from home? Because I don't know. We, we, we are going to admit you for some time to evaluate you and because of the breathlessness you are having, right. And then we'll start you on on intravenous, intravenous… erm That's OK. That's cool. Culture and sensitivity could take about 72 hours to.. to five days before it will be ready. Do you understand? Yeah, no problem, Doctor. Thank you. No problem, Doctor. Thank you very much. I think that's fine. I will just, yeah, I'll just do the labs and wait for just for you to start the treatment. Thank you.</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>301.248</v>
+        <v>794.144</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -749,367 +937,391 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Hello. Hello. Good afternoon. Good afternoon. I'm Dr. Yemi and I'll be the one attending to you this afternoon. All right, so can you tell me what brought you to the hospital? I've been having, um, my body has been feeling hot for a while now. It's very hot. Oh, I'm so sorry to hear about that. So I'd like to know more about this so I know how best to, you know, help you. So when did it start? Started a week ago. Was this sudden or was it gradual? It was gradual. And how has it been since then? Has it progressed? Has it gotten better? It has gotten worse. It has gotten worse. Okay. Aside from this high body temperature, do you have any other associated symptom? Yes, I've been having this very bad headache. Okay. Body pains. Okay. And sometimes I shiver. Okay. Okay. So all these symptoms are, do they start with the high body temperature? Yes, and it especially gets Worse at night. At night, okay, okay. So you feel like what of during the day? How, how do you feel during the day? During the day, um, I vomit. Okay. I vomited, for example, today and I vomited like four times this morning. Okay. So the headache, what part of your head are you having this headache? My front part of my head. Front part of your head. Are you describing it like in any as your eye pain? No. Okay. I would like to ask you, when was your last menstrual period? Last month. Okay, so you've had a missed period? Yeah. Okay, alright, thank you very much. So aside from this, I'd like to, so what have you done since it started so far? I haven't done, I haven't taken any paracetamol. Any relief with paracetamol? Just for a short while. Okay, okay, okay. So I'd just like to ask some other systemic questions to be sure that everything is fine with our systems. So from any any neck pain or stiffness no any cough or chest pain no have you been um going to have you any urinary symptoms no any diarrhea no okay so like from what you told me so far you said you've been having um high body temperature yes there was headache and um body pain and you shiver for about a week now am i correct and also this happens more in the evenings okay and there's also been vomiting how about appetite I your appetite's been fine. It does reduced. Reduced appetite. Okay, okay. So are you being me? I would like to ask for your past medical history now. Have you been married for any medical condition? No. In the past. Are you on any routine medications? No. Do you drink alcohol? No. Do you smoke cigarettes? No. Have you had surgery before in the past? No. Have you ever been admitted in the hospital? No. You have been transfused with blood. No. Okay. Are you married? No. Okay. Are you sexually active? No. Okay, that's, that's, that's it. And what do you do for work? I'm a student. Okay. Where do you go? You know, I. Okay. Now, I'm most, I would like to ask for this consultation. Are you paying out of pocket or are you under insurance? I'm paying out of pocket. And how are your finances? Like, you know, Well, depend, I'm depending on my. Okay, okay, okay, alright, that sounds very good. So, um, aside to is it, is there any other thing that you think is important that I must have missed out in the cause of this conversation? None for now. Okay, alright, thank you very much. So, I'd like to examine you now. I'll do a general examination and systemic examinations. So, um, well, from what you've told me so far, let's just, you know, do a quick recap. Said you've been having headache, body pains and fever for about week we're vomiting so and it's causing more in the evenings so i'm thinking you are having a condition you are having malaria so but what we need to do is we need to confirm we'll take um blood samples to the lab we'll do malaria parasite tests so if it comes out positive we'll give you medications for malaria but for now we'll give you um paracetamol for the fever and the um headache and the body pains so also like you to you know bed rest if you need um notes for school to maybe exempt you from school we can also issue that for you do you have any other thing would like you know like me to help with so i'll direct you to the lab and we'll do the test and well i wish the test results alright have any other thing no alright thank you so much for your time thank you very much alright have a lovely day you too bye あ！</t>
+          <t>Good afternoon, sir. I am Doctor Shadak. Good afternoon, good afternoon, doctor. How are you doing today, sir? Doctor, I'm not, I'm not too fine, not too fine. That's why I came to you today. What was the complaints? So, doctor, I've been coughing for about a week now, and I've been also, also at, yes. You also have what so and I also have um i've also been running temperature for about five days so it's been really yes yes and the cough has been for the cough has been for how long for about a week now a week yes okay alright so um the cough did it start suddenly or gradually the cough started suddenly just started like that i just Was there was there any symptoms like Qatar or any um any difficulty in swallowing before the cough started? No, none like that. I had nothing like that. Nothing like that. You had nothing like that. Yes. So now the cough, how does it sound? Does it sound like the barking? Does it sound like a? and it comes in and then you have to take a deep breath when you say barking are you do you mean like a dog or what do you mean by barking yes yes sounds like a dog barking no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no Substance from my mouth, yes. So what's the colour of the substance? Yeah, it's about yeah, it's clear, it's whitish, it's normal, it's just normal, it's looking like saliva, but it's very thick. It's very thick. Was there blood in it at any point? No, there was no blood in it. There was no blood in it at any point. And after you cough, do you feel like vomiting or do you vomit? No. I don't i don't i don't feel like i'm i don't vomit at all okay and you did not have catarrh or difficulty swallowing prior to onset of the cough no no that was not in my i was not i had nothing my my even when i was coughing my chest was not burning me nothing it was just the cough and i i discovered after a few days after that i was running temperature too my body was very very hot it was very hot i was shivering So you're telling me there is no there is no cough there is no chest pain. No, there's there's no chest pain. My chest was not pain in me at all. The chest was not pain in me. Is there anybody coughing around you? No, there's nobody. I stay alone right now so I have nobody around me. I don't stay with people so I don't remember anybody around me that is coughing too. And I walk to there's nobody coughing around me so. Okay, so you stay alone. You're not in a crowded place. Yes. but yes but doctor i noticed what actually prompted me to come is the fact that about two days ago i noticed that the cough became worsened and i was i started to have some difficulty in breathing so like that got me really scared i was i was feeling breathless for a moment comes and goes and and since that since then the breathlessness have become more worsened so that's what exactly prompted me to come quickly to see you So you're finding it difficult to breathe. Yes, the cough. Yes. When you sleep at night, do you sweat excessively? No, at all. I don't, I don't sleep, I don't sweat in a sleep department. Yes. Okay. So what's, what removes the breathlessness? Any changing position that relieves the breathlessness or is constant? No, it's not associated with any, any position, nothing. and it just comes and goes like i just feel breathless with a while then it releases me then it comes again especially when especially when i'm coughing okay has this worsened progressively yes yes that's gotten very bad doctor that's why i came to the hospital does it affect does it affect your daily activities yes it does doctor i've not been able to walk for the past two days because of the cough and the fact that i have not been feeling well generally So, no, no, this fever that you were having, was it, did it start suddenly or gradually? Started, it started gradually, then became, I became very hot and has been like that. It has been like that. So the fever is high grade, very hot. Yes, yes, it's I, do you have any points that you can check by yourself at home, your temperature? Yes, I did, I did, I have a stomach. I was about there was about thirty eight point nine thirty point nine okay and uh what do what do you do that releases the fever? Well i took some i took some past more it relieved the bit then but it didn't last long i just i became hot again and it has been like that ever since. So I just want to ask you some questions. Has this happened before in the past? Okay. Has it happened in the past? No, no, no, no. This is the first time I'm expressing this. This is the first time I'm expressing this kind of thing. Okay, this is the first time. Are you, do you have any medical condition? Like, are you asthmatic? Do you, do you need a blood pressure? No, I'm not to doctor. I'm fine. No, I have not. No. Are you a hypertensive or diabetic? Are you a hypertensive or diabetic? None, none, none. None. No, I have none of them. I have none of them. So what have you what have you done to care for yourself so far? I just try to get some cough syrup up but they didn't they didn't seem to work properly they didn't seem to work and since um the difficulty in breathing started i knew i knew i know i needed to like because to speak to someone to a doctor so that's why i came today for you to like for me to like know what's wrong with me and treat myself basically have you been have you been admitted before no not not not that current But none. Have you done any surgical procedure before? No, no. Okay, so I'm just going to ask you some other questions just to know what exactly could be related to your so the symptoms you're having. So do you have headache? Headache, it just comes once in a while, maybe because the cough, I've not been able to sleep really, so kind of, yeah, kind of yes. Okay, so any loss of consciousness? No, no, no, no. Okay, do you have catar? No at all. Okay, do you have any abdominal pain? No, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, no, No, no, the most of the just the shouters of breath have been happening, the difficulty in breathing have been happening. So that's the summary you're telling me, in summary you're telling me you had, you've had cough, fever and difficulty in breathing, yes, right, and your cough is productive, yes. Alright, so I'm going to have to have to examine you, right? I'm going to have to examine you, and I'm going to have to listen to your chest to know, to know whatever is going on in your chest. there's a chest infection that is causing you to have a fever and the and the cough do you understand and then we are going to have you do some investigations like a chest x-ray a complete blood count or a full blood count to tell us whether there's an infection going on depending on the parameters that are elevated or reduced do you understand we are going to do a neutrophil segmentation rate to know whether there's an inflammatory process brain on do you understand and then we're also going to take your sputum your the phlegm and we're going to um send it for culture sensitivity to know what bacteria is uh is being cultured um please i just want to ask you do you smoke no no i don't so doctor i'm a good christian i don't smoke i don't drink you don't you don't drink alcohol either i don't i don't do any of those i don't do jobs i don't do any of that i'm going to ask you some other questions um do you have um there are kind of personal questions can i go ahead yeah i just want to know doctor i just want to i just want to be fine i just want to know how soon you can start treating me and what i don't want to ask if i don't want to ask if you have multiple sexual partners and your sexual practices no no Oral sex. No, none at all, not at all. So we are going to start you from the history and the examination we have done and then we're going to ask you to do some investigations. However, we have some differentials like diagnoses, the cause of what is causing the cough and the fever. We have some just in the back of our mind which could be the cause, do you understand? We think you have a pneumonia, pneumonia, chest infection, so we are going to start you on a broad spectrum antibiotics, right, and then we are going to start you on cough syrup, right, to treat the cough while we wait for the results of our investigations, do you understand? Okay. And then, since there's no history of asthma, by the time you start treatments with the antibiotics and the cough syrup, there'll be the breathlessness. business is going to reduce but we your we would have checked your oxygen saturation and we see that it is fine so there'll be no need to place you on on oxygen so you're against having you do full block out in um um sputum and end microscopic culture sensitivity are going to have you doing the enteric site sedimentation rates and are going to do a chest x-ray so let's see if it's structural problem or a functional problem do you understand Okay. Do you want to ask a question? Do you have any questions? Yes, I was going to ask that, are you going to keep me in your hospital or do I have to go home? Can I be treated from home? Because I don't know. We are going to admit you for some time to evaluate you and because of the breathlessness you are having, right? Okay, that's fine. So thank you very much i think that's fine i will just yeah i will just do the laps and wait for is for you to start the treatment. Thank you.</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Hello. Hello. Good afternoon. Good afternoon. I'm Doctor Yemi and I'll be the one attending to you this afternoon. Alright, so can you tell me what brought you to the hospital? I've been having my body has been feeling hot for a while now. It's very hot. Oh, I'm so sorry to hear about that. So, I'd like to know more about this so I'd know how best to help you. When did it start? It started a week ago. sorry to hear about that so i'd like to know more about this so i'd know how best to you know help you so when did it start started a week ago was this sudden onset it was gradual it was gradual and how has it been since then has it progressed has it gotten better it has gotten worse it has gotten worse okay aside from this high body temperature do you have any other associated dead Yes, I've been having this very bad headache. Okay. Body pains. Okay. And sometimes I shiver. Okay. Okay. So all these symptoms, do they start with the high body temperature? Yes. And it especially gets worse at night. At night. Okay. Okay. So you feel like, what during the day? How do you feel during the day during the day um i vomit like i vomited for example today and i vomited like four times okay okay so the headache what part of your head are you having this headache my front part of my front part of your head i will describe it like in any actual eye pain no okay i'd like to ask you um when was your last menstrual period um last morning okay so you've done you've all had the missed period yeah okay all right thank you very much so aside from this i'd like to um so what have you done since it started so far i haven't done i'm i won't take you first with paracetamol just for a short while okay okay okay so um i'd just like to ask some other systemic questions to be sure that everything is fine with our systems so from um any um neck pain or stiffness no any cough or chest pain have pain? No. Have you been going to... Have you any urinary symptoms? No. Any diarrhea? No. Okay. So, like, from what you told me so far, you said you've been having high body temperature. Yes. There was headache and body pain, and you shivered for about a week now. Am I correct i correct and also this happens more in the evenings okay and there's also been vomiting how about your appetite are you ever tired of being fine uh that's reduced reduced appetite okay okay so are you being me um i'd like to ask for your past medical history now i've been married to any medical condition in the past are you on any routine medications um do you drink alcohol do you smoke cigarettes have you had surgery before in the past have you ever been addicted in the hospital no you have been transfused with blood okay um are you married no okay are you sexually active no okay that's that's that's okay and what do you do for work i'm a student oh okay where do you school um you know okay now um i would like to ask for this um consultation are you paying out of pocket or yeah under insurance i'm paying out of pocket and how are your finances like you know um well depend i'm depending on my parents okay okay okay all right that's that's very good so um is there any other thing that you think is important that i must have missed out in the course of this um conversation none for now okay all right thank you very much so i'd like to um examine you now i'll do a general examination and and systemic examinations so um well from what you've told me so far let's just you know do a quick recap he said you've been having headache body pains and fever for about a week you're vomiting so and it's your cause more in the evenings so i'm thinking you're having a condition you're having malaria so but what we need to do is we need to confirm we take blood samples to the lab we'll do a malaria parasite test so if it comes out positive we'll give you medications for malaria but for now we'll give you um paracetamol for the fever and the headache and the body pains so i would also like you to you know bed rest if you need notes for school to maybe exempt you from school we can also issue that for you do you have any other thing would like you know like me to help with so i'll direct you to the lab where they'll do the test and well which the test results all right have any other thing no all right thank you so much for your time all right have a lovely day bye</t>
+          <t xml:space="preserve"> Good afternoon, sir. I am Dr. Shadekoff. Good afternoon, doctor. How are you doing today, sir? Doctor, I'm not too fine. I'm not too fine. That's why I came to the hospital today. What are the complaints? So, doctor, I've been coughing for about a week now. and I've been also at What's the complaints? So, doctor, I've been coughing for about a week now. And I've been also... You also have what? So, and I also have... I've also been running temperature for about five days. So, it's been really... You've been running temperature for five days? Yes, yes. And the cough has been for... The cough has been for how long? For about a week now. A week? Yes. yes. And the cough has been for how long? For about a week now. A week? Yes. Okay. All right. So the cough, did it start suddenly or gradually? The cough started suddenly. It started like that. So I just woke up one morning and started coughing. By a week ago, yes. Was there any symptoms like catarrh or any difficulty in swallowing before the cough started? None like that. I had nothing like that. You had nothing like that? Yes. So now the cough, how does it sound? Does it sound like barking? Does it sound like it comes in barking? And then you have to take a deep breath. When you say barking, do you mean like a dog? Or what do you mean by barking? Yes, yes. It sounds like a dog barking. No, no, no, no, no. Mine is not like that. I didn't experience anything like that. Okay. So is the cough productive or phlegm? Yes, yes, it's productive. When I cough, I bring out some substance from my mouth. Yes. So what's the colour of the substance stuff yeah it's about yeah it's clear it's whitish it's not it's just normal it's looking like saliva but it's very thick it's very thick was there blood in it at any point no there was no blood in it there was no blood in it there was no blood in it at any point? Yes. And after you cough, do you feel like vomiting or do you vomit? No, I don't. I don't. I don't feel like vomiting. I don't vomit at all. Okay. And you did not have catarrh or difficulty swallowing prior to onset of the cough? cough? No. I was not in, I was not, I had nothing. Even when I was coughing, my chest was not paining me it was just the cough and i discovered after a few days after that i was tired running temperature too my body was very very hot it was very hot i was shivering so you're telling me there is no there is no cough there is no chest pain no there, there is no chest pain. My chest was not paining me at all. Is there anybody coughing around you? No, there is nobody. I stay alone right now so I have nobody around me. I don't stay with people so I don't have anybody around me that is coughing too. And I walk too, there is nobody coughing around me so okay so you stay in the room you're not in a crowded place yes but yes but doctor i noticed what actually tell me to come is the fact that about two days ago i noticed that the cough became worsened and i was i said to have some difficulty in breathing. So that got me really scared. I was feeling breathless for a moment. And since then, the breathlessness has become more worsened. So that's what exactly prompted me to come quickly to see you. You're finding it difficult to breathe? Yes. When you sleep at night, do you sweat excessively? No, at all. I don't sweat. So what relieves the breathlessness? Any changing position that relieves the breathlessness or is it constant, it's not associated with any position or nothing. It just comes and goes. I just feel breathlessness for a while, then it releases me. Then it comes again, especially when I'm coughing. Has this worsened progressively? Yes, yes. It's gotten very bad, doctor, that's why I came to the hospital. Does it affect your daily activities? Yes, it does doctor. I have not been able to walk for the past two days because of the cough and the fact that I have not been feeling well generally in my body. Now, this fever that you were having, did it start suddenly or gradually? It started gradually then I became very hot and it has been like that. So the fever is high grade, you're very hot? Yes, yes it's high. Did you at attend the question time check by yourself at your temporary job? Yes, I did. I did. I was about 38.9. It's about 37.9. 37.9. OK. And what do you do that released the fever? I took some Prost more. It relieved a bit then, but it didn't last long. It just became hot again and it has been like that ever since. So I just want to ask you some questions. Has this thing happened before in the past? Okay. Has it happened in the past? No, no, no, no. This is the first time I'm expressing this kind of thing. Okay. This is the first time. Do you have any any medical condition like are you asthmatic do you need a blood group on genotype oh no i'm not a doctor i'm fine no i have not seen no i am are you a potential user i can't hear you properly are you hypertensive or diabetic none none no no no i have none of them i have none of them so what have you what have you done to care for yourself so far um i just i just tried to try to get some cough syrup but they didn't probably didn't seem to work properly. They didn't seem to work and since the difficulty in breathing started, I knew I needed to speak to someone, to a doctor, so that's why I came today. For you to know what's wrong with me and treat myself basically. Have you been admitted before? No, not that I can remember. Have you done any surgical procedure before? No. Okay, so I'm just going to ask you some other questions just to know what exactly could be related to the symptoms you're having. So, do you have a headache? Headache? It just comes once in a while. Maybe because the cough, I've not been able to sleep. So, kind of, yeah, kind of, yes. Okay. So, any loss of consciousness? No, no, no. No. Okay. Do you have kata? No, at all. Okay. Do you have any abdominal pain? No, no. Do you have any abdominal pain? No, I have no abdominal pain at all. No. Do you have any bone pain? Yes. Hmm? Thank you. No, I've not vomited at all. No. Do you have any bone pain? Yes. Hmm? No. It's just the shoulders of breath that have been having. The difficulty in breathing that have been having. So, in summary, you're telling me you've had cough, fever, and difficulty in breathing. Yes. Right. And your cough is productive. Yes. All right. So I'm going to have to examine you. Right. I'm going to have to examine you. And I'm going to have to listen to your chest to know whatever is going on in your chest, whether it's a chest infection that is causing you to have a fever and a cough. Do you understand? And then we are going to have you do some investigations like a chest x-ray, a complete blood count, a full blood count, which will tell us whether there's an infection going on depending on the parameters that are elevated or reduced. Do you understand? We are going to do um, ifide segmentation rates to know whether there's an inflammatory process going on. Do you understand? And then we're also going to take your sputum, your deflame, and we're going to send it for culture sensitivity to know what bacteria is being cultured. Please, I just want to ask you, do you smoke? No, no, I don't. I'm a good Christian. I don't smoke, I don't drink. You don't drink alcohol either? I don't drink any of those. I don't do drugs. I don't drink any of that. I'm going to ask you some other questions do you have they are kind of personal questions can I go ahead yeah I just want to know I just want to be fine I just want to know how soon you can start treating me I just want to ask if I just want to ask if you have multiple sexual partners and then your sexual practice no no you have oral sex i'm married no not at all not at all i'm already i'm free so we are going to start you from the history and the examination you have done and then i'm going to ask you to do some investigations however we have some um different house like diagnosis because what the cost of what is causing the cough and the fever we have some um just in the back of our mind which could be the cause you understand you think you have a pneumonia pneumonia chest infection so we're going to start you on the blood spectrum antibiotics right and then we're going to start your cough serum right to treat the cough while we wait for the results of our investigations do you understand okay and then since there's no history of asthma by the time you start start treatment with the antibiotics and the cough syrup, the breathlessness is going to reduce. But we would have checked your oxygen saturation, and we see that it is fine. So there will be no need to place you on oxygen. So we are going to have you do a full blood count, a sputum, and microscop contrast sensitivity. You are going to have you do an ultrasound segmentation rate, and you are going to do a chest x-ray. So let's see if it is a structural problem or a functional problem. Do you understand? Okay, doctor. Okay. You want to ask me a question? Do you have any question? question yes i was going to ask that i'm able to keep me in your speech or do i can i can i be treated from home because i don't know we we are going to um admit you uh for some time to evaluate you because because of the breathlessness you're having, right? Okay. Okay. Okay. Okay. Okay. Okay. Okay. Okay. Okay. Okay. Okay. Okay. Okay. Okay. Okay. Okay. Okay. Okay. Okay. Okay. Okay. Okay. Okay. Okay. Okay. Okay. Okay. Okay. Okay. Okay. Okay. Okay. Okay. Okay. Okay. Okay. Okay. Okay. Okay. Okay. Okay. Okay. Okay. Okay. Okay. Okay. Okay. Okay. Okay. Okay. Okay. Okay. Okay. Okay. Okay. Okay. for the investigation. Cultural sensitivity could take about 72 hours to find this for you to be ready. Do you understand? No problem, doctor. Thank you. No problem, doctor. Thank you very much. I think that's fine. I will just do the labs and wait for you to start the treatment. Thank you very much. I think that's fine. I will just, yeah, I'll just do the labs and wait for, just for you to start the treatment. Thank you. No, I don't promise.</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>hello hello good afternoon good afternoon i am doctor yemi and ill be the one attending to you this afternoon all right so can you tell me what brought you to the hospital i have been havingerm my body has been feeling hot for a while now as in very hot oh i am so sorry to hear about that so id like to know more about this so i would know how best to you know help you so when did it start started a week ago was is sudden in onset or it was gradual it was gradual and how has it been since then has it progressed has it gotten better or it has gotten worse it has gotten worse ok aside from this high body temperature do you have any other associated symptom yes i have been having this very bad headache ok body pains ok ok ok so all these symptoms now did it starts with the high body temperature yes and it especially it gets worse at night at night ok ok so you feel like what of during the day how how do you feel during the day during the day erm i vomit like i vomited for example today now i vomited like four times ok this morning ok so the headache what part of your head are you have having this headache the my front part of my head front part of your head i will do you describe it like any associated eye pain no ok hmm last month ok so you have not you have not had a missed yeah ok alright thank you very much so aside from this id like to ermso what have you done since it started so far i have not done i have i have only taken paracetamol you have only taken para and any any any relief with paracetamol just for a short while ok ok ok so erm id just like to ask some other systemic questions to be sure that everything is fine with other systems so from any uhm neck pain or stiffness no any cough or chest pain no have you been going to have you any urinary symptoms no any diarrhea no ok so like from what you told me so far you said you have been having high body temperature yes there was headache and body pain and you shiver for about a week now am i correct and also this happens more in the evenings ok and there is also been vomiting how about your appetite has your appetite been fine it has reduced reduced appetite ok ok so are you being erm i would like to ask for your past medical history now are you been managed for any medical condition no in the past are you on any routine medications no do you drink alcohol no do you smoke cigarettes no have you had surgery before in the past no have you ever been admitted in the hospital no have you ever been transfused with blood no ok erm are you married no ok are you sexually active no ok that is that is that is that is ok and what do you do for work i am a student oh ok where do you school unilag ok now i am most i would like to ask for this erm consultation are you paying out of pocket or you are under insurance i am paying out of pocket and how are your finances like you know well depend i am depending on my parents ok ok ok alright that is that is very good so erm asides this is there any other thing that you think its important that i might have missed out in the course of this conversation none for now ok alright thank you very much so id like to examine you now ill do a general examination and for and focus and systemic examinations so well from what you have told me so far let us just you know do a quick recap you said you have been having headache body pains and fever for about a week with vomiting so and this it occurs more in the evenings so i am thinking you are having a condition you are having malaria so but what what would need to do is well need to confirm well take blood samples to the lab well do erm malaria parasite test so if it comes out positive well give you medications for malaria but for now wed give you paracetamol for the fever and the erm headache and the body pains so wed also like you to you know bed rest if you need erm notes for school to maybe exempt you from school we can also issue that for you do you have any other thing you would like you know like me to help with so ill direct you to the lab where they will do the test and while we await the test results alright have any other thing no alright thank you so much for your time thank you very much alright have a lovely day you too bye</t>
+          <t>Good afternoon, sir. I am Dr. Shadakoff. Good afternoon. Good afternoon, Doctor. How are you doing today, sir? Doctor, I'm not, I'm not too fine on not too fine. That's why I came to the hospital today. What's the complaints? So, doctor, I've been coughing for about a week now. And I've been also at yes. You also have what? So, and I also have also been running temperature for about five days. It's been really five days. Yes, yes. And the cough has been for the cough has been for how long? For about a week now. A week. Yes. Okay. All right. So, um, the cough, did this start soddening the or gradually? The cough started suddenly just started like that. I just woke up more morning and started coughing by a week ago. Yes. Was there any symptoms like Qatar or any difficulty in swallowing before the cough started? No, none like that. I had nothing like that. Nothing like that. You had nothing like that. Yes. Okay. So now the cough, how does it sound? Does it sound like backing? Does this sound like it comes in body? And then you have to take a different when you say backing, are you? Do you mean like a dog or what do you mean by backing? Yes, yes, sounds like a dog back. No, no, no, no, no. Mine is not that. Okay. So is the cough productive of flame? Yes, yes, it's productive. Yes, when I cough, I bring out some substance from my mouth. Yes. So what's the colour of the substance? Yeah, it's about, yeah, it's clear. It's whitish. It's just normal. It's looking like saliva, but it's very thick. It's very thick. Was there blood in it at any point? No, there was no blood in it. There was no blood in it. There was no blood in it at any point. Okay. And after you cough, do you feel like vomiting or do you vomit? No, I don't. I don't. I don't feel like I don't vomit at all. Okay. And you did not have catar or difficulty in swallowing prior to the onset of the cough. No, no, no, I was nothing. I was not, I had nothing. Even when I was coughing, my chest was not painting me. Nothing. It was just the cough. And I discovered after a few days after that I was hired running temperature too. My body was very, very hot. It was very hot. I was shivering. So you're telling me there is no cough. There is no chest pain. No, there is no chest pain. My chest was not paining me at all. It just was not pain. Is there anybody coughing around you? No, there's nobody. I stay alone right now. So I have nobody around me. I don't tell you people. So I don't remember coughing too. And I walk too. There's nobody coughing around me. Okay. So you stay alone. You're not in an overcrowded place. Yes. But yes, but doctor, I noticed what actually prompted me to come is the fact that about two days ago, I noticed that the cough became worsened and I said to have some difficulty in breathing. So like that got me really scared. I was feeling breathless for a moment, comes and goes. And since that, since then, the breathlessness has become more worsened. So that's what exactly prompted me to come quickly to see you. You're finding it difficult to breathe. Yes. Yes. When you sleep at night, do you sweat excessively? No, at all. I don't sleep. I don't sweat. Yes. Okay. Okay. So what's what relieves the breathlessness? Any change in position that relieves the breathlessness or this constant? No, it's not associated with any position, nothing. I just it just comes and goes like I just feel breathless for a while, then it relieves me. Then it comes again. Especially when I'm sitting when I'm coughing. Has this worsened progressively? Yes, yes. That's gotten very bad, doctor. That's why I came to the hospital. Does it affect, does it affect your daily activities? Yes, it does, doctor. I've not been able to work for the past two days because of the cough and the fact that I've not been feeling well generally in my body. So that's... Now, this fever that you were having, was it, did you start sodding it gradually? It started gradually, then I became very hot and has been like that. It has been like that. So the fever is high-grade. You're very hot. Yes, yes, it's high. Did you attend a question to try and check by yourself at your temperature? Yes, I did. I did. I average thermometer. I was about 38.9. 30.9. Okay. And what do you do that relieves the fever? I took some past more. It relieved the bit then, but it did. It didn't last long. It's just it became what again and it has been like that ever since. So I just want to ask you some questions. Has this thing happened before in the past? Okay. Has it happened in the past? No, no, no, no. This is the first time I'm expressing as I am. This is the first time I'm experiencing this kind of thing. Okay. It's the first time. Are you, do you have any medical condition? Like, are you asthmatic? Do you need a blood group and genotype? Oh, no, I'm not. Doctor, I'm fine. No, I have nothing. Are you hypocensing? I can't hear you properly, sir. Are you hypertensive or diabetic? None, none. No. No, no, I have none of them. I have none of them. So what have you? What have you done to care for yourself so far? I just tried to get some coughs here up, but they didn't seem to work properly. They didn't seem to work. And since the difficulty in breathing started, I know I needed to speak to someone to a doctor. So that's why I came today for you to like, for me to know what's wrong with me and treat myself basically. Have you been admitted before? No, not that current, but none. Have you done any surgical procedure before? No, no. Okay. So I'm just going to ask you some other questions just to know what exactly could be related to your to the symptoms you're having. So do you have headache? Headache. Yes, it comes once in a while. Maybe because the cough, I've not been able to sleep really. So kind of, yeah, kind of, yes. Okay. So any loss of consciousness? No, no, no. No. Okay. Okay. Do you have catar? No, at all. Okay. Do you have any abdominal pain? No, no. I don't have a problem. No, I'm not vomited at all. You have any bone pain? Yes. No, no, the most it's just the shortness of breath I've been having. The difficulty in breathing has been having. So in summary, you're telling me, some are telling me you had, you've had cough, fever, and difficulty in breathing. Yes. Right? And your cough is productive. Yes. All right. So I'm going to have to have to examine you, right? I'm going to have to examine you and I'm going to have to listen to your chest to know if to know whatever is going on in your chest, whether there's a chest infection that is causing you to have a fever and the cough. Do you understand? And then we are going to have you do some investigations like a chest x-ray, a complete blood count of a full blood count to tell us whether there's an infection going on, depending on the parameters that are indicated or reduced. Do you understand? We are going to do a neutrocyte segmentation rate to know whether there's an inflammatory process going on. Do you understand? And then we're also going to take your sputum, the flame, and we're going to send it for cultural sensitivity to know what bacteria is being caught. Please, I just want to ask you, do you smoke? No, no, I don't. So, Doctor, I'm a good Christian. I just spoke, I don't think. You don't drink alcohol either? I don't drink any of those. I don't do drugs. I don't drink of that. I'm going to ask you some other questions. Do you have there are kind of personal questions? Can I go ahead? Yeah, I just want to know. Doctor, I just want to, I just want to be fine. I just want to know how soon you can start with me. I just want to ask if I just want to ask if you have multiple sexual partners and your sexual practices. No, no. Do you have oral sex? I'm married. No, not at all. Not at all. So we are going to start you from the history and the examination you have done. And then we're going to ask you to do some investigations. However, we have some differentials, like diagnosis. The cause of what is causing the cough and the fever. We have some at the back of our mind, which could be the cause. You understand? We think you have a pneumonia, a chest infection. So we are going to start you on a broad spectrum antibiotics, right? And then we are going to start on the cough syrup, right? To treat the cough while we wait for the results of our investigations. Do you understand? Okay. And then since there is no history of asthma, by the time you start treatment with the antibiotics and the cough syrup, there will be the breathlessness is going to reduce. But we'll have checked your oxygen saturation and we see that it is fine. So there'll be no need to place you on oxygen. So we are going to have you do a full block count, a sputum and microscopic control sensitivity. I'm going to have you do an intrusive sedimentation rate. And we're going to do a chest x-ray. So let's see if it's a structural problem or a functional problem. Do you understand? Okay, doctor. Okay. You want to ask me a question? Do you have any questions? Yes, I was going to ask that. Are you going to keep me in your hospital? Can I be treated from home? Because I don't know. We are going to admit you for some time to evaluate you. And because of the breathlessness you're having, right? Okay. Okay, that's fine. 72 hours to five days for you to be ready. Do you understand? No problem, doctor. No problem, doctor. Thank you very much. I think that's fine. I will just, yeah, I'll just do the labs and wait for you to start the treatment. Thank you.</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>hello hello good afternoon good afternoon i am doctor yemi and ill be the one attending to you this afternoon alright so can you tell me what brought you to the hospital i have been having my body has been feeling hot for a while now its very hot oh i am so sorry to hear about that so id like to know more about this so id know how best to help you when did it start it started a week ago sorry to hear about that so id like to know more about this so id know how best to you know help you so when did it start started a week ago was this sudden onset it was gradual it was gradual and how has it been since then has it progressed has it gotten better it has gotten worse it has gotten worse okay aside from this high body temperature do you have any other associated dead yes i have been having this very bad headache okay body pains okay and sometimes i shiver okay okay so all these symptoms do they start with the high body temperature yes and it especially gets worse at night at night okay okay so you feel like what during the day how do you feel during the day during the day um i vomit like i vomited for example today and i vomited like four times okay okay so the headache what part of your head are you having this headache my front part of my front part of your head i will describe it like in any actual eye pain no okay id like to ask you um when was your last menstrual period um last morning okay so you have done you have all had the missed period yeah okay all right thank you very much so aside from this id like to um so what have you done since it started so far i have not done i am i will not take you first with paracetamol just for a short while okay okay okay so um id just like to ask some other systemic questions to be sure that everything is fine with our systems so from um any um neck pain or stiffness no any cough or chest pain have pain no have you been going to have you any urinary symptoms no any diarrhea no okay so like from what you told me so far you said you have been having high body temperature yes there was headache and body pain and you shivered for about a week now am i correct i correct and also this happens more in the evenings okay and there is also been vomiting how about your appetite are you ever tired of being fine uh that is reduced reduced appetite okay okay so are you being me um id like to ask for your past medical history now i have been married to any medical condition in the past are you on any routine medications um do you drink alcohol do you smoke cigarettes have you had surgery before in the past have you ever been addicted in the hospital no you have been transfused with blood okay um are you married no okay are you sexually active no okay that is that is that is okay and what do you do for work i am a student oh okay where do you school um you know okay now um i would like to ask for this um consultation are you paying out of pocket or yeah under insurance i am paying out of pocket and how are your finances like you know um well depend i am depending on my parents okay okay okay all right that is that is very good so um is there any other thing that you think is important that i must have missed out in the course of this um conversation none for now okay all right thank you very much so id like to um examine you now ill do a general examination and and systemic examinations so um well from what you have told me so far let us just you know do a quick recap he said you have been having headache body pains and fever for about a week you are vomiting so and its your because more in the evenings so i am thinking you are having a condition you are having malaria so but what we need to do is we need to confirm we take blood samples to the lab well do a malaria parasite test so if it comes out positive well give you medications for malaria but for now well give you um paracetamol for the fever and the headache and the body pains so i would also like you to you know bed rest if you need notes for school to maybe exempt you from school we can also issue that for you do you have any other thing would like you know like me to help with so ill direct you to the lab where they will do the test and well which the test results all right have any other thing no all right thank you so much for your time all right have a lovely day bye</t>
+          <t>good afternoon sir i am doctor sadeko good afternoon good afternoon doctor how are you doing today sir doctor i am not i am not too fine not too fine that is why i came to the hospital today what was the complaints so doctor i have been coughing for about a week now and i have been also also have you also have what so and i also have  i have also been running temperature for about five days so you have running temperature for five days yes yes for about a week now a week yes okay all right so the cough did it start suddenly or gradually the cough started suddenly just started like that i just just woke up more morning and started coughing about a week ago yes was there was there any symptoms like catarrh or  any  any difficulty in swallowing before the cough started no none like that i had nothing like that nothing like that you had nothing like that yes okay so now the cough how does it sound does it sound like barking does it sound like it is comes in bouts and then you have to take a deep breath when when you say barking do you are you do you mean like a dog or what do you mean by barking yes yes sounds like a dog barking no no no no no no mine is not that i did not i did not experience anything like that okay so is the cough productive of phlegm yes yes it is productive when i yes when i cough i bring out some some substance from my mouth yes so what is the colour of the substance err it is about  it is clear it is whitish it is not it is just normal it is looking like saliva but it is very thick it is very thick was there blood in it at any point no there was no blood in it there was no blood in it there was no blood in it at any point yes and after you cough do you feel like vomiting or do you vomit no i do not i do not i do not feel like vomiting i do not vomit at all okay and you did not have catarrh or difficulty in swallowing prior to onset of the cough no no there was nothing i was not i had nothing my my even when i was coughing my chest was not paining me nothing it was just the cough then i i discovered after a few days after that i just started running temperature too my body was very very hot it was very hot that i was shivering so you are telling me there is no there is no cough there is no chest pain no there is there is no chest pain my chest was not paining me at all your chest was not paining me is there anybody coughing around you no there nobody i stay alone right now so i have nobody around me i do not stay with people so i do not have anybody around me that is coughing too and at work too there is nobody coughing around me so okay so you stay alone you are not here in an overcrowded place yes but yes but doctor i noticed what actually prompted me to come is the fact that about two days ago i noticed that the cough became worsened and i was i started to have some difficulty in breathing so like that got me really scared like i was i was i was just feeling breathless for a moment comes and goes then and since that since then the breathlessness has become more worsened so that is what exactly prompted me to completely to see you you are finding it difficult to breathe yes yes when you sleep at night you sweat excessively no at all i do not i do not slept i do not sweat when i sleep at night okay so what is what relieves the breathlessness any change in position that relieves the breathlessness or it is constant no it is not associated with  any any position nothing i just it just comes and goes like i just feel breathless for a while then it relieves me then it comes again especially when i am especially when i am coughing okay has this worsened progressively yes yes it has gotten very bad doctor that is why i came to the hospital does it affect does it affect your daily activities yes it does doctor i have not been able to work for the past two days because of the cough and the fact that i have i have not been feeling well generally in my body so that is so now this fever that you were having was it did it start suddenly or gradually it started it started gradually then became i became very hot and it has been like that it has been like that so the fever is high grade you are very hot yes yes it is high did you at any point yes check by yourself at home your temperature yes i did i did i have a thermometer it was about was about thirtyeightnine thirtyeightnine okay and what does what do you do that relieves the fever i took some i took some paracetamol it relieved a bit then but it did did not last long i just i i became hot again and it has been like that ever since so i just want to ask you some questions has anything happened before in the past okay has it happened in the past no no no no this is the first time i am experiencing that is why i am this is the first time i am experiencing this kind of thing okay this is the first time are you do you have any medical condition like are you asthmatic during your blood group and genotype no i am not doctor i am fine no i have nothing and that is why this is surprising are you hypertensive what did you say i cannot hear you properly sir are you hypertensive or diabetic none none none none no no i have none of them i have none of them so what have you what have you done to care for yourself so far i just i just i just tried to get some cough syrup but they did not they did not seem to work properly they did not seem to work and since the difficulty breathing started i knew i knew i know i needed to like come to speak to someone to a doctor so that is why i came today for you to like for me to like know what is wrong with me and treat myself basically have you been have you been admitted before no not not not that i can remember have you done any surgical procedure before no no okay so i am just going to ask you some other questions just to know what exactly could be related to your to the symptoms you are having so do you have headache headache just comes once in a while maybe because the cough i have not been able to sleep really so kind of yeah kind of yes okay so any loss of consciousness no no no no okay okay do you have catarrh no at all okay do you have any abdominal pain no no i do not have any diarrhea or vomiting no i have not vomited at all you have any bone pain yes no the no the most it is just it is just the shortest of breath i have been having the difficulty in breathing i have been having that is just that is just so in summary you are telling me in summary you are telling me you had you you have had cough fever and difficulty in breathing yes right and your cough is productive yes all right so i am going to have to have to examine you right i am going to have to examine you and i am going to have to listen to your chest to know if to know whatever is going on in your chest whether there is a chest infection that is causing you to have a fever and the and the cough do you understand and then we are going to have you do some investigations like a chest xray a complete blood count a full blood count which will tell us whether there is an infection going on depending on the parameters that are elevated or reduced do you understand we are going to do you know electrocyte segmentation rates to know whether there is an inflammatory process going on do you understand and then we are also going to take your sputum your the phlegm and we are going to send it for culture sensitivity to know what bacteria is is being cultured  please i just want to ask you do you smoke no no i do not doctor i am a good christian i do not smoke i do not drink you do not you do not drink alcohol either i do not i do not do any of those i do not do drugs i do not do any of that i am going to ask you some other questions do you have their kind of personal questions can i go ahead yeah i just want to know doctor i just want to i just want to be fine i just want to know how soon you can start treating me and what i will need to take basically i just want to ask ifi just want to ask if you have multiple sexual partners and then your sexual practices no no you have oral sex i am married no not at all not at all i am married so we are going to start you from the history and the examination we have done and then we are going to ask you to do some investigations however we have some differentials like diagnosis the because the because of what is causing the cough and the fever we have some this thing at the back of our mind which could be the because do you understand we think you have a pneumonia pneumonia a chest infection so we are going to start you on a broad spectrum antibiotics right and then we are going to start you on the cough syrup right to treat the cough while we wait for the results of our investigations do you understand okay and then since there is no history of asthma by the time you will start treatment with the antibiotics and and the cough syrup there will be the breathlessness is going to reduce but we your we would have checked your your oxygen saturation and we will see that it is fine so there will be no need to place you on on oxygen so you are going to have you do a full blood count in sputum and microscopy culture sensitivity you are going to have you do any erythrocyte segmentation rate and you are going to do a chest xray so let us see if it is a structural problem or a functional problem do you understand okay doctor so doctor do i do you want to ask the question if you have any questions yes i was going to ask that are you going to keep me in the hospital or do i that can i can i be treated from home because i do not know we we we are going to admit you for some time to evaluate you and because of the breathlessness you are having right and then we will start you on on intravenous intravenous  that is okay that is cool culture and sensitivity could take about seventytwo hours to to five days before it will be ready do you understand yeah no problem doctor thank you no problem doctor thank you very much i think that is fine i will just yeah i will just do the labs and wait for just for you to start the treatment thank you</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t xml:space="preserve">hello hello good afternoon good afternoon i am dr yemi and ill be the one attending to you this afternoon all right so can you tell me what brought you to the hospital i have been having um my body has been feeling hot for a while now its very hot oh i am so sorry to hear about that so id like to know more about this so i know how best to you know help you so when did it start started a week ago was this sudden or was it gradual it was gradual and how has it been since then has it progressed has it gotten better it has gotten worse it has gotten worse okay aside from this high body temperature do you have any other associated symptom yes i have been having this very bad headache okay body pains okay and sometimes i shiver okay okay so all these symptoms are do they start with the high body temperature yes and it especially gets worse at night at night okay okay so you feel like what of during the day how how do you feel during the day during the day um i vomit okay i vomited for example today and i vomited like four times this morning okay so the headache what part of your head are you having this headache my front part of my head front part of your head are you describing it like in any as your eye pain no okay i would like to ask you when was your last menstrual period last month okay so you have had a missed period yeah okay alright thank you very much so aside from this id like to so what have you done since it started so far i have not done i have not taken any paracetamol any relief with paracetamol just for a short while okay okay okay so id just like to ask some other systemic questions to be sure that everything is fine with our systems so from any any neck pain or stiffness no any cough or chest pain no have you been um going to have you any urinary symptoms no any diarrhea no okay so like from what you told me so far you said you have been having um high body temperature yes there was headache and um body pain and you shiver for about a week now am i correct and also this happens more in the evenings okay and there is also been vomiting how about appetite i your appetites been fine it does reduced reduced appetite okay okay so are you being me i would like to ask for your past medical history now have you been married for any medical condition no in the past are you on any routine medications no do you drink alcohol no do you smoke cigarettes no have you had surgery before in the past no have you ever been admitted in the hospital no you have been transfused with blood no okay are you married no okay are you sexually active no okay that is that is that is it and what do you do for work i am a student okay where do you go you know i okay now i am most i would like to ask for this consultation are you paying out of pocket or are you under insurance i am paying out of pocket and how are your finances like you know well depend i am depending on my okay okay okay alright that sounds very good so um aside to is it is there any other thing that you think is important that i must have missed out in the because of this conversation none for now okay alright thank you very much so id like to examine you now ill do a general examination and systemic examinations so um well from what you have told me so far let us just you know do a quick recap said you have been having headache body pains and fever for about week were vomiting so and its causing more in the evenings so i am thinking you are having a condition you are having malaria so but what we need to do is we need to confirm well take um blood samples to the lab well do malaria parasite tests so if it comes out positive well give you medications for malaria but for now well give you um paracetamol for the fever and the um headache and the body pains so also like you to you know bed rest if you need um notes for school to maybe exempt you from school we can also issue that for you do you have any other thing would like you know like me to help with so ill direct you to the lab and well do the test and well i wish the test results alright have any other thing no alright thank you so much for your time thank you very much alright have a lovely day you too bye </t>
-        </is>
-      </c>
-      <c r="K3" t="n">
-        <v>0.2537313432835821</v>
-      </c>
-      <c r="L3" t="n">
-        <v>68</v>
+          <t>good afternoon sir i am doctor shadekoff good afternoon doctor how are you doing today sir doctor i am not too fine i am not too fine that is why i came to the hospital today what are the complaints so doctor i have been coughing for about a week now and i have been also at what is the complaints so doctor i have been coughing for about a week now and i have been also you also have what so and i also have i have also been running temperature for about five days so it is been really you have been running temperature for five days yes yes and the cough has been for the cough has been for how long for about a week now a week yes yes and the cough has been for how long for about a week now a week yes okay all right so the cough did it start suddenly or gradually the cough started suddenly it started like that so i just woke up one morning and started coughing by a week ago yes was there any symptoms like catarrh or any difficulty in swallowing before the cough started none like that i had nothing like that you had nothing like that yes so now the cough how does it sound does it sound like barking does it sound like it comes in barking and then you have to take a deep breath when you say barking do you mean like a dog or what do you mean by barking yes yes it sounds like a dog barking no no no no no mine is not like that i did not experience anything like that okay so is the cough productive or phlegm yes yes it is productive when i cough i bring out some substance from my mouth yes so what is the colour of the substance stuff yeah it is about yeah it is clear it is whitish it is not it is just normal it is looking like saliva but it is very thick it is very thick was there blood in it at any point no there was no blood in it there was no blood in it there was no blood in it at any point yes and after you cough do you feel like vomiting or do you vomit no i do not i do not i do not feel like vomiting i do not vomit at all okay and you did not have catarrh or difficulty swallowing prior to onset of the cough cough no i was not in i was not i had nothing even when i was coughing my chest was not paining me it was just the cough and i discovered after a few days after that i was tired running temperature too my body was very very hot it was very hot i was shivering so you are telling me there is no there is no cough there is no chest pain no there there is no chest pain my chest was not paining me at all is there anybody coughing around you no there is nobody i stay alone right now so i have nobody around me i do not stay with people so i do not have anybody around me that is coughing too and i walk too there is nobody coughing around me so okay so you stay in the room you are not in a crowded place yes but yes but doctor i noticed what actually tell me to come is the fact that about two days ago i noticed that the cough became worsened and i was i said to have some difficulty in breathing so that got me really scared i was feeling breathless for a moment and since then the breathlessness has become more worsened so that is what exactly prompted me to come quickly to see you you are finding it difficult to breathe yes when you sleep at night do you sweat excessively no at all i do not sweat so what relieves the breathlessness any changing position that relieves the breathlessness or is it constant it is not associated with any position or nothing it just comes and goes i just feel breathlessness for a while then it releases me then it comes again especially when i am coughing has this worsened progressively yes yes it is gotten very bad doctor that is why i came to the hospital does it affect your daily activities yes it does doctor i have not been able to walk for the past two days because of the cough and the fact that i have not been feeling well generally in my body now this fever that you were having did it start suddenly or gradually it started gradually then i became very hot and it has been like that so the fever is high grade you are very hot yes yes it is high did you at attend the question time check by yourself at your temporary job yes i did i did i was about thirtyeightnine it is about thirtysevennine thirtysevennine okay and what do you do that released the fever i took some prost more it relieved a bit then but it did not last long it just became hot again and it has been like that ever since so i just want to ask you some questions has this thing happened before in the past okay has it happened in the past no no no no this is the first time i am expressing this kind of thing okay this is the first time do you have any any medical condition like are you asthmatic do you need a blood group on genotype oh no i am not a doctor i am fine no i have not seen no i am are you a potential user i cannot hear you properly are you hypertensive or diabetic none none no no no i have none of them i have none of them so what have you what have you done to care for yourself so far  i just i just tried to try to get some cough syrup but they did not probably did not seem to work properly they did not seem to work and since the difficulty in breathing started i knew i needed to speak to someone to a doctor so that is why i came today for you to know what is wrong with me and treat myself basically have you been admitted before no not that i can remember have you done any surgical procedure before no okay so i am just going to ask you some other questions just to know what exactly could be related to the symptoms you are having so do you have a headache headache it just comes once in a while maybe because the cough i have not been able to sleep so kind of yeah kind of yes okay so any loss of consciousness no no no no okay do you have kata no at all okay do you have any abdominal pain no no do you have any abdominal pain no i have no abdominal pain at all no do you have any bone pain yes hmm thank you no i have not vomited at all no do you have any bone pain yes hmm no it is just the shoulders of breath that have been having the difficulty in breathing that have been having so in summary you are telling me you have had cough fever and difficulty in breathing yes right and your cough is productive yes all right so i am going to have to examine you right i am going to have to examine you and i am going to have to listen to your chest to know whatever is going on in your chest whether it is a chest infection that is causing you to have a fever and a cough do you understand and then we are going to have you do some investigations like a chest xray a complete blood count a full blood count which will tell us whether there is an infection going on depending on the parameters that are elevated or reduced do you understand we are going to do  ifide segmentation rates to know whether there is an inflammatory process going on do you understand and then we are also going to take your sputum your deflame and we are going to send it for culture sensitivity to know what bacteria is being cultured please i just want to ask you do you smoke no no i do not i am a good christian i do not smoke i do not drink you do not drink alcohol either i do not drink any of those i do not do drugs i do not drink any of that i am going to ask you some other questions do you have they are kind of personal questions can i go ahead yeah i just want to know i just want to be fine i just want to know how soon you can start treating me i just want to ask if i just want to ask if you have multiple sexual partners and then your sexual practice no no you have oral sex i am married no not at all not at all i am already i am free so we are going to start you from the history and the examination you have done and then i am going to ask you to do some investigations however we have some  different house like diagnosis because what the cost of what is causing the cough and the fever we have some  just in the back of our mind which could be the because you understand you think you have a pneumonia pneumonia chest infection so we are going to start you on the blood spectrum antibiotics right and then we are going to start your cough serum right to treat the cough while we wait for the results of our investigations do you understand okay and then since there is no history of asthma by the time you start start treatment with the antibiotics and the cough syrup the breathlessness is going to reduce but we would have checked your oxygen saturation and we see that it is fine so there will be no need to place you on oxygen so we are going to have you do a full blood count a sputum and microscop contrast sensitivity you are going to have you do an ultrasound segmentation rate and you are going to do a chest xray so let us see if it is a structural problem or a functional problem do you understand okay doctor okay you want to ask me a question do you have any question question yes i was going to ask that i am able to keep me in your speech or do i can i can i be treated from home because i do not know we we are going to  admit you  for some time to evaluate you because because of the breathlessness you are having right okay okay okay okay okay okay okay okay okay okay okay okay okay okay okay okay okay okay okay okay okay okay okay okay okay okay okay okay okay okay okay okay okay okay okay okay okay okay okay okay okay okay okay okay okay okay okay okay okay okay okay okay okay okay okay okay for the investigation cultural sensitivity could take about seventytwo hours to find this for you to be ready do you understand no problem doctor thank you no problem doctor thank you very much i think that is fine i will just do the labs and wait for you to start the treatment thank you very much i think that is fine i will just yeah i will just do the labs and wait for just for you to start the treatment thank you no i do not promise</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>good afternoon sir i am doctor shadak good afternoon good afternoon doctor how are you doing today sir doctor i am not i am not too fine not too fine that is why i came to you today what was the complaints so doctor i have been coughing for about a week now and i have been also also at yes you also have what so and i also have  i have also been running temperature for about five days so it is been really yes yes and the cough has been for the cough has been for how long for about a week now a week yes okay alright so  the cough did it start suddenly or gradually the cough started suddenly just started like that i just was there was there any symptoms like qatar or any  any difficulty in swallowing before the cough started no none like that i had nothing like that nothing like that you had nothing like that yes so now the cough how does it sound does it sound like the barking does it sound like a and it comes in and then you have to take a deep breath when you say barking are you do you mean like a dog or what do you mean by barking yes yes sounds like a dog barking no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no substance from my mouth yes so what is the colour of the substance yeah it is about yeah it is clear it is whitish it is normal it is just normal it is looking like saliva but it is very thick it is very thick was there blood in it at any point no there was no blood in it there was no blood in it at any point and after you cough do you feel like vomiting or do you vomit no i do not i do not i do not feel like i am i do not vomit at all okay and you did not have catarrh or difficulty swallowing prior to onset of the cough no no that was not in my i was not i had nothing my my even when i was coughing my chest was not burning me nothing it was just the cough and i i discovered after a few days after that i was running temperature too my body was very very hot it was very hot i was shivering so you are telling me there is no there is no cough there is no chest pain no there is there is no chest pain my chest was not pain in me at all the chest was not pain in me is there anybody coughing around you no there is nobody i stay alone right now so i have nobody around me i do not stay with people so i do not remember anybody around me that is coughing too and i walk to there is nobody coughing around me so okay so you stay alone you are not in a crowded place yes but yes but doctor i noticed what actually prompted me to come is the fact that about two days ago i noticed that the cough became worsened and i was i started to have some difficulty in breathing so like that got me really scared i was i was feeling breathless for a moment comes and goes and and since that since then the breathlessness have become more worsened so that is what exactly prompted me to come quickly to see you so you are finding it difficult to breathe yes the cough yes when you sleep at night do you sweat excessively no at all i do not i do not sleep i do not sweat in a sleep department yes okay so what is what removes the breathlessness any changing position that relieves the breathlessness or is constant no it is not associated with any any position nothing and it just comes and goes like i just feel breathless with a while then it releases me then it comes again especially when especially when i am coughing okay has this worsened progressively yes yes that is gotten very bad doctor that is why i came to the hospital does it affect does it affect your daily activities yes it does doctor i have not been able to walk for the past two days because of the cough and the fact that i have not been feeling well generally so no no this fever that you were having was it did it start suddenly or gradually started it started gradually then became i became very hot and has been like that it has been like that so the fever is high grade very hot yes yes it is i do you have any points that you can check by yourself at home your temperature yes i did i did i have a stomach i was about there was about thirty eight point nine thirty point nine okay and  what do what do you do that releases the fever well i took some i took some past more it relieved the bit then but it did not last long i just i became hot again and it has been like that ever since so i just want to ask you some questions has this happened before in the past okay has it happened in the past no no no no this is the first time i am expressing this this is the first time i am expressing this kind of thing okay this is the first time are you do you have any medical condition like are you asthmatic do you do you need a blood pressure no i am not to doctor i am fine no i have not no are you a hypertensive or diabetic are you a hypertensive or diabetic none none none none no i have none of them i have none of them so what have you what have you done to care for yourself so far i just try to get some cough syrup up but they did not they did not seem to work properly they did not seem to work and since  the difficulty in breathing started i knew i knew i know i needed to like because to speak to someone to a doctor so that is why i came today for you to like for me to like know what is wrong with me and treat myself basically have you been have you been admitted before no not not not that current but none have you done any surgical procedure before no no okay so i am just going to ask you some other questions just to know what exactly could be related to your so the symptoms you are having so do you have headache headache it just comes once in a while maybe because the cough i have not been able to sleep really so kind of yeah kind of yes okay so any loss of consciousness no no no no okay do you have catar no at all okay do you have any abdominal pain no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no no the most of the just the shouters of breath have been happening the difficulty in breathing have been happening so that is the summary you are telling me in summary you are telling me you had you have had cough fever and difficulty in breathing yes right and your cough is productive yes alright so i am going to have to have to examine you right i am going to have to examine you and i am going to have to listen to your chest to know to know whatever is going on in your chest there is a chest infection that is causing you to have a fever and the and the cough do you understand and then we are going to have you do some investigations like a chest xray a complete blood count or a full blood count to tell us whether there is an infection going on depending on the parameters that are elevated or reduced do you understand we are going to do a neutrophil segmentation rate to know whether there is an inflammatory process brain on do you understand and then we are also going to take your sputum your the phlegm and we are going to  send it for culture sensitivity to know what bacteria is  is being cultured  please i just want to ask you do you smoke no no i do not so doctor i am a good christian i do not smoke i do not drink you do not you do not drink alcohol either i do not i do not do any of those i do not do jobs i do not do any of that i am going to ask you some other questions  do you have  there are kind of personal questions can i go ahead yeah i just want to know doctor i just want to i just want to be fine i just want to know how soon you can start treating me and what i do not want to ask if i do not want to ask if you have multiple sexual partners and your sexual practices no no oral sex no none at all not at all so we are going to start you from the history and the examination we have done and then we are going to ask you to do some investigations however we have some differentials like diagnoses the because of what is causing the cough and the fever we have some just in the back of our mind which could be the because do you understand we think you have a pneumonia pneumonia chest infection so we are going to start you on a broad spectrum antibiotics right and then we are going to start you on cough syrup right to treat the cough while we wait for the results of our investigations do you understand okay and then since there is no history of asthma by the time you start treatments with the antibiotics and the cough syrup there will be the breathlessness business is going to reduce but we your we would have checked your oxygen saturation and we see that it is fine so there will be no need to place you on on oxygen so you are against having you do full block out in   sputum and end microscopic culture sensitivity are going to have you doing the enteric site sedimentation rates and are going to do a chest xray so let us see if it is structural problem or a functional problem do you understand okay do you want to ask a question do you have any questions yes i was going to ask that are you going to keep me in your hospital or do i have to go home can i be treated from home because i do not know we are going to admit you for some time to evaluate you and because of the breathlessness you are having right okay that is fine so thank you very much i think that is fine i will just yeah i will just do the laps and wait for is for you to start the treatment thank you</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>good afternoon sir i am doctor shadakoff good afternoon good afternoon doctor how are you doing today sir doctor i am not i am not too fine on not too fine that is why i came to the hospital today what is the complaints so doctor i have been coughing for about a week now and i have been also at yes you also have what so and i also have also been running temperature for about five days it is been really five days yes yes and the cough has been for the cough has been for how long for about a week now a week yes okay all right so  the cough did this start soddening the or gradually the cough started suddenly just started like that i just woke up more morning and started coughing by a week ago yes was there any symptoms like qatar or any difficulty in swallowing before the cough started no none like that i had nothing like that nothing like that you had nothing like that yes okay so now the cough how does it sound does it sound like backing does this sound like it comes in body and then you have to take a different when you say backing are you do you mean like a dog or what do you mean by backing yes yes sounds like a dog back no no no no no mine is not that okay so is the cough productive of flame yes yes it is productive yes when i cough i bring out some substance from my mouth yes so what is the colour of the substance yeah it is about yeah it is clear it is whitish it is just normal it is looking like saliva but it is very thick it is very thick was there blood in it at any point no there was no blood in it there was no blood in it there was no blood in it at any point okay and after you cough do you feel like vomiting or do you vomit no i do not i do not i do not feel like i do not vomit at all okay and you did not have catar or difficulty in swallowing prior to the onset of the cough no no no i was nothing i was not i had nothing even when i was coughing my chest was not painting me nothing it was just the cough and i discovered after a few days after that i was hired running temperature too my body was very very hot it was very hot i was shivering so you are telling me there is no cough there is no chest pain no there is no chest pain my chest was not paining me at all it just was not pain is there anybody coughing around you no there is nobody i stay alone right now so i have nobody around me i do not tell you people so i do not remember coughing too and i walk too there is nobody coughing around me okay so you stay alone you are not in an overcrowded place yes but yes but doctor i noticed what actually prompted me to come is the fact that about two days ago i noticed that the cough became worsened and i said to have some difficulty in breathing so like that got me really scared i was feeling breathless for a moment comes and goes and since that since then the breathlessness has become more worsened so that is what exactly prompted me to come quickly to see you you are finding it difficult to breathe yes yes when you sleep at night do you sweat excessively no at all i do not sleep i do not sweat yes okay okay so what is what relieves the breathlessness any change in position that relieves the breathlessness or this constant no it is not associated with any position nothing i just it just comes and goes like i just feel breathless for a while then it relieves me then it comes again especially when i am sitting when i am coughing has this worsened progressively yes yes that is gotten very bad doctor that is why i came to the hospital does it affect does it affect your daily activities yes it does doctor i have not been able to work for the past two days because of the cough and the fact that i have not been feeling well generally in my body so that is now this fever that you were having was it did you start sodding it gradually it started gradually then i became very hot and has been like that it has been like that so the fever is highgrade you are very hot yes yes it is high did you attend a question to try and check by yourself at your temperature yes i did i did i average thermometer i was about thirtyeightnine thirtynine okay and what do you do that relieves the fever i took some past more it relieved the bit then but it did it did not last long it is just it became what again and it has been like that ever since so i just want to ask you some questions has this thing happened before in the past okay has it happened in the past no no no no this is the first time i am expressing as i am this is the first time i am experiencing this kind of thing okay it is the first time are you do you have any medical condition like are you asthmatic do you need a blood group and genotype oh no i am not doctor i am fine no i have nothing are you hypocensing i cannot hear you properly sir are you hypertensive or diabetic none none no no no i have none of them i have none of them so what have you what have you done to care for yourself so far i just tried to get some coughs here up but they did not seem to work properly they did not seem to work and since the difficulty in breathing started i know i needed to speak to someone to a doctor so that is why i came today for you to like for me to know what is wrong with me and treat myself basically have you been admitted before no not that current but none have you done any surgical procedure before no no okay so i am just going to ask you some other questions just to know what exactly could be related to your to the symptoms you are having so do you have headache headache yes it comes once in a while maybe because the cough i have not been able to sleep really so kind of yeah kind of yes okay so any loss of consciousness no no no no okay okay do you have catar no at all okay do you have any abdominal pain no no i do not have a problem no i am not vomited at all you have any bone pain yes no no the most it is just the shortness of breath i have been having the difficulty in breathing has been having so in summary you are telling me some are telling me you had you have had cough fever and difficulty in breathing yes right and your cough is productive yes all right so i am going to have to have to examine you right i am going to have to examine you and i am going to have to listen to your chest to know if to know whatever is going on in your chest whether there is a chest infection that is causing you to have a fever and the cough do you understand and then we are going to have you do some investigations like a chest xray a complete blood count of a full blood count to tell us whether there is an infection going on depending on the parameters that are indicated or reduced do you understand we are going to do a neutrocyte segmentation rate to know whether there is an inflammatory process going on do you understand and then we are also going to take your sputum the flame and we are going to send it for cultural sensitivity to know what bacteria is being caught please i just want to ask you do you smoke no no i do not so doctor i am a good christian i just spoke i do not think you do not drink alcohol either i do not drink any of those i do not do drugs i do not drink of that i am going to ask you some other questions do you have there are kind of personal questions can i go ahead yeah i just want to know doctor i just want to i just want to be fine i just want to know how soon you can start with me i just want to ask if i just want to ask if you have multiple sexual partners and your sexual practices no no do you have oral sex i am married no not at all not at all so we are going to start you from the history and the examination you have done and then we are going to ask you to do some investigations however we have some differentials like diagnosis the because of what is causing the cough and the fever we have some at the back of our mind which could be the because you understand we think you have a pneumonia a chest infection so we are going to start you on a broad spectrum antibiotics right and then we are going to start on the cough syrup right to treat the cough while we wait for the results of our investigations do you understand okay and then since there is no history of asthma by the time you start treatment with the antibiotics and the cough syrup there will be the breathlessness is going to reduce but we will have checked your oxygen saturation and we see that it is fine so there will be no need to place you on oxygen so we are going to have you do a full block count a sputum and microscopic control sensitivity i am going to have you do an intrusive sedimentation rate and we are going to do a chest xray so let us see if it is a structural problem or a functional problem do you understand okay doctor okay you want to ask me a question do you have any questions yes i was going to ask that are you going to keep me in your hospital can i be treated from home because i do not know we are going to admit you for some time to evaluate you and because of the breathlessness you are having right okay okay that is fine seventytwo hours to five days for you to be ready do you understand no problem doctor no problem doctor thank you very much i think that is fine i will just yeah i will just do the labs and wait for you to start the treatment thank you</t>
+        </is>
       </c>
       <c r="M3" t="n">
-        <v>49</v>
+        <v>0.2589199614271938</v>
       </c>
       <c r="N3" t="n">
-        <v>104</v>
+        <v>171</v>
       </c>
       <c r="O3" t="n">
-        <v>0.1802525832376579</v>
+        <v>224</v>
       </c>
       <c r="P3" t="n">
-        <v>27</v>
+        <v>142</v>
       </c>
       <c r="Q3" t="n">
-        <v>45</v>
+        <v>0.4966248794599807</v>
       </c>
       <c r="R3" t="n">
-        <v>85</v>
-      </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>['right', 'in', 'in', 'or', 'or', 'starts', 'it', 'of', 'how', 'morning', 'ok', 'have', 'the', 'head', 'do', 'you', 'paracetamol', 'only', 'taken', 'para', 'and', 'any', 'any', 'any', 'relief', 'no', 'no', 'no', 'no', 'have', 'erm', 'is', 'ok', 'are', 'asides', 'this', 'for', 'focus', 'and', 'would', 'erm', 'erm', 'you', 'await', 'very', 'much', 'alright', 'you', 'too']</t>
-        </is>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>['id', 'know', 'how', 'best', 'to', 'help', 'you', 'when', 'did', 'it', 'start', 'it', 'started', 'a', 'week', 'ago', 'sorry', 'to', 'hear', 'about', 'that', 'so', 'id', 'more', 'about', 'this', 'so', 'id', 'know', 'okay', 'and', 'sometimes', 'i', 'in', 'okay', 'id', 'like', 'to', 'ask', 'you', 'um', 'when', 'menstrual', 'period', 'um', 'last', 'period', 'okay', 'um', 'um', 'have', 'pain', 'i', 'correct', 'are', 'you', 'uh', 'um', 'okay', 'um', 'okay', 'um', 'um', 'you', 'um', 'i', 'all', 'all']</t>
-        </is>
-      </c>
-      <c r="U3" t="inlineStr">
-        <is>
-          <t>['all', 'havingerm', 'as', 'i', 'would', 'is', 'ok', 'symptom', 'ok', 'ok', 'ok', 'ok', 'now', 'did', 'it', 'ok', 'ok', 'erm', 'now', 'ok', 'this', 'associated', 'ok', 'hmm', 'month', 'ok', 'not', 'not', 'a', 'ok', 'alright', 'ermso', 'have', 'have', 'only', 'taken', 'have', 'ok', 'ok', 'ok', 'erm', 'other', 'uhm', 'ok', 'shiver', 'ok', 'has', 'your', 'appetite', 'been', 'it', 'has', 'ok', 'ok', 'erm', 'i', 'would', 'are', 'you', 'managed', 'for', 'no', 'admitted', 'ever', 'no', 'ok', 'ok', 'ok', 'that', 'ok', 'unilag', 'ok', 'now', 'i', 'am', 'most', 'erm', 'you', 'ok', 'ok', 'ok', 'alright', 'erm', 'its', 'might', 'ok', 'alright', 'you', 'with', 'this', 'it', 'occurs', 'what', 'well', 'well', 'erm', 'wed', 'wed', 'while', 'we', 'alright', 'alright', 'thank', 'you']</t>
-        </is>
-      </c>
-      <c r="V3" t="inlineStr">
-        <is>
-          <t>['in', 'would', 'or', 'was', 'or', 'it', 'ok', 'have', 'the', 'will', 'do', 'not', 'have', 'only', 'paracetamol', 'you', 'have', 'only', 'taken', 'para', 'and', 'erm', 'your', 'have', 'erm', 'is', 'ok', 'ok', 'erm', 'are', 'ok', 'that', 'is', 'for', 'and', 'focus', 'and', 'you', 'a', 'occurs', 'would', 'erm', 'wed', 'you', 'will']</t>
-        </is>
-      </c>
-      <c r="W3" t="inlineStr">
-        <is>
-          <t>['having', 'okay', 'and', 'sometimes', 'i', 'in', 'as', 'okay', 'i', 'would', 'like', 'to', 'ask', 'you', 'when', 'period', 'um', 'um', 'um', 'go', 'you', 'are', 'it', 'is', 'um', 'um', 'um']</t>
-        </is>
-      </c>
-      <c r="X3" t="inlineStr">
-        <is>
-          <t>['doctor', 'havingerm', 'as', 'is', 'in', 'onset', 'ok', 'ok', 'ok', 'ok', 'ok', 'now', 'did', 'it', 'starts', 'ok', 'ok', 'erm', 'like', 'now', 'ok', 'i', 'describe', 'associated', 'ok', 'hmm', 'month', 'ok', 'so', 'you', 'have', 'not', 'ok', 'ermso', 'i', 'any', 'ok', 'ok', 'ok', 'other', 'uhm', 'ok', 'ok', 'has', 'appetite', 'has', 'ok', 'ok', 'erm', 'are', 'managed', 'ever', 'ok', 'ok', 'ok', 'that', 'oh', 'school', 'unilag', 'ok', 'parents', 'ok', 'ok', 'is', 'erm', 'asides', 'this', 'its', 'might', 'course', 'ok', 'with', 'this', 'it', 'what', 'well', 'test', 'wed', 'erm', 'erm', 'where', 'they', 'while', 'we', 'await']</t>
-        </is>
+        <v>673</v>
+      </c>
+      <c r="S3" t="n">
+        <v>163</v>
+      </c>
+      <c r="T3" t="n">
+        <v>194</v>
+      </c>
+      <c r="U3" t="n">
+        <v>0.1769527483124397</v>
+      </c>
+      <c r="V3" t="n">
+        <v>38</v>
+      </c>
+      <c r="W3" t="n">
+        <v>208</v>
+      </c>
+      <c r="X3" t="n">
+        <v>121</v>
       </c>
       <c r="Y3" t="inlineStr">
         <is>
-          <t xml:space="preserve">     ref_ix  hyp_ix  reference hypothesis operation  index_edit_ops
-0         0       0      hello      hello         =            &lt;NA&gt;
-1         1       1      hello      hello         =            &lt;NA&gt;
-2         2       2       good       good         =            &lt;NA&gt;
-3         3       3  afternoon  afternoon         =            &lt;NA&gt;
-4         4       4       good       good         =            &lt;NA&gt;
-..      ...     ...        ...        ...       ...             ...
-934     866     887     lovely     lovely         =            &lt;NA&gt;
-935     867     888        day        day         =            &lt;NA&gt;
-936     868    &lt;NA&gt;        you          _       del             219
-937     869    &lt;NA&gt;        too          _       del             220
-938     870     889        bye        bye         =            &lt;NA&gt;
-[939 rows x 6 columns]</t>
+          <t>['good', 'afternoon', 'not', 'too', 'fine', 'just', 'was', 'there', 'any', 'no', 'nothing', 'like', 'that', 'okay', 'is', 'when', 'are', 'you', 'do', 'you', 'no', 'i', 'did', 'not', 'yes', 'when', 'i', 'some', 'in', 'my', 'my', 'nothing', 'i', 'that', 'is', 'your', 'chest', 'was', 'not', 'paining', 'me', 'here', 'like', 'like', 'i', 'was', 'i', 'was', 'just', 'comes', 'goes', 'then', 'and', 'that', 'since', 'yes', 'i', 'do', 'not', 'slept', 'i', 'do', 'not', 'when', 'i', 'sleep', 'at', 'night', 'okay', 'is', 'what', 'in', 'is', 'no', 'i', 'just', 'like', 'especially', 'when', 'i', 'am', 'okay', 'does', 'it', 'affect', 'i', 'have', 'so', 'that', 'is', 'so', 'was', 'it', 'it', 'started', 'became', 'it', 'has', 'been', 'like', 'that', 'thirtyeightnine', 'thirtyeightnine', 'does', 'what', 'some', 'paracetamol', 'did', 'i', 'i', 'that', 'is', 'why', 'i', 'am', 'is', 'the', 'first', 'time', 'i', 'am', 'experiencing', 'this', 'are', 'you', 'this', 'is', 'surprising', 'you', 'say', 'sir', 'none', 'knew', 'i', 'know', 'i', 'like', 'come', 'to', 'like', 'for', 'me', 'to', 'like', 'have', 'you', 'been', 'not', 'not', 'no', 'your', 'to', 'really', 'okay', 'i', 'vomiting', 'that', 'is', 'just', 'that', 'is', 'just', 'in', 'summary', 'are', 'telling', 'me', 'you', 'had', 'you', 'you', 'have', 'to', 'if', 'to', 'know', 'and', 'the', 'know', 'electrocyte', 'phlegm', 'is', 'doctor', 'you', 'do', 'not', 'do', 'not', 'do', 'doctor', 'i', 'just', 'want', 'to', 'and', 'what', 'will', 'need', 'to', 'take', 'basically', 'i', 'at', 'do', 'a', 'on', 'the', 'and', 'there', 'will', 'be', 'your', 'we', 'your', 'will', 'on', 'doctor', 'do', 'i', 'do', 'that', 'we', 'will', 'yeah']</t>
         </is>
       </c>
       <c r="Z3" t="inlineStr">
         <is>
-          <t xml:space="preserve">     ref_ix  hyp_ix  reference hypothesis operation  index_edit_ops
-0         0       0      hello      hello         =            &lt;NA&gt;
-1         1       1      hello      hello         =            &lt;NA&gt;
-2         2       2       good       good         =            &lt;NA&gt;
-3         3       3  afternoon  afternoon         =            &lt;NA&gt;
-4         4       4       good       good         =            &lt;NA&gt;
-..      ...     ...        ...        ...       ...             ...
-893     866     848     lovely     lovely         =            &lt;NA&gt;
-894     867     849        day        day         =            &lt;NA&gt;
-895     868     850        you        you         =            &lt;NA&gt;
-896     869     851        too        too         =            &lt;NA&gt;
-897     870     852        bye        bye         =            &lt;NA&gt;
-[898 rows x 6 columns]</t>
+          <t>['too', 'fine', 'at', 'what', 'is', 'the', 'complaints', 'so', 'doctor', 'been', 'coughing', 'for', 'about', 'a', 'week', 'now', 'and', 'i', 'have', 'been', 'also', 'it', 'is', 'been', 'really', 'been', 'and', 'the', 'cough', 'has', 'been', 'the', 'cough', 'has', 'been', 'for', 'how', 'long', 'for', 'yes', 'and', 'the', 'cough', 'has', 'been', 'for', 'how', 'long', 'for', 'about', 'a', 'week', 'now', 'a', 'week', 'yes', 'so', 'it', 'like', 'stuff', 'yeah', 'not', 'is', 'in', 'the', 'come', 'do', 'is', 'attend', 'this', 'any', 'do', 'you', 'oh', 'a', 'in', 'a', 'it', 'no', 'no', 'do', 'hmm', 'thank', 'you', 'i', 'have', 'not', 'vomited', 'at', 'do', 'you', 'have', 'any', 'they', 'if', 'already', 'i', 'am', 'different', 'me', 'question', 'okay', 'okay', 'okay', 'okay', 'okay', 'okay', 'okay', 'okay', 'okay', 'okay', 'okay', 'okay', 'okay', 'okay', 'okay', 'okay', 'okay', 'okay', 'okay', 'okay', 'okay', 'okay', 'okay', 'okay', 'okay', 'okay', 'okay', 'okay', 'okay', 'okay', 'okay', 'okay', 'okay', 'okay', 'okay', 'okay', 'okay', 'okay', 'okay', 'okay', 'okay', 'okay', 'do', 'the', 'labs', 'and', 'wait', 'for', 'you', 'to', 'start', 'the', 'treatment', 'thank', 'you', 'very', 'much', 'i', 'think', 'that', 'is', 'fine', 'i', 'will', 'just', 'no', 'i', 'do', 'not', 'promise']</t>
         </is>
       </c>
       <c r="AA3" t="inlineStr">
         <is>
-          <t>hello hello good afternoon good afternoon i am doctor yemi and ill be the one attending to you this afternoon [SUB:all-&gt;alright] [DEL:right] so can you tell me what brought you to the hospital i have been [SUB:havingerm-&gt;having] my body has been feeling hot for a while now [SUB:as-&gt;its] [DEL:in] very hot oh i am so sorry to hear about that so id like to know more about this so [INS:id] [INS:know] [INS:how] [INS:best] [INS:to] [INS:help] [INS:you] [INS:when] [INS:did] [INS:it] [INS:start] [INS:it] [INS:started] [INS:a] [INS:week] [INS:ago] [INS:sorry] [INS:to] [INS:hear] [INS:about] [INS:that] [INS:so] [INS:id] [SUB:i-&gt;like] [SUB:would-&gt;to] know [INS:more] [INS:about] [INS:this] [INS:so] [INS:id] [INS:know] how best to you know help you so when did it start started a week ago was [SUB:is-&gt;this] sudden [DEL:in] onset [DEL:or] it was gradual it was gradual and how has it been since then has it progressed has it gotten better [DEL:or] it has gotten worse it has gotten worse [SUB:ok-&gt;okay] aside from this high body temperature do you have any other associated [SUB:symptom-&gt;dead] yes i have been having this very bad headache [SUB:ok-&gt;okay] body pains [INS:okay] [INS:and] [INS:sometimes] [INS:i] [SUB:ok-&gt;shiver] [SUB:ok-&gt;okay] [SUB:ok-&gt;okay] so all these symptoms [SUB:now-&gt;do] [SUB:did-&gt;they] [SUB:it-&gt;start] [DEL:starts] with the high body temperature yes and it especially [DEL:it] gets worse at night at night [SUB:ok-&gt;okay] [SUB:ok-&gt;okay] so you feel like what [DEL:of] during the day how [DEL:how] do you feel during the day during the day [SUB:erm-&gt;um] i vomit like i vomited for example today [SUB:now-&gt;and] i vomited like four times [SUB:ok-&gt;okay] [SUB:this-&gt;okay] [DEL:morning] [DEL:ok] so the headache what part of your head are you [DEL:have] having this headache [DEL:the] my front part of my [DEL:head] front part of your head i will [DEL:do] [DEL:you] describe it like [INS:in] any [SUB:associated-&gt;actual] eye pain no [INS:okay] [INS:id] [INS:like] [INS:to] [INS:ask] [INS:you] [INS:um] [INS:when] [SUB:ok-&gt;was] [SUB:hmm-&gt;your] last [INS:menstrual] [INS:period] [INS:um] [INS:last] [SUB:month-&gt;morning] [SUB:ok-&gt;okay] so you have [SUB:not-&gt;done] you have [SUB:not-&gt;all] had [SUB:a-&gt;the] missed [INS:period] yeah [INS:okay] [SUB:ok-&gt;all] [SUB:alright-&gt;right] thank you very much so aside from this id like to [INS:um] [SUB:ermso-&gt;so] what have you done since it started so far i have not done i [SUB:have-&gt;am] i [SUB:have-&gt;will] [SUB:only-&gt;not] [SUB:taken-&gt;take] [DEL:paracetamol] you [SUB:have-&gt;first] [DEL:only] [DEL:taken] [DEL:para] [DEL:and] [DEL:any] [DEL:any] [DEL:any] [DEL:relief] with paracetamol just for a short while [SUB:ok-&gt;okay] [SUB:ok-&gt;okay] [SUB:ok-&gt;okay] so [SUB:erm-&gt;um] id just like to ask some other systemic questions to be sure that everything is fine with [SUB:other-&gt;our] systems so from [INS:um] any [SUB:uhm-&gt;um] neck pain or stiffness no any cough or chest pain [INS:have] [INS:pain] no have you been going to have you any urinary symptoms no any diarrhea no [SUB:ok-&gt;okay] so like from what you told me so far you said you have been having high body temperature yes there was headache and body pain and you [SUB:shiver-&gt;shivered] for about a week now am i correct [INS:i] [INS:correct] and also this happens more in the evenings [SUB:ok-&gt;okay] and there is also been vomiting how about your appetite [INS:are] [INS:you] [SUB:has-&gt;ever] [SUB:your-&gt;tired] [SUB:appetite-&gt;of] [SUB:been-&gt;being] fine [INS:uh] [SUB:it-&gt;that] [SUB:has-&gt;is] reduced reduced appetite [SUB:ok-&gt;okay] [SUB:ok-&gt;okay] so are you being [SUB:erm-&gt;me] [SUB:i-&gt;um] [SUB:would-&gt;id] like to ask for your past medical history now [SUB:are-&gt;i] [SUB:you-&gt;have] been [SUB:managed-&gt;married] [SUB:for-&gt;to] any medical condition [DEL:no] in the past are you on any routine medications [SUB:no-&gt;um] do you drink alcohol [DEL:no] do you smoke cigarettes [DEL:no] have you had surgery before in the past [DEL:no] have you ever been [SUB:admitted-&gt;addicted] in the hospital no [DEL:have] you [SUB:ever-&gt;have] been transfused with blood [SUB:no-&gt;okay] [SUB:ok-&gt;um] [DEL:erm] are you married no [SUB:ok-&gt;okay] are you sexually active no [SUB:ok-&gt;okay] that is that is that is [SUB:that-&gt;okay] [DEL:is] [DEL:ok] and what do you do for work i am a student oh [SUB:ok-&gt;okay] where do you school [SUB:unilag-&gt;um] [SUB:ok-&gt;you] [SUB:now-&gt;know] [SUB:i-&gt;okay] [SUB:am-&gt;now] [SUB:most-&gt;um] i would like to ask for this [SUB:erm-&gt;um] consultation are you paying out of pocket or [SUB:you-&gt;yeah] [DEL:are] under insurance i am paying out of pocket and how are your finances like you know [INS:um] well depend i am depending on my parents [INS:okay] [SUB:ok-&gt;okay] [SUB:ok-&gt;okay] [SUB:ok-&gt;all] [SUB:alright-&gt;right] that is that is very good so [SUB:erm-&gt;um] [DEL:asides] [DEL:this] is there any other thing that you think [SUB:its-&gt;is] important that i [SUB:might-&gt;must] have missed out in the course of this [INS:um] conversation none for now [INS:okay] [SUB:ok-&gt;all] [SUB:alright-&gt;right] thank you very much so id like to [INS:um] examine you now ill do a general examination and [DEL:for] and [DEL:focus] [DEL:and] systemic examinations so [INS:um] well from what you have told me so far let us just you know do a quick recap [SUB:you-&gt;he] said you have been having headache body pains and fever for about a week [INS:you] [SUB:with-&gt;are] vomiting so and [SUB:this-&gt;its] [SUB:it-&gt;your] [SUB:occurs-&gt;because] more in the evenings so i am thinking you are having a condition you are having malaria so but what [SUB:what-&gt;we] [DEL:would] need to do is [SUB:well-&gt;we] need to confirm [SUB:well-&gt;we] take blood samples to the lab well do [SUB:erm-&gt;a] malaria parasite test so if it comes out positive well give you medications for malaria but for now [SUB:wed-&gt;well] give you [INS:um] paracetamol for the fever and the [DEL:erm] headache and the body pains so [INS:i] [SUB:wed-&gt;would] also like you to you know bed rest if you need [DEL:erm] notes for school to maybe exempt you from school we can also issue that for you do you have any other thing [DEL:you] would like you know like me to help with so ill direct you to the lab where they will do the test and [SUB:while-&gt;well] [SUB:we-&gt;which] [DEL:await] the test results [INS:all] [SUB:alright-&gt;right] have any other thing no [INS:all] [SUB:alright-&gt;right] thank you so much for your time [SUB:thank-&gt;all] [SUB:you-&gt;right] [DEL:very] [DEL:much] [DEL:alright] have a lovely day [DEL:you] [DEL:too] bye</t>
+          <t>['sadeko', 'was', 'also', 'just', 'more', 'about', 'bouts', 'of', 'err', 'no', 'there', 'nothing', 'then', 'just', 'started', 'at', 'work', 'alone', 'an', 'overcrowded', 'prompted', 'started', 'completely', 'change', 'any', 'position', 'breathless', 'relieves', 'has', 'work', 'any', 'point', 'yes', 'home', 'your', 'temperature', 'have', 'a', 'thermometer', 'was', 'was', 'about', 'relieves', 'i', 'took', 'i', 'anything', 'experiencing', 'during', 'your', 'and', 'nothing', 'and', 'that', 'is', 'why', 'hypertensive', 'what', 'did', 'none', 'i', 'just', 'tried', 'they', 'catarrh', 'not', 'diarrhea', 'or', 'not', 'vomited', 'the', 'the', 'most', 'it', 'is', 'just', 'shortest', 'i', 'i', 'there', 'the', 'you', 'the', 'i', 'do', 'their', 'ifi', 'practices', 'married', 'we', 'we', 'are', 'differentials', 'the', 'because', 'because', 'this', 'thing', 'we', 'a', 'broad', 'you', 'syrup', 'will', 'you', 'in', 'microscopy', 'culture', 'any', 'erythrocyte', 'so', 'the', 'if', 'questions', 'are', 'you', 'going', 'the', 'hospital', 'and', 'and', 'then', 'we', 'will', 'start', 'you', 'on', 'on', 'intravenous', 'intravenous', 'that', 'is', 'that', 'is', 'cool', 'culture', 'and', 'to', 'five', 'days', 'before', 'it']</t>
         </is>
       </c>
       <c r="AB3" t="inlineStr">
         <is>
-          <t>hello hello good afternoon good afternoon i am [SUB:doctor-&gt;dr] yemi and ill be the one attending to you this afternoon all right so can you tell me what brought you to the hospital i have been [INS:having] [SUB:havingerm-&gt;um] my body has been feeling hot for a while now [SUB:as-&gt;its] [DEL:in] very hot oh i am so sorry to hear about that so id like to know more about this so i [DEL:would] know how best to you know help you so when did it start started a week ago was [SUB:is-&gt;this] sudden [SUB:in-&gt;or] [SUB:onset-&gt;was] [DEL:or] it [DEL:was] gradual it was gradual and how has it been since then has it progressed has it gotten better [DEL:or] it has gotten worse it has gotten worse [SUB:ok-&gt;okay] aside from this high body temperature do you have any other associated symptom yes i have been having this very bad headache [SUB:ok-&gt;okay] body pains [INS:okay] [INS:and] [INS:sometimes] [INS:i] [SUB:ok-&gt;shiver] [SUB:ok-&gt;okay] [SUB:ok-&gt;okay] so all these symptoms [SUB:now-&gt;are] [SUB:did-&gt;do] [SUB:it-&gt;they] [SUB:starts-&gt;start] with the high body temperature yes and it especially [DEL:it] gets worse at night at night [SUB:ok-&gt;okay] [SUB:ok-&gt;okay] so you feel like what of during the day how how do you feel during the day during the day [SUB:erm-&gt;um] i vomit [SUB:like-&gt;okay] i vomited for example today [SUB:now-&gt;and] i vomited like four times [DEL:ok] this morning [SUB:ok-&gt;okay] so the headache what part of your head are you [DEL:have] having this headache [DEL:the] my front part of my head front part of your head [SUB:i-&gt;are] [DEL:will] [DEL:do] you [SUB:describe-&gt;describing] it like [INS:in] any [INS:as] [SUB:associated-&gt;your] eye pain no [INS:okay] [INS:i] [INS:would] [INS:like] [INS:to] [INS:ask] [INS:you] [INS:when] [SUB:ok-&gt;was] [SUB:hmm-&gt;your] last [SUB:month-&gt;menstrual] [SUB:ok-&gt;period] [SUB:so-&gt;last] [SUB:you-&gt;month] [SUB:have-&gt;okay] [SUB:not-&gt;so] you have [DEL:not] had a missed [INS:period] yeah [SUB:ok-&gt;okay] alright thank you very much so aside from this id like to [SUB:ermso-&gt;so] what have you done since it started so far i have not done i have [SUB:i-&gt;not] [DEL:have] [DEL:only] taken [DEL:paracetamol] [DEL:you] [DEL:have] [DEL:only] [DEL:taken] [DEL:para] [DEL:and] any [SUB:any-&gt;paracetamol] any relief with paracetamol just for a short while [SUB:ok-&gt;okay] [SUB:ok-&gt;okay] [SUB:ok-&gt;okay] so [DEL:erm] id just like to ask some other systemic questions to be sure that everything is fine with [SUB:other-&gt;our] systems so from any [SUB:uhm-&gt;any] neck pain or stiffness no any cough or chest pain no have you been [INS:um] going to have you any urinary symptoms no any diarrhea no [SUB:ok-&gt;okay] so like from what you told me so far you said you have been having [INS:um] high body temperature yes there was headache and [INS:um] body pain and you shiver for about a week now am i correct and also this happens more in the evenings [SUB:ok-&gt;okay] and there is also been vomiting how about [DEL:your] appetite [SUB:has-&gt;i] your [SUB:appetite-&gt;appetites] been fine it [SUB:has-&gt;does] reduced reduced appetite [SUB:ok-&gt;okay] [SUB:ok-&gt;okay] so are you being [SUB:erm-&gt;me] i would like to ask for your past medical history now [SUB:are-&gt;have] you been [SUB:managed-&gt;married] for any medical condition no in the past are you on any routine medications no do you drink alcohol no do you smoke cigarettes no have you had surgery before in the past no have you ever been admitted in the hospital no [DEL:have] you [SUB:ever-&gt;have] been transfused with blood no [SUB:ok-&gt;okay] [DEL:erm] are you married no [SUB:ok-&gt;okay] are you sexually active no [SUB:ok-&gt;okay] that is that is that is [SUB:that-&gt;it] [DEL:is] [DEL:ok] and what do you do for work i am a student [SUB:oh-&gt;okay] [DEL:ok] where do you [INS:go] [INS:you] [SUB:school-&gt;know] [SUB:unilag-&gt;i] [SUB:ok-&gt;okay] now i am most i would like to ask for this [DEL:erm] consultation are you paying out of pocket or [INS:are] you [DEL:are] under insurance i am paying out of pocket and how are your finances like you know well depend i am depending on my [SUB:parents-&gt;okay] [SUB:ok-&gt;okay] [SUB:ok-&gt;okay] [DEL:ok] alright that [SUB:is-&gt;sounds] [DEL:that] [DEL:is] very good so [SUB:erm-&gt;um] [SUB:asides-&gt;aside] [SUB:this-&gt;to] is [INS:it] [INS:is] there any other thing that you think [SUB:its-&gt;is] important that i [SUB:might-&gt;must] have missed out in the [SUB:course-&gt;because] of this conversation none for now [SUB:ok-&gt;okay] alright thank you very much so id like to examine you now ill do a general examination and [DEL:for] [DEL:and] [DEL:focus] [DEL:and] systemic examinations so [INS:um] well from what you have told me so far let us just you know do a quick recap [DEL:you] said you have been having headache body pains and fever for about [DEL:a] week [SUB:with-&gt;were] vomiting so and [SUB:this-&gt;its] [SUB:it-&gt;causing] [DEL:occurs] more in the evenings so i am thinking you are having a condition you are having malaria so but what [SUB:what-&gt;we] [DEL:would] need to do is [SUB:well-&gt;we] need to confirm well take [INS:um] blood samples to the lab well do [DEL:erm] malaria parasite [SUB:test-&gt;tests] so if it comes out positive well give you medications for malaria but for now [SUB:wed-&gt;well] give you [INS:um] paracetamol for the fever and the [SUB:erm-&gt;um] headache and the body pains so [DEL:wed] also like you to you know bed rest if you need [SUB:erm-&gt;um] notes for school to maybe exempt you from school we can also issue that for you do you have any other thing [DEL:you] would like you know like me to help with so ill direct you to the lab [SUB:where-&gt;and] [SUB:they-&gt;well] [DEL:will] do the test and [SUB:while-&gt;well] [SUB:we-&gt;i] [SUB:await-&gt;wish] the test results alright have any other thing no alright thank you so much for your time thank you very much alright have a lovely day you too bye</t>
+          <t>['hospital', 'right', 'just', 'woke', 'up', 'more', 'morning', 'and', 'started', 'coughing', 'about', 'a', 'week', 'ago', 'yes', 'okay', 'is', 'bouts', 'when', 'do', 'you', 'there', 'was', 'no', 'blood', 'in', 'it', 'yes', 'in', 'started', 'that', 'here', 'like', 'i', 'was', 'just', 'in', 'it', 'just', 'i', 'am', 'i', 'have', 'in', 'my', 'body', 'so', 'now', 'it', 'it', 'you', 'are', 'did', 'i', 'is', 'why', 'i', 'am', 'that', 'is', 'why', 'this', 'is', 'surprising', 'say', 'i', 'cannot', 'hear', 'sir', 'are', 'you', 'no', 'just', 'i', 'just', 'tried', 'okay', 'i', 'i', 'is', 'just', 'so', 'in', 'you', 'right', 'if', 'whether', 'will', 'electrocyte', 'to', 'ask', 'ifi', 'just', 'then', 'you', 'have', 'i', 'am', 'married', 'i', 'am', 'married', 'the', 'because', 'at', 'a', 'the', 'will', 'and', 'your', 'will', 'have', 'a', 'you', 'you', 'a', 'doctor', 'so', 'doctor', 'i', 'do', 'we', 'we', 'and', 'then', 'we', 'will', 'start', 'you', 'on', 'on', 'intravenous', 'intravenous', 'that', 'is', 'and', 'sensitivity', 'could', 'take', 'about', 'seventytwo', 'hours', 'to', 'to', 'five', 'days', 'before', 'it', 'will', 'be', 'ready', 'do', 'you', 'understand', 'yeah', 'no', 'problem', 'doctor', 'no', 'problem', 'doctor', 'thank', 'you']</t>
+        </is>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>['at', 'it', 'is', 'been', 'really', 'yes', 'yes', 'and', 'how', 'long', 'for', 'the', 'a', 'and', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'yeah', 'i', 'not', 'in', 'pain', 'pain', 'is', 'come', 'so', 'the', 'cough', 'do', 'points', 'that', 'there', 'thirty', 'eight', 'point', 'nine', 'thirty', 'well', 'past', 'do', 'you', 'to', 'a', 'up', 'in', 'it', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'no', 'or', 'so', 'there', 'do', 'business', 'end', 'doing', 'have']</t>
+        </is>
+      </c>
+      <c r="AD3" t="inlineStr">
+        <is>
+          <t>['sadeko', 'the', 'have', 'you', 'have', 'running', 'temperature', 'five', 'days', 'yes', 'yes', 'all', 'catarrh', 'mine', 'is', 'not', 'that', 'i', 'did', 'not', 'i', 'did', 'not', 'experience', 'anything', 'like', 'that', 'okay', 'so', 'is', 'the', 'cough', 'productive', 'of', 'phlegm', 'yes', 'yes', 'it', 'is', 'productive', 'when', 'i', 'yes', 'when', 'i', 'cough', 'i', 'bring', 'out', 'some', 'some', 'err', 'not', 'vomiting', 'there', 'nothing', 'paining', 'then', 'just', 'paining', 'your', 'paining', 'have', 'at', 'work', 'too', 'an', 'overcrowded', 'then', 'has', 'completely', 'slept', 'when', 'i', 'at', 'night', 'relieves', 'change', 'i', 'for', 'relieves', 'it', 'has', 'work', 'that', 'is', 'high', 'did', 'at', 'point', 'yes', 'thermometer', 'it', 'thirtyeightnine', 'thirtyeightnine', 'does', 'relieves', 'paracetamol', 'a', 'anything', 'experiencing', 'that', 'experiencing', 'during', 'your', 'blood', 'group', 'and', 'genotype', 'nothing', 'and', 'what', 'did', 'you', 'properly', 'i', 'come', 'i', 'can', 'remember', 'to', 'catarrh', 'i', 'do', 'not', 'have', 'any', 'diarrhea', 'or', 'vomiting', 'i', 'have', 'not', 'vomited', 'at', 'all', 'you', 'have', 'any', 'bone', 'pain', 'yes', 'the', 'the', 'most', 'it', 'is', 'just', 'it', 'is', 'shortest', 'having', 'having', 'that', 'just', 'all', 'which', 'you', 'know', 'rates', 'going', 'drugs', 'their', 'will', 'need', 'take', 'basically', 'just', 'want', 'not', 'diagnosis', 'this', 'thing', 'treatment', 'going', 'to', 'blood', 'count', 'microscopy', 'do', 'any', 'erythrocyte', 'segmentation', 'rate', 'the', 'if', 'the', 'that', 'can', 'i', 'cool', 'culture', 'labs', 'just']</t>
+        </is>
+      </c>
+      <c r="AE3" t="inlineStr">
+        <is>
+          <t>['i', 'have', 'temperature', 'for', 'just', 'was', 'there', 'any', 'is', 'breath', 'when', 'do', 'you', 'no', 'i', 'did', 'not', 'i', 'did', 'not', 'experience', 'anything', 'like', 'that', 'when', 'i', 'some', 'not', 'it', 'is', 'vomiting', 'my', 'my', 'i', 'that', 'there', 'is', 'no', 'there', 'is', 'me', 'anybody', 'around', 'me', 'that', 'is', 'so', 'here', 'i', 'started', 'like', 'i', 'was', 'i', 'was', 'just', 'then', 'do', 'not', 'slept', 'sleep', 'at', 'night', 'is', 'any', 'okay', 'i', 'have', 'so', 'it', 'started', 'became', 'it', 'grade', 'home', 'a', 'was', 'about', 'does', 'what', 'some', 'paracetamol', 'i', 'is', 'why', 'and', 'that', 'is', 'why', 'this', 'is', 'surprising', 'what', 'did', 'you', 'say', 'none', 'i', 'just', 'i', 'just', 'they', 'did', 'not', 'knew', 'i', 'knew', 'i', 'like', 'come', 'to', 'like', 'have', 'you', 'been', 'not', 'not', 'or', 'vomiting', 'the', 'it', 'is', 'just', 'have', 'that', 'is', 'just', 'that', 'is', 'just', 'summary', 'you', 'you', 'and', 'the', 'will', 'electrocyte', 'your', 'is', 'smoke', 'you', 'do', 'not', 'do', 'not', 'do', 'any', 'and', 'what', 'will', 'need', 'to', 'take', 'basically', 'i', 'then', 'i', 'am', 'married', 'the', 'because', 'this', 'thing', 'do', 'pneumonia', 'you', 'will', 'and', 'we', 'would', 'your', 'will', 'on', 'doctor', 'do', 'i', 'do', 'or', 'do', 'i', 'that', 'can', 'i', 'we', 'we', 'then', 'we', 'will', 'start', 'you', 'on', 'on', 'intravenous', 'intravenous', 'that', 'is', 'culture', 'and', 'sensitivity', 'could', 'take', 'about', 'to', 'yeah', 'thank', 'you', 'for', 'just']</t>
+        </is>
+      </c>
+      <c r="AF3" t="inlineStr">
+        <is>
+          <t>['on', 'and', 'the', 'cough', 'has', 'been', 'the', 'cough', 'has', 'been', 'for', 'how', 'long', 'for', 'soddening', 'yeah', 'the', 'no', 'is', 'come', 'do', 'attend', 'a', 'it', 'it', 'this', 'do', 'you', 'oh', 'coughs', 'in', 'yes', 'of', 'so', 'there', 'if', 'do', 'me']</t>
+        </is>
+      </c>
+      <c r="AG3" t="inlineStr">
+        <is>
+          <t>['sadeko', 'was', 'also', 'have', 'so', 'you', 'have', 'running', 'it', 'suddenly', 'about', 'catarrh', 'barking', 'it', 'bouts', 'deep', 'barking', 'barking', 'barking', 'phlegm', 'err', 'yes', 'catarrh', 'there', 'paining', 'then', 'just', 'started', 'your', 'chest', 'paining', 'stay', 'with', 'have', 'at', 'work', 'was', 'completely', 'i', 'when', 'i', 'it', 'especially', 'it', 'has', 'it', 'suddenly', 'or', 'high', 'at', 'any', 'point', 'yes', 'have', 'it', 'thirtyeightnine', 'i', 'took', 'a', 'i', 'i', 'hot', 'anything', 'experiencing', 'that', 'this', 'during', 'your', 'hypertensive', 'none', 'cough', 'syrup', 'i', 'can', 'remember', 'just', 'catarrh', 'any', 'diarrhea', 'have', 'shortest', 'i', 'in', 'which', 'elevated', 'you', 'know', 'rates', 'phlegm', 'culture', 'cultured', 'do', 'not', 'drink', 'i', 'do', 'their', 'treating', 'ifi', 'we', 'your', 'you', 'blood', 'in', 'microscopy', 'culture', 'you', 'are', 'any', 'erythrocyte', 'segmentation', 'you', 'so', 'the', 'if', 'the', 'and', 'cool', 'before', 'it', 'will']</t>
+        </is>
+      </c>
+      <c r="AH3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">      ref_ix  hyp_ix  reference hypothesis operation  index_edit_ops
+0          0       0       good       good         =            &lt;NA&gt;
+1          1       1  afternoon  afternoon         =            &lt;NA&gt;
+2          2       2        sir        sir         =            &lt;NA&gt;
+3          3       3          i          i         =            &lt;NA&gt;
+4          4       4         am         am         =            &lt;NA&gt;
+...      ...     ...        ...        ...       ...             ...
+2240    &lt;NA&gt;    2016          _         no       ins             532
+2241    &lt;NA&gt;    2017          _          i       ins             533
+2242    &lt;NA&gt;    2018          _         do       ins             534
+2243    &lt;NA&gt;    2019          _        not       ins             535
+2244    &lt;NA&gt;    2020          _    promise       ins             536
+[2245 rows x 6 columns]</t>
+        </is>
+      </c>
+      <c r="AI3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">      ref_ix  hyp_ix  reference hypothesis operation  index_edit_ops
+0          0       0       good       good         =            &lt;NA&gt;
+1          1       1  afternoon  afternoon         =            &lt;NA&gt;
+2          2       2        sir        sir         =            &lt;NA&gt;
+3          3       3          i          i         =            &lt;NA&gt;
+4          4       4         am         am         =            &lt;NA&gt;
+...      ...     ...        ...        ...       ...             ...
+2742    2069    2579      start      start         =            &lt;NA&gt;
+2743    2070    2580        the        the         =            &lt;NA&gt;
+2744    2071    2581  treatment  treatment         =            &lt;NA&gt;
+2745    2072    2582      thank      thank         =            &lt;NA&gt;
+2746    2073    2583        you        you         =            &lt;NA&gt;
+[2747 rows x 6 columns]</t>
+        </is>
+      </c>
+      <c r="AJ3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">      ref_ix  hyp_ix  reference hypothesis operation  index_edit_ops
+0          0       0       good       good         =            &lt;NA&gt;
+1          1       1  afternoon  afternoon         =            &lt;NA&gt;
+2          2       2        sir        sir         =            &lt;NA&gt;
+3          3       3          i          i         =            &lt;NA&gt;
+4          4       4         am         am         =            &lt;NA&gt;
+...      ...     ...        ...        ...       ...             ...
+2107    2069    1899      start      start         =            &lt;NA&gt;
+2108    2070    1900        the        the         =            &lt;NA&gt;
+2109    2071    1901  treatment  treatment         =            &lt;NA&gt;
+2110    2072    1902      thank      thank         =            &lt;NA&gt;
+2111    2073    1903        you        you         =            &lt;NA&gt;
+[2112 rows x 6 columns]</t>
+        </is>
+      </c>
+      <c r="AK3" t="inlineStr">
+        <is>
+          <t>good afternoon sir i am doctor [SUB:sadeko-&gt;shadekoff] good afternoon [DEL:good] [DEL:afternoon] doctor how are you doing today sir doctor i am not [INS:too] [INS:fine] i am not too fine [DEL:not] [DEL:too] [DEL:fine] that is why i came to the hospital today what [SUB:was-&gt;are] the complaints so doctor i have been coughing for about a week now and i have been also [INS:at] [INS:what] [INS:is] [INS:the] [INS:complaints] [INS:so] [INS:doctor] [SUB:also-&gt;i] have [INS:been] [INS:coughing] [INS:for] [INS:about] [INS:a] [INS:week] [INS:now] [INS:and] [INS:i] [INS:have] [INS:been] [INS:also] you also have what so and i also have i have also been running temperature for about five days so [INS:it] [INS:is] [INS:been] [INS:really] you have [INS:been] running temperature for five days yes yes [INS:and] [INS:the] [INS:cough] [INS:has] [INS:been] for [INS:the] [INS:cough] [INS:has] [INS:been] [INS:for] [INS:how] [INS:long] [INS:for] about a week now a week yes [INS:yes] [INS:and] [INS:the] [INS:cough] [INS:has] [INS:been] [INS:for] [INS:how] [INS:long] [INS:for] [INS:about] [INS:a] [INS:week] [INS:now] [INS:a] [INS:week] [INS:yes] okay all right so the cough did it start suddenly or gradually the cough started suddenly [SUB:just-&gt;it] started like that [INS:so] i just [DEL:just] woke up [SUB:more-&gt;one] morning and started coughing [SUB:about-&gt;by] a week ago yes was there [DEL:was] [DEL:there] any symptoms like catarrh or any [DEL:any] difficulty in swallowing before the cough started [DEL:no] none like that i had nothing like that [DEL:nothing] [DEL:like] [DEL:that] you had nothing like that yes [DEL:okay] so now the cough how does it sound does it sound like barking does it sound like it [DEL:is] comes in [SUB:bouts-&gt;barking] and then you have to take a deep breath when [DEL:when] you say barking do you [DEL:are] [DEL:you] [DEL:do] [DEL:you] mean like a dog or what do you mean by barking yes yes [INS:it] sounds like a dog barking no no no no no [DEL:no] mine is not [INS:like] that i did not [DEL:i] [DEL:did] [DEL:not] experience anything like that okay so is the cough productive [SUB:of-&gt;or] phlegm yes yes it is productive when i [DEL:yes] [DEL:when] [DEL:i] cough i bring out some [DEL:some] substance from my mouth yes so what is the colour of the substance [INS:stuff] [SUB:err-&gt;yeah] it is about [INS:yeah] it is clear it is whitish it is not it is just normal it is looking like saliva but it is very thick it is very thick was there blood in it at any point no there was no blood in it there was no blood in it there was no blood in it at any point yes and after you cough do you feel like vomiting or do you vomit no i do not i do not i do not feel like vomiting i do not vomit at all okay and you did not have catarrh or difficulty [DEL:in] swallowing prior to onset of the cough [SUB:no-&gt;cough] no [SUB:there-&gt;i] was [INS:not] [SUB:nothing-&gt;in] i was not i had nothing [DEL:my] [DEL:my] even when i was coughing my chest was not paining me [DEL:nothing] it was just the cough [SUB:then-&gt;and] i [DEL:i] discovered after a few days after that i [SUB:just-&gt;was] [SUB:started-&gt;tired] running temperature too my body was very very hot it was very hot [DEL:that] i was shivering so you are telling me there is no there is no cough there is no chest pain no there [DEL:is] there is no chest pain my chest was not paining me at all [DEL:your] [DEL:chest] [DEL:was] [DEL:not] [DEL:paining] [DEL:me] is there anybody coughing around you no there [INS:is] nobody i stay alone right now so i have nobody around me i do not stay with people so i do not have anybody around me that is coughing too and [SUB:at-&gt;i] [SUB:work-&gt;walk] too there is nobody coughing around me so okay so you stay [INS:in] [INS:the] [SUB:alone-&gt;room] you are not [DEL:here] in [SUB:an-&gt;a] [SUB:overcrowded-&gt;crowded] place yes but yes but doctor i noticed what actually [SUB:prompted-&gt;tell] me to come is the fact that about two days ago i noticed that the cough became worsened and i was i [SUB:started-&gt;said] to have some difficulty in breathing so [DEL:like] that got me really scared [DEL:like] i was [DEL:i] [DEL:was] [DEL:i] [DEL:was] [DEL:just] feeling breathless for a moment [DEL:comes] and [DEL:goes] [DEL:then] [DEL:and] since [DEL:that] [DEL:since] then the breathlessness has become more worsened so that is what exactly prompted me to [INS:come] [SUB:completely-&gt;quickly] to see you you are finding it difficult to breathe yes [DEL:yes] when you sleep at night [INS:do] you sweat excessively no at all i do not [DEL:i] [DEL:do] [DEL:not] [DEL:slept] [DEL:i] [DEL:do] [DEL:not] sweat [DEL:when] [DEL:i] [DEL:sleep] [DEL:at] [DEL:night] [DEL:okay] so what [DEL:is] [DEL:what] relieves the breathlessness any [SUB:change-&gt;changing] [DEL:in] position that relieves the breathlessness or [INS:is] it [DEL:is] constant [DEL:no] it is not associated with any [SUB:any-&gt;position] [SUB:position-&gt;or] nothing [DEL:i] [DEL:just] it just comes and goes [DEL:like] i just feel [SUB:breathless-&gt;breathlessness] for a while then it [SUB:relieves-&gt;releases] me then it comes again especially when i am [DEL:especially] [DEL:when] [DEL:i] [DEL:am] coughing [DEL:okay] has this worsened progressively yes yes it [SUB:has-&gt;is] gotten very bad doctor that is why i came to the hospital does it affect [DEL:does] [DEL:it] [DEL:affect] your daily activities yes it does doctor i have not been able to [SUB:work-&gt;walk] for the past two days because of the cough and the fact that i have [DEL:i] [DEL:have] not been feeling well generally in my body [DEL:so] [DEL:that] [DEL:is] [DEL:so] now this fever that you were having [DEL:was] [DEL:it] did it start suddenly or gradually it started [DEL:it] [DEL:started] gradually then [DEL:became] i became very hot and it has been like that [DEL:it] [DEL:has] [DEL:been] [DEL:like] [DEL:that] so the fever is high grade you are very hot yes yes it is high did you at [INS:attend] [SUB:any-&gt;the] [SUB:point-&gt;question] [SUB:yes-&gt;time] check by yourself at [SUB:home-&gt;your] [SUB:your-&gt;temporary] [SUB:temperature-&gt;job] yes i did i did i [SUB:have-&gt;was] [SUB:a-&gt;about] [SUB:thermometer-&gt;thirtyeightnine] it [SUB:was-&gt;is] about [SUB:was-&gt;thirtysevennine] [SUB:about-&gt;thirtysevennine] [DEL:thirtyeightnine] [DEL:thirtyeightnine] okay and what [DEL:does] [DEL:what] do you do that [SUB:relieves-&gt;released] the fever i took some [SUB:i-&gt;prost] [SUB:took-&gt;more] [DEL:some] [DEL:paracetamol] it relieved a bit then but it did [DEL:did] not last long [SUB:i-&gt;it] just [DEL:i] [DEL:i] became hot again and it has been like that ever since so i just want to ask you some questions has [INS:this] [SUB:anything-&gt;thing] happened before in the past okay has it happened in the past no no no no this is the first time i am [SUB:experiencing-&gt;expressing] [DEL:that] [DEL:is] [DEL:why] [DEL:i] [DEL:am] this [DEL:is] [DEL:the] [DEL:first] [DEL:time] [DEL:i] [DEL:am] [DEL:experiencing] [DEL:this] kind of thing okay this is the first time [DEL:are] [DEL:you] do you have any [INS:any] medical condition like are you asthmatic [INS:do] [INS:you] [SUB:during-&gt;need] [SUB:your-&gt;a] blood group [SUB:and-&gt;on] genotype [INS:oh] no i am not [INS:a] doctor i am fine no i have [SUB:nothing-&gt;not] [SUB:and-&gt;seen] [SUB:that-&gt;no] [SUB:is-&gt;i] [SUB:why-&gt;am] [DEL:this] [DEL:is] [DEL:surprising] are you [SUB:hypertensive-&gt;a] [SUB:what-&gt;potential] [SUB:did-&gt;user] [DEL:you] [DEL:say] i cannot hear you properly [DEL:sir] are you hypertensive or diabetic none none [SUB:none-&gt;no] [DEL:none] no no i have none of them i have none of them so what have you what have you done to care for yourself so far i just i just [SUB:i-&gt;tried] [SUB:just-&gt;to] [SUB:tried-&gt;try] to get some cough syrup but they did not [SUB:they-&gt;probably] did not seem to work properly they did not seem to work and since the difficulty [INS:in] breathing started i knew i [DEL:knew] [DEL:i] [DEL:know] [DEL:i] needed to [DEL:like] [DEL:come] [DEL:to] speak to someone to a doctor so that is why i came today for you to [DEL:like] [DEL:for] [DEL:me] [DEL:to] [DEL:like] know what is wrong with me and treat myself basically have you been [DEL:have] [DEL:you] [DEL:been] admitted before no not [DEL:not] [DEL:not] that i can remember have you done any surgical procedure before no [DEL:no] okay so i am just going to ask you some other questions just to know what exactly could be related to [DEL:your] [DEL:to] the symptoms you are having so do you have [INS:a] headache headache [INS:it] just comes once in a while maybe because the cough i have not been able to sleep [DEL:really] so kind of yeah kind of yes okay so any loss of consciousness no no no no okay [DEL:okay] do you have [SUB:catarrh-&gt;kata] no at all okay do you have any abdominal pain no no [DEL:i] do [SUB:not-&gt;you] have any [SUB:diarrhea-&gt;abdominal] [SUB:or-&gt;pain] [DEL:vomiting] no i have [INS:no] [SUB:not-&gt;abdominal] [SUB:vomited-&gt;pain] at all [INS:no] [INS:do] you have any bone pain yes [INS:hmm] [INS:thank] [INS:you] no [INS:i] [INS:have] [INS:not] [INS:vomited] [INS:at] [SUB:the-&gt;all] no [INS:do] [INS:you] [INS:have] [INS:any] [SUB:the-&gt;bone] [SUB:most-&gt;pain] [SUB:it-&gt;yes] [SUB:is-&gt;hmm] [SUB:just-&gt;no] it is just the [SUB:shortest-&gt;shoulders] of breath [SUB:i-&gt;that] have been having the difficulty in breathing [SUB:i-&gt;that] have been having [DEL:that] [DEL:is] [DEL:just] [DEL:that] [DEL:is] [DEL:just] so in summary you are telling me [DEL:in] [DEL:summary] you [DEL:are] [DEL:telling] [DEL:me] [DEL:you] [DEL:had] [DEL:you] [DEL:you] have had cough fever and difficulty in breathing yes right and your cough is productive yes all right so i am going to have to [DEL:have] [DEL:to] examine you right i am going to have to examine you and i am going to have to listen to your chest to know [DEL:if] [DEL:to] [DEL:know] whatever is going on in your chest whether [SUB:there-&gt;it] is a chest infection that is causing you to have a fever and [SUB:the-&gt;a] [DEL:and] [DEL:the] cough do you understand and then we are going to have you do some investigations like a chest xray a complete blood count a full blood count which will tell us whether there is an infection going on depending on the parameters that are elevated or reduced do you understand we are going to do [SUB:you-&gt;ifide] [DEL:know] [DEL:electrocyte] segmentation rates to know whether there is an inflammatory process going on do you understand and then we are also going to take your sputum your [SUB:the-&gt;deflame] [DEL:phlegm] and we are going to send it for culture sensitivity to know what bacteria is [DEL:is] being cultured please i just want to ask you do you smoke no no i do not [DEL:doctor] i am a good christian i do not smoke i do not drink you do not [DEL:you] [DEL:do] [DEL:not] drink alcohol either i do not [SUB:i-&gt;drink] [DEL:do] [DEL:not] [DEL:do] any of those i do not do drugs i do not [SUB:do-&gt;drink] any of that i am going to ask you some other questions do you have [INS:they] [SUB:their-&gt;are] kind of personal questions can i go ahead yeah i just want to know [DEL:doctor] i just want to [DEL:i] [DEL:just] [DEL:want] [DEL:to] be fine i just want to know how soon you can start treating me [DEL:and] [DEL:what] i [DEL:will] [DEL:need] [DEL:to] [DEL:take] [DEL:basically] [DEL:i] just want to ask [INS:if] [SUB:ifi-&gt;i] just want to ask if you have multiple sexual partners and then your sexual [SUB:practices-&gt;practice] no no you have oral sex i am married no not at all not at all i am [INS:already] [INS:i] [INS:am] [SUB:married-&gt;free] so we are going to start you from the history and the examination [SUB:we-&gt;you] have done and then [SUB:we-&gt;i] [SUB:are-&gt;am] going to ask you to do some investigations however we have some [INS:different] [SUB:differentials-&gt;house] like diagnosis [SUB:the-&gt;because] [SUB:because-&gt;what] the [SUB:because-&gt;cost] of what is causing the cough and the fever we have some [SUB:this-&gt;just] [SUB:thing-&gt;in] [DEL:at] the back of our mind which could be the because [DEL:do] you understand [SUB:we-&gt;you] think you have a pneumonia pneumonia [DEL:a] chest infection so we are going to start you on [SUB:a-&gt;the] [SUB:broad-&gt;blood] spectrum antibiotics right and then we are going to start [SUB:you-&gt;your] [DEL:on] [DEL:the] cough [SUB:syrup-&gt;serum] right to treat the cough while we wait for the results of our investigations do you understand okay and then since there is no history of asthma by the time you [SUB:will-&gt;start] start treatment with the antibiotics and [DEL:and] the cough syrup [DEL:there] [DEL:will] [DEL:be] the breathlessness is going to reduce but we [DEL:your] [DEL:we] would have checked your [DEL:your] oxygen saturation and we [DEL:will] see that it is fine so there will be no need to place you on [DEL:on] oxygen so [SUB:you-&gt;we] are going to have you do a full blood count [SUB:in-&gt;a] sputum and [SUB:microscopy-&gt;microscop] [SUB:culture-&gt;contrast] sensitivity you are going to have you do [SUB:any-&gt;an] [SUB:erythrocyte-&gt;ultrasound] segmentation rate and you are going to do a chest xray so let us see if it is a structural problem or a functional problem do you understand okay doctor [SUB:so-&gt;okay] [DEL:doctor] [DEL:do] [DEL:i] [DEL:do] you want to ask [INS:me] [SUB:the-&gt;a] question [SUB:if-&gt;do] you have any [INS:question] [SUB:questions-&gt;question] yes i was going to ask that [SUB:are-&gt;i] [SUB:you-&gt;am] [SUB:going-&gt;able] to keep me in [SUB:the-&gt;your] [SUB:hospital-&gt;speech] or do i [DEL:that] can i can i be treated from home because i do not know we we [DEL:we] are going to admit you for some time to evaluate you [SUB:and-&gt;because] because of the breathlessness you are having right [SUB:and-&gt;okay] [SUB:then-&gt;okay] [SUB:we-&gt;okay] [SUB:will-&gt;okay] [SUB:start-&gt;okay] [SUB:you-&gt;okay] [SUB:on-&gt;okay] [SUB:on-&gt;okay] [SUB:intravenous-&gt;okay] [SUB:intravenous-&gt;okay] [SUB:that-&gt;okay] [SUB:is-&gt;okay] okay [INS:okay] [INS:okay] [INS:okay] [INS:okay] [INS:okay] [INS:okay] [INS:okay] [INS:okay] [INS:okay] [INS:okay] [INS:okay] [INS:okay] [INS:okay] [INS:okay] [INS:okay] [INS:okay] [INS:okay] [INS:okay] [INS:okay] [INS:okay] [INS:okay] [INS:okay] [INS:okay] [INS:okay] [INS:okay] [INS:okay] [INS:okay] [INS:okay] [INS:okay] [INS:okay] [INS:okay] [INS:okay] [INS:okay] [INS:okay] [INS:okay] [INS:okay] [INS:okay] [INS:okay] [INS:okay] [INS:okay] [INS:okay] [INS:okay] [SUB:that-&gt;okay] [SUB:is-&gt;for] [SUB:cool-&gt;the] [SUB:culture-&gt;investigation] [SUB:and-&gt;cultural] sensitivity could take about seventytwo hours to [SUB:to-&gt;find] [SUB:five-&gt;this] [SUB:days-&gt;for] [SUB:before-&gt;you] [SUB:it-&gt;to] [DEL:will] be ready do you understand [DEL:yeah] no problem doctor thank you no problem doctor thank you very much i think that is fine i will just [INS:do] [INS:the] [INS:labs] [INS:and] [INS:wait] [INS:for] [INS:you] [INS:to] [INS:start] [INS:the] [INS:treatment] [INS:thank] [INS:you] [INS:very] [INS:much] [INS:i] [INS:think] [INS:that] [INS:is] [INS:fine] [INS:i] [INS:will] [INS:just] yeah i will just do the labs and wait for just for you to start the treatment thank you [INS:no] [INS:i] [INS:do] [INS:not] [INS:promise]</t>
+        </is>
+      </c>
+      <c r="AL3" t="inlineStr">
+        <is>
+          <t>good afternoon sir i am doctor [SUB:sadeko-&gt;shadak] good afternoon good afternoon doctor how are you doing today sir doctor i am not i am not too fine not too fine that is why i came to [SUB:the-&gt;you] [DEL:hospital] today what was the complaints so doctor i have been coughing for about a week now and i have been also also [INS:at] [SUB:have-&gt;yes] you also have what so and i also have i have also been running temperature for about five days so [INS:it] [INS:is] [INS:been] [INS:really] [INS:yes] [INS:yes] [INS:and] [SUB:you-&gt;the] [SUB:have-&gt;cough] [SUB:running-&gt;has] [SUB:temperature-&gt;been] for [SUB:five-&gt;the] [SUB:days-&gt;cough] [SUB:yes-&gt;has] [SUB:yes-&gt;been] for [INS:how] [INS:long] [INS:for] about a week now a week yes okay [SUB:all-&gt;alright] [DEL:right] so the cough did it start suddenly or gradually the cough started suddenly just started like that i just [DEL:just] [DEL:woke] [DEL:up] [DEL:more] [DEL:morning] [DEL:and] [DEL:started] [DEL:coughing] [DEL:about] [DEL:a] [DEL:week] [DEL:ago] [DEL:yes] was there was there any symptoms like [SUB:catarrh-&gt;qatar] or any any difficulty in swallowing before the cough started no none like that i had nothing like that nothing like that you had nothing like that yes [DEL:okay] so now the cough how does it sound does it sound like [INS:the] barking does it sound like [INS:a] [INS:and] it [DEL:is] comes in [DEL:bouts] and then you have to take a deep breath when [DEL:when] you say barking [DEL:do] [DEL:you] are you do you mean like a dog or what do you mean by barking yes yes sounds like a dog barking no no no no no no [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [SUB:mine-&gt;no] [SUB:is-&gt;no] [SUB:not-&gt;no] [SUB:that-&gt;no] [SUB:i-&gt;no] [SUB:did-&gt;no] [SUB:not-&gt;no] [SUB:i-&gt;no] [SUB:did-&gt;no] [SUB:not-&gt;no] [SUB:experience-&gt;no] [SUB:anything-&gt;no] [SUB:like-&gt;no] [SUB:that-&gt;no] [SUB:okay-&gt;no] [SUB:so-&gt;no] [SUB:is-&gt;no] [SUB:the-&gt;no] [SUB:cough-&gt;no] [SUB:productive-&gt;no] [SUB:of-&gt;no] [SUB:phlegm-&gt;no] [SUB:yes-&gt;no] [SUB:yes-&gt;no] [SUB:it-&gt;no] [SUB:is-&gt;no] [SUB:productive-&gt;no] [SUB:when-&gt;no] [SUB:i-&gt;no] [SUB:yes-&gt;no] [SUB:when-&gt;no] [SUB:i-&gt;no] [SUB:cough-&gt;no] [SUB:i-&gt;no] [SUB:bring-&gt;no] [SUB:out-&gt;no] [SUB:some-&gt;no] [SUB:some-&gt;no] substance from my mouth yes so what is the colour of the substance [SUB:err-&gt;yeah] it is about [INS:yeah] it is clear it is whitish it is [SUB:not-&gt;normal] it is just normal it is looking like saliva but it is very thick it is very thick was there blood in it at any point no there was no blood in it there was no blood in it [DEL:there] [DEL:was] [DEL:no] [DEL:blood] [DEL:in] [DEL:it] at any point [DEL:yes] and after you cough do you feel like vomiting or do you vomit no i do not i do not i do not feel like [INS:i] [SUB:vomiting-&gt;am] i do not vomit at all okay and you did not have catarrh or difficulty [DEL:in] swallowing prior to onset of the cough no no [SUB:there-&gt;that] was [INS:not] [INS:in] [SUB:nothing-&gt;my] i was not i had nothing my my even when i was coughing my chest was not [SUB:paining-&gt;burning] me nothing it was just the cough [SUB:then-&gt;and] i i discovered after a few days after that i [SUB:just-&gt;was] [DEL:started] running temperature too my body was very very hot it was very hot [DEL:that] i was shivering so you are telling me there is no there is no cough there is no chest pain no there is there is no chest pain my chest was not [INS:pain] [SUB:paining-&gt;in] me at all [SUB:your-&gt;the] chest was not [INS:pain] [SUB:paining-&gt;in] me is there anybody coughing around you no there [INS:is] nobody i stay alone right now so i have nobody around me i do not stay with people so i do not [SUB:have-&gt;remember] anybody around me that is coughing too and [SUB:at-&gt;i] [SUB:work-&gt;walk] [SUB:too-&gt;to] there is nobody coughing around me so okay so you stay alone you are not [DEL:here] in [SUB:an-&gt;a] [SUB:overcrowded-&gt;crowded] place yes but yes but doctor i noticed what actually prompted me to come is the fact that about two days ago i noticed that the cough became worsened and i was i started to have some difficulty in breathing so like that got me really scared [DEL:like] i was i was [DEL:i] [DEL:was] [DEL:just] feeling breathless for a moment comes and goes [SUB:then-&gt;and] and since that since then the breathlessness [SUB:has-&gt;have] become more worsened so that is what exactly prompted me to [INS:come] [SUB:completely-&gt;quickly] to see you [INS:so] you are finding it difficult to breathe yes [INS:the] [INS:cough] yes when you sleep at night [INS:do] you sweat excessively no at all i do not i do not [SUB:slept-&gt;sleep] i do not sweat [SUB:when-&gt;in] [SUB:i-&gt;a] sleep [SUB:at-&gt;department] [SUB:night-&gt;yes] okay so what is what [SUB:relieves-&gt;removes] the breathlessness any [SUB:change-&gt;changing] [DEL:in] position that relieves the breathlessness or [DEL:it] is constant no it is not associated with any any position nothing [SUB:i-&gt;and] [DEL:just] it just comes and goes like i just feel breathless [SUB:for-&gt;with] a while then it [SUB:relieves-&gt;releases] me then it comes again especially when [DEL:i] [DEL:am] especially when i am coughing okay has this worsened progressively yes yes [SUB:it-&gt;that] [SUB:has-&gt;is] gotten very bad doctor that is why i came to the hospital does it affect does it affect your daily activities yes it does doctor i have not been able to [SUB:work-&gt;walk] for the past two days because of the cough and the fact that i have [DEL:i] [DEL:have] not been feeling well generally [DEL:in] [DEL:my] [DEL:body] so [SUB:that-&gt;no] [SUB:is-&gt;no] [DEL:so] [DEL:now] this fever that you were having was it did it start suddenly or gradually [DEL:it] started it started gradually then became i became very hot and [DEL:it] has been like that it has been like that so the fever is high grade [DEL:you] [DEL:are] very hot yes yes it is [SUB:high-&gt;i] [SUB:did-&gt;do] you [SUB:at-&gt;have] any [INS:points] [INS:that] [SUB:point-&gt;you] [SUB:yes-&gt;can] check by yourself at home your temperature yes i did i did i have a [SUB:thermometer-&gt;stomach] [SUB:it-&gt;i] was about [INS:there] was about [INS:thirty] [INS:eight] [INS:point] [INS:nine] [INS:thirty] [SUB:thirtyeightnine-&gt;point] [SUB:thirtyeightnine-&gt;nine] okay and what [SUB:does-&gt;do] what do you do that [SUB:relieves-&gt;releases] the fever [INS:well] i took some i took some [INS:past] [SUB:paracetamol-&gt;more] it relieved [SUB:a-&gt;the] bit then but it did [DEL:did] not last long i just i [DEL:i] became hot again and it has been like that ever since so i just want to ask you some questions has [SUB:anything-&gt;this] happened before in the past okay has it happened in the past no no no no this is the first time i am [SUB:experiencing-&gt;expressing] [SUB:that-&gt;this] [DEL:is] [DEL:why] [DEL:i] [DEL:am] this is the first time i am [SUB:experiencing-&gt;expressing] this kind of thing okay this is the first time are you do you have any medical condition like are you asthmatic [INS:do] [INS:you] [SUB:during-&gt;do] [SUB:your-&gt;you] [SUB:blood-&gt;need] [SUB:group-&gt;a] [SUB:and-&gt;blood] [SUB:genotype-&gt;pressure] no i am not [INS:to] doctor i am fine no i have [SUB:nothing-&gt;not] [SUB:and-&gt;no] [DEL:that] [DEL:is] [DEL:why] [DEL:this] [DEL:is] [DEL:surprising] are you [INS:a] hypertensive [SUB:what-&gt;or] [SUB:did-&gt;diabetic] [SUB:you-&gt;are] [DEL:say] [DEL:i] [DEL:cannot] [DEL:hear] you [SUB:properly-&gt;a] [DEL:sir] [DEL:are] [DEL:you] hypertensive or diabetic none none none none no [DEL:no] i have none of them i have none of them so what have you what have you done to care for yourself so far i just [SUB:i-&gt;try] [DEL:just] [DEL:i] [DEL:just] [DEL:tried] to get some cough syrup [INS:up] but they did not they did not seem to work properly they did not seem to work and since the difficulty [INS:in] breathing started i knew i knew i know i needed to like [SUB:come-&gt;because] to speak to someone to a doctor so that is why i came today for you to like for me to like know what is wrong with me and treat myself basically have you been have you been admitted before no not not not that [SUB:i-&gt;current] [SUB:can-&gt;but] [SUB:remember-&gt;none] have you done any surgical procedure before no no okay so i am just going to ask you some other questions just to know what exactly could be related to your [SUB:to-&gt;so] the symptoms you are having so do you have headache headache [INS:it] just comes once in a while maybe because the cough i have not been able to sleep really so kind of yeah kind of yes okay so any loss of consciousness no no no no okay [DEL:okay] do you have [SUB:catarrh-&gt;catar] no at all okay do you have any abdominal pain no no [SUB:i-&gt;no] [SUB:do-&gt;no] [SUB:not-&gt;no] [SUB:have-&gt;no] [SUB:any-&gt;no] [SUB:diarrhea-&gt;no] [SUB:or-&gt;no] [SUB:vomiting-&gt;no] no [SUB:i-&gt;no] [SUB:have-&gt;no] [SUB:not-&gt;no] [SUB:vomited-&gt;no] [SUB:at-&gt;no] [SUB:all-&gt;no] [SUB:you-&gt;no] [SUB:have-&gt;no] [SUB:any-&gt;no] [SUB:bone-&gt;no] [SUB:pain-&gt;no] [SUB:yes-&gt;no] no [SUB:the-&gt;no] no [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [INS:no] [SUB:the-&gt;no] [SUB:most-&gt;no] [SUB:it-&gt;no] [SUB:is-&gt;the] [SUB:just-&gt;most] [SUB:it-&gt;of] [SUB:is-&gt;the] just the [SUB:shortest-&gt;shouters] of breath [DEL:i] have been [SUB:having-&gt;happening] the difficulty in breathing [DEL:i] have been [SUB:having-&gt;happening] [SUB:that-&gt;so] [DEL:is] [DEL:just] that is [SUB:just-&gt;the] [DEL:so] [DEL:in] summary you are telling me in summary you are telling me you had you [DEL:you] have had cough fever and difficulty in breathing yes right and your cough is productive yes [SUB:all-&gt;alright] [DEL:right] so i am going to have to have to examine you right i am going to have to examine you and i am going to have to listen to your chest to know [DEL:if] to know whatever is going on in your chest [DEL:whether] there is a chest infection that is causing you to have a fever and the and the cough do you understand and then we are going to have you do some investigations like a chest xray a complete blood count [INS:or] a full blood count [SUB:which-&gt;to] [DEL:will] tell us whether there is an infection going on depending on the parameters that are elevated or reduced do you understand we are going to do [SUB:you-&gt;a] [SUB:know-&gt;neutrophil] [DEL:electrocyte] segmentation [SUB:rates-&gt;rate] to know whether there is an inflammatory process [SUB:going-&gt;brain] on do you understand and then we are also going to take your sputum your the phlegm and we are going to send it for culture sensitivity to know what bacteria is is being cultured please i just want to ask you do you smoke no no i do not [INS:so] doctor i am a good christian i do not smoke i do not drink you do not you do not drink alcohol either i do not i do not do any of those i do not do [SUB:drugs-&gt;jobs] i do not do any of that i am going to ask you some other questions do you have [INS:there] [SUB:their-&gt;are] kind of personal questions can i go ahead yeah i just want to know doctor i just want to i just want to be fine i just want to know how soon you can start treating me and what i [INS:do] [SUB:will-&gt;not] [SUB:need-&gt;want] to [SUB:take-&gt;ask] [SUB:basically-&gt;if] i [SUB:just-&gt;do] [SUB:want-&gt;not] [DEL:to] [DEL:ask] [DEL:ifi] [DEL:just] want to ask if you have multiple sexual partners and [DEL:then] your sexual practices no no [DEL:you] [DEL:have] oral sex [DEL:i] [DEL:am] [DEL:married] no [SUB:not-&gt;none] at all not at all [DEL:i] [DEL:am] [DEL:married] so we are going to start you from the history and the examination we have done and then we are going to ask you to do some investigations however we have some differentials like [SUB:diagnosis-&gt;diagnoses] the because [DEL:the] [DEL:because] of what is causing the cough and the fever we have some [SUB:this-&gt;just] [SUB:thing-&gt;in] [DEL:at] the back of our mind which could be the because do you understand we think you have a pneumonia pneumonia [DEL:a] chest infection so we are going to start you on a broad spectrum antibiotics right and then we are going to start you on [DEL:the] cough syrup right to treat the cough while we wait for the results of our investigations do you understand okay and then since there is no history of asthma by the time you [DEL:will] start [SUB:treatment-&gt;treatments] with the antibiotics and [DEL:and] the cough syrup there will be the breathlessness [INS:business] is going to reduce but we your we would have checked your [DEL:your] oxygen saturation and we [DEL:will] see that it is fine so there will be no need to place you on on oxygen so you are [SUB:going-&gt;against] [SUB:to-&gt;having] [DEL:have] you do [DEL:a] full [SUB:blood-&gt;block] [SUB:count-&gt;out] in sputum and [INS:end] [SUB:microscopy-&gt;microscopic] culture sensitivity [DEL:you] are going to have you [INS:doing] [SUB:do-&gt;the] [SUB:any-&gt;enteric] [SUB:erythrocyte-&gt;site] [SUB:segmentation-&gt;sedimentation] [SUB:rate-&gt;rates] and [DEL:you] are going to do a chest xray so let us see if it is [DEL:a] structural problem or a functional problem do you understand okay [DEL:doctor] [DEL:so] [DEL:doctor] do [DEL:i] [DEL:do] you want to ask [SUB:the-&gt;a] question [SUB:if-&gt;do] you have any questions yes i was going to ask that are you going to keep me in [SUB:the-&gt;your] hospital or do i [INS:have] [SUB:that-&gt;to] [SUB:can-&gt;go] [SUB:i-&gt;home] can i be treated from home because i do not know we [DEL:we] [DEL:we] are going to admit you for some time to evaluate you and because of the breathlessness you are having right [DEL:and] [DEL:then] [DEL:we] [DEL:will] [DEL:start] [DEL:you] [DEL:on] [DEL:on] [DEL:intravenous] [DEL:intravenous] [DEL:that] [DEL:is] okay that is [SUB:cool-&gt;fine] [SUB:culture-&gt;so] [DEL:and] [DEL:sensitivity] [DEL:could] [DEL:take] [DEL:about] [DEL:seventytwo] [DEL:hours] [DEL:to] [DEL:to] [DEL:five] [DEL:days] [DEL:before] [DEL:it] [DEL:will] [DEL:be] [DEL:ready] [DEL:do] [DEL:you] [DEL:understand] [DEL:yeah] [DEL:no] [DEL:problem] [DEL:doctor] thank you [DEL:no] [DEL:problem] [DEL:doctor] [DEL:thank] [DEL:you] very much i think that is fine i will just yeah i will just do the [SUB:labs-&gt;laps] and wait for [SUB:just-&gt;is] for you to start the treatment thank you</t>
+        </is>
+      </c>
+      <c r="AM3" t="inlineStr">
+        <is>
+          <t>good afternoon sir i am doctor [SUB:sadeko-&gt;shadakoff] good afternoon good afternoon doctor how are you doing today sir doctor i am not i am not too fine [INS:on] not too fine that is why i came to the hospital today what [SUB:was-&gt;is] the complaints so doctor i have been coughing for about a week now and i have been also [SUB:also-&gt;at] [SUB:have-&gt;yes] you also have what so and i also have [DEL:i] [DEL:have] also been running temperature for about five days [SUB:so-&gt;it] [SUB:you-&gt;is] [SUB:have-&gt;been] [SUB:running-&gt;really] [DEL:temperature] [DEL:for] five days yes yes [INS:and] [INS:the] [INS:cough] [INS:has] [INS:been] for [INS:the] [INS:cough] [INS:has] [INS:been] [INS:for] [INS:how] [INS:long] [INS:for] about a week now a week yes okay all right so the cough did [SUB:it-&gt;this] start [INS:soddening] [SUB:suddenly-&gt;the] or gradually the cough started suddenly just started like that i just [DEL:just] woke up more morning and started coughing [SUB:about-&gt;by] a week ago yes was there [DEL:was] [DEL:there] any symptoms like [SUB:catarrh-&gt;qatar] or any [DEL:any] difficulty in swallowing before the cough started no none like that i had nothing like that nothing like that you had nothing like that yes okay so now the cough how does it sound does it sound like [SUB:barking-&gt;backing] does [SUB:it-&gt;this] sound like it [DEL:is] comes in [SUB:bouts-&gt;body] and then you have to take a [SUB:deep-&gt;different] [DEL:breath] when [DEL:when] you say [SUB:barking-&gt;backing] [DEL:do] [DEL:you] are you do you mean like a dog or what do you mean by [SUB:barking-&gt;backing] yes yes sounds like a dog [SUB:barking-&gt;back] no no no no no [DEL:no] mine is not that [DEL:i] [DEL:did] [DEL:not] [DEL:i] [DEL:did] [DEL:not] [DEL:experience] [DEL:anything] [DEL:like] [DEL:that] okay so is the cough productive of [SUB:phlegm-&gt;flame] yes yes it is productive [DEL:when] [DEL:i] yes when i cough i bring out some [DEL:some] substance from my mouth yes so what is the colour of the substance [SUB:err-&gt;yeah] it is about [INS:yeah] it is clear it is whitish it is [DEL:not] [DEL:it] [DEL:is] just normal it is looking like saliva but it is very thick it is very thick was there blood in it at any point no there was no blood in it there was no blood in it there was no blood in it at any point [SUB:yes-&gt;okay] and after you cough do you feel like vomiting or do you vomit no i do not i do not i do not feel like [DEL:vomiting] i do not vomit at all okay and you did not have [SUB:catarrh-&gt;catar] or difficulty in swallowing prior to [INS:the] onset of the cough no no [INS:no] [SUB:there-&gt;i] was nothing i was not i had nothing [DEL:my] [DEL:my] even when i was coughing my chest was not [SUB:paining-&gt;painting] me nothing it was just the cough [SUB:then-&gt;and] i [DEL:i] discovered after a few days after that i [SUB:just-&gt;was] [SUB:started-&gt;hired] running temperature too my body was very very hot it was very hot [DEL:that] i was shivering so you are telling me there is no [DEL:there] [DEL:is] [DEL:no] cough there is no chest pain no there is [DEL:there] [DEL:is] no chest pain my chest was not paining me at all [SUB:your-&gt;it] [SUB:chest-&gt;just] was not [SUB:paining-&gt;pain] [DEL:me] is there anybody coughing around you no there [INS:is] nobody i stay alone right now so i have nobody around me i do not [SUB:stay-&gt;tell] [SUB:with-&gt;you] people so i do not [SUB:have-&gt;remember] [DEL:anybody] [DEL:around] [DEL:me] [DEL:that] [DEL:is] coughing too and [SUB:at-&gt;i] [SUB:work-&gt;walk] too there is nobody coughing around me [DEL:so] okay so you stay alone you are not [DEL:here] in an overcrowded place yes but yes but doctor i noticed what actually prompted me to come is the fact that about two days ago i noticed that the cough became worsened and i [SUB:was-&gt;said] [DEL:i] [DEL:started] to have some difficulty in breathing so like that got me really scared [DEL:like] i was [DEL:i] [DEL:was] [DEL:i] [DEL:was] [DEL:just] feeling breathless for a moment comes and goes [DEL:then] and since that since then the breathlessness has become more worsened so that is what exactly prompted me to [INS:come] [SUB:completely-&gt;quickly] to see you you are finding it difficult to breathe yes yes when you sleep at night [INS:do] you sweat excessively no at all i do not [SUB:i-&gt;sleep] [DEL:do] [DEL:not] [DEL:slept] i do not sweat [SUB:when-&gt;yes] [SUB:i-&gt;okay] [DEL:sleep] [DEL:at] [DEL:night] okay so what is what relieves the breathlessness any change in position that relieves the breathlessness or [SUB:it-&gt;this] [DEL:is] constant no it is not associated with any [DEL:any] position nothing i just it just comes and goes like i just feel breathless for a while then it relieves me then it comes again especially when i am [SUB:especially-&gt;sitting] when i am coughing [DEL:okay] has this worsened progressively yes yes [SUB:it-&gt;that] [SUB:has-&gt;is] gotten very bad doctor that is why i came to the hospital does it affect does it affect your daily activities yes it does doctor i have not been able to work for the past two days because of the cough and the fact that i have [DEL:i] [DEL:have] not been feeling well generally in my body so that is [DEL:so] now this fever that you were having was it did [SUB:it-&gt;you] start [SUB:suddenly-&gt;sodding] [SUB:or-&gt;it] gradually it started [DEL:it] [DEL:started] gradually then [DEL:became] i became very hot and [DEL:it] has been like that it has been like that so the fever is [SUB:high-&gt;highgrade] [DEL:grade] you are very hot yes yes it is high did you [INS:attend] [INS:a] [SUB:at-&gt;question] [SUB:any-&gt;to] [SUB:point-&gt;try] [SUB:yes-&gt;and] check by yourself at [DEL:home] your temperature yes i did i did i [SUB:have-&gt;average] [DEL:a] thermometer [SUB:it-&gt;i] was about [DEL:was] [DEL:about] thirtyeightnine [SUB:thirtyeightnine-&gt;thirtynine] okay and what [DEL:does] [DEL:what] do you do that relieves the fever i took some [SUB:i-&gt;past] [SUB:took-&gt;more] [DEL:some] [DEL:paracetamol] it relieved [SUB:a-&gt;the] bit then but it did [INS:it] did not last long [INS:it] [SUB:i-&gt;is] just [SUB:i-&gt;it] [DEL:i] became [SUB:hot-&gt;what] again and it has been like that ever since so i just want to ask you some questions has [INS:this] [SUB:anything-&gt;thing] happened before in the past okay has it happened in the past no no no no this is the first time i am [SUB:experiencing-&gt;expressing] [SUB:that-&gt;as] [DEL:is] [DEL:why] i am this is the first time i am experiencing this kind of thing okay [SUB:this-&gt;it] is the first time are you do you have any medical condition like are you asthmatic [INS:do] [INS:you] [SUB:during-&gt;need] [SUB:your-&gt;a] blood group and genotype [INS:oh] no i am not doctor i am fine no i have nothing [DEL:and] [DEL:that] [DEL:is] [DEL:why] [DEL:this] [DEL:is] [DEL:surprising] are you [SUB:hypertensive-&gt;hypocensing] [DEL:what] [DEL:did] [DEL:you] [DEL:say] i cannot hear you properly sir are you hypertensive or diabetic none none [SUB:none-&gt;no] [DEL:none] no no i have none of them i have none of them so what have you what have you done to care for yourself so far i just [DEL:i] [DEL:just] [DEL:i] [DEL:just] tried to get some [INS:coughs] [SUB:cough-&gt;here] [SUB:syrup-&gt;up] but they did not [DEL:they] [DEL:did] [DEL:not] seem to work properly they did not seem to work and since the difficulty [INS:in] breathing started i [DEL:knew] [DEL:i] [DEL:knew] [DEL:i] know i needed to [DEL:like] [DEL:come] [DEL:to] speak to someone to a doctor so that is why i came today for you to like for me to [DEL:like] know what is wrong with me and treat myself basically have you been [DEL:have] [DEL:you] [DEL:been] admitted before no not [DEL:not] [DEL:not] that [SUB:i-&gt;current] [SUB:can-&gt;but] [SUB:remember-&gt;none] have you done any surgical procedure before no no okay so i am just going to ask you some other questions just to know what exactly could be related to your to the symptoms you are having so do you have headache headache [INS:yes] [SUB:just-&gt;it] comes once in a while maybe because the cough i have not been able to sleep really so kind of yeah kind of yes okay so any loss of consciousness no no no no okay okay do you have [SUB:catarrh-&gt;catar] no at all okay do you have any abdominal pain no no i do not have [SUB:any-&gt;a] [SUB:diarrhea-&gt;problem] [DEL:or] [DEL:vomiting] no i [SUB:have-&gt;am] not vomited at all you have any bone pain yes no [DEL:the] no the most it is just [DEL:it] [DEL:is] [DEL:just] the [SUB:shortest-&gt;shortness] of breath i have been having the difficulty in breathing [SUB:i-&gt;has] [DEL:have] been having [DEL:that] [DEL:is] [DEL:just] [DEL:that] [DEL:is] [DEL:just] so in summary you are telling me [SUB:in-&gt;some] [DEL:summary] [DEL:you] are telling me you had you [DEL:you] have had cough fever and difficulty in breathing yes right and your cough is productive yes all right so i am going to have to have to examine you right i am going to have to examine you and i am going to have to listen to your chest to know if to know whatever is going on in your chest whether there is a chest infection that is causing you to have a fever and the [DEL:and] [DEL:the] cough do you understand and then we are going to have you do some investigations like a chest xray a complete blood count [INS:of] a full blood count [SUB:which-&gt;to] [DEL:will] tell us whether there is an infection going on depending on the parameters that are [SUB:elevated-&gt;indicated] or reduced do you understand we are going to do [SUB:you-&gt;a] [SUB:know-&gt;neutrocyte] [DEL:electrocyte] segmentation [SUB:rates-&gt;rate] to know whether there is an inflammatory process going on do you understand and then we are also going to take your sputum [DEL:your] the [SUB:phlegm-&gt;flame] and we are going to send it for [SUB:culture-&gt;cultural] sensitivity to know what bacteria is [DEL:is] being [SUB:cultured-&gt;caught] please i just want to ask you do you smoke no no i do not [INS:so] doctor i am a good christian i [SUB:do-&gt;just] [SUB:not-&gt;spoke] [DEL:smoke] i do not [SUB:drink-&gt;think] you do not [DEL:you] [DEL:do] [DEL:not] drink alcohol either i do not [SUB:i-&gt;drink] [DEL:do] [DEL:not] [DEL:do] any of those i do not do drugs i do not [SUB:do-&gt;drink] [DEL:any] of that i am going to ask you some other questions do you have [INS:there] [SUB:their-&gt;are] kind of personal questions can i go ahead yeah i just want to know doctor i just want to i just want to be fine i just want to know how soon you can start [SUB:treating-&gt;with] me [DEL:and] [DEL:what] i [DEL:will] [DEL:need] [DEL:to] [DEL:take] [DEL:basically] [DEL:i] just want to ask [INS:if] [SUB:ifi-&gt;i] just want to ask if you have multiple sexual partners and [DEL:then] your sexual practices no no [INS:do] you have oral sex i am married no not at all not at all [DEL:i] [DEL:am] [DEL:married] so we are going to start you from the history and the examination [SUB:we-&gt;you] have done and then we are going to ask you to do some investigations however we have some differentials like diagnosis the because [DEL:the] [DEL:because] of what is causing the cough and the fever we have some [DEL:this] [DEL:thing] at the back of our mind which could be the because [DEL:do] you understand we think you have a pneumonia [DEL:pneumonia] a chest infection so we are going to start you on a broad spectrum antibiotics right and then we are going to start [DEL:you] on the cough syrup right to treat the cough while we wait for the results of our investigations do you understand okay and then since there is no history of asthma by the time you [DEL:will] start treatment with the antibiotics and [DEL:and] the cough syrup there will be the breathlessness is going to reduce but we [SUB:your-&gt;will] [DEL:we] [DEL:would] have checked your [DEL:your] oxygen saturation and we [DEL:will] see that it is fine so there will be no need to place you on [DEL:on] oxygen so [SUB:you-&gt;we] are going to have you do a full [SUB:blood-&gt;block] count [SUB:in-&gt;a] sputum and [SUB:microscopy-&gt;microscopic] [SUB:culture-&gt;control] sensitivity [SUB:you-&gt;i] [SUB:are-&gt;am] going to have you do [SUB:any-&gt;an] [SUB:erythrocyte-&gt;intrusive] [SUB:segmentation-&gt;sedimentation] rate and [SUB:you-&gt;we] are going to do a chest xray so let us see if it is a structural problem or a functional problem do you understand okay doctor [SUB:so-&gt;okay] [DEL:doctor] [DEL:do] [DEL:i] [DEL:do] you want to ask [INS:me] [SUB:the-&gt;a] question [SUB:if-&gt;do] you have any questions yes i was going to ask that are you going to keep me in [SUB:the-&gt;your] hospital [DEL:or] [DEL:do] [DEL:i] [DEL:that] can i [DEL:can] [DEL:i] be treated from home because i do not know we [DEL:we] [DEL:we] are going to admit you for some time to evaluate you and because of the breathlessness you are having right [SUB:and-&gt;okay] [DEL:then] [DEL:we] [DEL:will] [DEL:start] [DEL:you] [DEL:on] [DEL:on] [DEL:intravenous] [DEL:intravenous] [DEL:that] [DEL:is] okay that is [SUB:cool-&gt;fine] [DEL:culture] [DEL:and] [DEL:sensitivity] [DEL:could] [DEL:take] [DEL:about] seventytwo hours to [DEL:to] five days [SUB:before-&gt;for] [SUB:it-&gt;you] [SUB:will-&gt;to] be ready do you understand [DEL:yeah] no problem doctor [DEL:thank] [DEL:you] no problem doctor thank you very much i think that is fine i will just yeah i will just do the labs and wait [DEL:for] [DEL:just] for you to start the treatment thank you</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>RES0073</t>
+          <t>2_Diarrhea</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>data/final_audio/RES0073.mp3</t>
+          <t>data/final_audio/2_Diarrhea.wav</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>D: Would you mind by starting with what brought you in?
-P: Yeah, so over the last week I've just been feeling some symptoms. It kind of first started with, like a runny nose. That was around like 5 days ago and then it turned into just a lot of congestion, like around my nose and like my throat. And now over the last two days I've been just feeling so much pressure around my nose and around my jaw so I've been getting a lot of pain there as well.
-D: OK, is your nose still running?
-P: Yeah, I'm still getting some discharge and I also feel like I'm getting some dripping at the back of my throat too, especially when I wake up.
-D: OK, and could you describe the discharge? Is it clear, yellow, greenish?
-P: Uh, it's fairly clear and sometimes, like a bit white, but like, it's not like green or yellow.
-D: OK, uh, and have you felt that it's difficult to breathe in through either of your nostrils, like it's obstructed?
-P: Yeah, so at night sometimes I have to like turn because one side of my nose gets difficult to breathe from and then it kind of balances out on the other side. So yeah, I do have some obstruction.
-D: OK, and have you had any changes to your sense of smell?
-P: Yeah, so just in the last three days when the congestion got really bad I started losing the ability to smell.
-D: OK, have you had any changes to your sense of taste?
-P: No, taste is fine. 
-D: OK, and have you had any cough or sore throat?
-P: Uh, no. No cough or sore throat.
-D: OK, and the symptoms have gone on for five days. Have you had a period of time where you got better and then got sick again? 
-P: I did kind of have a runny nose last week as well, so probably like 8 days ago but then the runny nose discontinued a little bit but really got worse 5 days ago, but all these other symptoms just happened in the last few days.
-D: OK, and you have pain. Do you feel it in your jaw or do you feel it in the in the front of your nose?
-P: Yes, I would say mainly over the cheeks. It can kind of go near the front of my teeth as well, so like I would say like mostly around the cheeks, jaws and up to the front of my teeth. 
-D: OK, And do you grind your teeth at all at night? or have you had, TMJ issues before?
-P: No nothing like that. I think it's not so much on and around my teeth, it's more so just to right below my nose, above my teeth and just around my cheeks.
-D: OK, so no pain in your mouth or anything like that?
-P: No, not inside my mouth.
-D: OK, have you had any fevers or chills?
-P: Uhm, I Don't think I've had a fever. I did feel some chills over the last few days, but just very brief episodes.
-D: OK, and over the last few weeks have you had any weight loss? 
-P: No.
-D: OK, and you said you didn't have a cough or a sore throat, but have you had any wheezing?
-P: No wheezing.
-D: How about any shortness of breath?
-P: Uh, not shortness of breath. Just sometimes when my nose gets like really congested, I just turn into like a mouth breather, but that's about it.
-D: I see, OK, and have you had any chest pain?
-P: No, no chest pain. 
-D: Alright, and any lightheadedness or feeling dizzy?
-P: No.
-D: OK, have you had any nausea or vomiting?
-P: Nope. 
-D: Any abdominal pain? 
-P: No.
-D: Have you had any diarrhea?
-P: Sorry, what was that?
-D: Have you had any diarrhea?
-P: No diarrhea. 
-D: OK, and have you had any urinary problems?
-P: Uh, no.
-D: And have you had any rashes or skin changes?
-P: No, not that I know.
-D: OK, then how about any muscle aches or joint aches? 
-P: Uh, no.
-D: OK, and have you had any muscle weakness?
-P: No.
-D: And how has your energy been? Any fatigue?
-P: Uhm, it's been mainly OK, just maybe sometimes difficult to get to sleep with all the all the congestion, but I don't think my energy has been affected too much, no.
-D: OK, and, uh, sorry to go back to this, I don't think I asked. Did you notice any discharge from your eyes or any eye redness?
-P: Not discharge, but yeah, maybe a little bit of redness.
-D: OK, have your eyes been itchy?
-P: Uhm Yeah, a little bit. I would say they have been a bit itchy.
-D: OK, alright then, do you have any medical conditions that you see a physician for regularly? 
-P: Uh, just uhm, its called dyslipidemia. 
-D: OK, I see, and any medications you take for that?
-P: Just like a Statin medication.
-D: OK, do you take any other medications? over the counter? prescribed?
-P: No, other than that I take multivitamins.
-D: OK, and do you have any allergies to medications or like environmental allergies that might be getting worse?
-P: Uh, no, not that I know.
-D: OK, so you don't experience any symptoms like this when the seasons change?
-P: I don't think so. I have had this happen to me, Uh, I would say like once before. It happened like two years ago. It was pretty similar. 
-D: OK, uhm, and what was done at that time?
-P: At that time it kind of just went away on it's own. It got better. I feel it's definitely worse this time. But at that time I didn't even go to the doctor, it kind of just went away.
-D: OK, I see. Any recent hospitalizations?
-P: No hospitalizations.
-D: Any surgeries?
-P: Nope. 
-D: Alright, and could you tell me where abouts you're living currently and who you're living with?
-P: Yeah, so I'm currently living in an apartment by myself, just outside of London.
-D: OK, and anybody that you've been around who's had any symptoms?
-P: Uh, no, not that I know of.
-D: OK, so no sick Contacts. And have you traveled anywhere out of the city or province?
-P: No, I've tried to stay home, besides going to work. I just work at the grocery store. Besides that, no, nowhere else.
-D: OK, and any of your coworkers have any symptoms? Or any coworkers being off sick?
-P: No, we're pretty careful right now with the pandemic.
-D: I see, yeah, that's great. OK, and do you smoke cigarettes?
-P: No, I quit just a couple of years ago.
-D: Oh, that's great. It's not easy to quit, so that's awesome. And do you drink alcohol?
-P: Just maybe like red wine a couple of times a week.
-D: I see, OK, and do you use any recreational drugs? 
-P: Uh, just, in a month, maybe once or twice, I smoke a joint.
-D: OK, uh, and anybody in the family have any lung or heart conditions?
-P: No, not that I know of.
-D: Alright, and how about any cancer in the family?
-P: Uh, no, no cancers.
-D: OK, I think I that was everything I wanted to ask about today. Was there any other symptoms or anything else that you wanted to make sure I knew about today?
-P: No,  I think that's all. I just didn't know if I needed any, like, medications or if I needed to get tested. I just wanted to make sure.
-D: Yeah, so well, certainly check your temperature to see if you have a fever. And if you do and it's high enough, that will increase the chance that you have a bacterial sinusitis,  and if so, with some of your symptoms, including the discharge, obstruction, loss of smell, and facial pain, that all fits the picture for it and also you had a period where you felt a little bit better and then worse again. So that might require antibiotics, but we will check your temperature and go from there. 
-P: Alright, sounds good, thank you so much.
-D: Thank you.</t>
+          <t>OK, Good afternoon, my name is Doctor Sadeko. Yeah, good afternoon. How may I help you? Yeah, good afternoon, my name is Miss Sharon, erm… yes. OK. So, do you have any complaints? Yes, Doctor. I have been stooling for about four days now and I've been abdominal pain, two alongside. So, that’s… those are my 2 complaints. OK, OK, so which one started first, the stooling or the abdominal pain? Yeah, the stooling started first about four days ago. OK, so now like what is the consistency of the of the stool? Is it watery, Is he semi solid or it's in normal form, well formed stools? It's very watery. Very watery. Very watery, Yes. OK All right. So like, how many episodes of erm… you said you've been stolen for over 4 days, right? Yes. And how many episodes do you… do you have per day of stooling. My… about six… about six to seven episodes, actually about around that of passage of watery stool? Yes, Yes, Yes, Doctor. OK, OK. So erm… is the stool containing mucus, Is it mucoid? No, no, there's no mucus. No mucus in it. Was there any blood in it? No blood at all. There's no blood in it, OK. Did you change… Did you eat a… from a new restaurant or did you Did you eat something different? Erm…Actually, a few days ago I, like just before it started, I actually had a take out in a restaurant with my family, which all of us ate and erm… one of... my child actually vomited but vomiting stopped and he feels good now. So it's just me right now with the complaints I have of the of the loose stool Are you also vomiting? Yes, I…I vomited about two, two episodes about two times, yes. What… what… What… What was inside the vomit? What was the components of the vomitus? Was it what you ate or was it greenish or was there blood in it? No, there was no blood. It was just the content of what I ate. Was the vomiting, Was it projectile? So what do you mean by projectile Erm…when it comes with force, When it comes with force. Well, I really don't know. It just… I just vomited that’s all. I… I can't really remember how you came out, to be honest. OK. Was there any, is there any abdominal distension? Distension, like a swelling, Swelling. Yeah, was there swelling in your stomach? No, just the abdominal pain. The pain is just at my, the lower part of my stomach. OK.uhm.. All right. All right. Thank you. So, you said your son also ate… ate the same the same food that you bought and he's now vomiting. How is he feeling now? He feels… he's OK. He… after the episode of vomiting he… he got… he got well and he's OK. How is your appetite like? My appetite is.. is here and there. Know… it's not really good like. So now let's… OK, OK. So, let's talk about… let's talk about your… the pain you were having. So, can you describe the pain for me? What's the, what's the nature of the pain? Is it a sharp pain or a pain that holds you and leaves you? What…What kind of pain is it? Yeah, I'll describe it like, like has a cramp pain, like the pain I feel during menstruation. So, that's the kind of pain. Like, that's the way I can describe it. And where… where is this pain located In your abdomen? The lower part, the lower part? Does this pain… does it move to another part of your body when you start feeling it? No, just just the lower part of my... like moving to the back just the lower part it doesn’t move to your back? No, no, not at all It stays in the same space? Yes, Yes. OK. OK. So what, what do you think makes this pain worse? Well maybe if I… if I don't eat, I don't know. If I don't eat something around that. Yeah, but I don't feel like if it just comes and goes, I don't feel like anything that makes it worse per se. But I will say maybe If I don't eat, yes. OK. What… What… What relieves the pain? Erm… Nothing I don't know, I don't know anything that reduce the pain, it just comes and goes on its one. OK, so on a scale of zero to 10, let's say 0 means that you don't have any pain at all and 10 is the worst pain you've felt in your life, So what would you give this pain? I will the pain like five or ten? 5 / 10 Yes. No problem. So uhm, let's yeah, take some history. Do you have… are you hypertensive? No, I'm not. Are you diabetic? No I'm not. Do you? Are you a known peptic also patient? No, no. Are you lactose intolerant? No, the only the only ailment I’m being treated for… I'm being treated for is asthma. I’m a known asthmatic and and I am on… I use inhalers and how many… how many exacerbations do you have in a year? about… in the last one just one. OK, OK that is good. Have you had any previous history of blood transfusion? Any history of surgeries? No, no, none at all. OK. erm… erm…   Do you drink alcohol or do you smoke? No, I don't, I don't do any of those. I don't at all. And since you've been feeling these symptoms that you're having has… has it progressively worsened. Yeah, I I feel so. So that's why I actually came to the hospital just today, to see the doctor and properly know what's wrong with me and take care of it, basically. Have you been feeling very thirsty? Have you been feeling like your body is dry? Has your urine reduced? No, not at all. No, No. Do you feel weak? Yeah, I feel kind of weak. Yeah. Yeah. My… my… I feel sometimes my mouth is kind of dry to kind of. OK, OK, OK, No problem. So, do you… asides the asthma, do you have any other ailments you think the doctor should know about? No, not at all. At all, I have no other…. no other medical condition. Do you have any drug allergies? No, I don't react. No at all, I don't react to any drugs at all. OK. Please, are you married? Yes, I'm married With two kids. Erm… yes. OK. And you, you live with your husband? Yes, Yes, I do. And your kids live with you? Yeah, what did you say, doctor? And your kids live with you as well? Yes, they are. So, aside your… your son or your child, who had the, the vomiting, was there any… any of your family members that also had the same symptoms? No, no, no, no, no, other. Just me… just me and My son, yes. OK, no problem. OK. Do you… I'm just going to ask some questions just to rule out every other thing. Do you do you have headaches? No, Doctor. Do you have chest pain? No, doctor. At all no. Do you have an abdominal pain? Oh, do you... you have an abdominal pain. Do you have any change in your bowel habits? uhm… I don't know how to answer that. Other than the… just the .... the OK, I think. I think… I think that is fine. Your urine, Your… your urine, has it… has it changed in quantity? No, not at all. How about the frequency of urination, has it changed? No, No. My urination is fine. Do you have any, do you have any bone pain? No. All right, no problem. So, erm…thank you for… for answering my questions. Those questions are basically there so that we can pinpoint where and where there is a problem. And they can also come to have differential diagnosis of what could be the cause of your symptoms. And we’d like to examine you right? Check your level of hydration, check your general physical appearance to see whether you… and access your… your general health right. We also like to do an abdominal examination, right, to… to also give us more information on the abdominal pain you're having. If you could lead us to what is causing the symptoms you're having, the abdominal pain and the… the stooling. Do you understand? Yes Although… although, it seems like what you ate… the restaurants you got food from there must have been where you got some infection. Which could have… which could have caused the diarrhea. You want to say something? So, what exactly is wrong… What exactly is wrong? What exactly is the cause? OK. It's just the food I ate right? So, yeah, it looks like you've had a food poisoning… had a food poisoning. But, however we are going to have to evaluate you and find out what exactly is the cause. So we are going to do some very series of tests. I'm going to check your blood count to know if there's a… there's some infection which could be gastroenteritis. We want to do your erythrocyte sedimentation rates to know if there's any sign any, any type of kind of inflammatory disorder that could cause diarrhea like inflammatory bowel disease, right. And then we’d also want to do a stool culture microscopy and sensitivity and to look out for parasites and some bacteria that could cause you to be having diarrhea. We also check your retroviral status to know if you have retroviral disease which could also be a cause of of diarrhea although that comes in the chronic… chronic setting, however, would also need to just rule that out. Do you understand? OK doctor, OK. However, we are going to start you on, on some… some fluids to you know give you some strength and restore your hydration level because you've been losing some fluid from… from the stooling and the vomiting. We’ll also check your electrolytes, electrolytes to know what's your electrolyte picture looks like and the ones that will be needed to be that will… that will need to be corrected. Do you understand? OK And also lastly, we'd also want to check do an abdominal scan throughout any structural or functional problems that could be in the abdominal which would be could be causing the diarrhea and the… the… the abdominal pain. Do you understand? Yes. Thank you, Doctor. Thank you very much, Yes. Do you have any more questions for me? No, I'm fine, I'm fine. I'm good. Let's just get on with it. You’re fine . Yeah. So that'll be fine. Thank you. So you'll be attended to. All right. Thank you very much, Doctor.</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>711.9243125</v>
+        <v>735.5839999999999</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>us_medical</t>
+          <t>med-convo-nig</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Would you mind by starting with what brought you in? Yeah, so over the last week I've just been feeling some symptoms of, so it kind of first started with just like I had like a runny nose and then, so that was around like five days ago and then it turned into just a lot of congestion like around my nose and like my throat and now over the last two days I've been just feeling so much pressure around around my nose around my jaw so having having getting a lot of pain there as well okay is your nose still running yeah I'm still getting some discharge and I also feel like I'm getting some dripping at the back of my throat too especially when I wake up okay And could you describe the discharge? Is it clear, yellow, greenish? It's fairly clear and sometimes like a bit white but like it's not like green or yellow. Okay. And have you felt that it's difficult to breathe in through either of your nostrils like it's obstructed? Yeah, so I at night sometimes I I have to like turn because one side of my nose gets difficult to breathe from and then it kind of balances around the other side. So I do have some obstruction. Okay. And have you had any changes to your sense of smell? Yeah, so just in the last three days when the congestion got really bad, I started losing the ability to smell. Okay. Have you had any changes to your sense of taste? No, taste is fine. Okay. And have you had any cough or sore throat? No, no cough or sore throat. Okay. And the symptoms have gone on for five days. Have you had a period of time where you got better and then got sick again? again? I did kind of have a runny nose last week as well so probably like eight days ago and but that the runny nose has continued a little bit but really got worse five days ago but all these other symptoms just happened in the last few days. Okay. And you have pain is it you feel it in your jaw or do you feel it in the in the front of your nose or? Yes, I would say mainly over the cheeks. It can kind of go near the front of my teeth as well. So I would say like mostly around the cheeks, jaws, and up to the front of my teeth. Okay. Do you grind your teeth at all at night or have you had TMJ issues before? No, nothing like that. I think it's not so more like on and around my teeth, it's more so just right below my nose, above my teeth and just around my cheeks. Okay, so no pain in your mouth or anything like that? No, not inside my mouth. Okay, have you had any fevers or chills? I don't think I've had a fever. I did feel feel some chills over the last few days but just very brief episodes. Okay and over the last few weeks have you had any weight loss? No. Okay. And so you didn't have a cough or a sore throat but have you had any wheezing? No wheezing. How about any shortness of breath? Not shortness of breath, just sometimes in my neck nose gets like really congested it's I just I just turn into like a mouth breather but that's about it. I see okay and have you had any chest pain? No no chest pain. All right and any lightheadedness or feeling dizzy? No. Okay have you had any nausea or vomiting? Nope. Any abdominal pain? No. Have you had any diarrhea? Sorry, what was that? Have you had any diarrhea? No diarrhea. Okay, and have you had any urinary problems? No. And have you had any rashes or skin changes? No, not that I know of. Okay, and then how about any muscle aches or joint aches? No No. Okay. And have you any muscle weakness? No. And how's your energy been? Have you any fatigue? It's been mainly okay, just maybe sometimes difficult to get to sleep with all the congestion, but I don't think my energy's been affected too much. Okay. And sorry to go back to this, I don't think I asked. Did you have, notice any discharge from your eyes or any eye redness? Not discharge, but yeah, maybe a little bit of redness. Okay. Have your eyes been itchy? Yeah, a little bit. I would say they have been a bit itchy. Okay. All right, then do you have any medical conditions that you see a physician for regularly? Just a, I have, what's it called? It's, it's called high, like, dyslipidemia. Okay, I see. And any medications you take for that? Just a, like a statin medication. Okay, do you take any other medications over the counter or prescribed? No, just other than that I take multivitamins. Okay, and do you have any allergies to medications or maybe like environmental allergies that might be getting worse? No, not that I know of. Okay, so you don't experience any symptoms like this when the seasons change? I don't I don't think so. I have had this happen to me. I would say like once before it happened like two years ago. Yeah. It was pretty similar. Okay. And did you have any... And what was done at that time? At that time it kind of just went away on its own. It got better. like I feel it's definitely worse this time but at that time I didn't even go to the doctor I kind of just went away. Okay I see and have any reasons for hospitalizations? No hospitalizations and no. Any surgeries? Nope. Alright and could you tell me whereabouts you're living currently and who you're living with? Yeah, so I'm currently living in an apartment by myself and just outside of London. Okay, and anybody that you've been around who's had any symptoms? No, not that I know of. Okay, so no sick contacts. And have you traveled anywhere out of the city or province? No, I've tried to stay home. I, besides going to work, I just work at the grocery store. Besides that, nowhere else. Okay, and anybody, any of your co-workers have any symptoms or any co-workers been off sick? No, we're pretty careful right now with the pandemic. I see, yeah, no, that's great. Okay, and do you smoke cigarettes? No, I quit just a couple of years ago. Oh that's great. It's not easy to quit so that's awesome. And do you drink alcohol? Just maybe like red wine a couple of times a week. I see. Okay. And do you use any recreational drugs? Just in a month maybe or twice I smoke a joint. Okay. And anybody in the family have any lung or heart conditions? No, not that I know of. All right. And how about any cancer in the family? No, no, no cancers. Okay. I think that was everything. wanted to ask about today. Was there any other symptoms or anything else that you wanted to make sure I knew about today? No, I think that's all. I just didn't know if I needed any medications or if I needed to get tested. I just wanted to make sure. Yeah, so we'll certainly check your temperature to see if you have a fever and if you do and it's high enough that will increase the chance that you have a bacterial sinusitis with and if so with some of your symptoms including the discharge obstruction loss of smell and facial pain that all fits the picture for it and also you you felt you had a period where you felt a little bit better and then worse again. So that might require antibiotics, but we will check your temperature and go from there. All right, sounds good. Thank you so much. Thank you.</t>
+          <t>Okay, good afternoon. My name is Dr. Shadekum. Good afternoon. My name is Miss Sharon. Yes. Okay, so do you have any complaints? Yes, doctor. I have been straining for about four days now and having abdominal pain. Alongside so that's just my two complaints. Okay, okay, so which one started first the stooling or the abdominal pain? Yeah, the stooling started first about four days ago. Okay, so now like what is the consistency of the of the stool? Is he watery? Is he semi solid or is it normal form well formed? It's very watery, very watery. So like how many episodes of um you said you've been stalling for over four days, right? Yes. And how many episodes do you do you have per day of stalling? About six or six to seven episodes actually, about around that number. Yes, of passage of the water riser tube. Yes, yes, yes, doctor. Okay, okay, so um uh is this Is it still containing mucus? Is it mucoid? No, no, there's no mucus in it. Was there any blood in it? No blood at all. There's no blood in it. Okay. Did you change, did you eat from a new restaurant or did you, did you eat something different? Actually, a few days ago, just before you started, I actually had the take out in a restaurant with my family. Which all was it and um all of my child actually vomited but the vomiting stopped and it feels good now so it's just right now with the complaint i have of the of the loose so are you also vomiting yes i i've vomited about two um two episodes about two times yes well what what was inside the vomit what was the con um components Was it what you ate or was it greenish or was there blood in it? No, there was no blood, it was just the contents of what I ate. Was the vomiting was it projectile? So what do you mean by projectile? When it comes with force, when it comes with force. Well, I really don't know, I just, I just want to tell you that's the line, I can't really remember how it came out to be honest. Is there any is there any abdominal distention? Distention like a swelling? Swelling yeah, is there swelling in your stomach? No, just the abdominal pain. The pain is just at my lower part of my stomach. Okay, alright, alright, thank you. So you said your son also ate ate the same the same food that you bought and is now vomiting. How is he feeling now? It feels it's okay after the he got he got well and it's okay how is your appetite like my appetite is yeah there no it's not really good like so now this like before okay okay so let's talk about let's talk about your the pain we're having so can you describe the pain for me what's the what's the nature of the pain is it a sharp pain or a pain that holds you and needs What kind of pain is it? I would describe it as a camp pain, like a pain I feel during menstruation, so that's the kind of pain I can describe it. And where is this pain located in your abdomen? The lower parts. The lower parts. Does this pain, does it move to any other part of your body when you start feeling it? No, just the lower part of my abdomen. The same space. Yes, yes. Okay, okay, so what do you think makes this play worse? Well, if I don't eat, I don't know, maybe something around that, yeah, but I don't feel like if it just comes and goes, I don't feel like anything that makes it worse, I say, but I was saying if I don't eat, yes. Okay, what really? How is the pain? Um, not saying i don't know i don't know i just comes and goes on this one. Okay, so on a scale of zero to ten, let's say zero means that you don't have any pain at all and ten is the worst pain you felt in your life. So what would you give this pain? I would give this pain like five out of ten. Five out of ten. No problem. Let's take some history. Do you are you hypertensive? No, I'm not. Are you diabetic? No, I'm not. Do you are you a non-peptic ulcer patient? No, no. Are you lactose intolerant? No, the only the only payment I will be treating for is asthma. I have been treated for is asthma. I have non-asthmatic and I am on I use inhalers and how many? Recently, how many exhibitions do you have in a year? How about last one, just one. Okay, okay, that was good. Have you had any previous history of blood transfusion? Any history of surgeries? No, no, none at all. Okay. Do you drink alcohol or do you smoke? No, I don't. I don't do any of those. and since you've been feeling these symptoms that you're having as it progressively worsened yeah i feel so so that's why i actually came to the hospital just to see the doctor and properly know what's wrong with me and take care of it basically have you been feeling very thirsty have you been feeling like your body's dry has your urine reduced no not at all no no do you feel weak Yeah, I feel kind of weak, yeah, yeah, my mouth is kind of dry to kind of okay, okay, no problem. So do you, aside the asthma, do you have any other ailments that you think the doctor should know about? No, not at all at all. I have no other medical condition. Do you have any drug allergies? No, I don't react to any drugs at all. Are you married? yes i'm married with two kids um yes okay and you you live with your husband yes yes i do and your kids live with you yeah what did you say doctor and your kids live with you as well yes they are so aside your your son or your child who are the the vomit symptoms was there any any of your family members that also had the same symptoms no no No, that just me and my son. Yes. No problem. Uh, okay. Do you, I'm just going to ask some questions just to rule out every other thing. Do you have headaches? No. Do you have chest pain? I know, doctor. I thought no. Do you have an abdominal pain? Do you have an abdominal pain? You have any change in your bowel habits? I don't know how to answer that. I think that is fine. Your urine, your urine, has it changed in quantity? No, not at all. How about the frequency of urination? Has it changed? No, no. Do you have any bone pain? No. So um thank you for for answering my questions. Those questions are basically there so that we can pinpoint where and where there is a problem and then can also come to have differential diagnosis of what could be the cause of your symptoms and they would like to examine you right check your level of hydration, check your um general um physical appearance to see whether you you and access your general health. We also like to do an abdominal examination, right, to also give us more information on the abdominal pain you're having, if it could lead us to what is causing the symptoms you're having, the abdominal pain and the, the stooling. Do you understand? Yes, yes. Although, although it seems like what you ate, the restaurants you got food from, there must have been where you got um some uh so infection which could have which could have caused the diarrhoea you want to say something yeah so what exactly is drawn what exactly is wrong what exactly is the cause it's it's just the food poisoning by the food poisoning but however we are going to have to evaluate you and find out what exactly is the cause so we are going to do some really series of tests i'm going to check your blood count to see if there's some infection be gastritis. We want to do your um erythrocyte sedimentation rate to know if there's any any any type kind of inflammatory disorder that could cause diarrhoea like inflammatory bowel disease right and they would also want to do is to culture microscopy and sensitivity and to look out for um parasites and some bacteria that could cause you to be having diarrhoea and also check your um retroviral status to know if uh uh your abdominal viral disease which could also be a cause of um of diarrhoea or do that comes in a chronic um a chronic um setting however we would also need to just rule that out do you understand okay doctor okay however we are going to start you on on some some fluids to uh you know give you some strength and restore your hydration level because you've been losing some fluid from um this tooling and the vomiting we also check your electrolytes electrolytes to know what your electrolyte picture looks like and the ones that will be needed to be that will need to be corrected do you understand and also lastly we would also want to check do an abdominal scan to rule out any structural or functional problems that could be in the abdomen which could be causing the diarrhoea and then the the abdominal pain do you understand yes thank you doctor thank you very much yes do you have any more questions for me I'm fine, I'm fine, I'm good. Let's just get on with it. So, yeah, so that can be fine. Thank you. So, you've been attended to. Alright, thank you very much, doctor.</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Would you mind by starting with what brought you in? Yeah, so over the last week, I've just been feeling some symptoms of, so it kind of first started with just like I had like a runny nose. And then, so that was around like five days ago. And then it turned into just a lot of congestion, like nose and my throat. And now over the last two days, I've been just feeling so much pressure around my nose, around my jaw. So I've been getting a lot of pain there as well. Okay. your nose still running yeah i'm still getting some discharge and i also feel like i'm getting some dripping at the back of my throat too especially when i wake up okay um and uh could you describe the the discharge is it clear yellow yellow, greenish? It's fairly clear and sometimes a bit white, but it's not green or yellow. Okay. And have you felt that it's difficult to breathe through either of your nostrilsrils like it's uh obstructed yeah so i at night sometimes i have to like um turn because one side of my nose gets uh difficult to breathe from and then it kind of balances around the other side so i do have some obstruction okay and uh have you had any changes to your sense of smell I don't know. have some obstruction. Okay. And have you had any changes to your sense of smell? Yeah. So just in the last three days when the congestion got really bad, I started losing the ability to smell. Okay. Have you had any changes to your sense of taste no taste is fine okay and have you had any cough or sore throat uh no no cough or sore throat okay um and the symptoms have gone on for five days. Have you had a period of time where you got better and then got sick again? I did. I did kind of have a runny nose last week as well. So probably like eight days ago. And but the runny nose has continued a little bit, but really got worse five days ago. But all these other symptoms just happened in the last few days. Okay. And you have pain. Is it you feel it in your jaw or do you feel it in the front of your nose?, so I would say mainly over the cheeks. It can kind of go near the front of my teeth as well. So, like, I would say, like, mostly around the cheeks, jaws and up to the front of my teeth. Okay. And do you grind your teeth at all at night or have you had like TMJ issues before? No, nothing like that. I think it's not so more like on and around my teeth. It's more so just right below my nose, above my teeth and just around my cheeks. Okay. So no pain in your mouth or anything like that? No, not inside my mouth. Okay. Have you had any fevers or chills? I don't think I've had a fever. I did feel some chills over the last few days, but just very brief episodes. Okay. And over the last few weeks, have you had any weight loss? No. Okay. And so you didn't have a cough or a sore throat, but have you had any wheezing? No wheezing. How about any shortness of breath um not shortness of breath just sometimes when my nose gets like really congested it's i i just i just turn into like a mouth breather but that's about it i see okay and have you had um any uh chest pain no no chest pain. All right. And any lightheadedness or feeling dizzy? No. Okay. Have you had any nausea or vomiting? Nope. Any abdominal pain? Nope. Have you had any diarrhea? Sorry, what was that? Have you had any diarrhea? No diarrhea. Okay. And have you had any urinary problems? No. And have you had any rashes or skin changes? No, not that I know of. Okay. And then how um any muscle aches or joint aches uh nope okay um and uh have you any muscle weakness no and how's your energy been have you any had any fatigue? It's been mainly okay. Just maybe sometimes difficult to get to sleep with all the congestion. But I don't think my energy's been affected too much, no. Okay. And sorry to go back to this. I don't think I asked. Did you notice any discharge from your eyes or any eye redness? Not discharge, but yeah, maybe a little bit of redness. Okay. Have your eyes been itchy? Yeah, a little bit. I would say they have been a bit itchy. Okay. All right. Do you have any medical conditions that you see a physician for regularly? Just I have, what's it called? It's called high, like dyslipidemia. Okay, I see. And any medications you take for that? Just like a statin medication. Okay. Do you take any other medications over the counter prescribed? No, just other than that, I take multivitamins. Okay. And do you have any allergies to medications or maybe like environmental allergies that might be getting worse? No, not that I know of. Okay. So you don't experience any symptoms like this when the seasons change? I don't think so. I have had this happen to me I would say like once before. It happened like two years ago. Yeah. It was pretty similar. Okay. And did you have any, what was done at that time? At that time, it kind of just went away on its own. It got better. Like, I feel it's definitely worse this time. But at that time, I didn't even go to the doctor. I kind of just went away. Okay. I see. Any reasons for hospitalizations? No hospitalizations. No. Any surgeries? Nope. All right. And could you tell me whereabouts you're living currently and who you're living with? Yeah, so I'm currently living in an apartment by myself in just outside of London. Okay. And anybody that you've been around who's had any symptoms? No, not that I know of. Okay, so no sick contacts. And have you traveled anywhere out of the city or province? No, I've tried to stay home. Besides going to work, I just work at the grocery store um besides that nowhere else okay and anybody any of your co-workers have any symptoms or any co-workers been off sick no we're pretty careful right now with the pandemic i see yeah no that that's great um Okay, and do you smoke cigarettes? No. I see yeah no that that's great um okay and uh do you smoke cigarettes no uh I quit just a couple years ago oh that's great um all right it's not yeah it's not easy to quit so that's awesome um and uh do you drink alcohol uh just, just, uh, maybe like, uh, red wine a couple of times a week. I see. Okay. And do you use any recreational drugs? Um, just in a month, maybe once or twice I smoke a joint. Okay. And anybody in the family have any lung or heart conditions? No, not that I know of. All right. And how about any cancer in the family? uh no no no cancers okay um i think uh that was everything i wanted to ask about today um was there any other symptoms or um anything else that that you wanted to make sure i knew about today uh no i think that's all i i just didn't know if i needed I needed any medications or if I needed to get tested. I just wanted to make sure. Yeah, so we'll certainly check your temperature to see if you have a fever. And if you do, and it's high enough, that will increase the chance that you have a bacterial sinusitis. And if so, with some of your symptoms, including the discharge, obstruction, loss of smell, and facial pain, that all fits the picture for it and also you you felt you had a period where you felt a little bit better and then worse again so that might require antibiotics but we will yeah check your temperature and go from there alright sounds good thank you so much thank you</t>
+          <t xml:space="preserve"> Okay, good afternoon. My name is Dr. Shadepo. Good afternoon. My name is Ms. Sharon. Yes. Okay, so do you have any complaints? Yes, doctor. I have been schooling for about about four days now and I've been abdominal pain too, alongside. So those are my two complaints. Okay. So which one started first, the stooling or the abdominal pain? The stooling started first about four days ago. okay so now like what is the consistency of the of this tool is he watery is he semi-solid or it's normal from well from the stores it's very watery very watery very much yes okay all right so like how many episodes of um you said you've been still in for over four days right yes and how many episodes do you you have for the of student anyways about six or six to seven episodes actually about around that of passage of what is to yes yes yes. Yes, doctor. Okay. Okay, so is the stool containing mucous? Is it mucoid? No. No. No, it's not mucous. No mucous in it. Was there any blood in it? No blood at all. There was no blood in it. Okay. Did from a new restaurant or did you eat something different? Actually, a few days ago, just before it started, I had a takeout in a restaurant with my family, which was all heads. And one of my children actually vomitedited but the vomiting stopped and it feels good now so it's just me right now with the complaints i have of the of the loose yes i i vomited about two episodes but two times yes yes. What was inside the vomit? What was the components of the vomit? Was it what you ate? Or was it greenish? Or was there blood in it? No, there was no blood. It was just the contents of what I ate. Was the vomiting, was it projectile? So what do you mean by projector um when it comes with force when it comes with force well i really don't know i just i just wanted to tell so like i can't really remember how it came out to be honest okay was there any is there any abdominal distension? Distension like swelling? Swelling, yeah. Was there swelling in your stomach? No. Just the muscle. Is there any abdominal distension? Distension like swelling? Swelling, yeah. Was there swelling in your stomach? No, just abdominal pain. The pain is just at the lower part of my stomach. Okay. Alright, alright. Thank you. So you said your son also ate the same food that you bought and he's now vomiting. How is he feeling now? He feels he's okay. After the episode of vomiting, he got well and he's okay. How is your appetite like? My appetite is here and there. No, it's not really good. Like before. Okay. So let's talk about the pain you were having. So can you describe the pain for me? What's the nature of the pain? Is it a sharp pain? Or a pain that holds you and needs you? What kind of pain is it? I'll describe it as a cramp pain. Like the pain I feel do you want me to show so that's a kind of pain is it i'll describe it like like as a cramp pain like it's been a few during menstruation so that's the kind of pain like that's the way i can describe it and where is this pain located in your abdomen the lower part the lower part does this pain does it move to another part of your body where you start feeling it no just back just go back no it stays in the same space yes yes okay okay so what what do you think makes this pain worse well maybe if i if i don't eat i don't know if i don't eat here maybe don't know. If I don't eat, yeah, maybe something around that. Yeah. But I don't feel like if it just comes and goes, I don't feel like there's anything that makes you to want to say. But I would say maybe if I don't eat. Yes. Okay. What relieves the pain? I'm not saying, I don't know. I didn't know when you said that it would he said that it just comes and goes on this one. Okay so on a scale of zero to ten let's say zero means that you don't have any pain at all and ten is the worst pain you've felt in your life so what would you give this pain? I'll give the pain like five out of ten. Five 5 over 10? Yes. No problem. So let's take some history. Are you hypertensive? No, I'm not. Are you diabetic? No, I'm not. Are you a non-peptic cause a patient? No. Are you lactose intolerant? No. I don't like to be treated. Are you a non-peptic ulcer patient? No. Are you lactose intolerant? No. The only ailment I've been treated for is asthmatic. And I use inhalers. How many exhibitions do you have in a year? Last one. Just one. Okay one okay, that's good have you had any previous history of blood transfusion? any history of surgeries? no, none at all do you drink alcohol or do you smoke? no, I don't do any of those. I don't. And since you've been feeling these symptoms that you're having, has it progressively worsened? Yeah, I feel so. So that's why I actually came to the hospital yesterday to see the doctor and Probably know what's wrong with me and take care of it, basically. Have you been feeling very thirsty? Have you been feeling like your body is dry? Has your urine reduced? No, not at all. No, no. Do you feel weak? Yeah, I feel kind of weak, yeah. When I feel something, my mouth is kind of dry too, kind of. Okay, okay. No problem. So, do you, aside the asthma, do you have any other ailments that you think the doctor should know about? No, not at all, at all. I have no other medical condition. Do you have any drug allergies? No, I don't react to any drugs at all. Are you married? Yes, I'm married with two kids. Do you live with your husband? Yes, I do. Are your kids living with you? Yes, what did you say, doctor? And your kids live with you as well? Yes, they are. So aside your son or your child who are the vomitting, was there any of your family members that also had the same symptoms? No, no, no, no, dad. Just me and my son, yes. Okay. Okay. I'm just going to ask some questions just to realize every other thing. Do you have headaches? No. Do you have chest pain? No, doctor. I don't know. Do you have an abdominal pain? Do you have an abdominal pain? Do you have any change in your bowel habits? I don't know how to answer that. I think that is fine. Your urine, has it changed in quantity? No, not at all. How about the frequency of urination? Has it changed? No, no. Urination is fine. Do you have any bone pain? No. All right, no problem. So, thank you for answering my questions. Those questions are basically there so that we can pinpoint where there is a problem. And you can also come to have a differential diagnosis of what could be the cause of your symptoms. And I would like to examine you, check your level of hydration, check your general physical appearance, see whether you can access your general health. We also like to do an abdominal examination, right? To also give us more information on the abdominal pain you're having, if it could lead us to what is causing the symptoms you're having, the abdominal pain and the stooling. Do you understand? Yes. Although it seems like what you ate, the restaurants you got food from, they must have been where you got some infection. It could have caused the diarrhea. You want to say something? So what exactly is drunk? What exactly is drunk? It's just the food I ate, right? Yeah, it looks like you've had a food poisoning. However, we are going to have to evaluate you and find out what exactly is the cause. So we are going to do some very serious tests. I'm going to check your blood count to make sure there's some infection I don't know. to evaluate you and find out what exactly is the cause so we are going to do some very series of tests i'm going to check your blood count to make this there's some infection which could be gastroenteritis you want to do your um erythrocyte segmentation rate to know if there's any any type of kind of inflammatory disorder that could cause diarrhea like inflammatory disease right And they would also want to do a stool culture microscopy and sensitivity to look out for parasites and some bacteria that could cause you to be having diarrhea. We also check your retroviral status to know if you have a retroviral disease, which could also be a cause of diarrhea. Although that comes in a chronic setting, however, we would also need to just rule that out. Do you understand? Okay, doctor, okay. However, we are going to start you on some fluids to give you some strength and restore your hydration level because you've been using some fluid from this tooling and the vomiting. We also check your electrolytes, electrolytes to know what your electrolyte picture looks like and the ones that will be needed to be, that will need to be corrected. Do you understand? And also lastly, we also want to do an abdominal scan to rule out any structural or functional problems that could be in the abdomen, which could be causing the diarrhea and the abdominal pain. Do you understand? Yes, thank you, doctor. Thank you very much. Do you have any more questions for me? No, I'm fine. I'm fine. I'm good. Let's just get out of here. So I can be fine. Thank you. So you'll be attended to. Alright, thank you very much.</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> would you mind by starting with what brought you in  yeah so over the last week i have just been feeling some symptoms it kind of first started with like a runny nose that was around like five days ago and then it turned into just a lot of congestion like around my nose and like my throat and now over the last two days i have been just feeling so much pressure around my nose and around my jaw so i have been getting a lot of pain there as well  ok is your nose still running  yeah i am still getting some discharge and i also feel like i am getting some dripping at the back of my throat too especially when i wake up  ok and could you describe the discharge is it clear yellow greenish  uh its fairly clear and sometimes like a bit white but like its not like green or yellow  ok uh and have you felt that its difficult to breathe in through either of your nostrils like its obstructed  yeah so at night sometimes i have to like turn because one side of my nose gets difficult to breathe from and then it kind of balances out on the other side so yeah i do have some obstruction  ok and have you had any changes to your sense of smell  yeah so just in the last three days when the congestion got really bad i started losing the ability to smell  ok have you had any changes to your sense of taste  no taste is fine  ok and have you had any cough or sore throat  uh no no cough or sore throat  ok and the symptoms have gone on for five days have you had a period of time where you got better and then got sick again  i did kind of have a runny nose last week as well so probably like eight days ago but then the runny nose discontinued a little bit but really got worse five days ago but all these other symptoms just happened in the last few days  ok and you have pain do you feel it in your jaw or do you feel it in the in the front of your nose  yes i would say mainly over the cheeks it can kind of go near the front of my teeth as well so like i would say like mostly around the cheeks jaws and up to the front of my teeth  ok and do you grind your teeth at all at night or have you had tmj issues before  no nothing like that i think its not so much on and around my teeth its more so just to right below my nose above my teeth and just around my cheeks  ok so no pain in your mouth or anything like that  no not inside my mouth  ok have you had any fevers or chills  uhm i do not think i have had a fever i did feel some chills over the last few days but just very brief episodes  ok and over the last few weeks have you had any weight loss  no  ok and you said you did not have a cough or a sore throat but have you had any wheezing  no wheezing  how about any shortness of breath  uh not shortness of breath just sometimes when my nose gets like really congested i just turn into like a mouth breather but that is about it  i see ok and have you had any chest pain  no no chest pain  alright and any lightheadedness or feeling dizzy  no  ok have you had any nausea or vomiting  nope  any abdominal pain  no  have you had any diarrhea  sorry what was that  have you had any diarrhea  no diarrhea  ok and have you had any urinary problems  uh no  and have you had any rashes or skin changes  no not that i know  ok then how about any muscle aches or joint aches  uh no  ok and have you had any muscle weakness  no  and how has your energy been any fatigue  uhm its been mainly ok just maybe sometimes difficult to get to sleep with all the all the congestion but i do not think my energy has been affected too much no  ok and uh sorry to go back to this i do not think i asked did you notice any discharge from your eyes or any eye redness  not discharge but yeah maybe a little bit of redness  ok have your eyes been itchy  uhm yeah a little bit i would say they have been a bit itchy  ok alright then do you have any medical conditions that you see a physician for regularly  uh just uhm its called dyslipidemia  ok i see and any medications you take for that  just like a statin medication  ok do you take any other medications over the counter prescribed  no other than that i take multivitamins  ok and do you have any allergies to medications or like environmental allergies that might be getting worse  uh no not that i know  ok so you do not experience any symptoms like this when the seasons change  i do not think so i have had this happen to me uh i would say like once before it happened like two years ago it was pretty similar  ok uhm and what was done at that time  at that time it kind of just went away on its own it got better i feel its definitely worse this time but at that time i did not even go to the doctor it kind of just went away  ok i see any recent hospitalizations  no hospitalizations  any surgeries  nope  alright and could you tell me where abouts you are living currently and who you are living with  yeah so i am currently living in an apartment by myself just outside of london  ok and anybody that you have been around who is had any symptoms  uh no not that i know of  ok so no sick contacts and have you traveled anywhere out of the city or province  no i have tried to stay home besides going to work i just work at the grocery store besides that no nowhere else  ok and any of your coworkers have any symptoms or any coworkers being off sick  no were pretty careful right now with the pandemic  i see yeah that is great ok and do you smoke cigarettes  no i quit just a couple of years ago  oh that is great its not easy to quit so that is awesome and do you drink alcohol  just maybe like red wine a couple of times a week  i see ok and do you use any recreational drugs  uh just in a month maybe once or twice i smoke a joint  ok uh and anybody in the family have any lung or heart conditions  no not that i know of  alright and how about any cancer in the family  uh no no cancers  ok i think i that was everything i wanted to ask about today was there any other symptoms or anything else that you wanted to make sure i knew about today  no i think that is all i just did not know if i needed any like medications or if i needed to get tested i just wanted to make sure  yeah so well certainly check your temperature to see if you have a fever and if you do and its high enough that will increase the chance that you have a bacterial sinusitis and if so with some of your symptoms including the discharge obstruction loss of smell and facial pain that all fits the picture for it and also you had a period where you felt a little bit better and then worse again so that might require antibiotics but we will check your temperature and go from there  alright sounds good thank you so much  thank you</t>
+          <t>Okay, good afternoon. My name is Dr. Shadiko. Yeah, good afternoon. Yeah, good afternoon. My name is Miss Sharon. Yes. Okay. So do you have any complaints? Yes, Doctor. I have been stooling for about four days now and having abdominal pain too alongside. So that's those are my two complaints. Okay. Okay. So which one started first? The stooling or the abdominal pain? Yeah, the stooling started first about four days ago. Okay. So now, like, what is the consistency of this tool? Is he watery? Is he semi-solid? Or it's a normal form, well-formed stool? It's very watery, very watery, very watchful. Yes. Okay. All right. So like, how many episodes of, you said you've been stooling for about four days, right? Yes. And how many episodes do you have per day of stooling? About six, about six to seven episodes, actually. About around that number. Yes. Of passage of watery stool. Yes, yes. Yes, doctor. Okay. Okay, so is this tool containing mucus? Is it mucoid? No. No, no, it's not mucus. No mucus. Was there any blood in it? No blood at all. There's no blood in it. Okay. Did you change, did you eat from a new restaurant or did you eat something different? Actually, a few days ago, I like just before I started, I actually had a takeout in a restaurant with my family, which all of us ate. And one of my child actually vomited, but the vomiting stopped and it feels good now. So it's just right now with the complaints I have of the loose. Yes, I've only said about two episodes. But two times, yes. Well, what was inside the vomit? What was the components of the vomiters? Was it what you ate, or was it greenish? Or was there blood in it? No, there was no blood. It was just the content of what I ate. Was the vomiting? Was it projectile? So what do you mean by projectile? When it comes with force, when it comes to force. Well, I really don't know. I just wanted to ask. I can't really remember how it came out, to be honest. Okay. Was there any, is there any abdominal distension? Distension, like a swelling? Swelling, yeah. Was there swelling in your stomach? No, just the abdominal pain. The pain is just at my lower part of my stomach. Okay. All right. All right. Thank you. So you said your son also bought and he's now vomiting. How is he feeling now? He feels he's okay. After the appearance of vomiting, he got well and it's okay. Okay. How is your appetite like? My appetite is here. Yeah. No, it's not really good. So now let's okay. Okay. So let's talk about, let's talk about your the pain you're having. So can you describe the pain for me? What's the what's the nature of the pain? Is it a sharp pain or a pain that holds you and leaves you? What kind of pain is it? I'll describe it like like as a cramp pain, like the pain I feel during my session. So that's the kind of pain. Like that's the way I can describe it. And where is this pain located in your abdomen? The lower part. The lower part. Does this pain, does it move to another part of your body when you start feeling it? No, just back. Just the lower part. No. Is this the same space? Yes, yes. Okay. So what do you think makes this pain worse? Maybe if I don't eat, I don't know. It's easier. Maybe something around that. Yeah. But I don't feel like if it just comes and goes, I don't feel like anything that makes it well, per se. But I would say maybe if I don't eat. Yes. Okay. What relieves the pain? Nothing. I don't know. I don't know if that just comes and goes on this one. Okay, so on a scale of zero to ten, let's say zero means that you don't have any pain at all. And 10 is the worst pain you felt in your life. So what would you give this pain? I'll give the pain like five or ten. Five over ten. Okay. No problem. So let's take some history. Are you hypertensive? No, I'm not. Are you diabetic? No, I'm not. Do you are you a non-peptic ulcer patient? No, no. Are you lactose in tolerant? No, the only aim I'm treating for, I have been treated for is asthma, my non-asmatic. And I am only, I use ALS. How many? How many examples do you have in a year? About last one, just one. Okay. Okay, that's good. Have you had any previous history of blood transfusion? Any history of surgeries? No, no, not at all. Okay. Do you drink alcohol or do you smoke? No, I don't. I don't do any of those. I don't have it at all. And since you've been feeling these symptoms that you're having, has it progressively worsened? Yeah, I feel so. So that's why I actually came to the hospital just today to see the doctor and probably know what's wrong with me and take care of it, basically. Have you been feeling very testy? Have you been feeling like your body is dry? Has your urine reduced? No, not at all. No, no. Do you feel weak? Yeah, I feel kind of weak. Yeah. Yeah. I feel sometimes my mouth is kind of dry to cut up. Okay. Okay. Okay, no problem. So do you have asides the asthma? Do you have any other ailments that you think the doctor should know about? No, not at all at all. I have no other medical condition. Do you have any drug allergies? No, I don't react at all. I don't react to any drugs at all. Are you married? Yes, I'm married. You took it. Yes. Okay. And you live with your husband? Yes, yes, I do. And your kids live with you? Yeah, what did you say, doctor? Are your kids live with you as well? Yes, they are. So asides your son or your child, who are the vomiting, was there any of your family members that also had the same symptoms? No, no, no, no, no, that's just me and just me and my son, yes. Okay, do you, I'm just going to ask some questions just to raise every other thing. Do you have headaches? No. Not at all. Do you have chest pain? No, doctor, at all. No. Do you have an abdominal pain? Do you have an abdominal pain? Do you have any change in your dowel habits? Yeah, I don't know how to answer that. Other than the... Okay, I think that is fine. Your urine, has it changed in quantity? No, not at all. How about the frequency of urination? Has it changed? No, no. My initial. You have any bone pain? No. All right, no problem. So thank you for answering my questions. Those questions are basically there so that we can pinpoint where there is a problem. And then we can also come to have differential diagnosis of what could be the cause of your symptoms. And then we would like to examine you, right? Check your level of vibration, check your general physical appearance to see whether you can access your general health. We also like to do an abdominal examination, right? So also give us more information on the abdominal pain you're having. If you could lead us to what is causing the symptoms you have in the abdominal pain and the stooling. Do you understand? Yes, although, although it seems like what you ate, the restaurant you got food from, there must have been where you got some infection. You want to say something? So what exactly is drug? What exactly is wrong? What exactly is the cause? Okay, it's just the food I had, right? Yeah, it looks like you've had a food poisoning or the food poisoning, but however, we are going to have to evaluate you and find out what exactly is the cause. So we are going to do some very serious tests. I'm going to check your blood count to make there's some infection, which could be a gastroenteritis. We want to do your erythrocyte sedimentation rate to know if there's any type of kind of inflammatory disorder that could cause diarrhea, like inflammatory disease, right? And then we would also want to do a stool culture microscopy and sensitivity to look out for parasites and some bacterias that could cause you to be having diarrhea. We also check your retroviral status to know if you have a retroviral disease, which could also be a cause of diarrhea, although that comes in a chronic, chronic setting. However, I would also need to just rule that out. Do you understand? Okay, doctor. Okay. However, we are going to start you on some foods to give you some strength and restore your hydration level because you've been losing some fluid from the stooling and the vomiting. We also check your electrolyte electrolytes to know what your electrolyte picture looks like and the ones that will be needed to be, that would need to be corrected. Do you understand? And also lastly, we also want to check do an abdominal scan to rule out any structural or functional problems that could be in the abdomen, which could be causing the diarrhea and the abdominal pain. Do you understand? Yes, thank you, Doctor. Thank you very much. Yes. Do you have any more questions for me? I'm fine. I'm fine. I'm good. Let's just get on with it. Thank you. So you'll be attended to. All right. Thank you very much, Dr.</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>would you mind by starting with what brought you in yeah so over the last week i have just been feeling some symptoms of so it kind of first started with just like i had like a runny nose and then so that was around like five days ago and then it turned into just a lot of congestion like nose and my throat and now over the last two days i have been just feeling so much pressure around my nose around my jaw so i have been getting a lot of pain there as well okay your nose still running yeah i am still getting some discharge and i also feel like i am getting some dripping at the back of my throat too especially when i wake up okay um and uh could you describe the the discharge is it clear yellow yellow greenish its fairly clear and sometimes a bit white but its not green or yellow okay and have you felt that its difficult to breathe through either of your nostrilsrils like its uh obstructed yeah so i at night sometimes i have to like um turn because one side of my nose gets uh difficult to breathe from and then it kind of balances around the other side so i do have some obstruction okay and uh have you had any changes to your sense of smell i do not know have some obstruction okay and have you had any changes to your sense of smell yeah so just in the last three days when the congestion got really bad i started losing the ability to smell okay have you had any changes to your sense of taste no taste is fine okay and have you had any cough or sore throat uh no no cough or sore throat okay um and the symptoms have gone on for five days have you had a period of time where you got better and then got sick again i did i did kind of have a runny nose last week as well so probably like eight days ago and but the runny nose has continued a little bit but really got worse five days ago but all these other symptoms just happened in the last few days okay and you have pain is it you feel it in your jaw or do you feel it in the front of your nose so i would say mainly over the cheeks it can kind of go near the front of my teeth as well so like i would say like mostly around the cheeks jaws and up to the front of my teeth okay and do you grind your teeth at all at night or have you had like tmj issues before no nothing like that i think its not so more like on and around my teeth its more so just right below my nose above my teeth and just around my cheeks okay so no pain in your mouth or anything like that no not inside my mouth okay have you had any fevers or chills i do not think i have had a fever i did feel some chills over the last few days but just very brief episodes okay and over the last few weeks have you had any weight loss no okay and so you did not have a cough or a sore throat but have you had any wheezing no wheezing how about any shortness of breath um not shortness of breath just sometimes when my nose gets like really congested its i i just i just turn into like a mouth breather but that is about it i see okay and have you had um any uh chest pain no no chest pain all right and any lightheadedness or feeling dizzy no okay have you had any nausea or vomiting nope any abdominal pain nope have you had any diarrhea sorry what was that have you had any diarrhea no diarrhea okay and have you had any urinary problems no and have you had any rashes or skin changes no not that i know of okay and then how um any muscle aches or joint aches uh nope okay um and uh have you any muscle weakness no and how is your energy been have you any had any fatigue its been mainly okay just maybe sometimes difficult to get to sleep with all the congestion but i do not think my energys been affected too much no okay and sorry to go back to this i do not think i asked did you notice any discharge from your eyes or any eye redness not discharge but yeah maybe a little bit of redness okay have your eyes been itchy yeah a little bit i would say they have been a bit itchy okay all right do you have any medical conditions that you see a physician for regularly just i have what is it called its called high like dyslipidemia okay i see and any medications you take for that just like a statin medication okay do you take any other medications over the counter prescribed no just other than that i take multivitamins okay and do you have any allergies to medications or maybe like environmental allergies that might be getting worse no not that i know of okay so you do not experience any symptoms like this when the seasons change i do not think so i have had this happen to me i would say like once before it happened like two years ago yeah it was pretty similar okay and did you have any what was done at that time at that time it kind of just went away on its own it got better like i feel its definitely worse this time but at that time i did not even go to the doctor i kind of just went away okay i see any reasons for hospitalizations no hospitalizations no any surgeries nope all right and could you tell me whereabouts you are living currently and who you are living with yeah so i am currently living in an apartment by myself in just outside of london okay and anybody that you have been around who is had any symptoms no not that i know of okay so no sick contacts and have you traveled anywhere out of the city or province no i have tried to stay home besides going to work i just work at the grocery store um besides that nowhere else okay and anybody any of your coworkers have any symptoms or any coworkers been off sick no were pretty careful right now with the pandemic i see yeah no that that is great um okay and do you smoke cigarettes no i see yeah no that that is great um okay and uh do you smoke cigarettes no uh i quit just a couple years ago oh that is great um all right its not yeah its not easy to quit so that is awesome um and uh do you drink alcohol uh just just uh maybe like uh red wine a couple of times a week i see okay and do you use any recreational drugs um just in a month maybe once or twice i smoke a joint okay and anybody in the family have any lung or heart conditions no not that i know of all right and how about any cancer in the family uh no no no cancers okay um i think uh that was everything i wanted to ask about today um was there any other symptoms or um anything else that that you wanted to make sure i knew about today uh no i think that is all i i just did not know if i needed i needed any medications or if i needed to get tested i just wanted to make sure yeah so well certainly check your temperature to see if you have a fever and if you do and its high enough that will increase the chance that you have a bacterial sinusitis and if so with some of your symptoms including the discharge obstruction loss of smell and facial pain that all fits the picture for it and also you you felt you had a period where you felt a little bit better and then worse again so that might require antibiotics but we will yeah check your temperature and go from there alright sounds good thank you so much thank you</t>
+          <t>okay good afternoon my name is doctor sadeko yeah good afternoon how may i help you yeah good afternoon my name is miss sharon  yes okay so do you have any complaints yes doctor i have been stooling for about four days now and i have been abdominal pain two alongside so that is those are my two complaints okay okay so which one started first the stooling or the abdominal pain yeah the stooling started first about four days ago okay so now like what is the consistency of the of the stool is it watery is he semi solid or it is in normal form well formed stools it is very watery very watery very watery yes okay all right so like how many episodes of  you said you have been stolen for over four days right yes and how many episodes do you do you have per day of stooling my about six about six to seven episodes actually about around that of passage of watery stool yes yes yes doctor okay okay so  is the stool containing mucus is it mucoid no no there is no mucus no mucus in it was there any blood in it no blood at all there is no blood in it okay did you change did you eat a from a new restaurant or did you did you eat something different ermactually a few days ago i like just before it started i actually had a take out in a restaurant with my family which all of us ate and  one of my child actually vomited but vomiting stopped and he feels good now so it is just me right now with the complaints i have of the of the loose stool are you also vomiting yes ii vomited about two two episodes about two times yes what what what what was inside the vomit what was the components of the vomitus was it what you ate or was it greenish or was there blood in it no there was no blood it was just the content of what i ate was the vomiting was it projectile so what do you mean by projectile ermwhen it comes with force when it comes with force well i really do not know it just i just vomited that is all i i cannot really remember how you came out to be honest okay was there any is there any abdominal distension distension like a swelling swelling yeah was there swelling in your stomach no just the abdominal pain the pain is just at my the lower part of my stomach okuhm all right all right thank you so you said your son also ate ate the same the same food that you bought and he is now vomiting how is he feeling now he feels he is okay he after the episode of vomiting he he got he got well and he is okay how is your appetite like my appetite is is here and there know it is not really good like so now let us okay okay so let us talk about let us talk about your the pain you were having so can you describe the pain for me what is the what is the nature of the pain is it a sharp pain or a pain that holds you and leaves you whatwhat kind of pain is it yeah i will describe it like like has a cramp pain like the pain i feel during menstruation so that is the kind of pain like that is the way i can describe it and where where is this pain located in your abdomen the lower part the lower part does this pain does it move to another part of your body when you start feeling it no just just the lower part of my like moving to the back just the lower part it does not move to your back no no not at all it stays in the same space yes yes okay okay so what what do you think makes this pain worse well maybe if i if i do not eat i do not know if i do not eat something around that yeah but i do not feel like if it just comes and goes i do not feel like anything that makes it worse per se but i will say maybe if i do not eat yes okay what what what relieves the pain  nothing i do not know i do not know anything that reduce the pain it just comes and goes on its one okay so on a scale of zero to ten let us say zero means that you do not have any pain at all and ten is the worst pain you have felt in your life so what would you give this pain i will the pain like five or ten five  ten yes no problem so  let us yeah take some history do you have are you hypertensive no i am not are you diabetic no i am not do you are you a known peptic also patient no no are you lactose intolerant no the only the only ailment i am being treated for i am being treated for is asthma i am a known asthmatic and and i am on i use inhalers and how many how many exacerbations do you have in a year about in the last one just one okay okay that is good have you had any previous history of blood transfusion any history of surgeries no no none at all okay   do you drink alcohol or do you smoke no i do not i do not do any of those i do not at all and since you have been feeling these symptoms that you are having has has it progressively worsened yeah i i feel so so that is why i actually came to the hospital just today to see the doctor and properly know what is wrong with me and take care of it basically have you been feeling very thirsty have you been feeling like your body is dry has your urine reduced no not at all no no do you feel weak yeah i feel kind of weak yeah yeah my my i feel sometimes my mouth is kind of dry to kind of okay okay okay no problem so do you asides the asthma do you have any other ailments you think the doctor should know about no not at all at all i have no other no other medical condition do you have any drug allergies no i do not react no at all i do not react to any drugs at all okay please are you married yes i am married with two kids  yes okay and you you live with your husband yes yes i do and your kids live with you yeah what did you say doctor and your kids live with you as well yes they are so aside your your son or your child who had the the vomiting was there any any of your family members that also had the same symptoms no no no no no other just me just me and my son yes okay no problem okay do you i am just going to ask some questions just to rule out every other thing do you do you have headaches no doctor do you have chest pain no doctor at all no do you have an abdominal pain oh do you you have an abdominal pain do you have any change in your bowel habits  i do not know how to answer that other than the just the  the okay i think i think i think that is fine your urine your your urine has it has it changed in quantity no not at all how about the frequency of urination has it changed no no my urination is fine do you have any do you have any bone pain no all right no problem so ermthank you for for answering my questions those questions are basically there so that we can pinpoint where and where there is a problem and they can also come to have differential diagnosis of what could be the because of your symptoms and we would like to examine you right check your level of hydration check your general physical appearance to see whether you and access your your general health right we also like to do an abdominal examination right to to also give us more information on the abdominal pain you are having if you could lead us to what is causing the symptoms you are having the abdominal pain and the the stooling do you understand yes although although it seems like what you ate the restaurants you got food from there must have been where you got some infection which could have which could have caused the diarrhea you want to say something so what exactly is wrong what exactly is wrong what exactly is the because okay it is just the food i ate right so yeah it looks like you have had a food poisoning had a food poisoning but however we are going to have to evaluate you and find out what exactly is the because so we are going to do some very series of tests i am going to check your blood count to know if there is a there is some infection which could be gastroenteritis we want to do your erythrocyte sedimentation rates to know if there is any sign any any type of kind of inflammatory disorder that could cause diarrhea like inflammatory bowel disease right and then we would also want to do a stool culture microscopy and sensitivity and to look out for parasites and some bacteria that could cause you to be having diarrhea we also check your retroviral status to know if you have retroviral disease which could also be a because of of diarrhea although that comes in the chronic chronic setting however would also need to just rule that out do you understand okay doctor okay however we are going to start you on on some some fluids to you know give you some strength and restore your hydration level because you have been losing some fluid from from the stooling and the vomiting we will also check your electrolytes electrolytes to know what is your electrolyte picture looks like and the ones that will be needed to be that will that will need to be corrected do you understand okay and also lastly we would also want to check do an abdominal scan throughout any structural or functional problems that could be in the abdominal which would be could be causing the diarrhea and the the the abdominal pain do you understand yes thank you doctor thank you very much yes do you have any more questions for me no i am fine i am fine i am good let us just get on with it you are fine  yeah so that will be fine thank you so you will be attended to all right thank you very much doctor</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>would you mind by starting with what brought you in yeah so over the last week i have just been feeling some symptoms of so it kind of first started with just like i had like a runny nose and then so that was around like five days ago and then it turned into just a lot of congestion like around my nose and like my throat and now over the last two days i have been just feeling so much pressure around around my nose around my jaw so having having getting a lot of pain there as well okay is your nose still running yeah i am still getting some discharge and i also feel like i am getting some dripping at the back of my throat too especially when i wake up okay and could you describe the discharge is it clear yellow greenish its fairly clear and sometimes like a bit white but like its not like green or yellow okay and have you felt that its difficult to breathe in through either of your nostrils like its obstructed yeah so i at night sometimes i i have to like turn because one side of my nose gets difficult to breathe from and then it kind of balances around the other side so i do have some obstruction okay and have you had any changes to your sense of smell yeah so just in the last three days when the congestion got really bad i started losing the ability to smell okay have you had any changes to your sense of taste no taste is fine okay and have you had any cough or sore throat no no cough or sore throat okay and the symptoms have gone on for five days have you had a period of time where you got better and then got sick again again i did kind of have a runny nose last week as well so probably like eight days ago and but that the runny nose has continued a little bit but really got worse five days ago but all these other symptoms just happened in the last few days okay and you have pain is it you feel it in your jaw or do you feel it in the in the front of your nose or yes i would say mainly over the cheeks it can kind of go near the front of my teeth as well so i would say like mostly around the cheeks jaws and up to the front of my teeth okay do you grind your teeth at all at night or have you had tmj issues before no nothing like that i think its not so more like on and around my teeth its more so just right below my nose above my teeth and just around my cheeks okay so no pain in your mouth or anything like that no not inside my mouth okay have you had any fevers or chills i do not think i have had a fever i did feel feel some chills over the last few days but just very brief episodes okay and over the last few weeks have you had any weight loss no okay and so you did not have a cough or a sore throat but have you had any wheezing no wheezing how about any shortness of breath not shortness of breath just sometimes in my neck nose gets like really congested its i just i just turn into like a mouth breather but that is about it i see okay and have you had any chest pain no no chest pain all right and any lightheadedness or feeling dizzy no okay have you had any nausea or vomiting nope any abdominal pain no have you had any diarrhea sorry what was that have you had any diarrhea no diarrhea okay and have you had any urinary problems no and have you had any rashes or skin changes no not that i know of okay and then how about any muscle aches or joint aches no no okay and have you any muscle weakness no and how is your energy been have you any fatigue its been mainly okay just maybe sometimes difficult to get to sleep with all the congestion but i do not think my energys been affected too much okay and sorry to go back to this i do not think i asked did you have notice any discharge from your eyes or any eye redness not discharge but yeah maybe a little bit of redness okay have your eyes been itchy yeah a little bit i would say they have been a bit itchy okay all right then do you have any medical conditions that you see a physician for regularly just a i have what is it called its its called high like dyslipidemia okay i see and any medications you take for that just a like a statin medication okay do you take any other medications over the counter or prescribed no just other than that i take multivitamins okay and do you have any allergies to medications or maybe like environmental allergies that might be getting worse no not that i know of okay so you do not experience any symptoms like this when the seasons change i do not i do not think so i have had this happen to me i would say like once before it happened like two years ago yeah it was pretty similar okay and did you have any and what was done at that time at that time it kind of just went away on its own it got better like i feel its definitely worse this time but at that time i did not even go to the doctor i kind of just went away okay i see and have any reasons for hospitalizations no hospitalizations and no any surgeries nope alright and could you tell me whereabouts you are living currently and who you are living with yeah so i am currently living in an apartment by myself and just outside of london okay and anybody that you have been around who is had any symptoms no not that i know of okay so no sick contacts and have you traveled anywhere out of the city or province no i have tried to stay home i besides going to work i just work at the grocery store besides that nowhere else okay and anybody any of your coworkers have any symptoms or any coworkers been off sick no were pretty careful right now with the pandemic i see yeah no that is great okay and do you smoke cigarettes no i quit just a couple of years ago oh that is great its not easy to quit so that is awesome and do you drink alcohol just maybe like red wine a couple of times a week i see okay and do you use any recreational drugs just in a month maybe or twice i smoke a joint okay and anybody in the family have any lung or heart conditions no not that i know of all right and how about any cancer in the family no no no cancers okay i think that was everything wanted to ask about today was there any other symptoms or anything else that you wanted to make sure i knew about today no i think that is all i just did not know if i needed any medications or if i needed to get tested i just wanted to make sure yeah so well certainly check your temperature to see if you have a fever and if you do and its high enough that will increase the chance that you have a bacterial sinusitis with and if so with some of your symptoms including the discharge obstruction loss of smell and facial pain that all fits the picture for it and also you you felt you had a period where you felt a little bit better and then worse again so that might require antibiotics but we will check your temperature and go from there all right sounds good thank you so much thank you</t>
-        </is>
-      </c>
-      <c r="K4" t="n">
-        <v>0.1676602086438152</v>
-      </c>
-      <c r="L4" t="n">
+          <t>okay good afternoon my name is doctor shadepo good afternoon my name is ms sharon yes okay so do you have any complaints yes doctor i have been schooling for about about four days now and i have been abdominal pain too alongside so those are my two complaints okay so which one started first the stooling or the abdominal pain the stooling started first about four days ago okay so now like what is the consistency of the of this tool is he watery is he semisolid or it is normal from well from the stores it is very watery very watery very much yes okay all right so like how many episodes of  you said you have been still in for over four days right yes and how many episodes do you you have for the of student anyways about six or six to seven episodes actually about around that of passage of what is to yes yes yes yes doctor okay okay so is the stool containing mucous is it mucoid no no no it is not mucous no mucous in it was there any blood in it no blood at all there was no blood in it okay did from a new restaurant or did you eat something different actually a few days ago just before it started i had a takeout in a restaurant with my family which was all heads and one of my children actually vomitedited but the vomiting stopped and it feels good now so it is just me right now with the complaints i have of the of the loose yes i i vomited about two episodes but two times yes yes what was inside the vomit what was the components of the vomit was it what you ate or was it greenish or was there blood in it no there was no blood it was just the contents of what i ate was the vomiting was it projectile so what do you mean by projector  when it comes with force when it comes with force well i really do not know i just i just wanted to tell so like i cannot really remember how it came out to be honest okay was there any is there any abdominal distension distension like swelling swelling yeah was there swelling in your stomach no just the muscle is there any abdominal distension distension like swelling swelling yeah was there swelling in your stomach no just abdominal pain the pain is just at the lower part of my stomach okay alright alright thank you so you said your son also ate the same food that you bought and he is now vomiting how is he feeling now he feels he is okay after the episode of vomiting he got well and he is okay how is your appetite like my appetite is here and there no it is not really good like before okay so let us talk about the pain you were having so can you describe the pain for me what is the nature of the pain is it a sharp pain or a pain that holds you and needs you what kind of pain is it i will describe it as a cramp pain like the pain i feel do you want me to show so that is a kind of pain is it i will describe it like like as a cramp pain like it is been a few during menstruation so that is the kind of pain like that is the way i can describe it and where is this pain located in your abdomen the lower part the lower part does this pain does it move to another part of your body where you start feeling it no just back just go back no it stays in the same space yes yes okay okay so what what do you think makes this pain worse well maybe if i if i do not eat i do not know if i do not eat here maybe do not know if i do not eat yeah maybe something around that yeah but i do not feel like if it just comes and goes i do not feel like there is anything that makes you to want to say but i would say maybe if i do not eat yes okay what relieves the pain i am not saying i do not know i did not know when you said that it would he said that it just comes and goes on this one okay so on a scale of zero to ten let us say zero means that you do not have any pain at all and ten is the worst pain you have felt in your life so what would you give this pain i will give the pain like five out of ten five five over ten yes no problem so let us take some history are you hypertensive no i am not are you diabetic no i am not are you a nonpeptic because a patient no are you lactose intolerant no i do not like to be treated are you a nonpeptic ulcer patient no are you lactose intolerant no the only ailment i have been treated for is asthmatic and i use inhalers how many exhibitions do you have in a year last one just one okay one okay that is good have you had any previous history of blood transfusion any history of surgeries no none at all do you drink alcohol or do you smoke no i do not do any of those i do not and since you have been feeling these symptoms that you are having has it progressively worsened yeah i feel so so that is why i actually came to the hospital yesterday to see the doctor and probably know what is wrong with me and take care of it basically have you been feeling very thirsty have you been feeling like your body is dry has your urine reduced no not at all no no do you feel weak yeah i feel kind of weak yeah when i feel something my mouth is kind of dry too kind of okay okay no problem so do you aside the asthma do you have any other ailments that you think the doctor should know about no not at all at all i have no other medical condition do you have any drug allergies no i do not react to any drugs at all are you married yes i am married with two kids do you live with your husband yes i do are your kids living with you yes what did you say doctor and your kids live with you as well yes they are so aside your son or your child who are the vomitting was there any of your family members that also had the same symptoms no no no no dad just me and my son yes okay okay i am just going to ask some questions just to realize every other thing do you have headaches no do you have chest pain no doctor i do not know do you have an abdominal pain do you have an abdominal pain do you have any change in your bowel habits i do not know how to answer that i think that is fine your urine has it changed in quantity no not at all how about the frequency of urination has it changed no no urination is fine do you have any bone pain no all right no problem so thank you for answering my questions those questions are basically there so that we can pinpoint where there is a problem and you can also come to have a differential diagnosis of what could be the because of your symptoms and i would like to examine you check your level of hydration check your general physical appearance see whether you can access your general health we also like to do an abdominal examination right to also give us more information on the abdominal pain you are having if it could lead us to what is causing the symptoms you are having the abdominal pain and the stooling do you understand yes although it seems like what you ate the restaurants you got food from they must have been where you got some infection it could have caused the diarrhea you want to say something so what exactly is drunk what exactly is drunk it is just the food i ate right yeah it looks like you have had a food poisoning however we are going to have to evaluate you and find out what exactly is the because so we are going to do some very serious tests i am going to check your blood count to make sure there is some infection i do not know to evaluate you and find out what exactly is the because so we are going to do some very series of tests i am going to check your blood count to make this there is some infection which could be gastroenteritis you want to do your  erythrocyte segmentation rate to know if there is any any type of kind of inflammatory disorder that could cause diarrhea like inflammatory disease right and they would also want to do a stool culture microscopy and sensitivity to look out for parasites and some bacteria that could cause you to be having diarrhea we also check your retroviral status to know if you have a retroviral disease which could also be a because of diarrhea although that comes in a chronic setting however we would also need to just rule that out do you understand okay doctor okay however we are going to start you on some fluids to give you some strength and restore your hydration level because you have been using some fluid from this tooling and the vomiting we also check your electrolytes electrolytes to know what your electrolyte picture looks like and the ones that will be needed to be that will need to be corrected do you understand and also lastly we also want to do an abdominal scan to rule out any structural or functional problems that could be in the abdomen which could be causing the diarrhea and the abdominal pain do you understand yes thank you doctor thank you very much do you have any more questions for me no i am fine i am fine i am good let us just get out of here so i can be fine thank you so you will be attended to alright thank you very much</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>okay good afternoon my name is doctor shadekum good afternoon my name is miss sharon yes okay so do you have any complaints yes doctor i have been straining for about four days now and having abdominal pain alongside so that is just my two complaints okay okay so which one started first the stooling or the abdominal pain yeah the stooling started first about four days ago okay so now like what is the consistency of the of the stool is he watery is he semi solid or is it normal form well formed it is very watery very watery so like how many episodes of  you said you have been stalling for over four days right yes and how many episodes do you do you have per day of stalling about six or six to seven episodes actually about around that number yes of passage of the water riser tube yes yes yes doctor okay okay so   is this is it still containing mucus is it mucoid no no there is no mucus in it was there any blood in it no blood at all there is no blood in it okay did you change did you eat from a new restaurant or did you did you eat something different actually a few days ago just before you started i actually had the take out in a restaurant with my family which all was it and  all of my child actually vomited but the vomiting stopped and it feels good now so it is just right now with the complaint i have of the of the loose so are you also vomiting yes i i have vomited about two  two episodes about two times yes well what what was inside the vomit what was the con  components was it what you ate or was it greenish or was there blood in it no there was no blood it was just the contents of what i ate was the vomiting was it projectile so what do you mean by projectile when it comes with force when it comes with force well i really do not know i just i just want to tell you that is the line i cannot really remember how it came out to be honest is there any is there any abdominal distention distention like a swelling swelling yeah is there swelling in your stomach no just the abdominal pain the pain is just at my lower part of my stomach okay alright alright thank you so you said your son also ate ate the same the same food that you bought and is now vomiting how is he feeling now it feels it is okay after the he got he got well and it is okay how is your appetite like my appetite is yeah there no it is not really good like so now this like before okay okay so let us talk about let us talk about your the pain we are having so can you describe the pain for me what is the what is the nature of the pain is it a sharp pain or a pain that holds you and needs what kind of pain is it i would describe it as a camp pain like a pain i feel during menstruation so that is the kind of pain i can describe it and where is this pain located in your abdomen the lower parts the lower parts does this pain does it move to any other part of your body when you start feeling it no just the lower part of my abdomen the same space yes yes okay okay so what do you think makes this play worse well if i do not eat i do not know maybe something around that yeah but i do not feel like if it just comes and goes i do not feel like anything that makes it worse i say but i was saying if i do not eat yes okay what really how is the pain  not saying i do not know i do not know i just comes and goes on this one okay so on a scale of zero to ten let us say zero means that you do not have any pain at all and ten is the worst pain you felt in your life so what would you give this pain i would give this pain like five out of ten five out of ten no problem let us take some history do you are you hypertensive no i am not are you diabetic no i am not do you are you a nonpeptic ulcer patient no no are you lactose intolerant no the only the only payment i will be treating for is asthma i have been treated for is asthma i have nonasthmatic and i am on i use inhalers and how many recently how many exhibitions do you have in a year how about last one just one okay okay that was good have you had any previous history of blood transfusion any history of surgeries no no none at all okay do you drink alcohol or do you smoke no i do not i do not do any of those and since you have been feeling these symptoms that you are having as it progressively worsened yeah i feel so so that is why i actually came to the hospital just to see the doctor and properly know what is wrong with me and take care of it basically have you been feeling very thirsty have you been feeling like your bodys dry has your urine reduced no not at all no no do you feel weak yeah i feel kind of weak yeah yeah my mouth is kind of dry to kind of okay okay no problem so do you aside the asthma do you have any other ailments that you think the doctor should know about no not at all at all i have no other medical condition do you have any drug allergies no i do not react to any drugs at all are you married yes i am married with two kids  yes okay and you you live with your husband yes yes i do and your kids live with you yeah what did you say doctor and your kids live with you as well yes they are so aside your your son or your child who are the the vomit symptoms was there any any of your family members that also had the same symptoms no no no that just me and my son yes no problem  okay do you i am just going to ask some questions just to rule out every other thing do you have headaches no do you have chest pain i know doctor i thought no do you have an abdominal pain do you have an abdominal pain you have any change in your bowel habits i do not know how to answer that i think that is fine your urine your urine has it changed in quantity no not at all how about the frequency of urination has it changed no no do you have any bone pain no so  thank you for for answering my questions those questions are basically there so that we can pinpoint where and where there is a problem and then can also come to have differential diagnosis of what could be the because of your symptoms and they would like to examine you right check your level of hydration check your  general  physical appearance to see whether you you and access your general health we also like to do an abdominal examination right to also give us more information on the abdominal pain you are having if it could lead us to what is causing the symptoms you are having the abdominal pain and the the stooling do you understand yes yes although although it seems like what you ate the restaurants you got food from there must have been where you got  some  so infection which could have which could have caused the diarrhoea you want to say something yeah so what exactly is drawn what exactly is wrong what exactly is the because it is it is just the food poisoning by the food poisoning but however we are going to have to evaluate you and find out what exactly is the because so we are going to do some really series of tests i am going to check your blood count to see if there is some infection be gastritis we want to do your  erythrocyte sedimentation rate to know if there is any any any type kind of inflammatory disorder that could cause diarrhoea like inflammatory bowel disease right and they would also want to do is to culture microscopy and sensitivity and to look out for  parasites and some bacteria that could cause you to be having diarrhoea and also check your  retroviral status to know if   your abdominal viral disease which could also be a because of  of diarrhoea or do that comes in a chronic  a chronic  setting however we would also need to just rule that out do you understand okay doctor okay however we are going to start you on on some some fluids to  you know give you some strength and restore your hydration level because you have been losing some fluid from  this tooling and the vomiting we also check your electrolytes electrolytes to know what your electrolyte picture looks like and the ones that will be needed to be that will need to be corrected do you understand and also lastly we would also want to check do an abdominal scan to rule out any structural or functional problems that could be in the abdomen which could be causing the diarrhoea and then the the abdominal pain do you understand yes thank you doctor thank you very much yes do you have any more questions for me i am fine i am fine i am good let us just get on with it so yeah so that can be fine thank you so you have been attended to alright thank you very much doctor</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>okay good afternoon my name is doctor shadiko yeah good afternoon yeah good afternoon my name is miss sharon yes okay so do you have any complaints yes doctor i have been stooling for about four days now and having abdominal pain too alongside so that is those are my two complaints okay okay so which one started first the stooling or the abdominal pain yeah the stooling started first about four days ago okay so now like what is the consistency of this tool is he watery is he semisolid or it is a normal form wellformed stool it is very watery very watery very watchful yes okay all right so like how many episodes of you said you have been stooling for about four days right yes and how many episodes do you have per day of stooling about six about six to seven episodes actually about around that number yes of passage of watery stool yes yes yes doctor okay okay so is this tool containing mucus is it mucoid no no no it is not mucus no mucus was there any blood in it no blood at all there is no blood in it okay did you change did you eat from a new restaurant or did you eat something different actually a few days ago i like just before i started i actually had a takeout in a restaurant with my family which all of us ate and one of my child actually vomited but the vomiting stopped and it feels good now so it is just right now with the complaints i have of the loose yes i have only said about two episodes but two times yes well what was inside the vomit what was the components of the vomiters was it what you ate or was it greenish or was there blood in it no there was no blood it was just the content of what i ate was the vomiting was it projectile so what do you mean by projectile when it comes with force when it comes to force well i really do not know i just wanted to ask i cannot really remember how it came out to be honest okay was there any is there any abdominal distension distension like a swelling swelling yeah was there swelling in your stomach no just the abdominal pain the pain is just at my lower part of my stomach okay all right all right thank you so you said your son also bought and he is now vomiting how is he feeling now he feels he is okay after the appearance of vomiting he got well and it is okay okay how is your appetite like my appetite is here yeah no it is not really good so now let us okay okay so let us talk about let us talk about your the pain you are having so can you describe the pain for me what is the what is the nature of the pain is it a sharp pain or a pain that holds you and leaves you what kind of pain is it i will describe it like like as a cramp pain like the pain i feel during my session so that is the kind of pain like that is the way i can describe it and where is this pain located in your abdomen the lower part the lower part does this pain does it move to another part of your body when you start feeling it no just back just the lower part no is this the same space yes yes okay so what do you think makes this pain worse maybe if i do not eat i do not know it is easier maybe something around that yeah but i do not feel like if it just comes and goes i do not feel like anything that makes it well per se but i would say maybe if i do not eat yes okay what relieves the pain nothing i do not know i do not know if that just comes and goes on this one okay so on a scale of zero to ten let us say zero means that you do not have any pain at all and ten is the worst pain you felt in your life so what would you give this pain i will give the pain like five or ten five over ten okay no problem so let us take some history are you hypertensive no i am not are you diabetic no i am not do you are you a nonpeptic ulcer patient no no are you lactose in tolerant no the only aim i am treating for i have been treated for is asthma my nonasmatic and i am only i use als how many how many examples do you have in a year about last one just one okay okay that is good have you had any previous history of blood transfusion any history of surgeries no no not at all okay do you drink alcohol or do you smoke no i do not i do not do any of those i do not have it at all and since you have been feeling these symptoms that you are having has it progressively worsened yeah i feel so so that is why i actually came to the hospital just today to see the doctor and probably know what is wrong with me and take care of it basically have you been feeling very testy have you been feeling like your body is dry has your urine reduced no not at all no no do you feel weak yeah i feel kind of weak yeah yeah i feel sometimes my mouth is kind of dry to cut up okay okay okay no problem so do you have asides the asthma do you have any other ailments that you think the doctor should know about no not at all at all i have no other medical condition do you have any drug allergies no i do not react at all i do not react to any drugs at all are you married yes i am married you took it yes okay and you live with your husband yes yes i do and your kids live with you yeah what did you say doctor are your kids live with you as well yes they are so asides your son or your child who are the vomiting was there any of your family members that also had the same symptoms no no no no no that is just me and just me and my son yes okay do you i am just going to ask some questions just to raise every other thing do you have headaches no not at all do you have chest pain no doctor at all no do you have an abdominal pain do you have an abdominal pain do you have any change in your dowel habits yeah i do not know how to answer that other than the okay i think that is fine your urine has it changed in quantity no not at all how about the frequency of urination has it changed no no my initial you have any bone pain no all right no problem so thank you for answering my questions those questions are basically there so that we can pinpoint where there is a problem and then we can also come to have differential diagnosis of what could be the because of your symptoms and then we would like to examine you right check your level of vibration check your general physical appearance to see whether you can access your general health we also like to do an abdominal examination right so also give us more information on the abdominal pain you are having if you could lead us to what is causing the symptoms you have in the abdominal pain and the stooling do you understand yes although although it seems like what you ate the restaurant you got food from there must have been where you got some infection you want to say something so what exactly is drug what exactly is wrong what exactly is the because okay it is just the food i had right yeah it looks like you have had a food poisoning or the food poisoning but however we are going to have to evaluate you and find out what exactly is the because so we are going to do some very serious tests i am going to check your blood count to make there is some infection which could be a gastroenteritis we want to do your erythrocyte sedimentation rate to know if there is any type of kind of inflammatory disorder that could cause diarrhea like inflammatory disease right and then we would also want to do a stool culture microscopy and sensitivity to look out for parasites and some bacterias that could cause you to be having diarrhea we also check your retroviral status to know if you have a retroviral disease which could also be a because of diarrhea although that comes in a chronic chronic setting however i would also need to just rule that out do you understand okay doctor okay however we are going to start you on some foods to give you some strength and restore your hydration level because you have been losing some fluid from the stooling and the vomiting we also check your electrolyte electrolytes to know what your electrolyte picture looks like and the ones that will be needed to be that would need to be corrected do you understand and also lastly we also want to check do an abdominal scan to rule out any structural or functional problems that could be in the abdomen which could be causing the diarrhea and the abdominal pain do you understand yes thank you doctor thank you very much yes do you have any more questions for me i am fine i am fine i am good let us just get on with it thank you so you will be attended to all right thank you very much doctor</t>
+        </is>
+      </c>
+      <c r="M4" t="n">
+        <v>0.2667731629392971</v>
+      </c>
+      <c r="N4" t="n">
         <v>126</v>
       </c>
-      <c r="M4" t="n">
-        <v>34</v>
-      </c>
-      <c r="N4" t="n">
-        <v>65</v>
-      </c>
       <c r="O4" t="n">
-        <v>0.1192250372578241</v>
+        <v>216</v>
       </c>
       <c r="P4" t="n">
-        <v>67</v>
+        <v>159</v>
       </c>
       <c r="Q4" t="n">
-        <v>33</v>
+        <v>0.1964856230031949</v>
       </c>
       <c r="R4" t="n">
-        <v>60</v>
-      </c>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>['around', 'my', 'like', 'and', 'is', 'uh', 'like', 'like', 'like', 'uh', 'in', 'on', 'then', 'in', 'the', 'to', 'uhm', 'said', 'uh', 'had', 'uhm', 'all', 'the', 'has', 'uh', 'uhm', 'uh', 'uh', 'abouts', 'uh', 'no', 'of', 'uh', 'like']</t>
-        </is>
-      </c>
-      <c r="T4" t="inlineStr">
-        <is>
-          <t>['of', 'so', 'just', 'i', 'had', 'like', 'and', 'then', 'so', 'okay', 'uh', 'the', 'yellow', 'uh', 'i', 'um', 'uh', 'i', 'do', 'have', 'some', 'obstruction', 'okay', 'and', 'uh', 'have', 'you', 'had', 'any', 'changes', 'to', 'your', 'sense', 'of', 'not', 'know', 'okay', 'i', 'did', 'and', 'has', 'is', 'like', 'more', 'its', 'i', 'i', 'just', 'um', 'uh', 'all', 'of', 'okay', 'nope', 'uh', 'have', 'you', 'had', 'any', 'just', 'i', 'have', 'what', 'high', 'like', 'just', 'maybe', 'of', 'yeah', 'okay', 'and', 'did', 'like', 'reasons', 'no', 'all', 'in', 'um', 'anybody', 'no', 'that', 'um', 'see', 'yeah', 'no', 'that', 'that', 'is', 'great', 'um', 'okay', 'and', 'uh', 'do', 'you', 'smoke', 'cigarettes', 'no', 'uh', 'i', 'um', 'all', 'right', 'yeah', 'its', 'not', 'um', 'uh', 'uh', 'just', 'uh', 'uh', 'all', 'no', 'okay', 'um', 'um', 'that', 'uh', 'i', 'i', 'needed', 'you', 'felt', 'you', 'yeah']</t>
-        </is>
-      </c>
-      <c r="U4" t="inlineStr">
-        <is>
-          <t>['ok', 'ok', 'ok', 'nostrils', 'out', 'yeah', 'ok', 'ok', 'ok', 'ok', 'discontinued', 'ok', 'do', 'yes', 'ok', 'much', 'ok', 'ok', 'ok', 'ok', 'you', 'uh', 'ok', 'alright', 'ok', 'no', 'ok', 'ok', 'about', 'no', 'ok', 'has', 'ok', 'energy', 'ok', 'ok', 'ok', 'alright', 'then', 'uh', 'just', 'uhm', 'ok', 'ok', 'ok', 'ok', 'ok', 'uhm', 'and', 'it', 'ok', 'recent', 'alright', 'where', 'ok', 'ok', 'ok', 'being', 'ok', 'ok', 'uh', 'ok', 'alright', 'ok', 'i']</t>
-        </is>
-      </c>
-      <c r="V4" t="inlineStr">
-        <is>
-          <t>['and', 'been', 'uh', 'uh', 'on', 'yeah', 'uh', 'like', 'and', 'to', 'uhm', 'said', 'uh', 'uh', 'had', 'uhm', 'all', 'the', 'has', 'ok', 'uh', 'uhm', 'uh', 'uh', 'abouts', 'uh', 'no', 'uh', 'once', 'uh', 'i', 'i', 'like']</t>
-        </is>
-      </c>
-      <c r="W4" t="inlineStr">
-        <is>
-          <t>['of', 'so', 'just', 'i', 'had', 'like', 'and', 'then', 'so', 'around', 'i', 'i', 'again', 'and', 'has', 'is', 'or', 'more', 'feel', 'neck', 'its', 'i', 'just', 'all', 'of', 'okay', 'have', 'you', 'have', 'okay', 'just', 'a', 'i', 'have', 'what', 'its', 'high', 'like', 'a', 'or', 'just', 'maybe', 'of', 'i', 'do', 'not', 'yeah', 'okay', 'and', 'did', 'you', 'like', 'and', 'have', 'reasons', 'and', 'no', 'and', 'i', 'anybody', 'no', 'all', 'with', 'you', 'felt', 'you', 'all']</t>
-        </is>
-      </c>
-      <c r="X4" t="inlineStr">
-        <is>
-          <t>['i', 'have', 'ok', 'ok', 'ok', 'out', 'ok', 'ok', 'ok', 'ok', 'then', 'discontinued', 'ok', 'do', 'ok', 'much', 'ok', 'ok', 'ok', 'ok', 'you', 'when', 'ok', 'alright', 'ok', 'ok', 'ok', 'uh', 'ok', 'has', 'ok', 'energy', 'no', 'ok', 'ok', 'alright', 'uh', 'just', 'uhm', 'ok', 'ok', 'ok', 'ok', 'ok', 'uhm', 'it', 'ok', 'recent', 'where', 'ok', 'ok', 'ok', 'being', 'ok', 'ok', 'ok', 'alright', 'uh', 'ok', 'alright']</t>
-        </is>
+        <v>37</v>
+      </c>
+      <c r="S4" t="n">
+        <v>203</v>
+      </c>
+      <c r="T4" t="n">
+        <v>129</v>
+      </c>
+      <c r="U4" t="n">
+        <v>0.1730564430244941</v>
+      </c>
+      <c r="V4" t="n">
+        <v>25</v>
+      </c>
+      <c r="W4" t="n">
+        <v>195</v>
+      </c>
+      <c r="X4" t="n">
+        <v>105</v>
       </c>
       <c r="Y4" t="inlineStr">
         <is>
-          <t xml:space="preserve">      ref_ix  hyp_ix reference hypothesis operation  index_edit_ops
-0          0       0     would      would         =            &lt;NA&gt;
-1          1       1       you        you         =            &lt;NA&gt;
-2          2       2      mind       mind         =            &lt;NA&gt;
-3          3       3        by         by         =            &lt;NA&gt;
-4          4       4  starting   starting         =            &lt;NA&gt;
-...      ...     ...       ...        ...       ...             ...
-1463    1337    1429       you        you         =            &lt;NA&gt;
-1464    1338    1430        so         so         =            &lt;NA&gt;
-1465    1339    1431      much       much         =            &lt;NA&gt;
-1466    1340    1432     thank      thank         =            &lt;NA&gt;
-1467    1341    1433       you        you         =            &lt;NA&gt;
-[1468 rows x 6 columns]</t>
+          <t>['yeah', 'how', 'may', 'i', 'help', 'you', 'yeah', 'good', 'afternoon', 'that', 'is', 'okay', 'yeah', 'solid', 'in', 'do', 'you', 'change', 'did', 'you', 'eat', 'a', 'did', 'you', 'i', 'like', 'actually', 'out', 'us', 'ate', 'also', 'vomiting', 'yes', 'ii', 'two', 'what', 'what', 'a', 'my', 'all', 'right', 'ate', 'the', 'same', 'he', 'he', 'he', 'got', 'is', 'now', 'let', 'us', 'okay', 'let', 'us', 'talk', 'about', 'your', 'what', 'is', 'the', 'where', 'just', 'the', 'lower', 'part', 'of', 'my', 'like', 'moving', 'to', 'the', 'lower', 'part', 'it', 'does', 'not', 'move', 'to', 'your', 'no', 'not', 'at', 'all', 'what', 'what', 'yeah', 'do', 'you', 'have', 'do', 'you', 'no', 'am', 'being', 'about', 'in', 'the', 'no', 'okay', 'i', 'not', 'do', 'at', 'all', 'has', 'i', 'today', 'my', 'my', 'okay', 'no', 'other', 'no', 'at', 'all', 'i', 'do', 'not', 'react', 'okay', 'please', 'okay', 'and', 'you', 'yes', 'your', 'vomiting', 'any', 'other', 'just', 'me', 'no', 'problem', 'do', 'you', 'out', 'do', 'you', 'doctor', 'oh', 'you', 'other', 'than', 'the', 'just', 'the', 'the', 'okay', 'i', 'think', 'i', 'think', 'your', 'your', 'urine', 'has', 'it', 'my', 'do', 'you', 'have', 'any', 'for', 'and', 'where', 'right', 'to', 'your', 'right', 'to', 'the', 'although', 'which', 'could', 'have', 'what', 'exactly', 'is', 'the', 'because', 'okay', 'so', 'a', 'there', 'is', 'sign', 'any', 'bowel', 'we', 'and', 'of', 'chronic', 'on', 'some', 'you', 'know', 'stooling', 'will', 'is', 'that', 'will', 'okay', 'would', 'check', 'would', 'be', 'the', 'the', 'yes', 'you', 'are', 'fine', 'yeah', 'right', 'doctor']</t>
         </is>
       </c>
       <c r="Z4" t="inlineStr">
         <is>
-          <t xml:space="preserve">      ref_ix  hyp_ix reference hypothesis operation  index_edit_ops
-0          0       0     would      would         =            &lt;NA&gt;
-1          1       1       you        you         =            &lt;NA&gt;
-2          2       2      mind       mind         =            &lt;NA&gt;
-3          3       3        by         by         =            &lt;NA&gt;
-4          4       4  starting   starting         =            &lt;NA&gt;
-...      ...     ...       ...        ...       ...             ...
-1404    1337    1371       you        you         =            &lt;NA&gt;
-1405    1338    1372        so         so         =            &lt;NA&gt;
-1406    1339    1373      much       much         =            &lt;NA&gt;
-1407    1340    1374     thank      thank         =            &lt;NA&gt;
-1408    1341    1375       you        you         =            &lt;NA&gt;
-[1409 rows x 6 columns]</t>
+          <t>['about', 'from', 'still', 'what', 'yes', 'no', 'was', 'the', 'muscle', 'is', 'there', 'any', 'distension', 'distension', 'like', 'swelling', 'swelling', 'yeah', 'was', 'there', 'swelling', 'in', 'your', 'stomach', 'no', 'just', 'abdominal', 'i', 'will', 'describe', 'it', 'as', 'a', 'cramp', 'pain', 'like', 'the', 'feel', 'do', 'you', 'want', 'me', 'to', 'show', 'so', 'that', 'is', 'a', 'kind', 'of', 'pain', 'is', 'it', 'i', 'it', 'here', 'maybe', 'do', 'not', 'know', 'if', 'i', 'do', 'not', 'eat', 'yeah', 'maybe', 'there', 'is', 'you', 'i', 'am', 'not', 'when', 'you', 'it', 'would', 'give', 'out', 'five', 'over', 'have', 'i', 'one', 'that', 'i', 'a', 'however', 'we', 'are', 'going', 'to', 'have', 'to', 'evaluate', 'you', 'and', 'find', 'out', 'do', 'some', 'very', 'serious', 'tests', 'i', 'am', 'check', 'your', 'blood', 'count', 'to', 'make', 'sure', 'there', 'is', 'some', 'infection', 'i', 'do', 'not', 'know', 'to', 'a', 'we', 'to', 'rule']</t>
         </is>
       </c>
       <c r="AA4" t="inlineStr">
         <is>
-          <t>would you mind by starting with what brought you in yeah so over the last week i have just been feeling some symptoms [INS:of] [INS:so] it kind of first started with [INS:just] like [INS:i] [INS:had] [INS:like] a runny nose [INS:and] [INS:then] [INS:so] that was around like five days ago and then it turned into just a lot of congestion like [DEL:around] [DEL:my] nose and [DEL:like] my throat and now over the last two days i have been just feeling so much pressure around my nose [DEL:and] around my jaw so i have been getting a lot of pain there as well [SUB:ok-&gt;okay] [DEL:is] your nose still running yeah i am still getting some discharge and i also feel like i am getting some dripping at the back of my throat too especially when i wake up [INS:okay] [SUB:ok-&gt;um] and [INS:uh] could you describe the [INS:the] discharge is it clear yellow [INS:yellow] greenish [DEL:uh] its fairly clear and sometimes [DEL:like] a bit white but [DEL:like] its not [DEL:like] green or yellow [SUB:ok-&gt;okay] [DEL:uh] and have you felt that its difficult to breathe [DEL:in] through either of your [SUB:nostrils-&gt;nostrilsrils] like its [INS:uh] obstructed yeah so [INS:i] at night sometimes i have to like [INS:um] turn because one side of my nose gets [INS:uh] difficult to breathe from and then it kind of balances [SUB:out-&gt;around] [DEL:on] the other side so [INS:i] [INS:do] [INS:have] [INS:some] [INS:obstruction] [INS:okay] [INS:and] [INS:uh] [INS:have] [INS:you] [INS:had] [INS:any] [INS:changes] [INS:to] [INS:your] [INS:sense] [INS:of] [SUB:yeah-&gt;smell] i do [INS:not] [INS:know] have some obstruction [SUB:ok-&gt;okay] and have you had any changes to your sense of smell yeah so just in the last three days when the congestion got really bad i started losing the ability to smell [SUB:ok-&gt;okay] have you had any changes to your sense of taste no taste is fine [SUB:ok-&gt;okay] and have you had any cough or sore throat uh no no cough or sore throat [INS:okay] [SUB:ok-&gt;um] and the symptoms have gone on for five days have you had a period of time where you got better and then got sick again i did [INS:i] [INS:did] kind of have a runny nose last week as well so probably like eight days ago [INS:and] but [DEL:then] the runny nose [INS:has] [SUB:discontinued-&gt;continued] a little bit but really got worse five days ago but all these other symptoms just happened in the last few days [SUB:ok-&gt;okay] and you have pain [INS:is] [SUB:do-&gt;it] you feel it in your jaw or do you feel it in the [DEL:in] [DEL:the] front of your nose [SUB:yes-&gt;so] i would say mainly over the cheeks it can kind of go near the front of my teeth as well so like i would say like mostly around the cheeks jaws and up to the front of my teeth [SUB:ok-&gt;okay] and do you grind your teeth at all at night or have you had [INS:like] tmj issues before no nothing like that i think its not so [INS:more] [SUB:much-&gt;like] on and around my teeth its more so just [DEL:to] right below my nose above my teeth and just around my cheeks [SUB:ok-&gt;okay] so no pain in your mouth or anything like that no not inside my mouth [SUB:ok-&gt;okay] have you had any fevers or chills [DEL:uhm] i do not think i have had a fever i did feel some chills over the last few days but just very brief episodes [SUB:ok-&gt;okay] and over the last few weeks have you had any weight loss no [SUB:ok-&gt;okay] and [SUB:you-&gt;so] [DEL:said] you did not have a cough or a sore throat but have you had any wheezing no wheezing how about any shortness of breath [SUB:uh-&gt;um] not shortness of breath just sometimes when my nose gets like really congested [INS:its] i [INS:i] just [INS:i] [INS:just] turn into like a mouth breather but that is about it i see [SUB:ok-&gt;okay] and have you had [INS:um] any [INS:uh] chest pain no no chest pain [INS:all] [SUB:alright-&gt;right] and any lightheadedness or feeling dizzy no [SUB:ok-&gt;okay] have you had any nausea or vomiting nope any abdominal pain [SUB:no-&gt;nope] have you had any diarrhea sorry what was that have you had any diarrhea no diarrhea [SUB:ok-&gt;okay] and have you had any urinary problems [DEL:uh] no and have you had any rashes or skin changes no not that i know [INS:of] [INS:okay] [SUB:ok-&gt;and] then how [SUB:about-&gt;um] any muscle aches or joint aches uh [INS:nope] [SUB:no-&gt;okay] [SUB:ok-&gt;um] and [INS:uh] have you [DEL:had] any muscle weakness no and how [SUB:has-&gt;is] your energy been [INS:have] [INS:you] any [INS:had] [INS:any] fatigue [DEL:uhm] its been mainly [SUB:ok-&gt;okay] just maybe sometimes difficult to get to sleep with all the [DEL:all] [DEL:the] congestion but i do not think my [SUB:energy-&gt;energys] [DEL:has] been affected too much no [SUB:ok-&gt;okay] and [DEL:uh] sorry to go back to this i do not think i asked did you notice any discharge from your eyes or any eye redness not discharge but yeah maybe a little bit of redness [SUB:ok-&gt;okay] have your eyes been itchy [DEL:uhm] yeah a little bit i would say they have been a bit itchy [SUB:ok-&gt;okay] [SUB:alright-&gt;all] [SUB:then-&gt;right] do you have any medical conditions that you see a physician for regularly [INS:just] [INS:i] [INS:have] [INS:what] [SUB:uh-&gt;is] [SUB:just-&gt;it] [SUB:uhm-&gt;called] its called [INS:high] [INS:like] dyslipidemia [SUB:ok-&gt;okay] i see and any medications you take for that just like a statin medication [SUB:ok-&gt;okay] do you take any other medications over the counter prescribed no [INS:just] other than that i take multivitamins [SUB:ok-&gt;okay] and do you have any allergies to medications or [INS:maybe] like environmental allergies that might be getting worse [DEL:uh] no not that i know [INS:of] [SUB:ok-&gt;okay] so you do not experience any symptoms like this when the seasons change i do not think so i have had this happen to me [DEL:uh] i would say like once before it happened like two years ago [INS:yeah] it was pretty similar [INS:okay] [INS:and] [INS:did] [SUB:ok-&gt;you] [SUB:uhm-&gt;have] [SUB:and-&gt;any] what was done at that time at that time it kind of just went away on its own it got better [INS:like] i feel its definitely worse this time but at that time i did not even go to the doctor [SUB:it-&gt;i] kind of just went away [SUB:ok-&gt;okay] i see any [INS:reasons] [SUB:recent-&gt;for] hospitalizations no hospitalizations [INS:no] any surgeries nope [INS:all] [SUB:alright-&gt;right] and could you tell me [SUB:where-&gt;whereabouts] [DEL:abouts] you are living currently and who you are living with yeah so i am currently living in an apartment by myself [INS:in] just outside of london [SUB:ok-&gt;okay] and anybody that you have been around who is had any symptoms [DEL:uh] no not that i know of [SUB:ok-&gt;okay] so no sick contacts and have you traveled anywhere out of the city or province no i have tried to stay home besides going to work i just work at the grocery store [INS:um] besides that [DEL:no] nowhere else [SUB:ok-&gt;okay] and [INS:anybody] any of your coworkers have any symptoms or any coworkers [SUB:being-&gt;been] off sick no were pretty careful right now with the pandemic i see yeah [INS:no] that [INS:that] is great [INS:um] [SUB:ok-&gt;okay] and do you smoke cigarettes no i [INS:see] [INS:yeah] [INS:no] [INS:that] [INS:that] [INS:is] [INS:great] [INS:um] [INS:okay] [INS:and] [INS:uh] [INS:do] [INS:you] [INS:smoke] [INS:cigarettes] [INS:no] [INS:uh] [INS:i] quit just a couple [DEL:of] years ago oh that is great [INS:um] [INS:all] [INS:right] its not [INS:yeah] [INS:its] [INS:not] easy to quit so that is awesome [INS:um] and [INS:uh] do you drink alcohol [INS:uh] just [INS:just] [INS:uh] maybe like [INS:uh] red wine a couple of times a week i see [SUB:ok-&gt;okay] and do you use any recreational drugs [SUB:uh-&gt;um] just in a month maybe once or twice i smoke a joint [SUB:ok-&gt;okay] [DEL:uh] and anybody in the family have any lung or heart conditions no not that i know of [INS:all] [SUB:alright-&gt;right] and how about any cancer in the family uh no no [INS:no] cancers [INS:okay] [SUB:ok-&gt;um] i think [SUB:i-&gt;uh] that was everything i wanted to ask about today [INS:um] was there any other symptoms or [INS:um] anything else that [INS:that] you wanted to make sure i knew about today [INS:uh] no i think that is all i [INS:i] just did not know if i needed [INS:i] [INS:needed] any [DEL:like] medications or if i needed to get tested i just wanted to make sure yeah so well certainly check your temperature to see if you have a fever and if you do and its high enough that will increase the chance that you have a bacterial sinusitis and if so with some of your symptoms including the discharge obstruction loss of smell and facial pain that all fits the picture for it and also you [INS:you] [INS:felt] [INS:you] had a period where you felt a little bit better and then worse again so that might require antibiotics but we will [INS:yeah] check your temperature and go from there alright sounds good thank you so much thank you</t>
+          <t>['sadeko', 'miss', 'stooling', 'two', 'the', 'stool', 'it', 'semi', 'form', 'formed', 'stools', 'watery', 'stolen', 'per', 'day', 'stooling', 'my', 'about', 'watery', 'stool', 'mucus', 'there', 'no', 'mucus', 'mucus', 'is', 'ermactually', 'take', 'of', 'child', 'vomited', 'he', 'stool', 'are', 'you', 'about', 'what', 'vomitus', 'content', 'projectile', 'ermwhen', 'it', 'vomited', 'that', 'is', 'all', 'i', 'you', 'okuhm', 'all', 'right', 'know', 'so', 'leaves', 'whatwhat', 'yeah', 'has', 'the', 'pain', 'i', 'feel', 'when', 'the', 'it', 'worse', 'per', 'se', 'will', 'nothing', 'do', 'anything', 'reduce', 'the', 'pain', 'its', 'or', 'known', 'peptic', 'also', 'the', 'only', 'the', 'only', 'ailment', 'i', 'for', 'i', 'am', 'being', 'treated', 'for', 'is', 'asthma', 'i', 'am', 'a', 'known', 'asthmatic', 'and', 'and', 'am', 'on', 'i', 'use', 'inhalers', 'how', 'many', 'exacerbations', 'just', 'properly', 'yeah', 'sometimes', 'to', 'asides', 'yes', 'and', 'live', 'yeah', 'had', 'the', 'no', 'rule', 'at', 'all', 'no', 'ermthank', 'they', 'we', 'and', 'you', 'there', 'which', 'wrong', 'wrong', 'had', 'a', 'food', 'poisoning', 'but', 'however', 'have', 'know', 'if', 'we', 'sedimentation', 'rates', 'then', 'the', 'losing', 'from', 'the', 'throughout', 'abdominal', 'on', 'with', 'it', 'that', 'will', 'all']</t>
         </is>
       </c>
       <c r="AB4" t="inlineStr">
         <is>
-          <t>would you mind by starting with what brought you in yeah so over the last week i have just been feeling some symptoms [INS:of] [INS:so] it kind of first started with [INS:just] like [INS:i] [INS:had] [INS:like] a runny nose [INS:and] [INS:then] [INS:so] that was around like five days ago and then it turned into just a lot of congestion like around my nose and like my throat and now over the last two days i have been just feeling so much pressure around [INS:around] my nose [DEL:and] around my jaw so [SUB:i-&gt;having] [SUB:have-&gt;having] [DEL:been] getting a lot of pain there as well [SUB:ok-&gt;okay] is your nose still running yeah i am still getting some discharge and i also feel like i am getting some dripping at the back of my throat too especially when i wake up [SUB:ok-&gt;okay] and could you describe the discharge is it clear yellow greenish [DEL:uh] its fairly clear and sometimes like a bit white but like its not like green or yellow [SUB:ok-&gt;okay] [DEL:uh] and have you felt that its difficult to breathe in through either of your nostrils like its obstructed yeah so [INS:i] at night sometimes i [INS:i] have to like turn because one side of my nose gets difficult to breathe from and then it kind of balances [SUB:out-&gt;around] [DEL:on] the other side so [DEL:yeah] i do have some obstruction [SUB:ok-&gt;okay] and have you had any changes to your sense of smell yeah so just in the last three days when the congestion got really bad i started losing the ability to smell [SUB:ok-&gt;okay] have you had any changes to your sense of taste no taste is fine [SUB:ok-&gt;okay] and have you had any cough or sore throat [DEL:uh] no no cough or sore throat [SUB:ok-&gt;okay] and the symptoms have gone on for five days have you had a period of time where you got better and then got sick again [INS:again] i did kind of have a runny nose last week as well so probably like eight days ago [INS:and] but [SUB:then-&gt;that] the runny nose [INS:has] [SUB:discontinued-&gt;continued] a little bit but really got worse five days ago but all these other symptoms just happened in the last few days [SUB:ok-&gt;okay] and you have pain [INS:is] [SUB:do-&gt;it] you feel it in your jaw or do you feel it in the in the front of your nose [INS:or] yes i would say mainly over the cheeks it can kind of go near the front of my teeth as well so [DEL:like] i would say like mostly around the cheeks jaws and up to the front of my teeth [SUB:ok-&gt;okay] [DEL:and] do you grind your teeth at all at night or have you had tmj issues before no nothing like that i think its not so [INS:more] [SUB:much-&gt;like] on and around my teeth its more so just [DEL:to] right below my nose above my teeth and just around my cheeks [SUB:ok-&gt;okay] so no pain in your mouth or anything like that no not inside my mouth [SUB:ok-&gt;okay] have you had any fevers or chills [DEL:uhm] i do not think i have had a fever i did feel [INS:feel] some chills over the last few days but just very brief episodes [SUB:ok-&gt;okay] and over the last few weeks have you had any weight loss no [SUB:ok-&gt;okay] and [SUB:you-&gt;so] [DEL:said] you did not have a cough or a sore throat but have you had any wheezing no wheezing how about any shortness of breath [DEL:uh] not shortness of breath just sometimes [SUB:when-&gt;in] my [INS:neck] nose gets like really congested [INS:its] i just [INS:i] [INS:just] turn into like a mouth breather but that is about it i see [SUB:ok-&gt;okay] and have you had any chest pain no no chest pain [INS:all] [SUB:alright-&gt;right] and any lightheadedness or feeling dizzy no [SUB:ok-&gt;okay] have you had any nausea or vomiting nope any abdominal pain no have you had any diarrhea sorry what was that have you had any diarrhea no diarrhea [SUB:ok-&gt;okay] and have you had any urinary problems [DEL:uh] no and have you had any rashes or skin changes no not that i know [INS:of] [INS:okay] [SUB:ok-&gt;and] then how about any muscle aches or joint aches [SUB:uh-&gt;no] no [SUB:ok-&gt;okay] and have you [DEL:had] any muscle weakness no and how [SUB:has-&gt;is] your energy been [INS:have] [INS:you] any fatigue [DEL:uhm] its been mainly [SUB:ok-&gt;okay] just maybe sometimes difficult to get to sleep with all the [DEL:all] [DEL:the] congestion but i do not think my [SUB:energy-&gt;energys] [DEL:has] been affected too much [SUB:no-&gt;okay] [DEL:ok] and [DEL:uh] sorry to go back to this i do not think i asked did you [INS:have] notice any discharge from your eyes or any eye redness not discharge but yeah maybe a little bit of redness [SUB:ok-&gt;okay] have your eyes been itchy [DEL:uhm] yeah a little bit i would say they have been a bit itchy [INS:okay] [SUB:ok-&gt;all] [SUB:alright-&gt;right] then do you have any medical conditions that you see a physician for regularly [INS:just] [INS:a] [INS:i] [INS:have] [INS:what] [SUB:uh-&gt;is] [SUB:just-&gt;it] [SUB:uhm-&gt;called] its [INS:its] called [INS:high] [INS:like] dyslipidemia [SUB:ok-&gt;okay] i see and any medications you take for that just [INS:a] like a statin medication [SUB:ok-&gt;okay] do you take any other medications over the counter [INS:or] prescribed no [INS:just] other than that i take multivitamins [SUB:ok-&gt;okay] and do you have any allergies to medications or [INS:maybe] like environmental allergies that might be getting worse [DEL:uh] no not that i know [INS:of] [SUB:ok-&gt;okay] so you do not experience any symptoms like this when the seasons change i do not [INS:i] [INS:do] [INS:not] think so i have had this happen to me [DEL:uh] i would say like once before it happened like two years ago [INS:yeah] it was pretty similar [INS:okay] [INS:and] [INS:did] [INS:you] [SUB:ok-&gt;have] [SUB:uhm-&gt;any] and what was done at that time at that time it kind of just went away on its own it got better [INS:like] i feel its definitely worse this time but at that time i did not even go to the doctor [SUB:it-&gt;i] kind of just went away [SUB:ok-&gt;okay] i see [INS:and] [INS:have] any [INS:reasons] [SUB:recent-&gt;for] hospitalizations no hospitalizations [INS:and] [INS:no] any surgeries nope alright and could you tell me [SUB:where-&gt;whereabouts] [DEL:abouts] you are living currently and who you are living with yeah so i am currently living in an apartment by myself [INS:and] just outside of london [SUB:ok-&gt;okay] and anybody that you have been around who is had any symptoms [DEL:uh] no not that i know of [SUB:ok-&gt;okay] so no sick contacts and have you traveled anywhere out of the city or province no i have tried to stay home [INS:i] besides going to work i just work at the grocery store besides that [DEL:no] nowhere else [SUB:ok-&gt;okay] and [INS:anybody] any of your coworkers have any symptoms or any coworkers [SUB:being-&gt;been] off sick no were pretty careful right now with the pandemic i see yeah [INS:no] that is great [SUB:ok-&gt;okay] and do you smoke cigarettes no i quit just a couple of years ago oh that is great its not easy to quit so that is awesome and do you drink alcohol just maybe like red wine a couple of times a week i see [SUB:ok-&gt;okay] and do you use any recreational drugs [DEL:uh] just in a month maybe [DEL:once] or twice i smoke a joint [SUB:ok-&gt;okay] [DEL:uh] and anybody in the family have any lung or heart conditions no not that i know of [INS:all] [SUB:alright-&gt;right] and how about any cancer in the family [SUB:uh-&gt;no] no no cancers [SUB:ok-&gt;okay] i think [DEL:i] that was everything [DEL:i] wanted to ask about today was there any other symptoms or anything else that you wanted to make sure i knew about today no i think that is all i just did not know if i needed any [DEL:like] medications or if i needed to get tested i just wanted to make sure yeah so well certainly check your temperature to see if you have a fever and if you do and its high enough that will increase the chance that you have a bacterial sinusitis [INS:with] and if so with some of your symptoms including the discharge obstruction loss of smell and facial pain that all fits the picture for it and also you [INS:you] [INS:felt] [INS:you] had a period where you felt a little bit better and then worse again so that might require antibiotics but we will check your temperature and go from there [INS:all] [SUB:alright-&gt;right] sounds good thank you so much thank you</t>
+          <t>['yeah', 'how', 'may', 'i', 'help', 'you', 'yeah', 'good', 'afternoon', 'have', 'been', 'two', 'are', 'it', 'stools', 'very', 'watery', 'yes', 'okay', 'all', 'right', 'my', 'no', 'mucus', 'a', 'i', 'like', 'ate', 'me', 'what', 'of', 'the', 'vomitus', 'was', 'the', 'all', 'right', 'he', 'he', 'episode', 'of', 'vomiting', 'he', 'here', 'and', 'whatwhat', 'yeah', 'like', 'has', 'like', 'that', 'is', 'the', 'way', 'where', 'just', 'moving', 'to', 'back', 'just', 'the', 'lower', 'part', 'it', 'does', 'not', 'move', 'to', 'your', 'back', 'no', 'no', 'not', 'at', 'all', 'it', 'stays', 'in', 'the', 'what', 'maybe', 'if', 'i', 'i', 'do', 'not', 'eat', 'maybe', 'that', 'reduce', 'the', 'pain', 'it', 'have', 'yes', 'so', 'yeah', 'have', 'also', 'known', 'asthmatic', 'and', 'in', 'the', 'i', 'do', 'not', 'at', 'all', 'has', 'i', 'today', 'is', 'my', 'i', 'feel', 'sometimes', 'my', 'okay', 'no', 'other', 'no', 'at', 'all', 'i', 'do', 'not', 'react', 'okay', 'please', 'no', 'other', 'just', 'me', 'okay', 'do', 'you', 'doctor', 'oh', 'you', 'do', 'other', 'than', 'the', 'just', 'the', 'the', 'okay', 'i', 'think', 'i', 'think', 'your', 'has', 'it', 'my', 'urination', 'is', 'fine', 'do', 'you', 'have', 'any', 'all', 'right', 'no', 'problem', 'your', 'right', 'to', 'i', 'ate', 'right', 'so', 'yeah', 'it', 'looks', 'like', 'you', 'have', 'had', 'a', 'food', 'a', 'there', 'is', 'which', 'could', 'sign', 'of', 'we', 'stooling', 'will', 'is', 'that', 'will', 'okay', 'would', 'be', 'no', 'are', 'fine', 'right']</t>
+        </is>
+      </c>
+      <c r="AC4" t="inlineStr">
+        <is>
+          <t>['number', 'yes', 'the', 'water', 'this', 'is', 'the', 'i', 'i', 'con', 'want', 'to', 'tell', 'this', 'any', 'not', 'would', 'out', 'out', 'of', 'is', 'asthma', 'recently', 'how', 'that', 'vomit', 'i', 'you', 'yes', 'so', 'yeah', 'it', 'diarrhoea', 'a', 'we', 'to', 'rule']</t>
+        </is>
+      </c>
+      <c r="AD4" t="inlineStr">
+        <is>
+          <t>['sadeko', 'stooling', 'i', 'those', 'it', 'in', 'stolen', 'stooling', 'about', 'watery', 'stool', 'the', 'stool', 'ermactually', 'it', 'a', 'of', 'us', 'one', 'he', 'complaints', 'stool', 'ii', 'what', 'content', 'ermwhen', 'it', 'vomited', 'all', 'i', 'you', 'okay', 'distension', 'distension', 'was', 'okuhm', 'all', 'right', 'he', 'he', 'he', 'is', 'know', 'let', 'us', 'you', 'were', 'leaves', 'you', 'will', 'like', 'cramp', 'the', 'part', 'part', 'another', 'like', 'pain', 'if', 'per', 'se', 'will', 'say', 'what', 'what', 'relieves', 'nothing', 'anything', 'its', 'will', 'the', 'or', 'known', 'peptic', 'ailment', 'am', 'being', 'treated', 'am', 'being', 'am', 'a', 'exacerbations', 'is', 'has', 'body', 'asides', 'had', 'vomiting', 'no', 'no', 'at', 'all', 'ermthank', 'they', 'we', 'you', 'diarrhea', 'wrong', 'okay', 'had', 'a', 'very', 'know', 'gastroenteritis', 'rates', 'diarrhea', 'then', 'a', 'stool', 'diarrhea', 'we', 'you', 'have', 'retroviral', 'diarrhea', 'although', 'the', 'from', 'the', 'throughout', 'abdominal', 'diarrhea', 'the', 'you', 'will', 'will', 'be', 'all']</t>
+        </is>
+      </c>
+      <c r="AE4" t="inlineStr">
+        <is>
+          <t>['how', 'may', 'i', 'help', 'you', 'have', 'been', 'the', 'stool', 'solid', 'stools', 'do', 'you', 'my', 'in', 'it', 'a', 'did', 'you', 'out', 'me', 'of', 'the', 'yes', 'ii', 'vomited', 'two', 'what', 'what', 'it', 'just', 'all', 'i', 'the', 'ate', 'ate', 'the', 'same', 'the', 'same', 'food', 'that', 'you', 'he', 'he', 'he', 'got', 'is', 'know', 'like', 'yeah', 'where', 'just', 'the', 'lower', 'part', 'of', 'my', 'like', 'moving', 'to', 'the', 'it', 'does', 'not', 'move', 'to', 'your', 'back', 'at', 'all', 'it', 'stays', 'in', 'okay', 'what', 'well', 'if', 'i', 'eat', 'what', 'what', 'reduce', 'the', 'pain', 'it', 'have', 'yeah', 'do', 'you', 'have', 'also', 'only', 'ailment', 'treated', 'a', 'known', 'asthmatic', 'and', 'and', 'in', 'the', 'has', 'i', 'my', 'my', 'no', 'other', 'no', 'okay', 'please', 'you', 'your', 'the', 'any', 'no', 'problem', 'okay', 'out', 'do', 'you', 'oh', 'you', 'just', 'the', 'the', 'i', 'think', 'i', 'think', 'your', 'your', 'urine', 'has', 'it', 'is', 'fine', 'do', 'do', 'you', 'have', 'any', 'for', 'and', 'where', 'your', 'right', 'to', 'the', 'which', 'could', 'have', 'which', 'could', 'have', 'caused', 'the', 'diarrhea', 'so', 'of', 'if', 'a', 'there', 'is', 'sign', 'any', 'any', 'bowel', 'and', 'of', 'on', 'fluids', 'you', 'know', 'from', 'will', 'is', 'that', 'will', 'okay', 'would', 'would', 'be', 'the', 'the', 'no', 'you', 'are', 'fine', 'yeah', 'so', 'that', 'will', 'be', 'fine']</t>
+        </is>
+      </c>
+      <c r="AF4" t="inlineStr">
+        <is>
+          <t>['number', 'yes', 'no', 'the', 'okay', 'my', 'give', 'over', 'in', 'have', 'it', 'have', 'that', 'that', 'and', 'not', 'at', 'yeah', 'then', 'then', 'a', 'a', 'i', 'to', 'rule']</t>
+        </is>
+      </c>
+      <c r="AG4" t="inlineStr">
+        <is>
+          <t>['sadeko', 'i', 'two', 'the', 'of', 'it', 'semi', 'in', 'well', 'formed', 'watery', 'stolen', 'over', 'the', 'stool', 'there', 'no', 'ermactually', 'it', 'take', 'he', 'stool', 'are', 'you', 'also', 'vomiting', 'about', 'what', 'vomitus', 'ermwhen', 'with', 'vomited', 'that', 'is', 'you', 'okuhm', 'episode', 'he', 'and', 'there', 'were', 'whatwhat', 'has', 'menstruation', 'no', 'not', 'if', 'i', 'do', 'not', 'worse', 'will', 'anything', 'its', 'yes', 'known', 'peptic', 'intolerant', 'the', 'being', 'am', 'being', 'i', 'am', 'on', 'inhalers', 'exacerbations', 'none', 'properly', 'thirsty', 'kind', 'of', 'with', 'two', 'kids', 'and', 'aside', 'had', 'other', 'rule', 'doctor', 'bowel', 'urination', 'ermthank', 'they', 'hydration', 'and', 'to', 'are', 'having', 'restaurants', 'wrong', 'ate', 'had', 'a', 'series', 'know', 'rates', 'bacteria', 'the', 'some', 'electrolytes', 'will', 'throughout', 'abdominal']</t>
+        </is>
+      </c>
+      <c r="AH4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">      ref_ix  hyp_ix  reference hypothesis operation  index_edit_ops
+0          0       0       okay       okay         =            &lt;NA&gt;
+1          1       1       good       good         =            &lt;NA&gt;
+2          2       2  afternoon  afternoon         =            &lt;NA&gt;
+3          3       3         my         my         =            &lt;NA&gt;
+4          4       4       name       name         =            &lt;NA&gt;
+...      ...     ...        ...        ...       ...             ...
+1999    1873    1784      thank      thank         =            &lt;NA&gt;
+2000    1874    1785        you        you         =            &lt;NA&gt;
+2001    1875    1786       very       very         =            &lt;NA&gt;
+2002    1876    1787       much       much         =            &lt;NA&gt;
+2003    1877    &lt;NA&gt;     doctor          _       del             500
+[2004 rows x 6 columns]</t>
+        </is>
+      </c>
+      <c r="AI4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">      ref_ix  hyp_ix  reference hypothesis operation  index_edit_ops
+0          0       0       okay       okay         =            &lt;NA&gt;
+1          1       1       good       good         =            &lt;NA&gt;
+2          2       2  afternoon  afternoon         =            &lt;NA&gt;
+3          3       3         my         my         =            &lt;NA&gt;
+4          4       4       name       name         =            &lt;NA&gt;
+...      ...     ...        ...        ...       ...             ...
+1910    1873    1707      thank      thank         =            &lt;NA&gt;
+1911    1874    1708        you        you         =            &lt;NA&gt;
+1912    1875    1709       very       very         =            &lt;NA&gt;
+1913    1876    1710       much       much         =            &lt;NA&gt;
+1914    1877    1711     doctor     doctor         =            &lt;NA&gt;
+[1915 rows x 6 columns]</t>
+        </is>
+      </c>
+      <c r="AJ4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">      ref_ix  hyp_ix  reference hypothesis operation  index_edit_ops
+0          0       0       okay       okay         =            &lt;NA&gt;
+1          1       1       good       good         =            &lt;NA&gt;
+2          2       2  afternoon  afternoon         =            &lt;NA&gt;
+3          3       3         my         my         =            &lt;NA&gt;
+4          4       4       name       name         =            &lt;NA&gt;
+...      ...     ...        ...        ...       ...             ...
+1898    1873    1703      thank      thank         =            &lt;NA&gt;
+1899    1874    1704        you        you         =            &lt;NA&gt;
+1900    1875    1705       very       very         =            &lt;NA&gt;
+1901    1876    1706       much       much         =            &lt;NA&gt;
+1902    1877    1707     doctor     doctor         =            &lt;NA&gt;
+[1903 rows x 6 columns]</t>
+        </is>
+      </c>
+      <c r="AK4" t="inlineStr">
+        <is>
+          <t>okay good afternoon my name is doctor [SUB:sadeko-&gt;shadepo] [DEL:yeah] good afternoon [DEL:how] [DEL:may] [DEL:i] [DEL:help] [DEL:you] [DEL:yeah] [DEL:good] [DEL:afternoon] my name is [SUB:miss-&gt;ms] sharon yes okay so do you have any complaints yes doctor i have been [SUB:stooling-&gt;schooling] for about [INS:about] four days now and i have been abdominal pain [SUB:two-&gt;too] alongside so [DEL:that] [DEL:is] those are my two complaints okay [DEL:okay] so which one started first the stooling or the abdominal pain [DEL:yeah] the stooling started first about four days ago okay so now like what is the consistency of the of [SUB:the-&gt;this] [SUB:stool-&gt;tool] is [SUB:it-&gt;he] watery is he [SUB:semi-&gt;semisolid] [DEL:solid] or it is [DEL:in] normal [SUB:form-&gt;from] well [INS:from] [SUB:formed-&gt;the] [SUB:stools-&gt;stores] it is very watery very watery very [SUB:watery-&gt;much] yes okay all right so like how many episodes of you said you have been [INS:still] [SUB:stolen-&gt;in] for over four days right yes and how many episodes do you [DEL:do] you have [SUB:per-&gt;for] [SUB:day-&gt;the] of [SUB:stooling-&gt;student] [SUB:my-&gt;anyways] about six [SUB:about-&gt;or] six to seven episodes actually about around that of passage of [INS:what] [SUB:watery-&gt;is] [SUB:stool-&gt;to] yes yes yes [INS:yes] doctor okay okay so is the stool containing [SUB:mucus-&gt;mucous] is it mucoid no no [INS:no] [SUB:there-&gt;it] is [SUB:no-&gt;not] [SUB:mucus-&gt;mucous] no [SUB:mucus-&gt;mucous] in it was there any blood in it no blood at all there [SUB:is-&gt;was] no blood in it okay did [DEL:you] [DEL:change] [DEL:did] [DEL:you] [DEL:eat] [DEL:a] from a new restaurant or did you [DEL:did] [DEL:you] eat something different [SUB:ermactually-&gt;actually] a few days ago [DEL:i] [DEL:like] just before it started i [DEL:actually] had a [SUB:take-&gt;takeout] [DEL:out] in a restaurant with my family which [INS:was] all [SUB:of-&gt;heads] [DEL:us] [DEL:ate] and one of my [SUB:child-&gt;children] actually [SUB:vomited-&gt;vomitedited] but [INS:the] vomiting stopped and [SUB:he-&gt;it] feels good now so it is just me right now with the complaints i have of the of the loose [SUB:stool-&gt;yes] [SUB:are-&gt;i] [SUB:you-&gt;i] [DEL:also] [DEL:vomiting] [DEL:yes] [DEL:ii] vomited about two [DEL:two] episodes [SUB:about-&gt;but] two times yes [SUB:what-&gt;yes] what [DEL:what] [DEL:what] was inside the vomit what was the components of the [SUB:vomitus-&gt;vomit] was it what you ate or was it greenish or was there blood in it no there was no blood it was just the [SUB:content-&gt;contents] of what i ate was the vomiting was it projectile so what do you mean by [SUB:projectile-&gt;projector] [SUB:ermwhen-&gt;when] it comes with force when it comes with force well i really do not know [SUB:it-&gt;i] just i just [SUB:vomited-&gt;wanted] [SUB:that-&gt;to] [SUB:is-&gt;tell] [SUB:all-&gt;so] [SUB:i-&gt;like] i cannot really remember how [SUB:you-&gt;it] came out to be honest okay was there any is there any abdominal distension distension like [DEL:a] swelling swelling yeah was there swelling in your stomach no just the [INS:muscle] [INS:is] [INS:there] [INS:any] abdominal [INS:distension] [INS:distension] [INS:like] [INS:swelling] [INS:swelling] [INS:yeah] [INS:was] [INS:there] [INS:swelling] [INS:in] [INS:your] [INS:stomach] [INS:no] [INS:just] [INS:abdominal] pain the pain is just at [DEL:my] the lower part of my stomach [SUB:okuhm-&gt;okay] [SUB:all-&gt;alright] [SUB:right-&gt;alright] [DEL:all] [DEL:right] thank you so you said your son also ate [DEL:ate] the same [DEL:the] [DEL:same] food that you bought and he is now vomiting how is he feeling now he feels he is okay [DEL:he] after the episode of vomiting he [DEL:he] got [DEL:he] [DEL:got] well and he is okay how is your appetite like my appetite is [DEL:is] here and there [SUB:know-&gt;no] it is not really good like [SUB:so-&gt;before] [DEL:now] [DEL:let] [DEL:us] okay [DEL:okay] so let us talk about [DEL:let] [DEL:us] [DEL:talk] [DEL:about] [DEL:your] the pain you were having so can you describe the pain for me what is the [DEL:what] [DEL:is] [DEL:the] nature of the pain is it a sharp pain or a pain that holds you and [SUB:leaves-&gt;needs] you [SUB:whatwhat-&gt;what] kind of pain is it [INS:i] [INS:will] [INS:describe] [INS:it] [INS:as] [INS:a] [INS:cramp] [INS:pain] [INS:like] [INS:the] [SUB:yeah-&gt;pain] i [INS:feel] [INS:do] [INS:you] [INS:want] [INS:me] [INS:to] [INS:show] [INS:so] [INS:that] [INS:is] [INS:a] [INS:kind] [INS:of] [INS:pain] [INS:is] [INS:it] [INS:i] will describe it like like [SUB:has-&gt;as] a cramp pain like [INS:it] [SUB:the-&gt;is] [SUB:pain-&gt;been] [SUB:i-&gt;a] [SUB:feel-&gt;few] during menstruation so that is the kind of pain like that is the way i can describe it and where [DEL:where] is this pain located in your abdomen the lower part the lower part does this pain does it move to another part of your body [SUB:when-&gt;where] you start feeling it no just [DEL:just] [DEL:the] [DEL:lower] [DEL:part] [DEL:of] [DEL:my] [DEL:like] [DEL:moving] [DEL:to] [DEL:the] back just [SUB:the-&gt;go] [DEL:lower] [DEL:part] [DEL:it] [DEL:does] [DEL:not] [DEL:move] [DEL:to] [DEL:your] back no [DEL:no] [DEL:not] [DEL:at] [DEL:all] it stays in the same space yes yes okay okay so what what do you think makes this pain worse well maybe if i if i do not eat i do not know if i do not eat [INS:here] [INS:maybe] [INS:do] [INS:not] [INS:know] [INS:if] [INS:i] [INS:do] [INS:not] [INS:eat] [INS:yeah] [INS:maybe] something around that yeah but i do not feel like if it just comes and goes i do not feel like [INS:there] [INS:is] anything that makes [INS:you] [SUB:it-&gt;to] [SUB:worse-&gt;want] [SUB:per-&gt;to] [SUB:se-&gt;say] but i [SUB:will-&gt;would] say maybe if i do not eat yes okay what [DEL:what] [DEL:what] relieves the pain [INS:i] [INS:am] [INS:not] [SUB:nothing-&gt;saying] i do not know i [SUB:do-&gt;did] not know [INS:when] [INS:you] [SUB:anything-&gt;said] that [INS:it] [INS:would] [SUB:reduce-&gt;he] [SUB:the-&gt;said] [SUB:pain-&gt;that] it just comes and goes on [SUB:its-&gt;this] one okay so on a scale of zero to ten let us say zero means that you do not have any pain at all and ten is the worst pain you have felt in your life so what would you give this pain i will [INS:give] the pain like five [INS:out] [SUB:or-&gt;of] ten five [INS:five] [INS:over] ten yes no problem so let us [DEL:yeah] take some history [DEL:do] [DEL:you] [DEL:have] are you hypertensive no i am not are you diabetic no i am not [DEL:do] [DEL:you] are you a [SUB:known-&gt;nonpeptic] [SUB:peptic-&gt;because] [SUB:also-&gt;a] patient no [DEL:no] are you lactose intolerant no [SUB:the-&gt;i] [SUB:only-&gt;do] [SUB:the-&gt;not] [SUB:only-&gt;like] [SUB:ailment-&gt;to] [SUB:i-&gt;be] [DEL:am] [DEL:being] treated [SUB:for-&gt;are] [SUB:i-&gt;you] [SUB:am-&gt;a] [SUB:being-&gt;nonpeptic] [SUB:treated-&gt;ulcer] [SUB:for-&gt;patient] [SUB:is-&gt;no] [SUB:asthma-&gt;are] [SUB:i-&gt;you] [SUB:am-&gt;lactose] [SUB:a-&gt;intolerant] [SUB:known-&gt;no] [SUB:asthmatic-&gt;the] [SUB:and-&gt;only] [SUB:and-&gt;ailment] i [INS:have] [SUB:am-&gt;been] [SUB:on-&gt;treated] [SUB:i-&gt;for] [SUB:use-&gt;is] [SUB:inhalers-&gt;asthmatic] and [INS:i] [SUB:how-&gt;use] [SUB:many-&gt;inhalers] how many [SUB:exacerbations-&gt;exhibitions] do you have in a year [DEL:about] [DEL:in] [DEL:the] last one just one okay [INS:one] okay that is good have you had any previous history of blood transfusion any history of surgeries no [DEL:no] none at all [DEL:okay] do you drink alcohol or do you smoke no i do not [DEL:i] do [DEL:not] [DEL:do] any of those i do not [DEL:at] [DEL:all] and since you have been feeling these symptoms that you are having has [DEL:has] it progressively worsened yeah i [DEL:i] feel so so that is why i actually came to the hospital [SUB:just-&gt;yesterday] [DEL:today] to see the doctor and [SUB:properly-&gt;probably] know what is wrong with me and take care of it basically have you been feeling very thirsty have you been feeling like your body is dry has your urine reduced no not at all no no do you feel weak yeah i feel kind of weak yeah [SUB:yeah-&gt;when] [DEL:my] [DEL:my] i feel [SUB:sometimes-&gt;something] my mouth is kind of dry [SUB:to-&gt;too] kind of okay okay [DEL:okay] no problem so do you [SUB:asides-&gt;aside] the asthma do you have any other ailments [INS:that] you think the doctor should know about no not at all at all i have no other [DEL:no] [DEL:other] medical condition do you have any drug allergies no i do not react [DEL:no] [DEL:at] [DEL:all] [DEL:i] [DEL:do] [DEL:not] [DEL:react] to any drugs at all [DEL:okay] [DEL:please] are you married yes i am married with two kids [SUB:yes-&gt;do] [DEL:okay] [DEL:and] you [DEL:you] live with your husband yes [DEL:yes] i do [SUB:and-&gt;are] your kids [SUB:live-&gt;living] with you [SUB:yeah-&gt;yes] what did you say doctor and your kids live with you as well yes they are so aside your [DEL:your] son or your child who [SUB:had-&gt;are] the [SUB:the-&gt;vomitting] [DEL:vomiting] was there any [DEL:any] of your family members that also had the same symptoms no no no no [SUB:no-&gt;dad] [DEL:other] just me [DEL:just] [DEL:me] and my son yes okay [DEL:no] [DEL:problem] okay [DEL:do] [DEL:you] i am just going to ask some questions just to [SUB:rule-&gt;realize] [DEL:out] every other thing do you [DEL:do] [DEL:you] have headaches no [DEL:doctor] do you have chest pain no doctor [INS:i] [SUB:at-&gt;do] [SUB:all-&gt;not] [SUB:no-&gt;know] do you have an abdominal pain [DEL:oh] do you [DEL:you] have an abdominal pain do you have any change in your bowel habits i do not know how to answer that [DEL:other] [DEL:than] [DEL:the] [DEL:just] [DEL:the] [DEL:the] [DEL:okay] i think [DEL:i] [DEL:think] [DEL:i] [DEL:think] that is fine your urine [DEL:your] [DEL:your] [DEL:urine] has it [DEL:has] [DEL:it] changed in quantity no not at all how about the frequency of urination has it changed no no [DEL:my] urination is fine do you have any [DEL:do] [DEL:you] [DEL:have] [DEL:any] bone pain no all right no problem so [SUB:ermthank-&gt;thank] you for [DEL:for] answering my questions those questions are basically there so that we can pinpoint where [DEL:and] [DEL:where] there is a problem and [SUB:they-&gt;you] can also come to have [INS:a] differential diagnosis of what could be the because of your symptoms and [SUB:we-&gt;i] would like to examine you [DEL:right] check your level of hydration check your general physical appearance [DEL:to] see whether you [SUB:and-&gt;can] access your [DEL:your] general health [DEL:right] we also like to do an abdominal examination right to [DEL:to] also give us more information on the abdominal pain you are having if [SUB:you-&gt;it] could lead us to what is causing the symptoms you are having the abdominal pain and the [DEL:the] stooling do you understand yes although [DEL:although] it seems like what you ate the restaurants you got food from [SUB:there-&gt;they] must have been where you got some infection [SUB:which-&gt;it] could have [DEL:which] [DEL:could] [DEL:have] caused the diarrhea you want to say something so what exactly is [SUB:wrong-&gt;drunk] what exactly is [SUB:wrong-&gt;drunk] [DEL:what] [DEL:exactly] [DEL:is] [DEL:the] [DEL:because] [DEL:okay] it is just the food i ate right [DEL:so] yeah it looks like you have had a food poisoning [INS:however] [INS:we] [INS:are] [INS:going] [INS:to] [INS:have] [INS:to] [INS:evaluate] [INS:you] [INS:and] [INS:find] [INS:out] [SUB:had-&gt;what] [SUB:a-&gt;exactly] [SUB:food-&gt;is] [SUB:poisoning-&gt;the] [SUB:but-&gt;because] [SUB:however-&gt;so] we are going to [INS:do] [INS:some] [INS:very] [INS:serious] [INS:tests] [INS:i] [INS:am] [SUB:have-&gt;going] to [INS:check] [INS:your] [INS:blood] [INS:count] [INS:to] [INS:make] [INS:sure] [INS:there] [INS:is] [INS:some] [INS:infection] [INS:i] [INS:do] [INS:not] [INS:know] [INS:to] evaluate you and find out what exactly is the because so we are going to do some very series of tests i am going to check your blood count to [SUB:know-&gt;make] [SUB:if-&gt;this] there is [DEL:a] [DEL:there] [DEL:is] some infection which could be gastroenteritis [SUB:we-&gt;you] want to do your erythrocyte [SUB:sedimentation-&gt;segmentation] [SUB:rates-&gt;rate] to know if there is any [DEL:sign] any [DEL:any] type of kind of inflammatory disorder that could cause diarrhea like inflammatory [DEL:bowel] disease right and [SUB:then-&gt;they] [DEL:we] would also want to do a stool culture microscopy and sensitivity [DEL:and] to look out for parasites and some bacteria that could cause you to be having diarrhea we also check your retroviral status to know if you have [INS:a] retroviral disease which could also be a because of [DEL:of] diarrhea although that comes in [SUB:the-&gt;a] chronic [DEL:chronic] setting however [INS:we] would also need to just rule that out do you understand okay doctor okay however we are going to start you on [DEL:on] some [DEL:some] fluids to [DEL:you] [DEL:know] give you some strength and restore your hydration level because you have been [SUB:losing-&gt;using] some fluid from [SUB:from-&gt;this] [SUB:the-&gt;tooling] [DEL:stooling] and the vomiting we [DEL:will] also check your electrolytes electrolytes to know what [DEL:is] your electrolyte picture looks like and the ones that will be needed to be that will [DEL:that] [DEL:will] need to be corrected do you understand [DEL:okay] and also lastly we [DEL:would] also want to [DEL:check] do an abdominal scan [INS:to] [INS:rule] [SUB:throughout-&gt;out] any structural or functional problems that could be in the [SUB:abdominal-&gt;abdomen] which [DEL:would] [DEL:be] could be causing the diarrhea and the [DEL:the] [DEL:the] abdominal pain do you understand yes thank you doctor thank you very much [DEL:yes] do you have any more questions for me no i am fine i am fine i am good let us just get [SUB:on-&gt;out] [SUB:with-&gt;of] [SUB:it-&gt;here] [DEL:you] [DEL:are] [DEL:fine] [DEL:yeah] so [SUB:that-&gt;i] [SUB:will-&gt;can] be fine thank you so you will be attended to [SUB:all-&gt;alright] [DEL:right] thank you very much [DEL:doctor]</t>
+        </is>
+      </c>
+      <c r="AL4" t="inlineStr">
+        <is>
+          <t>okay good afternoon my name is doctor [SUB:sadeko-&gt;shadekum] [DEL:yeah] good afternoon [DEL:how] [DEL:may] [DEL:i] [DEL:help] [DEL:you] [DEL:yeah] [DEL:good] [DEL:afternoon] my name is miss sharon yes okay so do you have any complaints yes doctor i have been [SUB:stooling-&gt;straining] for about four days now and [SUB:i-&gt;having] [DEL:have] [DEL:been] abdominal pain [DEL:two] alongside so that is [SUB:those-&gt;just] [DEL:are] my two complaints okay okay so which one started first the stooling or the abdominal pain yeah the stooling started first about four days ago okay so now like what is the consistency of the of the stool is [SUB:it-&gt;he] watery is he semi solid or [DEL:it] is [SUB:in-&gt;it] normal form well formed [DEL:stools] it is very watery very watery [DEL:very] [DEL:watery] [DEL:yes] [DEL:okay] [DEL:all] [DEL:right] so like how many episodes of you said you have been [SUB:stolen-&gt;stalling] for over four days right yes and how many episodes do you do you have per day of [SUB:stooling-&gt;stalling] [DEL:my] about six [SUB:about-&gt;or] six to seven episodes actually about around that [INS:number] [INS:yes] of passage of [INS:the] [INS:water] [SUB:watery-&gt;riser] [SUB:stool-&gt;tube] yes yes yes doctor okay okay so is [INS:this] [INS:is] [SUB:the-&gt;it] [SUB:stool-&gt;still] containing mucus is it mucoid no no there is no mucus [DEL:no] [DEL:mucus] in it was there any blood in it no blood at all there is no blood in it okay did you change did you eat [DEL:a] from a new restaurant or did you did you eat something different [SUB:ermactually-&gt;actually] a few days ago [DEL:i] [DEL:like] just before [SUB:it-&gt;you] started i actually had [SUB:a-&gt;the] take out in a restaurant with my family which all [SUB:of-&gt;was] [SUB:us-&gt;it] [DEL:ate] and [SUB:one-&gt;all] of my child actually vomited but [INS:the] vomiting stopped and [SUB:he-&gt;it] feels good now so it is just [DEL:me] right now with the [SUB:complaints-&gt;complaint] i have of the of the loose [SUB:stool-&gt;so] are you also vomiting yes [INS:i] [INS:i] [SUB:ii-&gt;have] vomited about two two episodes about two times yes [SUB:what-&gt;well] what what [DEL:what] was inside the vomit what was the [INS:con] components [DEL:of] [DEL:the] [DEL:vomitus] was it what you ate or was it greenish or was there blood in it no there was no blood it was just the [SUB:content-&gt;contents] of what i ate was the vomiting was it projectile so what do you mean by projectile [SUB:ermwhen-&gt;when] it comes with force when it comes with force well i really do not know [SUB:it-&gt;i] just i just [INS:want] [INS:to] [INS:tell] [SUB:vomited-&gt;you] that is [SUB:all-&gt;the] [SUB:i-&gt;line] i cannot really remember how [SUB:you-&gt;it] came out to be honest [SUB:okay-&gt;is] [DEL:was] there any is there any abdominal [SUB:distension-&gt;distention] [SUB:distension-&gt;distention] like a swelling swelling yeah [SUB:was-&gt;is] there swelling in your stomach no just the abdominal pain the pain is just at my [DEL:the] lower part of my stomach [SUB:okuhm-&gt;okay] [SUB:all-&gt;alright] [SUB:right-&gt;alright] [DEL:all] [DEL:right] thank you so you said your son also ate ate the same the same food that you bought and [DEL:he] is now vomiting how is he feeling now [SUB:he-&gt;it] feels [SUB:he-&gt;it] is okay [DEL:he] after the [DEL:episode] [DEL:of] [DEL:vomiting] he [DEL:he] got he got well and [SUB:he-&gt;it] is okay how is your appetite like my appetite is [SUB:is-&gt;yeah] [DEL:here] [DEL:and] there [SUB:know-&gt;no] it is not really good like so now [INS:this] [SUB:let-&gt;like] [SUB:us-&gt;before] okay okay so let us talk about let us talk about your the pain [SUB:you-&gt;we] [SUB:were-&gt;are] having so can you describe the pain for me what is the what is the nature of the pain is it a sharp pain or a pain that holds you and [SUB:leaves-&gt;needs] [SUB:you-&gt;what] [DEL:whatwhat] kind of pain is it [DEL:yeah] i [SUB:will-&gt;would] describe it [SUB:like-&gt;as] [DEL:like] [DEL:has] a [SUB:cramp-&gt;camp] pain like [SUB:the-&gt;a] pain i feel during menstruation so that is the kind of pain [DEL:like] [DEL:that] [DEL:is] [DEL:the] [DEL:way] i can describe it and where [DEL:where] is this pain located in your abdomen the lower [SUB:part-&gt;parts] the lower [SUB:part-&gt;parts] does this pain does it move to [INS:any] [SUB:another-&gt;other] part of your body when you start feeling it no just [DEL:just] the lower part of my [SUB:like-&gt;abdomen] [DEL:moving] [DEL:to] the [DEL:back] [DEL:just] [DEL:the] [DEL:lower] [DEL:part] [DEL:it] [DEL:does] [DEL:not] [DEL:move] [DEL:to] [DEL:your] [DEL:back] [DEL:no] [DEL:no] [DEL:not] [DEL:at] [DEL:all] [DEL:it] [DEL:stays] [DEL:in] [DEL:the] same space yes yes okay okay so what [DEL:what] do you think makes this [SUB:pain-&gt;play] worse well [DEL:maybe] if i [DEL:if] [DEL:i] do not eat i do not know [SUB:if-&gt;maybe] [DEL:i] [DEL:do] [DEL:not] [DEL:eat] something around that yeah but i do not feel like if it just comes and goes i do not feel like anything that makes it worse [SUB:per-&gt;i] [SUB:se-&gt;say] but i [SUB:will-&gt;was] [SUB:say-&gt;saying] [DEL:maybe] if i do not eat yes okay what [SUB:what-&gt;really] [SUB:what-&gt;how] [SUB:relieves-&gt;is] the pain [INS:not] [SUB:nothing-&gt;saying] i do not know i do not know [SUB:anything-&gt;i] [DEL:that] [DEL:reduce] [DEL:the] [DEL:pain] [DEL:it] just comes and goes on [SUB:its-&gt;this] one okay so on a scale of zero to ten let us say zero means that you do not have any pain at all and ten is the worst pain you [DEL:have] felt in your life so what would you give this pain i [INS:would] [SUB:will-&gt;give] [SUB:the-&gt;this] pain like five [INS:out] [SUB:or-&gt;of] ten five [INS:out] [INS:of] ten [DEL:yes] no problem [DEL:so] let us [DEL:yeah] take some history do you [DEL:have] are you hypertensive no i am not are you diabetic no i am not do you are you a [SUB:known-&gt;nonpeptic] [SUB:peptic-&gt;ulcer] [DEL:also] patient no no are you lactose intolerant no the only the only [SUB:ailment-&gt;payment] i [SUB:am-&gt;will] [SUB:being-&gt;be] [SUB:treated-&gt;treating] for [INS:is] [INS:asthma] i [SUB:am-&gt;have] [SUB:being-&gt;been] treated for is asthma i [SUB:am-&gt;have] [SUB:a-&gt;nonasthmatic] [DEL:known] [DEL:asthmatic] and [DEL:and] i am on i use inhalers and how many [INS:recently] how many [SUB:exacerbations-&gt;exhibitions] do you have in a year [INS:how] about [DEL:in] [DEL:the] last one just one okay okay that [SUB:is-&gt;was] good have you had any previous history of blood transfusion any history of surgeries no no none at all okay do you drink alcohol or do you smoke no i do not i do not do any of those [DEL:i] [DEL:do] [DEL:not] [DEL:at] [DEL:all] and since you have been feeling these symptoms that you are having [SUB:has-&gt;as] [DEL:has] it progressively worsened yeah i [DEL:i] feel so so that is why i actually came to the hospital just [DEL:today] to see the doctor and properly know what is wrong with me and take care of it basically have you been feeling very thirsty have you been feeling like your [SUB:body-&gt;bodys] [DEL:is] dry has your urine reduced no not at all no no do you feel weak yeah i feel kind of weak yeah yeah my [DEL:my] [DEL:i] [DEL:feel] [DEL:sometimes] [DEL:my] mouth is kind of dry to kind of okay okay [DEL:okay] no problem so do you [SUB:asides-&gt;aside] the asthma do you have any other ailments [INS:that] you think the doctor should know about no not at all at all i have no other [DEL:no] [DEL:other] medical condition do you have any drug allergies no i do not react [DEL:no] [DEL:at] [DEL:all] [DEL:i] [DEL:do] [DEL:not] [DEL:react] to any drugs at all [DEL:okay] [DEL:please] are you married yes i am married with two kids yes okay and you you live with your husband yes yes i do and your kids live with you yeah what did you say doctor and your kids live with you as well yes they are so aside your your son or your child who [SUB:had-&gt;are] the the [INS:vomit] [SUB:vomiting-&gt;symptoms] was there any any of your family members that also had the same symptoms no no no [SUB:no-&gt;that] [DEL:no] [DEL:other] just me [DEL:just] [DEL:me] and my son yes [DEL:okay] no problem okay do you i am just going to ask some questions just to rule out every other thing do you [DEL:do] [DEL:you] have headaches no [DEL:doctor] do you have chest pain [INS:i] [SUB:no-&gt;know] doctor [SUB:at-&gt;i] [SUB:all-&gt;thought] no do you have an abdominal pain [DEL:oh] do you [DEL:you] have an abdominal pain [DEL:do] you have any change in your bowel habits i do not know how to answer that [DEL:other] [DEL:than] [DEL:the] [DEL:just] [DEL:the] [DEL:the] [DEL:okay] i think [DEL:i] [DEL:think] [DEL:i] [DEL:think] that is fine your urine your [DEL:your] urine has it [DEL:has] [DEL:it] changed in quantity no not at all how about the frequency of urination has it changed no no [DEL:my] [DEL:urination] [DEL:is] [DEL:fine] do you have any [DEL:do] [DEL:you] [DEL:have] [DEL:any] bone pain no [DEL:all] [DEL:right] [DEL:no] [DEL:problem] so [SUB:ermthank-&gt;thank] you for for answering my questions those questions are basically there so that we can pinpoint where and where there is a problem and [SUB:they-&gt;then] can also come to have differential diagnosis of what could be the because of your symptoms and [SUB:we-&gt;they] would like to examine you right check your level of hydration check your general physical appearance to see whether you [INS:you] and access your [DEL:your] general health [DEL:right] we also like to do an abdominal examination right to [DEL:to] also give us more information on the abdominal pain you are having if [SUB:you-&gt;it] could lead us to what is causing the symptoms you are having the abdominal pain and the the stooling do you understand yes [INS:yes] although although it seems like what you ate the restaurants you got food from there must have been where you got some [INS:so] infection which could have which could have caused the [SUB:diarrhea-&gt;diarrhoea] you want to say something [INS:yeah] so what exactly is [SUB:wrong-&gt;drawn] what exactly is wrong what exactly is the because [INS:it] [SUB:okay-&gt;is] it is just the food [DEL:i] [DEL:ate] [DEL:right] [DEL:so] [DEL:yeah] [DEL:it] [DEL:looks] [DEL:like] [DEL:you] [DEL:have] [DEL:had] [DEL:a] [DEL:food] poisoning [SUB:had-&gt;by] [SUB:a-&gt;the] food poisoning but however we are going to have to evaluate you and find out what exactly is the because so we are going to do some [SUB:very-&gt;really] series of tests i am going to check your blood count to [SUB:know-&gt;see] if there is [DEL:a] [DEL:there] [DEL:is] some infection [DEL:which] [DEL:could] be [SUB:gastroenteritis-&gt;gastritis] we want to do your erythrocyte sedimentation [SUB:rates-&gt;rate] to know if there is any [DEL:sign] any any type [DEL:of] kind of inflammatory disorder that could cause [SUB:diarrhea-&gt;diarrhoea] like inflammatory bowel disease right and [SUB:then-&gt;they] [DEL:we] would also want to do [SUB:a-&gt;is] [SUB:stool-&gt;to] culture microscopy and sensitivity and to look out for parasites and some bacteria that could cause you to be having [SUB:diarrhea-&gt;diarrhoea] [SUB:we-&gt;and] also check your retroviral status to know if [SUB:you-&gt;your] [SUB:have-&gt;abdominal] [SUB:retroviral-&gt;viral] disease which could also be a because of of [INS:diarrhoea] [SUB:diarrhea-&gt;or] [SUB:although-&gt;do] that comes in [SUB:the-&gt;a] chronic [INS:a] chronic setting however [INS:we] would also need to just rule that out do you understand okay doctor okay however we are going to start you on on some some fluids to you know give you some strength and restore your hydration level because you have been losing some fluid from [SUB:from-&gt;this] [SUB:the-&gt;tooling] [DEL:stooling] and the vomiting we [DEL:will] also check your electrolytes electrolytes to know what [DEL:is] your electrolyte picture looks like and the ones that will be needed to be that will [DEL:that] [DEL:will] need to be corrected do you understand [DEL:okay] and also lastly we would also want to check do an abdominal scan [INS:to] [INS:rule] [SUB:throughout-&gt;out] any structural or functional problems that could be in the [SUB:abdominal-&gt;abdomen] which [DEL:would] [DEL:be] could be causing the [SUB:diarrhea-&gt;diarrhoea] and [SUB:the-&gt;then] the the abdominal pain do you understand yes thank you doctor thank you very much yes do you have any more questions for me [DEL:no] i am fine i am fine i am good let us just get on with it [SUB:you-&gt;so] [DEL:are] [DEL:fine] yeah so that [SUB:will-&gt;can] be fine thank you so you [SUB:will-&gt;have] [SUB:be-&gt;been] attended to [SUB:all-&gt;alright] [DEL:right] thank you very much doctor</t>
+        </is>
+      </c>
+      <c r="AM4" t="inlineStr">
+        <is>
+          <t>okay good afternoon my name is doctor [SUB:sadeko-&gt;shadiko] yeah good afternoon [DEL:how] [DEL:may] [DEL:i] [DEL:help] [DEL:you] yeah good afternoon my name is miss sharon yes okay so do you have any complaints yes doctor i have been stooling for about four days now and [SUB:i-&gt;having] [DEL:have] [DEL:been] abdominal pain [SUB:two-&gt;too] alongside so that is those are my two complaints okay okay so which one started first the stooling or the abdominal pain yeah the stooling started first about four days ago okay so now like what is the consistency of [SUB:the-&gt;this] [SUB:of-&gt;tool] [DEL:the] [DEL:stool] is [SUB:it-&gt;he] watery is he [SUB:semi-&gt;semisolid] [DEL:solid] or it is [SUB:in-&gt;a] normal form [SUB:well-&gt;wellformed] [SUB:formed-&gt;stool] [DEL:stools] it is very watery very watery very [SUB:watery-&gt;watchful] yes okay all right so like how many episodes of you said you have been [SUB:stolen-&gt;stooling] for [SUB:over-&gt;about] four days right yes and how many episodes do you [DEL:do] [DEL:you] have per day of stooling [DEL:my] about six about six to seven episodes actually about around that [INS:number] [INS:yes] of passage of watery stool yes yes yes doctor okay okay so is [SUB:the-&gt;this] [SUB:stool-&gt;tool] containing mucus is it mucoid no no [INS:no] [SUB:there-&gt;it] is [SUB:no-&gt;not] mucus no mucus [DEL:in] [DEL:it] was there any blood in it no blood at all there is no blood in it okay did you change did you eat [DEL:a] from a new restaurant or did you [DEL:did] [DEL:you] eat something different [SUB:ermactually-&gt;actually] a few days ago i like just before [SUB:it-&gt;i] started i actually had a [SUB:take-&gt;takeout] [DEL:out] in a restaurant with my family which all of us ate and one of my child actually vomited but [INS:the] vomiting stopped and [SUB:he-&gt;it] feels good now so it is just [DEL:me] right now with the complaints i have of the [DEL:of] [DEL:the] loose [SUB:stool-&gt;yes] [SUB:are-&gt;i] [SUB:you-&gt;have] [SUB:also-&gt;only] [SUB:vomiting-&gt;said] [DEL:yes] [DEL:ii] [DEL:vomited] about two [DEL:two] episodes [SUB:about-&gt;but] two times yes [SUB:what-&gt;well] what [DEL:what] [DEL:what] was inside the vomit what was the components of the [SUB:vomitus-&gt;vomiters] was it what you ate or was it greenish or was there blood in it no there was no blood it was just the content of what i ate was the vomiting was it projectile so what do you mean by projectile [SUB:ermwhen-&gt;when] it comes with force when it comes [SUB:with-&gt;to] force well i really do not know [DEL:it] [DEL:just] i just [SUB:vomited-&gt;wanted] [SUB:that-&gt;to] [SUB:is-&gt;ask] [DEL:all] i [DEL:i] cannot really remember how [SUB:you-&gt;it] came out to be honest okay was there any is there any abdominal distension distension like a swelling swelling yeah was there swelling in your stomach no just the abdominal pain the pain is just at my [DEL:the] lower part of my stomach [SUB:okuhm-&gt;okay] all right all right thank you so you said your son also [DEL:ate] [DEL:ate] [DEL:the] [DEL:same] [DEL:the] [DEL:same] [DEL:food] [DEL:that] [DEL:you] bought and he is now vomiting how is he feeling now he feels he is okay [DEL:he] after the [SUB:episode-&gt;appearance] of vomiting he [DEL:he] got [DEL:he] [DEL:got] well and [SUB:he-&gt;it] is okay [INS:okay] how is your appetite like my appetite is [DEL:is] here [SUB:and-&gt;yeah] [SUB:there-&gt;no] [DEL:know] it is not really good [DEL:like] so now let us okay okay so let us talk about let us talk about your the pain you [SUB:were-&gt;are] having so can you describe the pain for me what is the what is the nature of the pain is it a sharp pain or a pain that holds you and leaves you [SUB:whatwhat-&gt;what] kind of pain is it [DEL:yeah] i will describe it like like [SUB:has-&gt;as] a cramp pain like the pain i feel during [INS:my] [SUB:menstruation-&gt;session] so that is the kind of pain like that is the way i can describe it and where [DEL:where] is this pain located in your abdomen the lower part the lower part does this pain does it move to another part of your body when you start feeling it no just [DEL:just] [DEL:the] [DEL:lower] [DEL:part] [DEL:of] [DEL:my] [DEL:like] [DEL:moving] [DEL:to] [DEL:the] back just the lower part [DEL:it] [DEL:does] [DEL:not] [DEL:move] [DEL:to] [DEL:your] [DEL:back] no [SUB:no-&gt;is] [SUB:not-&gt;this] [DEL:at] [DEL:all] [DEL:it] [DEL:stays] [DEL:in] the same space yes yes okay [DEL:okay] so what [DEL:what] do you think makes this pain worse [DEL:well] maybe if i [DEL:if] [DEL:i] do not eat i do not know [SUB:if-&gt;it] [SUB:i-&gt;is] [SUB:do-&gt;easier] [SUB:not-&gt;maybe] [DEL:eat] something around that yeah but i do not feel like if it just comes and goes i do not feel like anything that makes it [SUB:worse-&gt;well] per se but i [SUB:will-&gt;would] say maybe if i do not eat yes okay what [DEL:what] [DEL:what] relieves the pain nothing i do not know i do not know [SUB:anything-&gt;if] that [DEL:reduce] [DEL:the] [DEL:pain] [DEL:it] just comes and goes on [SUB:its-&gt;this] one okay so on a scale of zero to ten let us say zero means that you do not have any pain at all and ten is the worst pain you [DEL:have] felt in your life so what would you give this pain i will [INS:give] the pain like five or ten five [INS:over] ten [SUB:yes-&gt;okay] no problem so let us [DEL:yeah] take some history [DEL:do] [DEL:you] [DEL:have] are you hypertensive no i am not are you diabetic no i am not do you are you a [SUB:known-&gt;nonpeptic] [SUB:peptic-&gt;ulcer] [DEL:also] patient no no are you lactose [INS:in] [SUB:intolerant-&gt;tolerant] no the only [SUB:the-&gt;aim] [DEL:only] [DEL:ailment] i am [SUB:being-&gt;treating] [DEL:treated] for i [SUB:am-&gt;have] [SUB:being-&gt;been] treated for is asthma [SUB:i-&gt;my] [SUB:am-&gt;nonasmatic] [DEL:a] [DEL:known] [DEL:asthmatic] and [DEL:and] i am [SUB:on-&gt;only] i use [SUB:inhalers-&gt;als] [DEL:and] how many how many [SUB:exacerbations-&gt;examples] do you have in a year about [DEL:in] [DEL:the] last one just one okay okay that is good have you had any previous history of blood transfusion any history of surgeries no no [SUB:none-&gt;not] at all okay do you drink alcohol or do you smoke no i do not i do not do any of those i do not [INS:have] [INS:it] at all and since you have been feeling these symptoms that you are having has [DEL:has] it progressively worsened yeah i [DEL:i] feel so so that is why i actually came to the hospital just today to see the doctor and [SUB:properly-&gt;probably] know what is wrong with me and take care of it basically have you been feeling very [SUB:thirsty-&gt;testy] have you been feeling like your body is dry has your urine reduced no not at all no no do you feel weak yeah i feel kind of weak yeah yeah [DEL:my] [DEL:my] i feel sometimes my mouth is kind of dry to [SUB:kind-&gt;cut] [SUB:of-&gt;up] okay okay okay no problem so do you [INS:have] asides the asthma do you have any other ailments [INS:that] you think the doctor should know about no not at all at all i have no other [DEL:no] [DEL:other] medical condition do you have any drug allergies no i do not react [DEL:no] at all i do not react to any drugs at all [DEL:okay] [DEL:please] are you married yes i am married [SUB:with-&gt;you] [SUB:two-&gt;took] [SUB:kids-&gt;it] yes okay and you [DEL:you] live with your husband yes yes i do and your kids live with you yeah what did you say doctor [SUB:and-&gt;are] your kids live with you as well yes they are so [SUB:aside-&gt;asides] your [DEL:your] son or your child who [SUB:had-&gt;are] the [DEL:the] vomiting was there any [DEL:any] of your family members that also had the same symptoms no no no no no [INS:that] [SUB:other-&gt;is] just me [INS:and] just me and my son yes okay [DEL:no] [DEL:problem] [DEL:okay] do you i am just going to ask some questions just to [SUB:rule-&gt;raise] [DEL:out] every other thing do you [DEL:do] [DEL:you] have headaches no [INS:not] [INS:at] [SUB:doctor-&gt;all] do you have chest pain no doctor at all no do you have an abdominal pain [DEL:oh] do you [DEL:you] have an abdominal pain do you have any change in your [SUB:bowel-&gt;dowel] habits [INS:yeah] i do not know how to answer that other than the [DEL:just] [DEL:the] [DEL:the] okay i think [DEL:i] [DEL:think] [DEL:i] [DEL:think] that is fine your urine [DEL:your] [DEL:your] [DEL:urine] has it [DEL:has] [DEL:it] changed in quantity no not at all how about the frequency of urination has it changed no no my [SUB:urination-&gt;initial] [DEL:is] [DEL:fine] [DEL:do] you have any [DEL:do] [DEL:you] [DEL:have] [DEL:any] bone pain no all right no problem so [SUB:ermthank-&gt;thank] you for [DEL:for] answering my questions those questions are basically there so that we can pinpoint where [DEL:and] [DEL:where] there is a problem and [INS:then] [SUB:they-&gt;we] can also come to have differential diagnosis of what could be the because of your symptoms and [INS:then] we would like to examine you right check your level of [SUB:hydration-&gt;vibration] check your general physical appearance to see whether you [SUB:and-&gt;can] access your [DEL:your] general health [DEL:right] we also like to do an abdominal examination right [SUB:to-&gt;so] [DEL:to] also give us more information on the abdominal pain you are having if you could lead us to what is causing the symptoms you [SUB:are-&gt;have] [SUB:having-&gt;in] the abdominal pain and the [DEL:the] stooling do you understand yes although although it seems like what you ate the [SUB:restaurants-&gt;restaurant] you got food from there must have been where you got some infection [DEL:which] [DEL:could] [DEL:have] [DEL:which] [DEL:could] [DEL:have] [DEL:caused] [DEL:the] [DEL:diarrhea] you want to say something so what exactly is [SUB:wrong-&gt;drug] what exactly is wrong what exactly is the because okay it is just the food i [SUB:ate-&gt;had] right [DEL:so] yeah it looks like you have had a food poisoning [SUB:had-&gt;or] [SUB:a-&gt;the] food poisoning but however we are going to have to evaluate you and find out what exactly is the because so we are going to do some very [SUB:series-&gt;serious] [DEL:of] tests i am going to check your blood count to [SUB:know-&gt;make] [DEL:if] there is [DEL:a] [DEL:there] [DEL:is] some infection which could be [INS:a] gastroenteritis we want to do your erythrocyte sedimentation [SUB:rates-&gt;rate] to know if there is any [DEL:sign] [DEL:any] [DEL:any] type of kind of inflammatory disorder that could cause diarrhea like inflammatory [DEL:bowel] disease right and then we would also want to do a stool culture microscopy and sensitivity [DEL:and] to look out for parasites and some [SUB:bacteria-&gt;bacterias] that could cause you to be having diarrhea we also check your retroviral status to know if you have [INS:a] retroviral disease which could also be a because of [DEL:of] diarrhea although that comes in [SUB:the-&gt;a] chronic chronic setting however [INS:i] would also need to just rule that out do you understand okay doctor okay however we are going to start you on [DEL:on] some [SUB:some-&gt;foods] [DEL:fluids] to [DEL:you] [DEL:know] give you some strength and restore your hydration level because you have been losing some fluid from [DEL:from] the stooling and the vomiting we [DEL:will] also check your [SUB:electrolytes-&gt;electrolyte] electrolytes to know what [DEL:is] your electrolyte picture looks like and the ones that will be needed to be that [SUB:will-&gt;would] [DEL:that] [DEL:will] need to be corrected do you understand [DEL:okay] and also lastly we [DEL:would] also want to check do an abdominal scan [INS:to] [INS:rule] [SUB:throughout-&gt;out] any structural or functional problems that could be in the [SUB:abdominal-&gt;abdomen] which [DEL:would] [DEL:be] could be causing the diarrhea and the [DEL:the] [DEL:the] abdominal pain do you understand yes thank you doctor thank you very much yes do you have any more questions for me [DEL:no] i am fine i am fine i am good let us just get on with it [DEL:you] [DEL:are] [DEL:fine] [DEL:yeah] [DEL:so] [DEL:that] [DEL:will] [DEL:be] [DEL:fine] thank you so you will be attended to all right thank you very much doctor</t>
         </is>
       </c>
     </row>

</xml_diff>